<commit_message>
Added Phase One data to milestones consolidated. THESE ENTRIES HAVE NOT BEEN CHECKED OR CONFIRMED YET.
</commit_message>
<xml_diff>
--- a/milestones-consolidated.xlsx
+++ b/milestones-consolidated.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-1860" yWindow="-16000" windowWidth="25520" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="3660" yWindow="-19280" windowWidth="25520" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="406">
   <si>
     <t>center</t>
   </si>
@@ -832,13 +832,418 @@
   </si>
   <si>
     <t>Use microenvironment microarray (MEMA) based platform to assess the impacts of ~3000 different pairwise combinations of ME perturbagens (MEPs) on 10 biological response endpoints.</t>
+  </si>
+  <si>
+    <t>PHASE ONE DATA</t>
+  </si>
+  <si>
+    <t>Moerke 2 Color Apoptosis</t>
+  </si>
+  <si>
+    <t>Moerke 2 Color Apoptosis: IA-LM, IST-MEL1, NCI-H1648, PC-9 and SK-LMS-1 cells. Dose response of anti-mitotic compounds in human cancer cell lines at 24, 48, and 72 hours to determine their effects on apoptosis.  In this assay, the cell-permeable DNA dye Hoechst 33342 is used to stain the nuclei of all cells.  The fluorescent caspase 3 reporter NucView488 stains the nuclei of cells undergoing apoptosis (in which caspase 3 is active).</t>
+  </si>
+  <si>
+    <t>COLO-800,epithelial-like,,skin,50012;IA-LM,,,lung,50017;IST-MEL1,epithelial-like,,skin,50020;NCI-H1648,,,lung,50032;PC-9,,,lung,50038</t>
+  </si>
+  <si>
+    <t>RO-3306,small molecule,10104-101,LSM-1104;BI-2536,small molecule,10041-101,LSM-1041;MPS-1-IN-1,small molecule,10105-101,LSM-1105;Staurosporine,small molecule,10103-101,LSM-1103;GW843682,small molecule,10014-101,LSM-1014;Tozasertib,small molecule,10021-101,LSM-1021;XMD-12,small molecule,10106-101,LSM-1106;Taxol,small molecule,10102-101,LSM-1102</t>
+  </si>
+  <si>
+    <t>false\small molecules,8</t>
+  </si>
+  <si>
+    <t>http://lincs.hms.harvard.edu/db/datasets/20001/</t>
+  </si>
+  <si>
+    <t>LP1</t>
+  </si>
+  <si>
+    <t>Moerke 3 Color Apoptosis</t>
+  </si>
+  <si>
+    <t>Moerke 3 Color Apoptosis: Dose response of anti-mitotic compounds in human cancer cell lines at 24 and 48 hours to determine their effects on apoptosis and cell death.  In this assay, the cell-permeable DNA dye Hoechst 33342 is used to stain the nuclei of all cells.  The fluorescent caspase 3 reporter NucView488 stains the nuclei of cells undergoing apoptosis (in which caspase 3 is active), and the cell-impermeable DNA dye TO-PRO3 stains only the nuclei of dead or dying cells in which membrane integrity is compromised.</t>
+  </si>
+  <si>
+    <t>5637.0,epithelial,,urinary bladder,50001;BPH-1,epitheloid,,prostate,50005;HUTU-80,epithelial,,intestine,50016;KYSE-140,,,esophagus,50024;KYSE-180,epitheloid,,esophagus,50026;NCI-H810,epithelial,,lung,50037;SK-LMS-1,,,uterus,50042</t>
+  </si>
+  <si>
+    <t>http://lincs.hms.harvard.edu/db/datasets/20002/</t>
+  </si>
+  <si>
+    <t>Tang Mitosis/Apoptosis ver.II -- Data from PMID: 23788527: Differential Determinants of Cancer Cell Insensitivity to Antimitotic Drugs Discriminated by a One-Step Cell Imaging Assay (2013).</t>
+  </si>
+  <si>
+    <t>Tang Mitosis/Apoptosis ver.II: Dose response of anti-mitotic compounds in human cancer cell lines at 24, 48 and 72 hours to determine effect on apoptosis, mitosis and cell death. In screening for small-molecule compounds that are effective at killing cancer cells, one-dimensional readout GI50, which is the EC50 value of growth inhibition, is usually used as the only criterion. A major problem with this one-readout approach is that other useful information is discarded, which could be critical for understanding the action of the compounds. In this screen, we use a single-cell-based imaging assay that can report multi-dimensional physiological responses in cells treated with small molecule kinase inhibitors. The data in this dataset are described in PMID: 23788527: Differential Determinants of Cancer Cell Insensitivity to Antimitotic Drugs Discriminated by a One-Step Cell Imaging Assay (J. Biomolecular Screening, 2013). The image analysis algorithm is available at https://github.com/xietiao/Tang_et_al_LINCS_cell_scoring.</t>
+  </si>
+  <si>
+    <t>5637.0,epithelial,,urinary bladder,50001;647-V,epithelial-like,,urinary bladder,50002;A375.S2,epithelial,,skin,50003;AGS,epithelial,,stomach,50004;Ca Ski,epithelial,,cervix,50006;Ca9-22,epithelial-like,,head &amp; neck,50007;CAL-51,epithelial-like,,breast,50008;Calu-1,epithelial,,lung,50009;Calu-3,epithelial,,lung,50010;COLO-679,fibroblastic,,skin,50011;FU97,epithelial-like,,stomach,50013;HEC-1,,,uterus,50014;HLF,,,liver,50015;Ishikawa,epithelial-like,,uterus,50018;Ishikawa (Heraklio) 02 ER-,epithelial,,uterus,50019;JHH-6,epithelial-like,,liver,50021;KMRC-20,epithelial-like,,kidney,50023;KYSE-140,,,esophagus,50024;KYSE-150,epitheloid,,esophagus,50025;KYSE-450,epitheloid,,esophagus,50027;LNZTA3WT4,,,brain,50028;MDA-MB-435S,melanocyte,,skin,50030;MT-3,epithelial,,breast,50031;NCI-H1651,epithelial,,lung,50033;NCI-H1915,large cell,,lung,50035;NCI-H2023,,,lung,50036;PE/CA-PJ15,epithelial-like,,head &amp; neck,50039;PL4,,,pancreas,50040;SK-OV-3,epithelial,,ovary,50044;SW527,epithelial,,breast,50046;SW620,epithelial,,intestine,50047;T24,epithelial,,urinary bladder,50048;WiDr,epithelial,,intestine,50049</t>
+  </si>
+  <si>
+    <t>33\cell lines</t>
+  </si>
+  <si>
+    <t>BI-2536,small molecule,10041-101,LSM-1041;MLN8054,small molecule,10066-101,LSM-1066;Tozasertib,small molecule,10021-101,LSM-1021;GSK1070916,small molecule,10062-101,LSM-1062;Barasertib,small molecule,10067-101,LSM-1067;KIN001-220,small molecule,10065-101,LSM-1065;MPS-1-IN-1,small molecule,10105-101,LSM-1105;Taxol,small molecule,10102-101,LSM-1102</t>
+  </si>
+  <si>
+    <t>http://lincs.hms.harvard.edu/db/datasets/20003/</t>
+  </si>
+  <si>
+    <t>Tang Proliferation/Mitosis</t>
+  </si>
+  <si>
+    <t>Tang Proliferation/Mitosis: Dose response of anti-mitotic compounds in human cancer cell lines at 24, 48 and 72 hours to determine effect on cell proliferation and mitosis.</t>
+  </si>
+  <si>
+    <t>5637.0,epithelial,,urinary bladder,50001;BPH-1,epitheloid,,prostate,50005;COLO-800,epithelial-like,,skin,50012;HUTU-80,epithelial,,intestine,50016;IA-LM,,,lung,50017;IST-MEL1,epithelial-like,,skin,50020;KATO III,spherical,,stomach,50022;KYSE-140,,,esophagus,50024;KYSE-180,epitheloid,,esophagus,50026;NCI-H1648,,,lung,50032;NCI-H1703,epithelial,,lung,50034;NCI-H810,epithelial,,lung,50037;PC-9,,,lung,50038;SJCRH30,fibroblast,,muscle,50041;SK-LMS-1,,,uterus,50042;SK-MES,epithelial,,lung,50043;SNB75,,,brain,50045</t>
+  </si>
+  <si>
+    <t>17\cell lines</t>
+  </si>
+  <si>
+    <t>http://lincs.hms.harvard.edu/db/datasets/20004/</t>
+  </si>
+  <si>
+    <t>MGH (CMT) Growth Inhibition Assay Protocol (9 compound doses: 10.24 uM to 0.04 uM) -- DNA Staining</t>
+  </si>
+  <si>
+    <t>The CMT platform uses a DNA stain or Resazurin based assay to determine cell viability following compound treatment, as indicated in the formatted assay data. A single cell line is seeded in each 384 well plate and assayed against a panel of compounds. In each 384 well plate, 4 to 8 test compounds are assayed at nine different doses.  In each plate, 42 Control wells are treated with DMSO only (no test compound), and 32 wells contain no cells.  After a 72 hour incubation, the relative cell number in each well is determined using bulk fluorescence measurement (either resazurin or Syto 60). For the Syto 60 assay, cells are fixed before staining.  We report an average FI : Control Ratio for each cell line and compound concentration.  This ratio is calculated by dividing the average FI for each condition by the averaged signal in Control (DMSO treated) wells.  Conditions where more cells are viable have a high ratio; conditions where fewer cells are viable have a lower ratio.- Cell Density at seeding time: variable (~15% confluence) to insure continuous growth during compound treatment.- Doses: 9 concentrations, 2-fold apart. Actual concentrations are provided and may vary among compounds. Concentrations used are based on published literature and pre-screening work done at CMT to estimate potency.- Compound treatment duration: 72h.</t>
+  </si>
+  <si>
+    <t>CAL-51,epithelial-like,,breast,50008;FU97,epithelial-like,,stomach,50013;KMRC-20,epithelial-like,,kidney,50023;MCF7,epithelial,,breast,50029;MDA-MB-435S,melanocyte,,skin,50030;NCI-H1703,epithelial,,lung,50034;PE/CA-PJ15,epithelial-like,,head &amp; neck,50039;SW527,epithelial,,breast,50046;MDA-MB-231,epithelial,,breast,50058;769-P,,,kidney,50072;786-O,,,kidney,50073;A2058,,,skin,50078;A-427,,,lung,50082;A549,,,lung,50084;ACHN,,,kidney,50087;ASH-3,,,thyroid,50089;AsPC-1,,,pancreas,50090;AU565,,,breast,50091;BT-20,,,breast,50105;BT-549,,,breast,50108;BxPC-3,,,pancreas,50109;Caki-1,,,kidney,50118;CAL-120,,,breast,50120;CAL-78,,,bone,50129;CAL-85-1,,,breast,50130;CAMA-1,,,breast,50131;COLO 792,,,skin,50146;COLO 858,,,skin,50149;DAN-G,,,pancreas,50161;DMS 273,,,lung,50167;EBC-1,,,lung,50173;EFM-192B,,,breast,50177;EFM-192C,,,breast,50178;EN,,,uterus,50183;G-292 Clone A141B1,,,bone,50193;G-401,,,kidney,50195;G-402,,,kidney,50196;HCC1143,,,breast,50205;HCC1395,,,breast,50206;HCC1419,,,breast,50207;HCC1428,,,breast,50208;HCC1806,,,breast,50211;HCC1937,,,breast,50212;HCC1954,,,breast,50213;HCC38,,,breast,50216;HCC-56,,,intestine,50218;HCC70,,,breast,50219;HCC-78,,,lung,50220;HDQ-P1,,,breast,50225;HLE,,,liver,50228;HN,,,head &amp; neck,50230;HO-1-u-1,,,head &amp; neck,50232;HPAC,,,pancreas,50234;HPAF-II,,,pancreas,50235;Hs 683,,,brain,50241;Hs 766T,,,pancreas,50243;HSC-4,,,head &amp; neck,50246;HT 1376,,,urinary bladder,50248;HUP-T3,,,pancreas,50260;HUP-T4,,,pancreas,50261;IHH-4,,,thyroid,50265;IM-95,,,stomach,50266;JHH-1,,,liver,50272;JHH-2,,,liver,50273;JHH-4,,,liver,50274;JHH-7,,,liver,50275;JIMT-1,,,breast,50276;KMH-2,,,thyroid,50283;KP-2,,,pancreas,50287;KP-4,,,pancreas,50290;KPL-1,,,breast,50291;LC-1 sq,,,lung,50301;LU99A,,,lung,50319;MB 157,,,breast,50324;MDA-MB-157,,,breast,50328;MDA-MB-175-VII,,,breast,50329;MDA-MB-415,,,breast,50332;MDA-MB-436,,,breast,50333;MDA-MB-453,,,breast,50334;MDA-MB-468,,,breast,50335;MES-SA/Dx-5,,,uterus,50341;MFE-319,,,uterus,50345;ML-1,,,thyroid,50355;NCI-H1568,,,lung,50366;NCI-H1688,,,lung,50371;NCI-H1792,,,lung,50376;NCI-H196,,,lung,50381;NCI-H2110,,,lung,50389;NCI-H2228,,,lung,50397;NCI-H23,,,lung,50400;NCI-H2444,,,lung,50404;NCI-H460,,,lung,50410;NCI-H647,,,lung,50415;NCI-H838,,,lung,50419;NY,,,bone,50426;OSC-20,,,head &amp; neck,50435;Panc 02.03,,,pancreas,50444;Panc 04.03,,,pancreas,50446;Panc 08.13,,,pancreas,50447;Panc 10.05,,,pancreas,50448;PANC-1,,,pancreas,50449;PA-TU-8902,,,pancreas,50450;PA-TU-8988S,,,pancreas,50451;PA-TU-8988T,,,pancreas,50452;PL45,,,pancreas,50456;RT4,,,urinary bladder,50474;SCaBER,,,urinary bladder,50482;SCC-15,,,head &amp; neck,50483;SKN,,,uterus,50503;SNU-182,,,liver,50512;SU.86.86,,,pancreas,50520;SUIT-2,,,pancreas,50521;SW 1271,,,lung,50524;SW 13,,,adrenal gland,50525;SW 1417,,,intestine,50526;SW 156,,,kidney,50528;T47D,,,breast,50541;TOV-112D,,,ovary,50547;UACC-893,,,breast,50557;UMC-11,,,lung,50558;VM-CUB1,,,urinary bladder,50561;VMRC-RCZ,,,kidney,50565;YAPC,,,pancreas,50572;ZR-75-1,,,breast,50574;ZR-75-30,,,breast,50575;HCC1500,epithelial,,breast,50579;CFPAC-1,,,pancreas,50609;ChaGo-K-1,,,lung,50610;KP-1N,,,pancreas,50695;KP-1NL,,,pancreas,50696;NCI-H1563,,,lung,50755;RH-30,,,muscle,50817;SK-MEL-3,,,skin,50834;SW 1990,,,pancreas,50853;BB65-RCC,,,kidney,50892;D-423MG,,,brain,50911;HA7-RCC,,,kidney,50950;LB1047-RCC,,,kidney,50978;LB2241-RCC,,,kidney,50979;LB996-RCC,,,kidney,50985;LXF-289,,,lung,50996;MZ1-PC,,,pancreas,51004;OC-314,,,ovary,51031;OS-RC-2,,,kidney,51035;RCC10RGB,,,kidney,51039;RXF393,,,kidney,51044;SK-MEL-5,,,skin,51051;SK-MG-1,,,brain,51052;TK10,,,kidney,51077;YH-13,,,brain,51080</t>
+  </si>
+  <si>
+    <t>150\cell lines</t>
+  </si>
+  <si>
+    <t>GSK1070916,small molecule,10062-101,LSM-1062</t>
+  </si>
+  <si>
+    <t>http://lincs.hms.harvard.edu/db/datasets/20015/</t>
+  </si>
+  <si>
+    <t>A549 cells -- High-throughput Secretomic Analysis of Single Cells: Data published in Lu, et al. (2013) Analytical Chem. PMID: 23339603</t>
+  </si>
+  <si>
+    <t>This micro-fluidics assay is performed using a microchip developed by Yale LINCS U01 team (http://www.eng.yale.edu/fanlab/Rong_Fan_Group/NIH_LINCS_-_Yale_Tech_U01.html ). This microchip consists of a PDMS microwell array containing &gt;5000 single-cell trapping chambers and a high-density antibody barcode array fabricated by Yale LINCS__ flow patterning method. The assay does not require external fluid handling equipment and can be performed anywhere in a typical cell biology lab.</t>
+  </si>
+  <si>
+    <t>A549,,,lung,50084</t>
+  </si>
+  <si>
+    <t>http://lincs.hms.harvard.edu/db/datasets/20121/</t>
+  </si>
+  <si>
+    <t>Breast cell line dose response to target inhibition measured by high throughput microscopy: Data published in Fallahi-Sichani et al. (2013) Nature Chemical Biology. PMID: 24013279</t>
+  </si>
+  <si>
+    <t>To investigate how a shallow dose-response curve might arise (as seen in data analyzed in Fallahi-Sichani et al. (2013) Nature Chemical Biology. PMID: 24013279), this assay focuses on drugs inhibiting the PI3K/Akt/mTOR pathway that varied widely in Hill slope (HS) and Emax values independent of proliferation rate. For six compounds with varying HS, target inhibition was measured by immunofluorescence microscopy and cell killing in four breast cell lines (HER2-amplified AU565 and HCC1954 cancer cells, hormone receptor-positive T47D cancer cells, and non-transformed MCF10A cells). The effects of the mTOR inhibitor PP242, PI3K inhibitor GSK1059615, dual specificity mTOR/PI3K inhibitor dactolisib (BEZ235), Akt inhibitors MK2206 and triciribine, and also an EGFR inhibitor gefitinib were probed 6 hr and 24 hr after drug exposure in 9-point dose-response assays using antibodies specific for p-ERK (Thr202/Tyr204), p-Akt (Ser473), p-4EBP1 (Thr37/46), and p-S6 (Ser235/236). A shallow dose-response curve is correlated with high cell-to-cell variability in target (p-4EBP1) inhibition by PP242 and dactolisib as compared to drugs for which HS ~ 1 or HS &gt; 1 (in four of four cell lines tested). This dataset refers to data shown in Figure 5 and Supplementary Figures 5, 7, 8 and 9 of the paper.</t>
+  </si>
+  <si>
+    <t>AU565,,,breast,50091;HCC1954,,,breast,50213;MCF 10A,epithelial,,breast,50583;T47D,,,breast,50541</t>
+  </si>
+  <si>
+    <t>Gefitinib,small molecule,10098-101,LSM-1098;PP242 hydrate,small molecule,10345-111,LSM-6357;GSK1059615,small molecule,10172-101,LSM-1173;MK2206,small molecule,10057-102,LSM-1057;Triciribine,small molecule,10280-101,LSM-3810;BEZ235,small molecule,10232-101,LSM-4255</t>
+  </si>
+  <si>
+    <t>false\small molecules,6</t>
+  </si>
+  <si>
+    <t>http://lincs.hms.harvard.edu/db/datasets/20136/</t>
+  </si>
+  <si>
+    <t>MGH (CMT) Growth Inhibition Assay Protocol (3 compound doses) -- DNA Staining</t>
+  </si>
+  <si>
+    <t>The CMT platform uses a DNA stain based assay to determine cell viability following compound treatment.</t>
+  </si>
+  <si>
+    <t>5637.0,epithelial,,urinary bladder,50001;647-V,epithelial-like,,urinary bladder,50002;A375.S2,epithelial,,skin,50003;AGS,epithelial,,stomach,50004;BPH-1,epitheloid,,prostate,50005;Ca Ski,epithelial,,cervix,50006;Ca9-22,epithelial-like,,head &amp; neck,50007;CAL-51,epithelial-like,,breast,50008;Calu-1,epithelial,,lung,50009;Calu-3,epithelial,,lung,50010;COLO-679,fibroblastic,,skin,50011;FU97,epithelial-like,,stomach,50013;HEC-1,,,uterus,50014;HLF,,,liver,50015;Ishikawa,epithelial-like,,uterus,50018;Ishikawa (Heraklio) 02 ER-,epithelial,,uterus,50019;JHH-6,epithelial-like,,liver,50021;KATO III,spherical,,stomach,50022;KMRC-20,epithelial-like,,kidney,50023;KYSE-140,,,esophagus,50024;KYSE-150,epitheloid,,esophagus,50025;KYSE-180,epitheloid,,esophagus,50026;KYSE-450,epitheloid,,esophagus,50027;LNZTA3WT4,,,brain,50028;MCF7,epithelial,,breast,50029;MDA-MB-435S,melanocyte,,skin,50030;MT-3,epithelial,,breast,50031;NCI-H1648,,,lung,50032;NCI-H1651,epithelial,,lung,50033;NCI-H1703,epithelial,,lung,50034;NCI-H1915,large cell,,lung,50035;NCI-H2023,,,lung,50036;NCI-H810,epithelial,,lung,50037;PC-9,,,lung,50038;PE/CA-PJ15,epithelial-like,,head &amp; neck,50039;PL4,,,pancreas,50040;SJCRH30,fibroblast,,muscle,50041;SK-MES,epithelial,,lung,50043;SK-OV-3,epithelial,,ovary,50044;SW527,epithelial,,breast,50046;SW620,epithelial,,intestine,50047;T24,epithelial,,urinary bladder,50048;WiDr,epithelial,,intestine,50049;Hep 3B2.1-7,epithelial,,liver,50051;Hep G2,epithelial,,liver,50052;Huh7,,,liver,50055;SK-BR-3,epithelial,,breast,50057;MDA-MB-231,epithelial,,breast,50058;A-375,epithelial,,skin,50060;HeLa,epithelial,,cervix,50061;1205Lu,,,skin,50062;1321N1,,,brain,50063;143B,,,bone,50064;143B PML BK TK,,,bone,50065;1A6,,,urinary bladder,50066;22RV1,,,prostate,50067;23132/87,,,stomach,50068;42-MG-BA,,,brain,50069;621-101,,,kidney,50070;639-V,,,ureter,50071;769-P,,,kidney,50072;786-O,,,kidney,50073;8305C,,,thyroid,50074;8505C,,,thyroid,50075;A172,,,brain,50076;A-204,,,muscle,50077;A2058,,,skin,50078;A2780,,,ovary,50079;A2780ADR,,,ovary,50080;A373-C6,,,skin,50081;A-427,,,lung,50082;A431,,,skin,50083;A549,,,lung,50084;A673,,,muscle,50085;ABC-1,,,lung,50086;ACHN,,,kidney,50087;AN3CA,,,uterus,50088;ASH-3,,,thyroid,50089;AsPC-1,,,pancreas,50090;AU565,,,breast,50091;AZ-521,,,stomach,50092;B-CPAP,,,thyroid,50093;BE(2)-C,,,nervous system,50094;BEN,,,lung,50095;BeWo,,,miscellaneous,50096;BFTC-905,,,urinary bladder,50097;BFTC-909,,,kidney,50098;BHT-101,,,thyroid,50099;BHY,,,head &amp; neck,50100;BICR 10,,,head &amp; neck,50101;BICR 22,,,head &amp; neck,50102;BICR 31,,,head &amp; neck,50103;BICR 78,,,head &amp; neck,50104;BT-20,,,breast,50105;BT-474,,,breast,50106;BT-483,,,breast,50107;BT-549,,,breast,50108;BxPC-3,,,pancreas,50109;C170,,,intestine,50110;C2BBe1,,,intestine,50111;C32,,,skin,50112;C-33 A,,,cervix,50113;C3A,,,liver,50114;C-4 I,,,cervix,50115;C-4 II,,,cervix,50116;Caco-2,,,intestine,50117;Caki-1,,,kidney,50118;CAL 27,,,head &amp; neck,50119;CAL-120,,,breast,50120;CAL-12T,,,lung,50121;CAL-148,,,breast,50122;CAL-29,,,urinary bladder,50123;CAL-33,,,head &amp; neck,50124;CAL-39,,,vulva,50125;CAL-54,,,kidney,50126;CAL-62,,,thyroid,50127;CAL-72,,,bone,50128;CAL-78,,,bone,50129;CAL-85-1,,,breast,50130;CAMA-1,,,breast,50131;Caov-3,,,ovary,50132;Caov-4,,,ovary,50133;Capan-1,,,pancreas,50134;Capan-2,,,pancreas,50135;CaR-1,,,intestine,50136;CCF-STTG1,,,brain,50137;CCK-81,,,intestine,50138;CHP-212,,,nervous system,50139;CL-40,,,intestine,50140;CoCM-1,,,intestine,50141;COLO 201,,,intestine,50142;COLO 205,,,intestine,50143;COLO 320DM,,,intestine,50144;COLO 741,,,intestine,50145;COLO 792,,,skin,50146;COLO 853,,,skin,50147;COLO 857,,,skin,50148;COLO 858,,,skin,50149;COLO-206F,,,intestine,50150;COLO-320,,,intestine,50151;COLO-678,,,intestine,50152;COLO-680N,,,esophagus,50153;COLO-783,,,skin,50154;COLO-818,,,skin,50155;COLO-824,,,breast,50156;COLO-849,,,skin,50157;COR-L 105,,,lung,50158;COR-L 23/CPR,,,lung,50159;COR-L23,,,lung,50160;DAN-G,,,pancreas,50161;Daoy,,,brain,50162;DBTRG-05MG,,,brain,50163;Detroit 562,,,head &amp; neck,50164;DK-MG,,,brain,50165;DLD-1,,,intestine,50166;DMS 273,,,lung,50167;DMS 53,,,lung,50168;DOK,,,head &amp; neck,50169;DoTc2 4510,,,cervix,50170;DU 145,,,prostate,50171;DV-90,,,lung,50172;EBC-1,,,lung,50173;EFE-184,,,uterus,50174;EFM-19,,,breast,50175;EFM-192A,,,breast,50176;EFM-192B,,,breast,50177;EFM-192C,,,breast,50178;EFO-21,,,ovary,50179;EFO-27,,,ovary,50180;EGI-1,,,biliary tract,50181;EJ138,,,urinary bladder,50182;EN,,,uterus,50183;EPLC-272H,,,lung,50184;ES-2,,,ovary,50185;ESS-1,,,uterus,50186;EVSA-T,,,breast,50187;FaDu,,,head &amp; neck,50188;FLYA13,,,miscellaneous,50189;FTC-133,,,thyroid,50190;FTC-238,,,thyroid,50191;FU-OV-1,,,ovary,50192;G-292 Clone A141B1,,,bone,50193;G-361,,,skin,50194;G-401,,,kidney,50195;G-402,,,kidney,50196;GAMG,,,brain,50197;GCT,,,miscellaneous,50198;GMS-10,,,brain,50199;GOS-3,,,brain,50200;GP5d,,,intestine,50201;H4,,,brain,50202;H69V,,,lung,50203;HARA,,,lung,50204;HCC1143,,,breast,50205;HCC1395,,,breast,50206;HCC1419,,,breast,50207;HCC1428,,,breast,50208;HCC-15,,,lung,50209;HCC1569,,,breast,50210;HCC1806,,,breast,50211;HCC1937,,,breast,50212;HCC1954,,,breast,50213;HCC202,,,breast,50214;HCC-366,,,lung,50215;HCC38,,,breast,50216;HCC-44,,,lung,50217;HCC-56,,,intestine,50218;HCC70,,,breast,50219;HCC-78,,,lung,50220;HCC-827,,,lung,50221;HCT 116,,,intestine,50222;HCT-15,,,intestine,50223;HCT-8,,,intestine,50224;HDQ-P1,,,breast,50225;H-EMC-SS,,,bone,50226;HGC-27,,,stomach,50227;HLE,,,liver,50228;HMVII,,,skin,50229;HN,,,head &amp; neck,50230;HO-1-N-1,,,head &amp; neck,50231;HO-1-u-1,,,head &amp; neck,50232;HOS,,,bone,50233;HPAC,,,pancreas,50234;HPAF-II,,,pancreas,50235;HRT-18,,,intestine,50236;Hs 257.T,,,intestine,50237;Hs 578T,,,breast,50238;Hs 588.T,,,cervix,50239;Hs 633T,,,miscellaneous,50240;Hs 683,,,brain,50241;Hs 746T,,,stomach,50242;Hs 766T,,,pancreas,50243;HSC-2,,,head &amp; neck,50244;HSC-3,,,head &amp; neck,50245;HSC-4,,,head &amp; neck,50246;HT 1080,,,miscellaneous,50247;HT 1376,,,urinary bladder,50248;HT115,,,intestine,50249;HT-1197,,,urinary bladder,50250;HT-29,,,intestine,50251;HT-3,,,cervix,50252;HT55,,,intestine,50253;HTC-C3,,,thyroid,50254;HuCCT1,,,biliary tract,50255;huH-1,,,liver,50256;HuO-3N1,,,bone,50257;HuO9,,,bone,50258;HuO9N2,,,bone,50259;HUP-T3,,,pancreas,50260;HUP-T4,,,pancreas,50261;IGR-1,,,skin,50262;IGR-37,,,skin,50263;IGR-39,,,skin,50264;IHH-4,,,thyroid,50265;IM-95,,,stomach,50266;IM-95m,,,stomach,50267;IMR-32,,,nervous system,50268;IPC-298,,,skin,50269;J82,,,urinary bladder,50270;JAR,,,miscellaneous,50271;JHH-1,,,liver,50272;JHH-2,,,liver,50273;JHH-4,,,liver,50274;JHH-7,,,liver,50275;JIMT-1,,,breast,50276;KELLY,,,nervous system,50277;KG-1-C,,,brain,50278;KHM-3S,,,lung,50279;KHOS/NP,,,bone,50280;KHOS-240S,,,bone,50281;KHOS-312H,,,bone,50282;KMH-2,,,thyroid,50283;KMRC-1,,,kidney,50284;KON,,,head &amp; neck,50285;KOSC-2 cl3-43,,,head &amp; neck,50286;KP-2,,,pancreas,50287;KP-3,,,pancreas,50288;KP-3L,,,pancreas,50289;KP-4,,,pancreas,50290;KPL-1,,,breast,50291;KU-19-19,,,urinary bladder,50292;KYSE-220,,,esophagus,50293;KYSE-270,,,esophagus,50294;KYSE-30,,,esophagus,50295;KYSE-410,,,esophagus,50296;KYSE-50,,,esophagus,50297;KYSE-510,,,esophagus,50298;KYSE-520,,,esophagus,50299;KYSE-70,,,esophagus,50300;LC-1 sq,,,lung,50301;LCLC-103H,,,lung,50302;LCLC-97TM1,,,lung,50303;LK-2,,,lung,50304;LN-18,,,brain,50305;LN-229,,,brain,50306;LN-405,,,brain,50307;LNZTA3WT11,,,brain,50308;LOU-NH91,,,lung,50309;LoVo,,,intestine,50310;LS174T,,,intestine,50311;LS180,,,intestine,50312;Lu-134-A-H,,,lung,50313;Lu-135,,,lung,50314;LU65,,,lung,50315;LU65A,,,lung,50316;LU65B,,,lung,50317;LU65C,,,lung,50318;LU99A,,,lung,50319;LU99B,,,lung,50320;LU99C,,,lung,50321;LUDLU-1,,,lung,50322;M059J,,,brain,50323;MB 157,,,breast,50324;MCAS,,,ovary,50325;MC-IXC,,,nervous system,50326;MDA-MB-134-VI,,,breast,50327;MDA-MB-157,,,breast,50328;MDA-MB-175-VII,,,breast,50329;MDA-MB-330,,,breast,50330;MDA-MB-361,,,breast,50331;MDA-MB-415,,,breast,50332;MDA-MB-436,,,breast,50333;MDA-MB-453,,,breast,50334;MDA-MB-468,,,breast,50335;MDST8,,,intestine,50336;ME-180,,,cervix,50337;MEL-HO,,,skin,50338;MEL-JUSO,,,skin,50339;MES-SA,,,uterus,50340;MES-SA/Dx-5,,,uterus,50341;MEWO,,,skin,50342;MFE-280,,,uterus,50343;MFE-296,,,uterus,50344;MFE-319,,,uterus,50345;MFM-223,,,breast,50346;MG-63,,,bone,50347;MHH-ES-1,,,nervous system,50348;MIA PaCa-2,,,pancreas,50349;MKN1,,,stomach,50350;MKN28,,,stomach,50351;MKN45,,,stomach,50352;MKN7,,,stomach,50353;MKN74,,,stomach,50354;ML-1,,,thyroid,50355;MOG-G-CCM,,,brain,50356;MOG-G-UVW,,,brain,50357;MS751,,,cervix,50358;MSTO-211H,,,pleura,50359;NB69,,,nervous system,50360;NCC-IT-A3,,,testes,50361;NCI-H1048,,,lung,50362;NCI-H1299,,,lung,50363;NCI-H1435,,,lung,50364;NCI-H1437,,,lung,50365;NCI-H1568,,,lung,50366;NCI-H1573,,,lung,50367;NCI-H1581,,,lung,50368;NCI-H1623,,,lung,50369;NCI-H1650,,,lung,50370;NCI-H1688,,,lung,50371;NCI-H1693,,,lung,50372;NCI-H1734,,,lung,50373;NCI-H1755,,,lung,50374;NCI-H1781,,,lung,50375;NCI-H1792,,,lung,50376;NCI-H1793,,,lung,50377;NCI-H1869,,,lung,50378;NCI-H1876,,,lung,50379;NCI-H1944,,,lung,50380;NCI-H196,,,lung,50381;NCI-H1993,,,lung,50382;NCI-H2009,,,lung,50383;NCI-H2029,,,lung,50384;NCI-H2030,,,lung,50385;NCI-H2073,,,lung,50386;NCI-H2085,,,lung,50387;NCI-H2087,,,lung,50388;NCI-H2110,,,lung,50389;NCI-H2122,,,lung,50390;NCI-H2135,,,lung,50391;NCI-H2170,,,lung,50392;NCI-H2172,,,lung,50393;NCI-H2195,,,lung,50394;NCI-H2196,,,lung,50395;NCI-H2198,,,lung,50396;NCI-H2228,,,lung,50397;NCI-H2286,,,lung,50398;NCI-H2291,,,lung,50399;NCI-H23,,,lung,50400;NCI-H2342,,,lung,50401;NCI-H2347,,,lung,50402;NCI-H2405,,,lung,50403;NCI-H2444,,,lung,50404;NCI-H2452,,,lung,50405;NCI-H3122,,,lung,50406;NCI-H322,,,lung,50407;NCI-H358,,,lung,50408;NCI-H441,,,lung,50409;NCI-H460,,,lung,50410;NCI-H520,,,lung,50411;NCI-H522,,,lung,50412;NCI-H596,,,lung,50413;NCI-H630,,,intestine,50414;NCI-H647,,,lung,50415;NCI-H650,,,lung,50416;NCI-H661,,,lung,50417;NCI-H727,,,lung,50418;NCI-H838,,,lung,50419;NCI-H841,,,lung,50420;NCI-N87,,,stomach,50421;NIH:OVCAR-3,,,ovary,50422;NUGC-2,,,stomach,50423;NUGC-3,,,stomach,50424;NUGC-4,,,stomach,50425;NY,,,bone,50426;OAW28,,,ovary,50427;OAW42,,,ovary,50428;OCUG-1,,,gall bladder,50429;OCUM-1,,,stomach,50430;OE19,,,esophagus,50431;OE21,,,esophagus,50432;OE33,,,esophagus,50433;OSC-19,,,head &amp; neck,50434;OSC-20,,,head &amp; neck,50435;OUMS-23,,,intestine,50436;OV-90,,,ovary,50437;OVISE,,,ovary,50438;OVKATE,,,ovary,50439;OVMIU,,,ovary,50440;OVSAYO,,,ovary,50441;OVTOKO,,,ovary,50442;PA-1,,,ovary,50443;Panc 02.03,,,pancreas,50444;Panc 03.27,,,pancreas,50445;Panc 04.03,,,pancreas,50446;Panc 08.13,,,pancreas,50447;Panc 10.05,,,pancreas,50448;PANC-1,,,pancreas,50449;PA-TU-8902,,,pancreas,50450;PA-TU-8988S,,,pancreas,50451;PA-TU-8988T,,,pancreas,50452;PC-14,,,lung,50453;PC-3,,,prostate,50454;PFSK-1,,,brain,50455;PL45,,,pancreas,50456;PLC/PRF/5,,,liver,50457;QGP-1,,,pancreas,50458;RCM-1,,,intestine,50459;RD,,,muscle,50460;RD-ES,,,nervous system,50461;RERF-GC-1B,,,stomach,50462;RERF-LC-Ad1,,,lung,50463;RERF-LC-KJ,,,lung,50464;RERF-LC-MA,,,lung,50465;RERF-LC-Sq1,,,lung,50466;RKN,,,ovary,50467;RMG-I,,,ovary,50468;RO82-W-1,,,thyroid,50469;RPMI 2650,,,head &amp; neck,50470;RPMI-7951,,,skin,50471;RT-112,,,urinary bladder,50472;RT112/84,,,urinary bladder,50473;RT4,,,urinary bladder,50474;RVH-421,,,skin,50475;S-117,,,thyroid,50476;Saos-2,,,bone,50477;SAS,,,head &amp; neck,50478;SAT,,,head &amp; neck,50479;SBC-3,,,lung,50480;SBC-5,,,lung,50481;SCaBER,,,urinary bladder,50482;SCC-15,,,head &amp; neck,50483;SCC-25,,,head &amp; neck,50484;SCC-4,,,head &amp; neck,50485;SCC-9,,,head &amp; neck,50486;SCCH-196,,,miscellaneous,50487;SCCH-26,,,nervous system,50488;SCH,,,stomach,50489;SCLC-21H,,,lung,50490;SHP-77,,,lung,50491;SH-SY5Y,,,nervous system,50492;SiHa,,,cervix,50493;SISO,,,cervix,50494;SK-CO-1,,,intestine,50495;SK-ES-1,,,bone,50496;SKG-IIIa,,,cervix,50497;SKG-IIIb,,,cervix,50498;SK-HEP-1,,,liver,50499;SK-LU-1,,,lung,50500;SK-MEL-2,,,skin,50501;SK-MEL-30,,,skin,50502;SKN,,,uterus,50503;SKN-3,,,head &amp; neck,50504;SK-N-AS,,,nervous system,50505;SK-N-DZ,,,nervous system,50506;SK-NEP-1,,,kidney,50507;SK-N-SH,,,nervous system,50508;SNG-M,,,uterus,50509;SNU-1,,,stomach,50510;SNU-16,,,stomach,50511;SNU-182,,,liver,50512;SNU-387,,,liver,50513;SNU-398,,,liver,50514;SNU-423,,,liver,50515;SNU-449,,,liver,50516;SNU-475,,,liver,50517;SNU-5,,,stomach,50518;STC 1,,,lung,50519;SU.86.86,,,pancreas,50520;SUIT-2,,,pancreas,50521;SW 1088,,,brain,50522;SW 1116,,,intestine,50523;SW 1271,,,lung,50524;SW 13,,,adrenal gland,50525;SW 1417,,,intestine,50526;SW 1463,,,intestine,50527;SW 156,,,kidney,50528;SW 1573,,,lung,50529;SW 1783,,,brain,50530;SW 48,,,intestine,50531;SW 626,,,ovary,50532;SW 780,,,urinary bladder,50533;SW 900,,,lung,50534;SW-1710,,,urinary bladder,50535;SW756,,,cervix,50536;SW837,,,intestine,50537;SW-948,,,intestine,50538;T.T,,,esophagus,50539;T.Tn,,,esophagus,50540;T47D,,,breast,50541;T84,,,intestine,50542;T98G,,,brain,50543;TASK1,,,nervous system,50544;TCCSUP,,,urinary bladder,50545;TGW,,,adrenal gland,50546;TOV-112D,,,ovary,50547;TOV-21G,,,ovary,50548;TT2609-C02,,,thyroid,50549;TYK-nu,,,ovary,50550;U-118 MG,,,brain,50551;U-138 MG,,,brain,50552;U-2 OS,,,bone,50553;U-251 MG,,,brain,50554;U373 MG,,,brain,50555;UACC-812,,,breast,50556;UACC-893,,,breast,50557;UMC-11,,,lung,50558;UM-UC-3,,,urinary bladder,50559;VCaP,,,prostate,50560;VM-CUB1,,,urinary bladder,50561;VMRC-LCP,,,lung,50562;VMRC-MELG,,,skin,50563;VMRC-RCW,,,kidney,50564;VMRC-RCZ,,,kidney,50565;WM 266-4,,,skin,50566;WM-115,,,skin,50567;WM1552C,,,skin,50568;WM278,,,skin,50569;WM35,,,skin,50570;WM793B,,,skin,50571;YAPC,,,pancreas,50572;YKG-1,,,brain,50573;ZR-75-1,,,breast,50574;ZR-75-30,,,breast,50575</t>
+  </si>
+  <si>
+    <t>564\cell lines</t>
+  </si>
+  <si>
+    <t>GSK461364,small molecule,10013-101,LSM-1013;Dasatinib,small molecule,10020-101,LSM-1020;Tozasertib,small molecule,10021-101,LSM-1021;GNF2,small molecule,10022-101,LSM-1022;Imatinib,small molecule,10023-103,LSM-1023;NVP-TAE684,small molecule,10024-101,LSM-1024;CGP60474,small molecule,10025-101,LSM-1025;PD173074,small molecule,10026-101,LSM-1026;Crizotinib,small molecule,10027-101,LSM-1027;Saracatinib,small molecule,10032-101,LSM-1032;WH-4-023,small molecule,10038-101,LSM-5613;WH-4-025,small molecule,10039-101,LSM-5431;BI-2536,small molecule,10041-101,LSM-1041;KIN001-127,small molecule,10043-101,LSM-1043;A443654,small molecule,10045-101,LSM-1045;AZ-628,small molecule,10050-101,LSM-1050;Lapatinib,small molecule,10051-104,LSM-1051;Torin1,small molecule,10079-101,LSM-1079;MG-132,small molecule,10107-101,LSM-1107;Geldanamycin,small molecule,10108-101,LSM-1108;Rapamycin,small molecule,10052-101,LSM-1052;(R)- Roscovitine,small molecule,10001-101,LSM-1001;Sorafenib,small molecule,10008-101,LSM-1008;Erlotinib,small molecule,10097-101,LSM-1097;XMD8-85,small molecule,10093-101,LSM-1093</t>
+  </si>
+  <si>
+    <t>false\small molecules,25</t>
+  </si>
+  <si>
+    <t>http://lincs.hms.harvard.edu/db/datasets/20006/</t>
+  </si>
+  <si>
+    <t>MGH (CMT) Growth Inhibition Assay Protocol (3 compound doses) -- DNA Staining (2nd)</t>
+  </si>
+  <si>
+    <t>5637.0,epithelial,,urinary bladder,50001;647-V,epithelial-like,,urinary bladder,50002;A375.S2,epithelial,,skin,50003;AGS,epithelial,,stomach,50004;BPH-1,epitheloid,,prostate,50005;Ca Ski,epithelial,,cervix,50006;Ca9-22,epithelial-like,,head &amp; neck,50007;CAL-51,epithelial-like,,breast,50008;Calu-1,epithelial,,lung,50009;Calu-3,epithelial,,lung,50010;COLO-679,fibroblastic,,skin,50011;FU97,epithelial-like,,stomach,50013;HEC-1,,,uterus,50014;HLF,,,liver,50015;Ishikawa,epithelial-like,,uterus,50018;Ishikawa (Heraklio) 02 ER-,epithelial,,uterus,50019;JHH-6,epithelial-like,,liver,50021;KMRC-20,epithelial-like,,kidney,50023;KYSE-140,,,esophagus,50024;KYSE-150,epitheloid,,esophagus,50025;KYSE-180,epitheloid,,esophagus,50026;KYSE-450,epitheloid,,esophagus,50027;LNZTA3WT4,,,brain,50028;MCF7,epithelial,,breast,50029;MDA-MB-435S,melanocyte,,skin,50030;MT-3,epithelial,,breast,50031;NCI-H1648,,,lung,50032;NCI-H1651,epithelial,,lung,50033;NCI-H1703,epithelial,,lung,50034;NCI-H1915,large cell,,lung,50035;NCI-H2023,,,lung,50036;NCI-H810,epithelial,,lung,50037;PE/CA-PJ15,epithelial-like,,head &amp; neck,50039;SJCRH30,fibroblast,,muscle,50041;SK-MES,epithelial,,lung,50043;SK-OV-3,epithelial,,ovary,50044;SW527,epithelial,,breast,50046;SW620,epithelial,,intestine,50047;T24,epithelial,,urinary bladder,50048;WiDr,epithelial,,intestine,50049;Hep 3B2.1-7,epithelial,,liver,50051;Hep G2,epithelial,,liver,50052;Huh7,,,liver,50055;SK-BR-3,epithelial,,breast,50057;MDA-MB-231,epithelial,,breast,50058;A-375,epithelial,,skin,50060;HeLa,epithelial,,cervix,50061;1205Lu,,,skin,50062;1321N1,,,brain,50063;143B,,,bone,50064;143B PML BK TK,,,bone,50065;1A6,,,urinary bladder,50066;22RV1,,,prostate,50067;23132/87,,,stomach,50068;42-MG-BA,,,brain,50069;639-V,,,ureter,50071;769-P,,,kidney,50072;786-O,,,kidney,50073;8305C,,,thyroid,50074;8505C,,,thyroid,50075;A172,,,brain,50076;A-204,,,muscle,50077;A2058,,,skin,50078;A2780,,,ovary,50079;A2780ADR,,,ovary,50080;A373-C6,,,skin,50081;A-427,,,lung,50082;A431,,,skin,50083;A549,,,lung,50084;A673,,,muscle,50085;ABC-1,,,lung,50086;ACHN,,,kidney,50087;AN3CA,,,uterus,50088;ASH-3,,,thyroid,50089;AsPC-1,,,pancreas,50090;AU565,,,breast,50091;AZ-521,,,stomach,50092;B-CPAP,,,thyroid,50093;BE(2)-C,,,nervous system,50094;BEN,,,lung,50095;BeWo,,,miscellaneous,50096;BFTC-905,,,urinary bladder,50097;BFTC-909,,,kidney,50098;BHT-101,,,thyroid,50099;BHY,,,head &amp; neck,50100;BICR 10,,,head &amp; neck,50101;BICR 22,,,head &amp; neck,50102;BICR 31,,,head &amp; neck,50103;BICR 78,,,head &amp; neck,50104;BT-20,,,breast,50105;BT-474,,,breast,50106;BT-483,,,breast,50107;BT-549,,,breast,50108;BxPC-3,,,pancreas,50109;C170,,,intestine,50110;C2BBe1,,,intestine,50111;C32,,,skin,50112;C-33 A,,,cervix,50113;C3A,,,liver,50114;C-4 I,,,cervix,50115;C-4 II,,,cervix,50116;Caco-2,,,intestine,50117;Caki-1,,,kidney,50118;CAL 27,,,head &amp; neck,50119;CAL-120,,,breast,50120;CAL-12T,,,lung,50121;CAL-148,,,breast,50122;CAL-29,,,urinary bladder,50123;CAL-33,,,head &amp; neck,50124;CAL-39,,,vulva,50125;CAL-54,,,kidney,50126;CAL-62,,,thyroid,50127;CAL-72,,,bone,50128;CAL-78,,,bone,50129;CAL-85-1,,,breast,50130;CAMA-1,,,breast,50131;Caov-3,,,ovary,50132;Caov-4,,,ovary,50133;Capan-1,,,pancreas,50134;Capan-2,,,pancreas,50135;CaR-1,,,intestine,50136;CCF-STTG1,,,brain,50137;CCK-81,,,intestine,50138;CHP-212,,,nervous system,50139;CL-40,,,intestine,50140;CoCM-1,,,intestine,50141;COLO 201,,,intestine,50142;COLO 205,,,intestine,50143;COLO 320DM,,,intestine,50144;COLO 741,,,intestine,50145;COLO 792,,,skin,50146;COLO 853,,,skin,50147;COLO 857,,,skin,50148;COLO 858,,,skin,50149;COLO-206F,,,intestine,50150;COLO-320,,,intestine,50151;COLO-678,,,intestine,50152;COLO-680N,,,esophagus,50153;COLO-783,,,skin,50154;COLO-818,,,skin,50155;COLO-824,,,breast,50156;COLO-849,,,skin,50157;COR-L 105,,,lung,50158;COR-L 23/CPR,,,lung,50159;COR-L23,,,lung,50160;DAN-G,,,pancreas,50161;Daoy,,,brain,50162;DBTRG-05MG,,,brain,50163;Detroit 562,,,head &amp; neck,50164;DK-MG,,,brain,50165;DLD-1,,,intestine,50166;DMS 273,,,lung,50167;DMS 53,,,lung,50168;DOK,,,head &amp; neck,50169;DoTc2 4510,,,cervix,50170;DU 145,,,prostate,50171;DV-90,,,lung,50172;EBC-1,,,lung,50173;EFE-184,,,uterus,50174;EFM-19,,,breast,50175;EFM-192A,,,breast,50176;EFM-192B,,,breast,50177;EFM-192C,,,breast,50178;EFO-21,,,ovary,50179;EFO-27,,,ovary,50180;EGI-1,,,biliary tract,50181;EJ138,,,urinary bladder,50182;EN,,,uterus,50183;EPLC-272H,,,lung,50184;ESS-1,,,uterus,50186;EVSA-T,,,breast,50187;FaDu,,,head &amp; neck,50188;FLYA13,,,miscellaneous,50189;FTC-133,,,thyroid,50190;FTC-238,,,thyroid,50191;FU-OV-1,,,ovary,50192;G-292 Clone A141B1,,,bone,50193;G-361,,,skin,50194;G-401,,,kidney,50195;G-402,,,kidney,50196;GAMG,,,brain,50197;GCT,,,miscellaneous,50198;GMS-10,,,brain,50199;GOS-3,,,brain,50200;GP5d,,,intestine,50201;H4,,,brain,50202;H69V,,,lung,50203;HARA,,,lung,50204;HCC1143,,,breast,50205;HCC1395,,,breast,50206;HCC1419,,,breast,50207;HCC1428,,,breast,50208;HCC-15,,,lung,50209;HCC1569,,,breast,50210;HCC1806,,,breast,50211;HCC1937,,,breast,50212;HCC1954,,,breast,50213;HCC202,,,breast,50214;HCC-366,,,lung,50215;HCC38,,,breast,50216;HCC-44,,,lung,50217;HCC-56,,,intestine,50218;HCC70,,,breast,50219;HCC-78,,,lung,50220;HCC-827,,,lung,50221;HCT 116,,,intestine,50222;HCT-15,,,intestine,50223;HCT-8,,,intestine,50224;HDQ-P1,,,breast,50225;H-EMC-SS,,,bone,50226;HGC-27,,,stomach,50227;HLE,,,liver,50228;HMVII,,,skin,50229;HN,,,head &amp; neck,50230;HO-1-N-1,,,head &amp; neck,50231;HO-1-u-1,,,head &amp; neck,50232;HOS,,,bone,50233;HPAC,,,pancreas,50234;HPAF-II,,,pancreas,50235;HRT-18,,,intestine,50236;Hs 257.T,,,intestine,50237;Hs 578T,,,breast,50238;Hs 588.T,,,cervix,50239;Hs 633T,,,miscellaneous,50240;Hs 683,,,brain,50241;Hs 746T,,,stomach,50242;Hs 766T,,,pancreas,50243;HSC-2,,,head &amp; neck,50244;HSC-3,,,head &amp; neck,50245;HSC-4,,,head &amp; neck,50246;HT 1080,,,miscellaneous,50247;HT 1376,,,urinary bladder,50248;HT115,,,intestine,50249;HT-1197,,,urinary bladder,50250;HT-29,,,intestine,50251;HT-3,,,cervix,50252;HT55,,,intestine,50253;HTC-C3,,,thyroid,50254;HuCCT1,,,biliary tract,50255;huH-1,,,liver,50256;HuO-3N1,,,bone,50257;HuO9,,,bone,50258;HuO9N2,,,bone,50259;HUP-T3,,,pancreas,50260;HUP-T4,,,pancreas,50261;IGR-1,,,skin,50262;IGR-37,,,skin,50263;IGR-39,,,skin,50264;IHH-4,,,thyroid,50265;IM-95,,,stomach,50266;IM-95m,,,stomach,50267;IPC-298,,,skin,50269;J82,,,urinary bladder,50270;JAR,,,miscellaneous,50271;JHH-1,,,liver,50272;JHH-2,,,liver,50273;JHH-4,,,liver,50274;JHH-7,,,liver,50275;JIMT-1,,,breast,50276;KELLY,,,nervous system,50277;KG-1-C,,,brain,50278;KHM-3S,,,lung,50279;KHOS/NP,,,bone,50280;KHOS-240S,,,bone,50281;KHOS-312H,,,bone,50282;KMH-2,,,thyroid,50283;KMRC-1,,,kidney,50284;KON,,,head &amp; neck,50285;KOSC-2 cl3-43,,,head &amp; neck,50286;KP-2,,,pancreas,50287;KP-3,,,pancreas,50288;KP-3L,,,pancreas,50289;KP-4,,,pancreas,50290;KPL-1,,,breast,50291;KU-19-19,,,urinary bladder,50292;KYSE-220,,,esophagus,50293;KYSE-270,,,esophagus,50294;KYSE-30,,,esophagus,50295;KYSE-410,,,esophagus,50296;KYSE-50,,,esophagus,50297;KYSE-510,,,esophagus,50298;KYSE-520,,,esophagus,50299;KYSE-70,,,esophagus,50300;LC-1 sq,,,lung,50301;LCLC-103H,,,lung,50302;LCLC-97TM1,,,lung,50303;LK-2,,,lung,50304;LN-18,,,brain,50305;LN-229,,,brain,50306;LN-405,,,brain,50307;LNZTA3WT11,,,brain,50308;LOU-NH91,,,lung,50309;LoVo,,,intestine,50310;LS174T,,,intestine,50311;LS180,,,intestine,50312;Lu-134-A-H,,,lung,50313;Lu-135,,,lung,50314;LU65A,,,lung,50316;LU65B,,,lung,50317;LU65C,,,lung,50318;LU99A,,,lung,50319;LU99B,,,lung,50320;LU99C,,,lung,50321;LUDLU-1,,,lung,50322;M059J,,,brain,50323;MB 157,,,breast,50324;MCAS,,,ovary,50325;MC-IXC,,,nervous system,50326;MDA-MB-157,,,breast,50328;MDA-MB-175-VII,,,breast,50329;MDA-MB-330,,,breast,50330;MDA-MB-361,,,breast,50331;MDA-MB-415,,,breast,50332;MDA-MB-436,,,breast,50333;MDA-MB-453,,,breast,50334;MDA-MB-468,,,breast,50335;MDST8,,,intestine,50336;ME-180,,,cervix,50337;MEL-HO,,,skin,50338;MEL-JUSO,,,skin,50339;MES-SA,,,uterus,50340;MES-SA/Dx-5,,,uterus,50341;MEWO,,,skin,50342;MFE-280,,,uterus,50343;MFE-296,,,uterus,50344;MFE-319,,,uterus,50345;MFM-223,,,breast,50346;MG-63,,,bone,50347;MHH-ES-1,,,nervous system,50348;MIA PaCa-2,,,pancreas,50349;MKN1,,,stomach,50350;MKN28,,,stomach,50351;MKN45,,,stomach,50352;MKN7,,,stomach,50353;MKN74,,,stomach,50354;ML-1,,,thyroid,50355;MOG-G-CCM,,,brain,50356;MOG-G-UVW,,,brain,50357;MS751,,,cervix,50358;MSTO-211H,,,pleura,50359;NB69,,,nervous system,50360;NCC-IT-A3,,,testes,50361;NCI-H1048,,,lung,50362;NCI-H1299,,,lung,50363;NCI-H1435,,,lung,50364;NCI-H1437,,,lung,50365;NCI-H1568,,,lung,50366;NCI-H1573,,,lung,50367;NCI-H1581,,,lung,50368;NCI-H1623,,,lung,50369;NCI-H1650,,,lung,50370;NCI-H1688,,,lung,50371;NCI-H1693,,,lung,50372;NCI-H1734,,,lung,50373;NCI-H1755,,,lung,50374;NCI-H1781,,,lung,50375;NCI-H1792,,,lung,50376;NCI-H1793,,,lung,50377;NCI-H1869,,,lung,50378;NCI-H1944,,,lung,50380;NCI-H196,,,lung,50381;NCI-H1993,,,lung,50382;NCI-H2009,,,lung,50383;NCI-H2029,,,lung,50384;NCI-H2030,,,lung,50385;NCI-H2073,,,lung,50386;NCI-H2085,,,lung,50387;NCI-H2087,,,lung,50388;NCI-H2110,,,lung,50389;NCI-H2122,,,lung,50390;NCI-H2135,,,lung,50391;NCI-H2170,,,lung,50392;NCI-H2172,,,lung,50393;NCI-H2195,,,lung,50394;NCI-H2196,,,lung,50395;NCI-H2228,,,lung,50397;NCI-H2286,,,lung,50398;NCI-H2291,,,lung,50399;NCI-H23,,,lung,50400;NCI-H2342,,,lung,50401;NCI-H2347,,,lung,50402;NCI-H2405,,,lung,50403;NCI-H2444,,,lung,50404;NCI-H2452,,,lung,50405;NCI-H322,,,lung,50407;NCI-H358,,,lung,50408;NCI-H441,,,lung,50409;NCI-H460,,,lung,50410;NCI-H520,,,lung,50411;NCI-H522,,,lung,50412;NCI-H596,,,lung,50413;NCI-H630,,,intestine,50414;NCI-H647,,,lung,50415;NCI-H650,,,lung,50416;NCI-H661,,,lung,50417;NCI-H727,,,lung,50418;NCI-H838,,,lung,50419;NCI-H841,,,lung,50420;NCI-N87,,,stomach,50421;NIH:OVCAR-3,,,ovary,50422;NUGC-2,,,stomach,50423;NUGC-3,,,stomach,50424;NUGC-4,,,stomach,50425;NY,,,bone,50426;OAW28,,,ovary,50427;OAW42,,,ovary,50428;OCUG-1,,,gall bladder,50429;OCUM-1,,,stomach,50430;OE19,,,esophagus,50431;OE21,,,esophagus,50432;OE33,,,esophagus,50433;OSC-19,,,head &amp; neck,50434;OSC-20,,,head &amp; neck,50435;OUMS-23,,,intestine,50436;OV-90,,,ovary,50437;OVISE,,,ovary,50438;OVKATE,,,ovary,50439;OVMIU,,,ovary,50440;OVSAYO,,,ovary,50441;OVTOKO,,,ovary,50442;PA-1,,,ovary,50443;Panc 02.03,,,pancreas,50444;Panc 03.27,,,pancreas,50445;Panc 04.03,,,pancreas,50446;Panc 08.13,,,pancreas,50447;Panc 10.05,,,pancreas,50448;PANC-1,,,pancreas,50449;PA-TU-8902,,,pancreas,50450;PA-TU-8988S,,,pancreas,50451;PA-TU-8988T,,,pancreas,50452;PC-14,,,lung,50453;PC-3,,,prostate,50454;PFSK-1,,,brain,50455;PL45,,,pancreas,50456;PLC/PRF/5,,,liver,50457;QGP-1,,,pancreas,50458;RCM-1,,,intestine,50459;RD,,,muscle,50460;RERF-GC-1B,,,stomach,50462;RERF-LC-Ad1,,,lung,50463;RERF-LC-KJ,,,lung,50464;RERF-LC-MA,,,lung,50465;RERF-LC-Sq1,,,lung,50466;RKN,,,ovary,50467;RMG-I,,,ovary,50468;RO82-W-1,,,thyroid,50469;RPMI 2650,,,head &amp; neck,50470;RPMI-7951,,,skin,50471;RT-112,,,urinary bladder,50472;RT112/84,,,urinary bladder,50473;RT4,,,urinary bladder,50474;RVH-421,,,skin,50475;S-117,,,thyroid,50476;Saos-2,,,bone,50477;SAS,,,head &amp; neck,50478;SAT,,,head &amp; neck,50479;SBC-3,,,lung,50480;SBC-5,,,lung,50481;SCaBER,,,urinary bladder,50482;SCC-25,,,head &amp; neck,50484;SCC-4,,,head &amp; neck,50485;SCC-9,,,head &amp; neck,50486;SCCH-196,,,miscellaneous,50487;SCCH-26,,,nervous system,50488;SCH,,,stomach,50489;SCLC-21H,,,lung,50490;SHP-77,,,lung,50491;SH-SY5Y,,,nervous system,50492;SiHa,,,cervix,50493;SISO,,,cervix,50494;SK-CO-1,,,intestine,50495;SK-ES-1,,,bone,50496;SKG-IIIa,,,cervix,50497;SKG-IIIb,,,cervix,50498;SK-HEP-1,,,liver,50499;SK-LU-1,,,lung,50500;SK-MEL-2,,,skin,50501;SK-MEL-30,,,skin,50502;SKN,,,uterus,50503;SKN-3,,,head &amp; neck,50504;SK-N-AS,,,nervous system,50505;SK-N-DZ,,,nervous system,50506;SK-NEP-1,,,kidney,50507;SK-N-SH,,,nervous system,50508;SNG-M,,,uterus,50509;SNU-1,,,stomach,50510;SNU-16,,,stomach,50511;SNU-182,,,liver,50512;SNU-387,,,liver,50513;SNU-398,,,liver,50514;SNU-423,,,liver,50515;SNU-449,,,liver,50516;SNU-475,,,liver,50517;SNU-5,,,stomach,50518;STC 1,,,lung,50519;SU.86.86,,,pancreas,50520;SUIT-2,,,pancreas,50521;SW 1088,,,brain,50522;SW 1116,,,intestine,50523;SW 1271,,,lung,50524;SW 13,,,adrenal gland,50525;SW 1417,,,intestine,50526;SW 1463,,,intestine,50527;SW 156,,,kidney,50528;SW 1573,,,lung,50529;SW 1783,,,brain,50530;SW 48,,,intestine,50531;SW 626,,,ovary,50532;SW 780,,,urinary bladder,50533;SW 900,,,lung,50534;SW-1710,,,urinary bladder,50535;SW756,,,cervix,50536;SW837,,,intestine,50537;SW-948,,,intestine,50538;T.T,,,esophagus,50539;T.Tn,,,esophagus,50540;T47D,,,breast,50541;T84,,,intestine,50542;T98G,,,brain,50543;TASK1,,,nervous system,50544;TCCSUP,,,urinary bladder,50545;TGW,,,adrenal gland,50546;TOV-112D,,,ovary,50547;TOV-21G,,,ovary,50548;TT2609-C02,,,thyroid,50549;TYK-nu,,,ovary,50550;U-118 MG,,,brain,50551;U-138 MG,,,brain,50552;U-2 OS,,,bone,50553;U-251 MG,,,brain,50554;U373 MG,,,brain,50555;UACC-812,,,breast,50556;UACC-893,,,breast,50557;UMC-11,,,lung,50558;UM-UC-3,,,urinary bladder,50559;VCaP,,,prostate,50560;VM-CUB1,,,urinary bladder,50561;VMRC-LCP,,,lung,50562;VMRC-MELG,,,skin,50563;VMRC-RCW,,,kidney,50564;VMRC-RCZ,,,kidney,50565;WM 266-4,,,skin,50566;WM-115,,,skin,50567;WM1552C,,,skin,50568;WM278,,,skin,50569;WM35,,,skin,50570;WM793B,,,skin,50571;YAPC,,,pancreas,50572;YKG-1,,,brain,50573;ZR-75-1,,,breast,50574;ZR-75-30,,,breast,50575;LU65,,,lung,50315;RD-ES,,,nervous system,50461;SCC-15,,,head &amp; neck,50483;ES-2,,,ovary,50185;IMR-32,,,nervous system,50268;MDA-MB-134-VI,,,breast,50327;NCI-H1876,,,lung,50379;NCI-H2198,,,lung,50396</t>
+  </si>
+  <si>
+    <t>559\cell lines</t>
+  </si>
+  <si>
+    <t>Neratinib,small molecule,10018-101,LSM-1018;Taxol,small molecule,10102-101,LSM-1102;PHA-665752,small molecule,10125-101,LSM-1125;Sunitinib,small molecule,10175-101,LSM-1176;Y-27632,small molecule,10176-101,LSM-1177;BMS-536924, KIN001-126,small molecule,10209-101,LSM-1210;Go 6976,small molecule,10210-101,LSM-1211;Go-6983,small molecule,10211-101,LSM-1212;KIN001-021/CGP082996,small molecule,10212-101,LSM-1213;KIN001-111/A770041,small molecule,10213-101,LSM-1214;KIN001-123/WZ-1-84,small molecule,10214-101,LSM-1215;KIN001-135,small molecule,10215-101,LSM-1216;KN-93,small molecule,10216-101,LSM-1217;S-Trityl-L-cysteine,small molecule,10217-101,LSM-1218;SU6656,small molecule,10218-101,LSM-1219;U-0126,small molecule,10219-101,LSM-1220</t>
+  </si>
+  <si>
+    <t>false\small molecules,16</t>
+  </si>
+  <si>
+    <t>http://lincs.hms.harvard.edu/db/datasets/20007/</t>
+  </si>
+  <si>
+    <t>MGH (CMT) Growth Inhibition Assay Protocol (9 compound doses: 8 uM to 0.03125 uM) -- DNA Staining</t>
+  </si>
+  <si>
+    <t>5637.0,epithelial,,urinary bladder,50001;647-V,epithelial-like,,urinary bladder,50002;A375.S2,epithelial,,skin,50003;AGS,epithelial,,stomach,50004;BPH-1,epitheloid,,prostate,50005;Ca Ski,epithelial,,cervix,50006;Ca9-22,epithelial-like,,head &amp; neck,50007;CAL-51,epithelial-like,,breast,50008;Calu-1,epithelial,,lung,50009;Calu-3,epithelial,,lung,50010;COLO-679,fibroblastic,,skin,50011;COLO-800,epithelial-like,,skin,50012;FU97,epithelial-like,,stomach,50013;HEC-1,,,uterus,50014;HLF,,,liver,50015;HUTU-80,epithelial,,intestine,50016;IA-LM,,,lung,50017;Ishikawa,epithelial-like,,uterus,50018;Ishikawa (Heraklio) 02 ER-,epithelial,,uterus,50019;IST-MEL1,epithelial-like,,skin,50020;JHH-6,epithelial-like,,liver,50021;KMRC-20,epithelial-like,,kidney,50023;KYSE-140,,,esophagus,50024;KYSE-150,epitheloid,,esophagus,50025;KYSE-180,epitheloid,,esophagus,50026;KYSE-450,epitheloid,,esophagus,50027;LNZTA3WT4,,,brain,50028;MCF7,epithelial,,breast,50029;MDA-MB-435S,melanocyte,,skin,50030;MT-3,epithelial,,breast,50031;NCI-H1648,,,lung,50032;NCI-H1651,epithelial,,lung,50033;NCI-H1703,epithelial,,lung,50034;NCI-H1915,large cell,,lung,50035;NCI-H2023,,,lung,50036;NCI-H810,epithelial,,lung,50037;PE/CA-PJ15,epithelial-like,,head &amp; neck,50039;SJCRH30,fibroblast,,muscle,50041;SK-LMS-1,,,uterus,50042;SK-MES,epithelial,,lung,50043;SK-OV-3,epithelial,,ovary,50044;SNB75,,,brain,50045;SW527,epithelial,,breast,50046;SW620,epithelial,,intestine,50047;T24,epithelial,,urinary bladder,50048;WiDr,epithelial,,intestine,50049;Hep 3B2.1-7,epithelial,,liver,50051;Hep G2,epithelial,,liver,50052;Huh7,,,liver,50055;SK-BR-3,epithelial,,breast,50057;MDA-MB-231,epithelial,,breast,50058;LNCaP,epithelial,,prostate,50059;A-375,epithelial,,skin,50060;HeLa,epithelial,,cervix,50061;1205Lu,,,skin,50062;1321N1,,,brain,50063;143B,,,bone,50064;143B PML BK TK,,,bone,50065;1A6,,,urinary bladder,50066;22RV1,,,prostate,50067;23132/87,,,stomach,50068;42-MG-BA,,,brain,50069;639-V,,,ureter,50071;769-P,,,kidney,50072;786-O,,,kidney,50073;8305C,,,thyroid,50074;8505C,,,thyroid,50075;A172,,,brain,50076;A-204,,,muscle,50077;A2058,,,skin,50078;A2780,,,ovary,50079;A2780ADR,,,ovary,50080;A373-C6,,,skin,50081;A-427,,,lung,50082;A431,,,skin,50083;A549,,,lung,50084;A673,,,muscle,50085;ABC-1,,,lung,50086;ACHN,,,kidney,50087;AN3CA,,,uterus,50088;ASH-3,,,thyroid,50089;AsPC-1,,,pancreas,50090;AU565,,,breast,50091;AZ-521,,,stomach,50092;B-CPAP,,,thyroid,50093;BE(2)-C,,,nervous system,50094;BEN,,,lung,50095;BeWo,,,miscellaneous,50096;BFTC-905,,,urinary bladder,50097;BFTC-909,,,kidney,50098;BHT-101,,,thyroid,50099;BHY,,,head &amp; neck,50100;BICR 10,,,head &amp; neck,50101;BICR 22,,,head &amp; neck,50102;BICR 31,,,head &amp; neck,50103;BICR 78,,,head &amp; neck,50104;BT-20,,,breast,50105;BT-474,,,breast,50106;BT-483,,,breast,50107;BT-549,,,breast,50108;BxPC-3,,,pancreas,50109;C170,,,intestine,50110;C2BBe1,,,intestine,50111;C32,,,skin,50112;C-33 A,,,cervix,50113;C3A,,,liver,50114;C-4 I,,,cervix,50115;C-4 II,,,cervix,50116;Caco-2,,,intestine,50117;Caki-1,,,kidney,50118;CAL 27,,,head &amp; neck,50119;CAL-120,,,breast,50120;CAL-12T,,,lung,50121;CAL-148,,,breast,50122;CAL-29,,,urinary bladder,50123;CAL-33,,,head &amp; neck,50124;CAL-39,,,vulva,50125;CAL-54,,,kidney,50126;CAL-62,,,thyroid,50127;CAL-72,,,bone,50128;CAL-78,,,bone,50129;CAL-85-1,,,breast,50130;CAMA-1,,,breast,50131;Caov-3,,,ovary,50132;Caov-4,,,ovary,50133;Capan-1,,,pancreas,50134;Capan-2,,,pancreas,50135;CaR-1,,,intestine,50136;CCF-STTG1,,,brain,50137;CCK-81,,,intestine,50138;CHP-212,,,nervous system,50139;CoCM-1,,,intestine,50141;COLO 201,,,intestine,50142;COLO 205,,,intestine,50143;COLO 320DM,,,intestine,50144;COLO 741,,,intestine,50145;COLO 792,,,skin,50146;COLO 853,,,skin,50147;COLO 857,,,skin,50148;COLO 858,,,skin,50149;COLO-206F,,,intestine,50150;COLO-320,,,intestine,50151;COLO-678,,,intestine,50152;COLO-680N,,,esophagus,50153;COLO-783,,,skin,50154;COLO-824,,,breast,50156;COLO-849,,,skin,50157;COR-L 105,,,lung,50158;COR-L 23/CPR,,,lung,50159;COR-L23,,,lung,50160;DAN-G,,,pancreas,50161;Daoy,,,brain,50162;DBTRG-05MG,,,brain,50163;Detroit 562,,,head &amp; neck,50164;DK-MG,,,brain,50165;DLD-1,,,intestine,50166;DMS 273,,,lung,50167;DMS 53,,,lung,50168;DOK,,,head &amp; neck,50169;DoTc2 4510,,,cervix,50170;DU 145,,,prostate,50171;DV-90,,,lung,50172;EBC-1,,,lung,50173;EFE-184,,,uterus,50174;EFM-19,,,breast,50175;EFM-192A,,,breast,50176;EFM-192B,,,breast,50177;EFM-192C,,,breast,50178;EFO-21,,,ovary,50179;EFO-27,,,ovary,50180;EGI-1,,,biliary tract,50181;EJ138,,,urinary bladder,50182;EN,,,uterus,50183;EPLC-272H,,,lung,50184;ES-2,,,ovary,50185;ESS-1,,,uterus,50186;EVSA-T,,,breast,50187;FaDu,,,head &amp; neck,50188;FLYA13,,,miscellaneous,50189;FTC-133,,,thyroid,50190;FTC-238,,,thyroid,50191;FU-OV-1,,,ovary,50192;G-292 Clone A141B1,,,bone,50193;G-361,,,skin,50194;G-401,,,kidney,50195;G-402,,,kidney,50196;GAMG,,,brain,50197;GCT,,,miscellaneous,50198;GMS-10,,,brain,50199;GOS-3,,,brain,50200;GP5d,,,intestine,50201;H4,,,brain,50202;HARA,,,lung,50204;HCC1143,,,breast,50205;HCC1395,,,breast,50206;HCC1419,,,breast,50207;HCC1428,,,breast,50208;HCC-15,,,lung,50209;HCC1569,,,breast,50210;HCC1806,,,breast,50211;HCC1937,,,breast,50212;HCC1954,,,breast,50213;HCC202,,,breast,50214;HCC-366,,,lung,50215;HCC38,,,breast,50216;HCC-44,,,lung,50217;HCC-56,,,intestine,50218;HCC70,,,breast,50219;HCC-78,,,lung,50220;HCC-827,,,lung,50221;HCT 116,,,intestine,50222;HCT-15,,,intestine,50223;HCT-8,,,intestine,50224;HDQ-P1,,,breast,50225;H-EMC-SS,,,bone,50226;HGC-27,,,stomach,50227;HLE,,,liver,50228;HMVII,,,skin,50229;HN,,,head &amp; neck,50230;HO-1-N-1,,,head &amp; neck,50231;HO-1-u-1,,,head &amp; neck,50232;HOS,,,bone,50233;HPAC,,,pancreas,50234;HPAF-II,,,pancreas,50235;HRT-18,,,intestine,50236;Hs 257.T,,,intestine,50237;Hs 578T,,,breast,50238;Hs 588.T,,,cervix,50239;Hs 633T,,,miscellaneous,50240;Hs 683,,,brain,50241;Hs 766T,,,pancreas,50243;HSC-2,,,head &amp; neck,50244;HSC-3,,,head &amp; neck,50245;HSC-4,,,head &amp; neck,50246;HT 1080,,,miscellaneous,50247;HT 1376,,,urinary bladder,50248;HT115,,,intestine,50249;HT-1197,,,urinary bladder,50250;HT-29,,,intestine,50251;HT-3,,,cervix,50252;HT55,,,intestine,50253;HTC-C3,,,thyroid,50254;HuCCT1,,,biliary tract,50255;huH-1,,,liver,50256;HuO-3N1,,,bone,50257;HuO9,,,bone,50258;HuO9N2,,,bone,50259;HUP-T3,,,pancreas,50260;HUP-T4,,,pancreas,50261;IGR-1,,,skin,50262;IGR-37,,,skin,50263;IGR-39,,,skin,50264;IHH-4,,,thyroid,50265;IM-95,,,stomach,50266;IM-95m,,,stomach,50267;IMR-32,,,nervous system,50268;IPC-298,,,skin,50269;J82,,,urinary bladder,50270;JAR,,,miscellaneous,50271;JHH-1,,,liver,50272;JHH-2,,,liver,50273;JHH-4,,,liver,50274;JHH-7,,,liver,50275;JIMT-1,,,breast,50276;KELLY,,,nervous system,50277;KG-1-C,,,brain,50278;KHOS/NP,,,bone,50280;KHOS-240S,,,bone,50281;KHOS-312H,,,bone,50282;KMH-2,,,thyroid,50283;KMRC-1,,,kidney,50284;KON,,,head &amp; neck,50285;KOSC-2 cl3-43,,,head &amp; neck,50286;KP-2,,,pancreas,50287;KP-3,,,pancreas,50288;KP-3L,,,pancreas,50289;KP-4,,,pancreas,50290;KPL-1,,,breast,50291;KU-19-19,,,urinary bladder,50292;KYSE-220,,,esophagus,50293;KYSE-270,,,esophagus,50294;KYSE-30,,,esophagus,50295;KYSE-410,,,esophagus,50296;KYSE-50,,,esophagus,50297;KYSE-510,,,esophagus,50298;KYSE-520,,,esophagus,50299;KYSE-70,,,esophagus,50300;LC-1 sq,,,lung,50301;LCLC-103H,,,lung,50302;LCLC-97TM1,,,lung,50303;LK-2,,,lung,50304;LN-18,,,brain,50305;LN-229,,,brain,50306;LN-405,,,brain,50307;LNZTA3WT11,,,brain,50308;LOU-NH91,,,lung,50309;LoVo,,,intestine,50310;LS174T,,,intestine,50311;LS180,,,intestine,50312;Lu-135,,,lung,50314;LU65,,,lung,50315;LU65A,,,lung,50316;LU65B,,,lung,50317;LU65C,,,lung,50318;LU99A,,,lung,50319;LU99B,,,lung,50320;LU99C,,,lung,50321;LUDLU-1,,,lung,50322;M059J,,,brain,50323;MB 157,,,breast,50324;MCAS,,,ovary,50325;MC-IXC,,,nervous system,50326;MDA-MB-134-VI,,,breast,50327;MDA-MB-157,,,breast,50328;MDA-MB-175-VII,,,breast,50329;MDA-MB-330,,,breast,50330;MDA-MB-361,,,breast,50331;MDA-MB-415,,,breast,50332;MDA-MB-436,,,breast,50333;MDA-MB-453,,,breast,50334;MDA-MB-468,,,breast,50335;MDST8,,,intestine,50336;ME-180,,,cervix,50337;MEL-HO,,,skin,50338;MEL-JUSO,,,skin,50339;MES-SA,,,uterus,50340;MES-SA/Dx-5,,,uterus,50341;MEWO,,,skin,50342;MFE-280,,,uterus,50343;MFE-296,,,uterus,50344;MFE-319,,,uterus,50345;MFM-223,,,breast,50346;MG-63,,,bone,50347;MHH-ES-1,,,nervous system,50348;MIA PaCa-2,,,pancreas,50349;MKN1,,,stomach,50350;MKN28,,,stomach,50351;MKN45,,,stomach,50352;MKN7,,,stomach,50353;MKN74,,,stomach,50354;ML-1,,,thyroid,50355;MOG-G-CCM,,,brain,50356;MOG-G-UVW,,,brain,50357;MS751,,,cervix,50358;MSTO-211H,,,pleura,50359;NB69,,,nervous system,50360;NCC-IT-A3,,,testes,50361;NCI-H1048,,,lung,50362;NCI-H1299,,,lung,50363;NCI-H1435,,,lung,50364;NCI-H1437,,,lung,50365;NCI-H1568,,,lung,50366;NCI-H1573,,,lung,50367;NCI-H1581,,,lung,50368;NCI-H1623,,,lung,50369;NCI-H1650,,,lung,50370;NCI-H1688,,,lung,50371;NCI-H1693,,,lung,50372;NCI-H1734,,,lung,50373;NCI-H1755,,,lung,50374;NCI-H1781,,,lung,50375;NCI-H1792,,,lung,50376;NCI-H1793,,,lung,50377;NCI-H1869,,,lung,50378;NCI-H1876,,,lung,50379;NCI-H1944,,,lung,50380;NCI-H196,,,lung,50381;NCI-H1993,,,lung,50382;NCI-H2009,,,lung,50383;NCI-H2029,,,lung,50384;NCI-H2030,,,lung,50385;NCI-H2073,,,lung,50386;NCI-H2085,,,lung,50387;NCI-H2087,,,lung,50388;NCI-H2110,,,lung,50389;NCI-H2122,,,lung,50390;NCI-H2135,,,lung,50391;NCI-H2170,,,lung,50392;NCI-H2172,,,lung,50393;NCI-H2195,,,lung,50394;NCI-H2196,,,lung,50395;NCI-H2198,,,lung,50396;NCI-H2228,,,lung,50397;NCI-H2286,,,lung,50398;NCI-H2291,,,lung,50399;NCI-H23,,,lung,50400;NCI-H2342,,,lung,50401;NCI-H2347,,,lung,50402;NCI-H2405,,,lung,50403;NCI-H2444,,,lung,50404;NCI-H2452,,,lung,50405;NCI-H322,,,lung,50407;NCI-H358,,,lung,50408;NCI-H441,,,lung,50409;NCI-H460,,,lung,50410;NCI-H520,,,lung,50411;NCI-H522,,,lung,50412;NCI-H596,,,lung,50413;NCI-H647,,,lung,50415;NCI-H650,,,lung,50416;NCI-H661,,,lung,50417;NCI-H727,,,lung,50418;NCI-H838,,,lung,50419;NCI-H841,,,lung,50420;NCI-N87,,,stomach,50421;NIH:OVCAR-3,,,ovary,50422;NUGC-3,,,stomach,50424;NUGC-4,,,stomach,50425;NY,,,bone,50426;OAW28,,,ovary,50427;OAW42,,,ovary,50428;OCUG-1,,,gall bladder,50429;OCUM-1,,,stomach,50430;OE19,,,esophagus,50431;OE21,,,esophagus,50432;OE33,,,esophagus,50433;OSC-19,,,head &amp; neck,50434;OSC-20,,,head &amp; neck,50435;OUMS-23,,,intestine,50436;OV-90,,,ovary,50437;OVISE,,,ovary,50438;OVKATE,,,ovary,50439;OVMIU,,,ovary,50440;OVSAYO,,,ovary,50441;OVTOKO,,,ovary,50442;PA-1,,,ovary,50443;Panc 02.03,,,pancreas,50444;Panc 03.27,,,pancreas,50445;Panc 04.03,,,pancreas,50446;Panc 08.13,,,pancreas,50447;Panc 10.05,,,pancreas,50448;PANC-1,,,pancreas,50449;PA-TU-8902,,,pancreas,50450;PA-TU-8988S,,,pancreas,50451;PA-TU-8988T,,,pancreas,50452;PC-14,,,lung,50453;PC-3,,,prostate,50454;PFSK-1,,,brain,50455;PL45,,,pancreas,50456;PLC/PRF/5,,,liver,50457;RCM-1,,,intestine,50459;RD,,,muscle,50460;RD-ES,,,nervous system,50461;RERF-GC-1B,,,stomach,50462;RERF-LC-Ad1,,,lung,50463;RERF-LC-KJ,,,lung,50464;RERF-LC-MA,,,lung,50465;RERF-LC-Sq1,,,lung,50466;RKN,,,ovary,50467;RMG-I,,,ovary,50468;RO82-W-1,,,thyroid,50469;RPMI 2650,,,head &amp; neck,50470;RPMI-7951,,,skin,50471;RT-112,,,urinary bladder,50472;RT112/84,,,urinary bladder,50473;RT4,,,urinary bladder,50474;RVH-421,,,skin,50475;S-117,,,thyroid,50476;Saos-2,,,bone,50477;SAS,,,head &amp; neck,50478;SAT,,,head &amp; neck,50479;SBC-3,,,lung,50480;SBC-5,,,lung,50481;SCaBER,,,urinary bladder,50482;SCC-15,,,head &amp; neck,50483;SCC-25,,,head &amp; neck,50484;SCC-4,,,head &amp; neck,50485;SCC-9,,,head &amp; neck,50486;SCCH-26,,,nervous system,50488;SCH,,,stomach,50489;SCLC-21H,,,lung,50490;SHP-77,,,lung,50491;SiHa,,,cervix,50493;SISO,,,cervix,50494;SK-CO-1,,,intestine,50495;SK-ES-1,,,bone,50496;SKG-IIIa,,,cervix,50497;SKG-IIIb,,,cervix,50498;SK-HEP-1,,,liver,50499;SK-LU-1,,,lung,50500;SK-MEL-2,,,skin,50501;SK-MEL-30,,,skin,50502;SKN,,,uterus,50503;SKN-3,,,head &amp; neck,50504;SK-N-AS,,,nervous system,50505;SK-N-DZ,,,nervous system,50506;SK-NEP-1,,,kidney,50507;SK-N-SH,,,nervous system,50508;SNG-M,,,uterus,50509;SNU-1,,,stomach,50510;SNU-16,,,stomach,50511;SNU-182,,,liver,50512;SNU-387,,,liver,50513;SNU-398,,,liver,50514;SNU-423,,,liver,50515;SNU-449,,,liver,50516;SNU-475,,,liver,50517;SNU-5,,,stomach,50518;SU.86.86,,,pancreas,50520;SUIT-2,,,pancreas,50521;SW 1088,,,brain,50522;SW 1271,,,lung,50524;SW 13,,,adrenal gland,50525;SW 1417,,,intestine,50526;SW 1463,,,intestine,50527;SW 156,,,kidney,50528;SW 1573,,,lung,50529;SW 1783,,,brain,50530;SW 48,,,intestine,50531;SW 626,,,ovary,50532;SW 780,,,urinary bladder,50533;SW 900,,,lung,50534;SW-1710,,,urinary bladder,50535;SW756,,,cervix,50536;SW837,,,intestine,50537;SW-948,,,intestine,50538;T.T,,,esophagus,50539;T.Tn,,,esophagus,50540;T47D,,,breast,50541;T84,,,intestine,50542;T98G,,,brain,50543;TASK1,,,nervous system,50544;TCCSUP,,,urinary bladder,50545;TGW,,,adrenal gland,50546;TOV-112D,,,ovary,50547;TOV-21G,,,ovary,50548;TT2609-C02,,,thyroid,50549;TYK-nu,,,ovary,50550;U-118 MG,,,brain,50551;U-138 MG,,,brain,50552;U-2 OS,,,bone,50553;U-251 MG,,,brain,50554;U373 MG,,,brain,50555;UACC-812,,,breast,50556;UACC-893,,,breast,50557;UMC-11,,,lung,50558;UM-UC-3,,,urinary bladder,50559;VCaP,,,prostate,50560;VM-CUB1,,,urinary bladder,50561;VMRC-LCP,,,lung,50562;VMRC-MELG,,,skin,50563;VMRC-RCW,,,kidney,50564;VMRC-RCZ,,,kidney,50565;WM 266-4,,,skin,50566;WM-115,,,skin,50567;WM1552C,,,skin,50568;WM278,,,skin,50569;WM35,,,skin,50570;WM793B,,,skin,50571;YAPC,,,pancreas,50572;YKG-1,,,brain,50573;ZR-75-1,,,breast,50574;ZR-75-30,,,breast,50575;DU4475,epithelial,,breast,50577;HCC1187,epithelial,,breast,50578;HCC1500,epithelial,,breast,50579;HCC1599,epithelial,,breast,50580;HCC2157,epithelial,,breast,50581;HCC2218,epithelial,,breast,50582;2B8,,,lymphatic system,50585;A2780cis,,,ovary,50586;A3,,,blood,50587;A3/KAW,,,lymphatic system,50588;AGR-ON,,,blood,50589;ALL-SIL,,,blood,50590;AMO-1,,,lymphatic system,50591;ARH-77,,,blood,50592;BALL-1,,,blood,50593;BC-1,,,lymphatic system,50594;BC-2,,,lymphatic system,50595;BC-3,,,lymphatic system,50596;BDCM,,,blood,50597;BE(2)-M17,,,nervous system,50598;BL-41,,,lymphatic system,50599;BL-70,,,lymphatic system,50600;C8166,,,blood,50601;CA46,,,lymphatic system,50602;CCRF-CEM,,,blood,50603;CCRF-HSB-2,,,blood,50604;CCRF-SB,,,blood,50605;CEM/C1,,,blood,50606;CEM/C2,,,blood,50607;CESS,,,blood,50608;CFPAC-1,,,pancreas,50609;ChaGo-K-1,,,lung,50610;CHP-126,,,nervous system,50611;CI-1,,,lymphatic system,50612;CL-11,,,intestine,50613;Clone 15 HL-60,,,blood,50614;CMK,,,blood,50615;COLO 684,,,uterus,50616;COLO-704,,,ovary,50617;COR-L279,,,lung,50618;COR-L51,,,lung,50619;COR-L88,,,lung,50620;COR-L95,,,lung,50621;CPC-N,,,lung,50622;CTV-1,,,blood,50623;D283 Med,,,brain,50624;Daudi,,,lymphatic system,50625;DB,,,lymphatic system,50626;DERL-2,,,lymphatic system,50627;DG-75,,,lymphatic system,50628;DMS 114,,,lung,50629;DMS 153,,,lung,50630;DMS 79,,,lung,50631;DND-41,,,blood,50632;EB1,,,lymphatic system,50633;EB2,,,lymphatic system,50634;EB-3,,,lymphatic system,50635;EHEB,,,blood,50636;EJM,,,blood,50637;Eos-HL-60,,,blood,50638;Farage,,,lymphatic system,50639;GA-10 (Clone 20),,,lymphatic system,50641;GDM-1,,,blood,50642;GOTO,,,nervous system,50643;Gp2D,,,intestine,50644;GRANTA-519,,,lymphatic system,50645;H33HJ-JA1,,,blood,50646;HC-1,,,blood,50647;HCC-33,,,lung,50648;HDLM-2,,,lymphatic system,50649;HD-MY-Z,,,lymphatic system,50650;HEL,,,blood,50651;HEL 92.1.7,,,blood,50652;HH,,,lymphatic system,50653;HL-60,,,blood,50654;HL60(S),,,blood,50655;HL-60/MX2,,,blood,50656;HL60RG,,,blood,50657;Hs 445,,,lymphatic system,50658;HS-Sultan,,,lymphatic system,50659;HT,,,lymphatic system,50660;HuT 78,,,lymphatic system,50661;I 2.1,,,blood,50662;I 9.2,,,blood,50663;IM-9,,,lymphatic system,50664;J.gamma1,,,blood,50665;J.gamma1.WT,,,blood,50666;J.RT3-T3.5,,,blood,50667;J45.01,,,blood,50668;Jiyoye,,,lymphatic system,50669;JJN-3,,,blood,50670;JKT-beta-del,,,blood,50671;JM1,,,lymphatic system,50672;JSC-1,,,lymphatic system,50673;Jurkat, Clone E6-1,,,blood,50674;JURL-MK1,,,blood,50675;JURL-MK2,,,blood,50676;K-562,,,blood,50677;K562/ADM,,,blood,50678;KARPAS-231,,,blood,50679;KARPAS-299,,,lymphatic system,50680;KARPAS-422,,,lymphatic system,50681;KARPAS-45,,,blood,50682;KARPAS-620,,,blood,50683;KCL-22,,,blood,50685;KE-37,,,blood,50686;KG-1,,,blood,50687;KG-1a,,,blood,50688;KM-H2,,,lymphatic system,50689;KMOE-2,,,blood,50690;KMS-12-BM,,,blood,50691;KMS-12-PE,,,blood,50692;KO52,,,blood,50693;KOPN-8,,,blood,50694;KP-1N,,,pancreas,50695;KP-1NL,,,pancreas,50696;KU812,,,blood,50697;KU812E,,,blood,50698;KU812F,,,blood,50699;KY821,,,blood,50700;KY821A3,,,blood,50701;KYM-1,,,muscle,50702;L-1236,,,lymphatic system,50703;L-363,,,blood,50704;L-428,,,lymphatic system,50705;L-540,,,lymphatic system,50706;LAMA-84,,,blood,50707;LC4-1,,,blood,50708;Loucy,,,blood,50709;LP-1,,,blood,50710;Lu-134-B,,,lung,50711;M059K,,,brain,50712;MC/CAR,,,lymphatic system,50713;MC116,,,lymphatic system,50714;ME-1,,,blood,50715;MEC-1,,,blood,50716;MEC-2,,,blood,50717;MEG-01,,,blood,50718;MHH-NB-11,,,nervous system,50719;MHH-PREB-1,,,lymphatic system,50720;MJ,,,lymphatic system,50721;ML-2,,,blood,50722;MLMA,,,blood,50723;MOLM-13,,,blood,50724;MOLP-8,,,blood,50725;MOLT-14,,,blood,50726;MOLT-16,,,blood,50727;MOLT-4,,,blood,50728;MOLT-4F,,,blood,50729;MONO-MAC-1,,,blood,50730;MONO-MAC-6,,,blood,50731;MRK-nu-1,,,breast,50732;MS-1-L,,,lung,50733;MV-4-11,,,blood,50734;MY,,,blood,50735;MY-M12,,,blood,50736;MY-M13,,,blood,50737;NALM-19,,,blood,50738;NALM-6,,,blood,50739;NAMALWA,,,lymphatic system,50740;NAMALWA.PNT,,,lymphatic system,50741;NB(TU)1-10,,,nervous system,50742;NB-1,,,nervous system,50743;NB-4,,,blood,50744;NC-37,,,lymphatic system,50745;NCI-H1092,,,lung,50746;NCI-H1155,,,lung,50747;NCI-H1304,,,lung,50748;NCI-H1385,,,lung,50749;NCI-H1395,,,lung,50750;NCI-H1404,,,lung,50751;NCI-H1417,,,lung,50752;NCI-H1436,,,lung,50753;NCI-H1522,,,lung,50754;NCI-H1563,,,lung,50755;NCI-H1618,,,lung,50756;NCI-H1666,,,lung,50757;NCI-H1694,,,lung,50758;NCI-H1770,,,lung,50759;NCI-H1836,,,lung,50760;NCI-H1838,,,lung,50761;NCI-H187,,,lung,50762;NCI-H1882,,,lung,50763;NCI-H1963,,,lung,50764;NCI-H1975,,,lung,50765;NCI-H2081,,,lung,50766;NCI-H209,,,lung,50767;NCI-H2106,,,lung,50768;NCI-H211,,,lung,50769;NCI-H2141,,,lung,50770;NCI-H2171,,,lung,50771;NCI-H220,,,lung,50772;NCI-H2227,,,lung,50773;NCI-H226,,,lung,50774;NCI-H345,,,lung,50775;NCI-H446,,,lung,50776;NCI-H510A,,,lung,50777;NCI-H524,,,lung,50778;NCI-H526,,,lung,50779;NCI-H69,,,lung,50780;NCI-H719,,,lung,50781;NCI-H720,,,lung,50782;NCI-H748,,,lung,50783;NCI-H82,,,lung,50784;NCI-H847,,,lung,50785;NCI-H889,,,lung,50786;NEC8,,,testes,50787;NH-12,,,nervous system,50788;NK-92MI,,,lymphatic system,50789;NOMO-1/ADM,,,blood,50790;NU-DUL-1,,,lymphatic system,50791;OCI-AML2,,,blood,50792;OCI-AML3,,,blood,50793;OCI-AML5,,,blood,50794;OCI-LY-19,,,lymphatic system,50795;OCI-M1,,,blood,50796;OPM-2,,,blood,50797;P116.cl39,,,blood,50798;P12-ICHIKAWA,,,blood,50799;P30/OHK,,,blood,50800;P31/FUJ,,,blood,50801;P32/ISH,,,lymphatic system,50802;P3HR-1,,,lymphatic system,50803;PC-3 [JPC-3],,,lung,50804;PEER,,,blood,50805;PF-382,,,blood,50806;Pfeiffer,,,lymphatic system,50807;PL-21,,,blood,50808;PSN1,,,pancreas,50809;Raji,,,lymphatic system,50810;Ramos (RA 1),,,blood,50811;RC-K8,,,lymphatic system,50812;REC-1,,,lymphatic system,50813;Reh,,,blood,50814;RERF-LC-MS,,,lung,50815;RH-1,,,bone,50816;RH-30,,,muscle,50817;RH-41,,,muscle,50818;RL,,,lymphatic system,50819;ROS-50,,,blood,50820;RPMI 1788,,,blood,50821;RPMI 6666,,,lymphatic system,50822;RPMI 8226,,,blood,50823;RPMI-8402,,,blood,50824;RS4;11,,,blood,50825;SBC-1,,,lung,50826;SBC-2,,,lung,50827;SC-1,,,lymphatic system,50828;SCC-3,,,lymphatic system,50829;Sci-1,,,lymphatic system,50830;SIG-M5,,,blood,50831;SIMA,,,nervous system,50832;SK-MEL-1,,,skin,50833;SK-MEL-3,,,skin,50834;SK-N-BE(2),,,nervous system,50835;SK-N-FI,,,nervous system,50836;SLVL,,,lymphatic system,50837;SNB-19,,,brain,50838;SR,,,lymphatic system,50839;ST486,,,lymphatic system,50840;SU-DHL-1,,,lymphatic system,50841;SU-DHL-16,,,lymphatic system,50843;SU-DHL-4,,,lymphatic system,50844;SU-DHL-5,,,lymphatic system,50845;SU-DHL-6,,,lymphatic system,50846;SU-DHL-8,,,lymphatic system,50847;SUP-B15,,,blood,50848;SUP-HD1,,,lymphatic system,50849;SUP-M2,,,lymphatic system,50850;SUP-T1,,,blood,50851;SW 1990,,,pancreas,50853;TALL-1,,,blood,50854;TANOUE,,,blood,50855;TC-71,,,bone,50856;Tera-1,,,testes,50857;TF-1,,,blood,50858;TF-1.CN5a.1,,,blood,50859;TF-1a,,,blood,50860;THP-1,,,blood,50861;TK,,,lymphatic system,50862;Toledo,,,lymphatic system,50863;TT,,,thyroid,50864;TUR,,,lymphatic system,50865;U266B1,,,blood,50866;U-698-M,,,blood,50867;U-87 MG,,,brain,50868;U-937,,,lymphatic system,50869;VAL,,,lymphatic system,50870;WIL2 NS,,,lymphatic system,50871;WILCL,,,blood,50872;WSU-DLCL2,,,lymphatic system,50873;WSU-NHL,,,lymphatic system,50874;YMB-1,,,breast,50875;YT,,,lymphatic system,50876;8-MG-BA,,,brain,50878;A101D,,,skin,50879;A253,,,head &amp; neck,50880;A388,,,miscellaneous,50881;A498,,,kidney,50882;A704,,,kidney,50884;ACN,,,nervous system,50885;ALL-PO,,,blood,50886;AM-38,,,brain,50887;ATN-1,,,blood,50888;BB30-HNC,,,head &amp; neck,50890;BB49-HNC,,,head &amp; neck,50891;BB65-RCC,,,kidney,50892;BE-13,,,blood,50893;Becker,,,brain,50894;BOKU,,,cervix,50895;BV-173,,,blood,50896;Calu-6,,,lung,50897;CAS-1,,,brain,50898;CGTH-W-1,,,thyroid,50899;COLO-320-HSR,,,intestine,50900;COLO-668,,,lung,50901;COLO-829,,,skin,50902;CP66-MEL,,,skin,50904;CW-2,,,intestine,50906;D-263MG,,,brain,50908;D-392MG,,,brain,50910;D-502MG,,,brain,50912;D-542MG,,,brain,50913;DEL,,,blood,50915;DJM-1,,,skin,50916;DOHH-2,,,lymphatic system,50917;DSH1,,,urinary tract,50918;ECC4,,,intestine,50921;EC-GI-10,,,esophagus,50922;EKVX,,,lung,50923;EM-2,,,blood,50924;EoL-1-cell,,,blood,50925;ES1,,,bone,50926;ES4,,,bone,50928;ES5,,,bone,50929;ES6,,,bone,50930;ES7,,,bone,50931;ES8,,,bone,50932;ETK-1,,,biliary tract,50933;EW-1,,,bone,50934;EW-11,,,bone,50935;EW-13,,,bone,50936;EW-16,,,bone,50937;EW-18,,,bone,50938;EW-24,,,bone,50939;EW-3,,,bone,50940;EW-7,,,bone,50941;GAK,,,skin,50942;GB-1,,,brain,50943;GCIY,,,stomach,50944;GI-1,,,brain,50945;GI-ME-N,,,nervous system,50946;GR-ST,,,blood,50947;GT3TKB,,,stomach,50948;HA7-RCC,,,kidney,50950;HAL-01,,,blood,50951;HCC2998,,,intestine,50952;HCE-T,,,head &amp; neck,50954;HOP-62,,,lung,50955;HT-144,,,skin,50956;IMR-5,,,nervous system,50957;IST-MES1,,,pleura,50958;IST-SL2,,,lung,50960;JVM-2,,,blood,50962;JVM-3,,,blood,50963;K5,,,thyroid,50964;KALS-1,,,brain,50965;KGN,,,ovary,50966;KINGS-1,,,brain,50967;KM12,,,intestine,50969;KNS-42,,,brain,50970;KNS-81-FD,,,brain,50971;KP-N-YS,,,nervous system,50973;KS-1,,,brain,50974;KURAMOCHI,,,ovary,50975;LAN-5,,,nervous system,50976;LAN-6,,,nervous system,50977;LB1047-RCC,,,kidney,50978;LB2241-RCC,,,kidney,50979;LB2518-MEL,,,skin,50980;LB373-MEL-D,,,skin,50981;LB771-HNC,,,head &amp; neck,50983;LB831-BLC,,,urinary tract,50984;LB996-RCC,,,kidney,50985;LC-2-ad,,,lung,50987;LOXIMVI,,,skin,50988;LS-1034,,,intestine,50989;LS-123,,,intestine,50990;LS-411N,,,intestine,50991;LS-513,,,intestine,50992;LU-134-A,,,lung,50993;LU-165,,,lung,50995;LXF-289,,,lung,50996;MFH-ino,,,miscellaneous,50997;MHH-CALL-2,,,blood,50998;MMAC-SF,,,skin,50999;MN-60,,,blood,51000;MPP-89,,,pleura,51002;MUTZ-1,,,blood,51003;MZ1-PC,,,pancreas,51004;MZ2-MEL,,,skin,51005;MZ7-mel,,,skin,51006;NB10,,,nervous system,51007;NB12,,,nervous system,51008;NB13,,,nervous system,51009;NB14,,,nervous system,51010;NB16,,,nervous system,51011;NB5,,,nervous system,51013;NB6,,,nervous system,51014;NB7,,,nervous system,51015;NCI-H1355,,,lung,51017;NCI-H157,,,lung,51018;NCI-H2126,,,lung,51019;NCI-H322M,,,lung,51020;NCI-H64,,,lung,51021;NCI-H716,,,intestine,51022;NCI-H747,,,intestine,51023;NKM-1,,,blood,51024;NMC-G1,,,brain,51025;no-10,,,brain,51026;no-11,,,brain,51027;NOMO-1,,,blood,51028;NOS-1,,,bone,51029;NTERA-S-cl-D1,,,testes,51030;OCUB-M,,,breast,51032;OMC-1,,,cervix,51033;ONS-76,,,brain,51034;OS-RC-2,,,kidney,51035;OVCAR-4,,,ovary,51036;QIMR-WIL,,,blood,51037;Ramos-2G6-4C10,,,lymphatic system,51038;RCC10RGB,,,kidney,51039;RKO,,,intestine,51041;RPMI-8866,,,blood,51043;RXF393,,,kidney,51044;SF126,,,brain,51045;SF268,,,brain,51046;SF539,,,brain,51047;SH-4,,,skin,51048;SJSA-1,,,bone,51049;SK-MM-2,,,blood,51053;SK-PN-DW,,,bone,51054;SK-UT-1,,,uterus,51055;SNU-C1,,,intestine,51056;SNU-C2B,,,intestine,51057;SW403,,,intestine,51058;SW684,,,miscellaneous,51059;SW872,,,miscellaneous,51060;SW954,,,vulva,51061;SW962,,,vulva,51062;SW982,,,miscellaneous,51063;TE-1,,,esophagus,51064;TE-10,,,esophagus,51065;TE-12,,,esophagus,51067;TE-15,,,esophagus,51068;TE-441-T,,,muscle,51069;TE-5,,,esophagus,51070;TE-6,,,esophagus,51071;TE-8,,,esophagus,51072;TE-9,,,esophagus,51073;TGBC11TKB,,,stomach,51074;TGBC1TKB,,,biliary tract,51075;TK10,,,kidney,51077;UACC-257,,,skin,51078;VA-ES-BJ,,,miscellaneous,51079;ECC10,,,stomach,50919;JEG-3,,,miscellaneous,50961;697.0,,,blood,50877;LU-139,,,lung,50994;CTB-1,,,lymphatic system,50905;ES3,,,bone,50927;TE-11,,,esophagus,51066;IST-SL1,,,lung,50959;TGBC24TKB,,,biliary tract,51076;KLE,,,uterus,50968;LC-1F,,,lung,50986;HCE-4,,,esophagus,50953;A4-Fuk,,,skin,50883;SK-MEL-24,,,skin,51050;CP50-MEL-B,,,skin,50903;YH-13,,,brain,51080;OC-314,,,ovary,51031;RF-48,,,stomach,51040;SK-MG-1,,,brain,51052;B2-17,,,brain,50889;Mo-T,,,blood,51001;KP-N-YN,,,nervous system,50972;D-423MG,,,brain,50911;H9,,,lymphatic system,50949;D-566MG,,,brain,50914;SK-MEL-5,,,skin,51051;NBsusSR,,,nervous system,51016;LB647-SCLC,,,lung,50982</t>
+  </si>
+  <si>
+    <t>1046\cell lines</t>
+  </si>
+  <si>
+    <t>BAY61-3606,small molecule,10166-107,LSM-1167;AS601245,small molecule,10034-101,LSM-1034;Pazopanib,small molecule,10114-101,LSM-1114</t>
+  </si>
+  <si>
+    <t>http://lincs.hms.harvard.edu/db/datasets/20008/</t>
+  </si>
+  <si>
+    <t>MGH (CMT) Growth Inhibition Assay Protocol (9 compound doses: 5.12 uM to 0.02 uM) -- DNA Staining</t>
+  </si>
+  <si>
+    <t>5637.0,epithelial,,urinary bladder,50001;647-V,epithelial-like,,urinary bladder,50002;A375.S2,epithelial,,skin,50003;AGS,epithelial,,stomach,50004;BPH-1,epitheloid,,prostate,50005;Ca Ski,epithelial,,cervix,50006;Ca9-22,epithelial-like,,head &amp; neck,50007;CAL-51,epithelial-like,,breast,50008;Calu-1,epithelial,,lung,50009;Calu-3,epithelial,,lung,50010;COLO-679,fibroblastic,,skin,50011;COLO-800,epithelial-like,,skin,50012;FU97,epithelial-like,,stomach,50013;HEC-1,,,uterus,50014;HLF,,,liver,50015;HUTU-80,epithelial,,intestine,50016;IA-LM,,,lung,50017;Ishikawa,epithelial-like,,uterus,50018;Ishikawa (Heraklio) 02 ER-,epithelial,,uterus,50019;IST-MEL1,epithelial-like,,skin,50020;JHH-6,epithelial-like,,liver,50021;KMRC-20,epithelial-like,,kidney,50023;KYSE-140,,,esophagus,50024;KYSE-150,epitheloid,,esophagus,50025;KYSE-180,epitheloid,,esophagus,50026;KYSE-450,epitheloid,,esophagus,50027;LNZTA3WT4,,,brain,50028;MCF7,epithelial,,breast,50029;MDA-MB-435S,melanocyte,,skin,50030;MT-3,epithelial,,breast,50031;NCI-H1648,,,lung,50032;NCI-H1651,epithelial,,lung,50033;NCI-H1703,epithelial,,lung,50034;NCI-H1915,large cell,,lung,50035;NCI-H2023,,,lung,50036;NCI-H810,epithelial,,lung,50037;PE/CA-PJ15,epithelial-like,,head &amp; neck,50039;SJCRH30,fibroblast,,muscle,50041;SK-LMS-1,,,uterus,50042;SK-MES,epithelial,,lung,50043;SK-OV-3,epithelial,,ovary,50044;SNB75,,,brain,50045;SW527,epithelial,,breast,50046;SW620,epithelial,,intestine,50047;T24,epithelial,,urinary bladder,50048;WiDr,epithelial,,intestine,50049;Hep 3B2.1-7,epithelial,,liver,50051;Hep G2,epithelial,,liver,50052;Huh7,,,liver,50055;SK-BR-3,epithelial,,breast,50057;MDA-MB-231,epithelial,,breast,50058;LNCaP,epithelial,,prostate,50059;A-375,epithelial,,skin,50060;HeLa,epithelial,,cervix,50061;1205Lu,,,skin,50062;1321N1,,,brain,50063;143B,,,bone,50064;143B PML BK TK,,,bone,50065;1A6,,,urinary bladder,50066;22RV1,,,prostate,50067;23132/87,,,stomach,50068;42-MG-BA,,,brain,50069;639-V,,,ureter,50071;769-P,,,kidney,50072;786-O,,,kidney,50073;8305C,,,thyroid,50074;8505C,,,thyroid,50075;A172,,,brain,50076;A-204,,,muscle,50077;A2058,,,skin,50078;A2780,,,ovary,50079;A2780ADR,,,ovary,50080;A373-C6,,,skin,50081;A-427,,,lung,50082;A431,,,skin,50083;A549,,,lung,50084;A673,,,muscle,50085;ABC-1,,,lung,50086;ACHN,,,kidney,50087;AN3CA,,,uterus,50088;ASH-3,,,thyroid,50089;AsPC-1,,,pancreas,50090;AU565,,,breast,50091;AZ-521,,,stomach,50092;B-CPAP,,,thyroid,50093;BE(2)-C,,,nervous system,50094;BEN,,,lung,50095;BeWo,,,miscellaneous,50096;BFTC-905,,,urinary bladder,50097;BFTC-909,,,kidney,50098;BHT-101,,,thyroid,50099;BHY,,,head &amp; neck,50100;BICR 10,,,head &amp; neck,50101;BICR 22,,,head &amp; neck,50102;BICR 31,,,head &amp; neck,50103;BICR 78,,,head &amp; neck,50104;BT-20,,,breast,50105;BT-474,,,breast,50106;BT-483,,,breast,50107;BT-549,,,breast,50108;BxPC-3,,,pancreas,50109;C170,,,intestine,50110;C2BBe1,,,intestine,50111;C32,,,skin,50112;C-33 A,,,cervix,50113;C3A,,,liver,50114;C-4 I,,,cervix,50115;C-4 II,,,cervix,50116;Caco-2,,,intestine,50117;Caki-1,,,kidney,50118;CAL 27,,,head &amp; neck,50119;CAL-120,,,breast,50120;CAL-12T,,,lung,50121;CAL-148,,,breast,50122;CAL-29,,,urinary bladder,50123;CAL-33,,,head &amp; neck,50124;CAL-39,,,vulva,50125;CAL-54,,,kidney,50126;CAL-62,,,thyroid,50127;CAL-72,,,bone,50128;CAL-78,,,bone,50129;CAL-85-1,,,breast,50130;CAMA-1,,,breast,50131;Caov-3,,,ovary,50132;Caov-4,,,ovary,50133;Capan-1,,,pancreas,50134;Capan-2,,,pancreas,50135;CaR-1,,,intestine,50136;CCF-STTG1,,,brain,50137;CCK-81,,,intestine,50138;CHP-212,,,nervous system,50139;CoCM-1,,,intestine,50141;COLO 201,,,intestine,50142;COLO 205,,,intestine,50143;COLO 320DM,,,intestine,50144;COLO 741,,,intestine,50145;COLO 792,,,skin,50146;COLO 853,,,skin,50147;COLO 857,,,skin,50148;COLO 858,,,skin,50149;COLO-206F,,,intestine,50150;COLO-320,,,intestine,50151;COLO-678,,,intestine,50152;COLO-680N,,,esophagus,50153;COLO-783,,,skin,50154;COLO-818,,,skin,50155;COLO-824,,,breast,50156;COLO-849,,,skin,50157;COR-L 105,,,lung,50158;COR-L 23/CPR,,,lung,50159;COR-L23,,,lung,50160;DAN-G,,,pancreas,50161;Daoy,,,brain,50162;DBTRG-05MG,,,brain,50163;Detroit 562,,,head &amp; neck,50164;DK-MG,,,brain,50165;DLD-1,,,intestine,50166;DMS 273,,,lung,50167;DMS 53,,,lung,50168;DOK,,,head &amp; neck,50169;DoTc2 4510,,,cervix,50170;DU 145,,,prostate,50171;DV-90,,,lung,50172;EBC-1,,,lung,50173;EFE-184,,,uterus,50174;EFM-19,,,breast,50175;EFM-192A,,,breast,50176;EFM-192B,,,breast,50177;EFM-192C,,,breast,50178;EFO-21,,,ovary,50179;EFO-27,,,ovary,50180;EGI-1,,,biliary tract,50181;EJ138,,,urinary bladder,50182;EN,,,uterus,50183;EPLC-272H,,,lung,50184;ES-2,,,ovary,50185;ESS-1,,,uterus,50186;EVSA-T,,,breast,50187;FaDu,,,head &amp; neck,50188;FLYA13,,,miscellaneous,50189;FTC-133,,,thyroid,50190;FTC-238,,,thyroid,50191;FU-OV-1,,,ovary,50192;G-292 Clone A141B1,,,bone,50193;G-361,,,skin,50194;G-401,,,kidney,50195;G-402,,,kidney,50196;GAMG,,,brain,50197;GCT,,,miscellaneous,50198;GMS-10,,,brain,50199;GOS-3,,,brain,50200;GP5d,,,intestine,50201;H4,,,brain,50202;HARA,,,lung,50204;HCC1143,,,breast,50205;HCC1395,,,breast,50206;HCC1419,,,breast,50207;HCC1428,,,breast,50208;HCC-15,,,lung,50209;HCC1569,,,breast,50210;HCC1806,,,breast,50211;HCC1937,,,breast,50212;HCC1954,,,breast,50213;HCC-366,,,lung,50215;HCC38,,,breast,50216;HCC-44,,,lung,50217;HCC-56,,,intestine,50218;HCC70,,,breast,50219;HCC-78,,,lung,50220;HCC-827,,,lung,50221;HCT 116,,,intestine,50222;HCT-15,,,intestine,50223;HCT-8,,,intestine,50224;HDQ-P1,,,breast,50225;H-EMC-SS,,,bone,50226;HGC-27,,,stomach,50227;HLE,,,liver,50228;HMVII,,,skin,50229;HN,,,head &amp; neck,50230;HO-1-N-1,,,head &amp; neck,50231;HO-1-u-1,,,head &amp; neck,50232;HOS,,,bone,50233;HPAC,,,pancreas,50234;HPAF-II,,,pancreas,50235;HRT-18,,,intestine,50236;Hs 257.T,,,intestine,50237;Hs 578T,,,breast,50238;Hs 588.T,,,cervix,50239;Hs 633T,,,miscellaneous,50240;Hs 683,,,brain,50241;Hs 746T,,,stomach,50242;Hs 766T,,,pancreas,50243;HSC-2,,,head &amp; neck,50244;HSC-3,,,head &amp; neck,50245;HSC-4,,,head &amp; neck,50246;HT 1080,,,miscellaneous,50247;HT 1376,,,urinary bladder,50248;HT115,,,intestine,50249;HT-1197,,,urinary bladder,50250;HT-29,,,intestine,50251;HT-3,,,cervix,50252;HT55,,,intestine,50253;HTC-C3,,,thyroid,50254;HuCCT1,,,biliary tract,50255;huH-1,,,liver,50256;HuO-3N1,,,bone,50257;HuO9,,,bone,50258;HuO9N2,,,bone,50259;HUP-T3,,,pancreas,50260;HUP-T4,,,pancreas,50261;IGR-1,,,skin,50262;IGR-37,,,skin,50263;IGR-39,,,skin,50264;IHH-4,,,thyroid,50265;IM-95,,,stomach,50266;IM-95m,,,stomach,50267;IMR-32,,,nervous system,50268;IPC-298,,,skin,50269;J82,,,urinary bladder,50270;JAR,,,miscellaneous,50271;JHH-1,,,liver,50272;JHH-2,,,liver,50273;JHH-4,,,liver,50274;JHH-7,,,liver,50275;JIMT-1,,,breast,50276;KELLY,,,nervous system,50277;KG-1-C,,,brain,50278;KHOS/NP,,,bone,50280;KHOS-240S,,,bone,50281;KHOS-312H,,,bone,50282;KMH-2,,,thyroid,50283;KMRC-1,,,kidney,50284;KON,,,head &amp; neck,50285;KOSC-2 cl3-43,,,head &amp; neck,50286;KP-2,,,pancreas,50287;KP-3,,,pancreas,50288;KP-3L,,,pancreas,50289;KP-4,,,pancreas,50290;KPL-1,,,breast,50291;KU-19-19,,,urinary bladder,50292;KYSE-220,,,esophagus,50293;KYSE-270,,,esophagus,50294;KYSE-30,,,esophagus,50295;KYSE-410,,,esophagus,50296;KYSE-50,,,esophagus,50297;KYSE-510,,,esophagus,50298;KYSE-520,,,esophagus,50299;KYSE-70,,,esophagus,50300;LC-1 sq,,,lung,50301;LCLC-103H,,,lung,50302;LCLC-97TM1,,,lung,50303;LK-2,,,lung,50304;LN-18,,,brain,50305;LN-229,,,brain,50306;LN-405,,,brain,50307;LNZTA3WT11,,,brain,50308;LOU-NH91,,,lung,50309;LoVo,,,intestine,50310;LS174T,,,intestine,50311;LS180,,,intestine,50312;Lu-135,,,lung,50314;LU65,,,lung,50315;LU65A,,,lung,50316;LU65B,,,lung,50317;LU65C,,,lung,50318;LU99A,,,lung,50319;LU99B,,,lung,50320;LU99C,,,lung,50321;LUDLU-1,,,lung,50322;M059J,,,brain,50323;MB 157,,,breast,50324;MCAS,,,ovary,50325;MC-IXC,,,nervous system,50326;MDA-MB-134-VI,,,breast,50327;MDA-MB-157,,,breast,50328;MDA-MB-175-VII,,,breast,50329;MDA-MB-330,,,breast,50330;MDA-MB-361,,,breast,50331;MDA-MB-415,,,breast,50332;MDA-MB-436,,,breast,50333;MDA-MB-453,,,breast,50334;MDA-MB-468,,,breast,50335;MDST8,,,intestine,50336;ME-180,,,cervix,50337;MEL-HO,,,skin,50338;MEL-JUSO,,,skin,50339;MES-SA,,,uterus,50340;MES-SA/Dx-5,,,uterus,50341;MEWO,,,skin,50342;MFE-280,,,uterus,50343;MFE-296,,,uterus,50344;MFE-319,,,uterus,50345;MFM-223,,,breast,50346;MG-63,,,bone,50347;MHH-ES-1,,,nervous system,50348;MIA PaCa-2,,,pancreas,50349;MKN1,,,stomach,50350;MKN28,,,stomach,50351;MKN45,,,stomach,50352;MKN7,,,stomach,50353;MKN74,,,stomach,50354;ML-1,,,thyroid,50355;MOG-G-CCM,,,brain,50356;MOG-G-UVW,,,brain,50357;MS751,,,cervix,50358;MSTO-211H,,,pleura,50359;NB69,,,nervous system,50360;NCC-IT-A3,,,testes,50361;NCI-H1048,,,lung,50362;NCI-H1299,,,lung,50363;NCI-H1435,,,lung,50364;NCI-H1437,,,lung,50365;NCI-H1568,,,lung,50366;NCI-H1573,,,lung,50367;NCI-H1581,,,lung,50368;NCI-H1623,,,lung,50369;NCI-H1650,,,lung,50370;NCI-H1688,,,lung,50371;NCI-H1693,,,lung,50372;NCI-H1734,,,lung,50373;NCI-H1755,,,lung,50374;NCI-H1781,,,lung,50375;NCI-H1792,,,lung,50376;NCI-H1793,,,lung,50377;NCI-H1869,,,lung,50378;NCI-H1876,,,lung,50379;NCI-H1944,,,lung,50380;NCI-H196,,,lung,50381;NCI-H1993,,,lung,50382;NCI-H2009,,,lung,50383;NCI-H2029,,,lung,50384;NCI-H2030,,,lung,50385;NCI-H2073,,,lung,50386;NCI-H2085,,,lung,50387;NCI-H2087,,,lung,50388;NCI-H2110,,,lung,50389;NCI-H2122,,,lung,50390;NCI-H2135,,,lung,50391;NCI-H2170,,,lung,50392;NCI-H2172,,,lung,50393;NCI-H2195,,,lung,50394;NCI-H2196,,,lung,50395;NCI-H2198,,,lung,50396;NCI-H2228,,,lung,50397;NCI-H2286,,,lung,50398;NCI-H2291,,,lung,50399;NCI-H23,,,lung,50400;NCI-H2342,,,lung,50401;NCI-H2347,,,lung,50402;NCI-H2405,,,lung,50403;NCI-H2444,,,lung,50404;NCI-H2452,,,lung,50405;NCI-H322,,,lung,50407;NCI-H358,,,lung,50408;NCI-H441,,,lung,50409;NCI-H460,,,lung,50410;NCI-H520,,,lung,50411;NCI-H522,,,lung,50412;NCI-H596,,,lung,50413;NCI-H630,,,intestine,50414;NCI-H647,,,lung,50415;NCI-H650,,,lung,50416;NCI-H661,,,lung,50417;NCI-H727,,,lung,50418;NCI-H838,,,lung,50419;NCI-H841,,,lung,50420;NCI-N87,,,stomach,50421;NIH:OVCAR-3,,,ovary,50422;NUGC-3,,,stomach,50424;NUGC-4,,,stomach,50425;NY,,,bone,50426;OAW28,,,ovary,50427;OAW42,,,ovary,50428;OCUG-1,,,gall bladder,50429;OCUM-1,,,stomach,50430;OE19,,,esophagus,50431;OE21,,,esophagus,50432;OE33,,,esophagus,50433;OSC-19,,,head &amp; neck,50434;OSC-20,,,head &amp; neck,50435;OUMS-23,,,intestine,50436;OV-90,,,ovary,50437;OVISE,,,ovary,50438;OVKATE,,,ovary,50439;OVMIU,,,ovary,50440;OVSAYO,,,ovary,50441;OVTOKO,,,ovary,50442;PA-1,,,ovary,50443;Panc 02.03,,,pancreas,50444;Panc 03.27,,,pancreas,50445;Panc 04.03,,,pancreas,50446;Panc 08.13,,,pancreas,50447;Panc 10.05,,,pancreas,50448;PANC-1,,,pancreas,50449;PA-TU-8902,,,pancreas,50450;PA-TU-8988S,,,pancreas,50451;PA-TU-8988T,,,pancreas,50452;PC-14,,,lung,50453;PC-3,,,prostate,50454;PFSK-1,,,brain,50455;PL45,,,pancreas,50456;PLC/PRF/5,,,liver,50457;RCM-1,,,intestine,50459;RD,,,muscle,50460;RD-ES,,,nervous system,50461;RERF-GC-1B,,,stomach,50462;RERF-LC-Ad1,,,lung,50463;RERF-LC-KJ,,,lung,50464;RERF-LC-MA,,,lung,50465;RERF-LC-Sq1,,,lung,50466;RKN,,,ovary,50467;RMG-I,,,ovary,50468;RO82-W-1,,,thyroid,50469;RPMI 2650,,,head &amp; neck,50470;RPMI-7951,,,skin,50471;RT-112,,,urinary bladder,50472;RT112/84,,,urinary bladder,50473;RT4,,,urinary bladder,50474;RVH-421,,,skin,50475;S-117,,,thyroid,50476;Saos-2,,,bone,50477;SAS,,,head &amp; neck,50478;SAT,,,head &amp; neck,50479;SBC-3,,,lung,50480;SBC-5,,,lung,50481;SCaBER,,,urinary bladder,50482;SCC-15,,,head &amp; neck,50483;SCC-25,,,head &amp; neck,50484;SCC-4,,,head &amp; neck,50485;SCC-9,,,head &amp; neck,50486;SCCH-26,,,nervous system,50488;SCH,,,stomach,50489;SCLC-21H,,,lung,50490;SHP-77,,,lung,50491;SiHa,,,cervix,50493;SISO,,,cervix,50494;SK-CO-1,,,intestine,50495;SK-ES-1,,,bone,50496;SKG-IIIa,,,cervix,50497;SKG-IIIb,,,cervix,50498;SK-HEP-1,,,liver,50499;SK-LU-1,,,lung,50500;SK-MEL-2,,,skin,50501;SK-MEL-30,,,skin,50502;SKN,,,uterus,50503;SKN-3,,,head &amp; neck,50504;SK-N-AS,,,nervous system,50505;SK-N-DZ,,,nervous system,50506;SK-NEP-1,,,kidney,50507;SK-N-SH,,,nervous system,50508;SNG-M,,,uterus,50509;SNU-1,,,stomach,50510;SNU-16,,,stomach,50511;SNU-182,,,liver,50512;SNU-387,,,liver,50513;SNU-398,,,liver,50514;SNU-423,,,liver,50515;SNU-449,,,liver,50516;SNU-475,,,liver,50517;SNU-5,,,stomach,50518;SU.86.86,,,pancreas,50520;SUIT-2,,,pancreas,50521;SW 1088,,,brain,50522;SW 1271,,,lung,50524;SW 13,,,adrenal gland,50525;SW 1417,,,intestine,50526;SW 1463,,,intestine,50527;SW 156,,,kidney,50528;SW 1573,,,lung,50529;SW 1783,,,brain,50530;SW 48,,,intestine,50531;SW 626,,,ovary,50532;SW 780,,,urinary bladder,50533;SW 900,,,lung,50534;SW-1710,,,urinary bladder,50535;SW756,,,cervix,50536;SW837,,,intestine,50537;SW-948,,,intestine,50538;T.T,,,esophagus,50539;T.Tn,,,esophagus,50540;T47D,,,breast,50541;T84,,,intestine,50542;T98G,,,brain,50543;TASK1,,,nervous system,50544;TCCSUP,,,urinary bladder,50545;TGW,,,adrenal gland,50546;TOV-112D,,,ovary,50547;TOV-21G,,,ovary,50548;TT2609-C02,,,thyroid,50549;TYK-nu,,,ovary,50550;U-118 MG,,,brain,50551;U-138 MG,,,brain,50552;U-2 OS,,,bone,50553;U-251 MG,,,brain,50554;U373 MG,,,brain,50555;UACC-812,,,breast,50556;UACC-893,,,breast,50557;UMC-11,,,lung,50558;UM-UC-3,,,urinary bladder,50559;VCaP,,,prostate,50560;VM-CUB1,,,urinary bladder,50561;VMRC-LCP,,,lung,50562;VMRC-MELG,,,skin,50563;VMRC-RCW,,,kidney,50564;VMRC-RCZ,,,kidney,50565;WM 266-4,,,skin,50566;WM-115,,,skin,50567;WM1552C,,,skin,50568;WM278,,,skin,50569;WM35,,,skin,50570;WM793B,,,skin,50571;YAPC,,,pancreas,50572;YKG-1,,,brain,50573;ZR-75-1,,,breast,50574;ZR-75-30,,,breast,50575;DU4475,epithelial,,breast,50577;HCC1187,epithelial,,breast,50578;HCC1500,epithelial,,breast,50579;HCC1599,epithelial,,breast,50580;HCC2157,epithelial,,breast,50581;HCC2218,epithelial,,breast,50582;2B8,,,lymphatic system,50585;A2780cis,,,ovary,50586;A3,,,blood,50587;A3/KAW,,,lymphatic system,50588;AGR-ON,,,blood,50589;ALL-SIL,,,blood,50590;AMO-1,,,lymphatic system,50591;ARH-77,,,blood,50592;BALL-1,,,blood,50593;BC-1,,,lymphatic system,50594;BC-2,,,lymphatic system,50595;BC-3,,,lymphatic system,50596;BDCM,,,blood,50597;BE(2)-M17,,,nervous system,50598;BL-41,,,lymphatic system,50599;BL-70,,,lymphatic system,50600;C8166,,,blood,50601;CA46,,,lymphatic system,50602;CCRF-CEM,,,blood,50603;CCRF-HSB-2,,,blood,50604;CCRF-SB,,,blood,50605;CEM/C1,,,blood,50606;CEM/C2,,,blood,50607;CESS,,,blood,50608;CFPAC-1,,,pancreas,50609;ChaGo-K-1,,,lung,50610;CHP-126,,,nervous system,50611;CI-1,,,lymphatic system,50612;CL-11,,,intestine,50613;Clone 15 HL-60,,,blood,50614;CMK,,,blood,50615;COLO 684,,,uterus,50616;COLO-704,,,ovary,50617;COR-L279,,,lung,50618;COR-L51,,,lung,50619;COR-L88,,,lung,50620;COR-L95,,,lung,50621;CPC-N,,,lung,50622;CTV-1,,,blood,50623;D283 Med,,,brain,50624;Daudi,,,lymphatic system,50625;DB,,,lymphatic system,50626;DERL-2,,,lymphatic system,50627;DG-75,,,lymphatic system,50628;DMS 114,,,lung,50629;DMS 153,,,lung,50630;DMS 79,,,lung,50631;DND-41,,,blood,50632;EB1,,,lymphatic system,50633;EB2,,,lymphatic system,50634;EB-3,,,lymphatic system,50635;EHEB,,,blood,50636;EJM,,,blood,50637;Eos-HL-60,,,blood,50638;Farage,,,lymphatic system,50639;GA-10,,,lymphatic system,50640;GA-10 (Clone 20),,,lymphatic system,50641;GDM-1,,,blood,50642;GOTO,,,nervous system,50643;Gp2D,,,intestine,50644;GRANTA-519,,,lymphatic system,50645;H33HJ-JA1,,,blood,50646;HC-1,,,blood,50647;HCC-33,,,lung,50648;HDLM-2,,,lymphatic system,50649;HD-MY-Z,,,lymphatic system,50650;HEL,,,blood,50651;HEL 92.1.7,,,blood,50652;HH,,,lymphatic system,50653;HL-60,,,blood,50654;HL60(S),,,blood,50655;HL-60/MX2,,,blood,50656;HL60RG,,,blood,50657;Hs 445,,,lymphatic system,50658;HS-Sultan,,,lymphatic system,50659;HT,,,lymphatic system,50660;HuT 78,,,lymphatic system,50661;I 2.1,,,blood,50662;I 9.2,,,blood,50663;IM-9,,,lymphatic system,50664;J.gamma1,,,blood,50665;J.gamma1.WT,,,blood,50666;J.RT3-T3.5,,,blood,50667;J45.01,,,blood,50668;Jiyoye,,,lymphatic system,50669;JJN-3,,,blood,50670;JKT-beta-del,,,blood,50671;JM1,,,lymphatic system,50672;JSC-1,,,lymphatic system,50673;Jurkat, Clone E6-1,,,blood,50674;JURL-MK1,,,blood,50675;JURL-MK2,,,blood,50676;K-562,,,blood,50677;K562/ADM,,,blood,50678;KARPAS-231,,,blood,50679;KARPAS-299,,,lymphatic system,50680;KARPAS-422,,,lymphatic system,50681;KARPAS-45,,,blood,50682;KARPAS-620,,,blood,50683;Kasumi-1,,,blood,50684;KCL-22,,,blood,50685;KE-37,,,blood,50686;KG-1,,,blood,50687;KG-1a,,,blood,50688;KM-H2,,,lymphatic system,50689;KMOE-2,,,blood,50690;KMS-12-BM,,,blood,50691;KMS-12-PE,,,blood,50692;KO52,,,blood,50693;KOPN-8,,,blood,50694;KP-1N,,,pancreas,50695;KP-1NL,,,pancreas,50696;KU812,,,blood,50697;KU812E,,,blood,50698;KU812F,,,blood,50699;KY821,,,blood,50700;KY821A3,,,blood,50701;KYM-1,,,muscle,50702;L-1236,,,lymphatic system,50703;L-363,,,blood,50704;L-428,,,lymphatic system,50705;L-540,,,lymphatic system,50706;LAMA-84,,,blood,50707;LC4-1,,,blood,50708;Loucy,,,blood,50709;LP-1,,,blood,50710;Lu-134-B,,,lung,50711;M059K,,,brain,50712;MC/CAR,,,lymphatic system,50713;MC116,,,lymphatic system,50714;ME-1,,,blood,50715;MEC-1,,,blood,50716;MEC-2,,,blood,50717;MEG-01,,,blood,50718;MHH-NB-11,,,nervous system,50719;MHH-PREB-1,,,lymphatic system,50720;MJ,,,lymphatic system,50721;ML-2,,,blood,50722;MLMA,,,blood,50723;MOLM-13,,,blood,50724;MOLP-8,,,blood,50725;MOLT-14,,,blood,50726;MOLT-16,,,blood,50727;MOLT-4,,,blood,50728;MOLT-4F,,,blood,50729;MONO-MAC-1,,,blood,50730;MONO-MAC-6,,,blood,50731;MRK-nu-1,,,breast,50732;MS-1-L,,,lung,50733;MV-4-11,,,blood,50734;MY,,,blood,50735;MY-M12,,,blood,50736;MY-M13,,,blood,50737;NALM-19,,,blood,50738;NALM-6,,,blood,50739;NAMALWA,,,lymphatic system,50740;NAMALWA.PNT,,,lymphatic system,50741;NB(TU)1-10,,,nervous system,50742;NB-1,,,nervous system,50743;NB-4,,,blood,50744;NC-37,,,lymphatic system,50745;NCI-H1092,,,lung,50746;NCI-H1155,,,lung,50747;NCI-H1304,,,lung,50748;NCI-H1385,,,lung,50749;NCI-H1395,,,lung,50750;NCI-H1404,,,lung,50751;NCI-H1417,,,lung,50752;NCI-H1436,,,lung,50753;NCI-H1522,,,lung,50754;NCI-H1563,,,lung,50755;NCI-H1618,,,lung,50756;NCI-H1666,,,lung,50757;NCI-H1694,,,lung,50758;NCI-H1770,,,lung,50759;NCI-H1836,,,lung,50760;NCI-H1838,,,lung,50761;NCI-H187,,,lung,50762;NCI-H1882,,,lung,50763;NCI-H1963,,,lung,50764;NCI-H1975,,,lung,50765;NCI-H2081,,,lung,50766;NCI-H209,,,lung,50767;NCI-H2106,,,lung,50768;NCI-H211,,,lung,50769;NCI-H2141,,,lung,50770;NCI-H2171,,,lung,50771;NCI-H220,,,lung,50772;NCI-H2227,,,lung,50773;NCI-H226,,,lung,50774;NCI-H345,,,lung,50775;NCI-H446,,,lung,50776;NCI-H510A,,,lung,50777;NCI-H524,,,lung,50778;NCI-H526,,,lung,50779;NCI-H69,,,lung,50780;NCI-H719,,,lung,50781;NCI-H720,,,lung,50782;NCI-H748,,,lung,50783;NCI-H82,,,lung,50784;NCI-H847,,,lung,50785;NCI-H889,,,lung,50786;NEC8,,,testes,50787;NH-12,,,nervous system,50788;NK-92MI,,,lymphatic system,50789;NOMO-1/ADM,,,blood,50790;NU-DUL-1,,,lymphatic system,50791;OCI-AML2,,,blood,50792;OCI-AML3,,,blood,50793;OCI-AML5,,,blood,50794;OCI-LY-19,,,lymphatic system,50795;OCI-M1,,,blood,50796;OPM-2,,,blood,50797;P116.cl39,,,blood,50798;P12-ICHIKAWA,,,blood,50799;P30/OHK,,,blood,50800;P31/FUJ,,,blood,50801;P32/ISH,,,lymphatic system,50802;P3HR-1,,,lymphatic system,50803;PC-3 [JPC-3],,,lung,50804;PEER,,,blood,50805;PF-382,,,blood,50806;Pfeiffer,,,lymphatic system,50807;PL-21,,,blood,50808;PSN1,,,pancreas,50809;Raji,,,lymphatic system,50810;Ramos (RA 1),,,blood,50811;RC-K8,,,lymphatic system,50812;REC-1,,,lymphatic system,50813;Reh,,,blood,50814;RERF-LC-MS,,,lung,50815;RH-1,,,bone,50816;RH-30,,,muscle,50817;RH-41,,,muscle,50818;RL,,,lymphatic system,50819;ROS-50,,,blood,50820;RPMI 1788,,,blood,50821;RPMI 6666,,,lymphatic system,50822;RPMI 8226,,,blood,50823;RPMI-8402,,,blood,50824;RS4;11,,,blood,50825;SBC-1,,,lung,50826;SBC-2,,,lung,50827;SC-1,,,lymphatic system,50828;SCC-3,,,lymphatic system,50829;Sci-1,,,lymphatic system,50830;SIG-M5,,,blood,50831;SIMA,,,nervous system,50832;SK-MEL-1,,,skin,50833;SK-MEL-3,,,skin,50834;SK-N-BE(2),,,nervous system,50835;SK-N-FI,,,nervous system,50836;SLVL,,,lymphatic system,50837;SNB-19,,,brain,50838;SR,,,lymphatic system,50839;ST486,,,lymphatic system,50840;SU-DHL-1,,,lymphatic system,50841;SU-DHL-10,,,lymphatic system,50842;SU-DHL-16,,,lymphatic system,50843;SU-DHL-4,,,lymphatic system,50844;SU-DHL-5,,,lymphatic system,50845;SU-DHL-6,,,lymphatic system,50846;SU-DHL-8,,,lymphatic system,50847;SUP-B15,,,blood,50848;SUP-HD1,,,lymphatic system,50849;SUP-M2,,,lymphatic system,50850;SUP-T1,,,blood,50851;SVG p12,,,brain,50852;SW 1990,,,pancreas,50853;TALL-1,,,blood,50854;TANOUE,,,blood,50855;TC-71,,,bone,50856;Tera-1,,,testes,50857;TF-1,,,blood,50858;TF-1.CN5a.1,,,blood,50859;TF-1a,,,blood,50860;THP-1,,,blood,50861;TK,,,lymphatic system,50862;Toledo,,,lymphatic system,50863;TT,,,thyroid,50864;TUR,,,lymphatic system,50865;U266B1,,,blood,50866;U-698-M,,,blood,50867;U-87 MG,,,brain,50868;U-937,,,lymphatic system,50869;VAL,,,lymphatic system,50870;WIL2 NS,,,lymphatic system,50871;WILCL,,,blood,50872;WSU-DLCL2,,,lymphatic system,50873;WSU-NHL,,,lymphatic system,50874;YMB-1,,,breast,50875;YT,,,lymphatic system,50876;8-MG-BA,,,brain,50878;A253,,,head &amp; neck,50880;A498,,,kidney,50882;A704,,,kidney,50884;ACN,,,nervous system,50885;ALL-PO,,,blood,50886;AM-38,,,brain,50887;ATN-1,,,blood,50888;BB30-HNC,,,head &amp; neck,50890;BB49-HNC,,,head &amp; neck,50891;BE-13,,,blood,50893;Becker,,,brain,50894;BOKU,,,cervix,50895;BV-173,,,blood,50896;Calu-6,,,lung,50897;CAS-1,,,brain,50898;COLO-320-HSR,,,intestine,50900;COLO-668,,,lung,50901;COLO-829,,,skin,50902;CP66-MEL,,,skin,50904;CW-2,,,intestine,50906;D-247MG,,,brain,50907;D-263MG,,,brain,50908;D-336MG,,,brain,50909;D-392MG,,,brain,50910;D-542MG,,,brain,50913;DEL,,,blood,50915;DJM-1,,,skin,50916;DOHH-2,,,lymphatic system,50917;DSH1,,,urinary tract,50918;ECC12,,,stomach,50920;ECC4,,,intestine,50921;EC-GI-10,,,esophagus,50922;EKVX,,,lung,50923;EM-2,,,blood,50924;EoL-1-cell,,,blood,50925;ES1,,,bone,50926;ES4,,,bone,50928;ES5,,,bone,50929;ES6,,,bone,50930;ES7,,,bone,50931;ES8,,,bone,50932;ETK-1,,,biliary tract,50933;EW-1,,,bone,50934;EW-11,,,bone,50935;EW-13,,,bone,50936;EW-16,,,bone,50937;EW-18,,,bone,50938;EW-24,,,bone,50939;EW-3,,,bone,50940;EW-7,,,bone,50941;GAK,,,skin,50942;GB-1,,,brain,50943;GI-1,,,brain,50945;GI-ME-N,,,nervous system,50946;GR-ST,,,blood,50947;GT3TKB,,,stomach,50948;HAL-01,,,blood,50951;HCC2998,,,intestine,50952;HCE-T,,,head &amp; neck,50954;HOP-62,,,lung,50955;HT-144,,,skin,50956;IMR-5,,,nervous system,50957;IST-MES1,,,pleura,50958;IST-SL2,,,lung,50960;JVM-2,,,blood,50962;JVM-3,,,blood,50963;K5,,,thyroid,50964;KALS-1,,,brain,50965;KGN,,,ovary,50966;KINGS-1,,,brain,50967;KM12,,,intestine,50969;KNS-42,,,brain,50970;KNS-81-FD,,,brain,50971;KP-N-YS,,,nervous system,50973;KS-1,,,brain,50974;KURAMOCHI,,,ovary,50975;LAN-5,,,nervous system,50976;LAN-6,,,nervous system,50977;LB1047-RCC,,,kidney,50978;LB2241-RCC,,,kidney,50979;LB2518-MEL,,,skin,50980;LB373-MEL-D,,,skin,50981;LB771-HNC,,,head &amp; neck,50983;LB831-BLC,,,urinary tract,50984;LB996-RCC,,,kidney,50985;LOXIMVI,,,skin,50988;LS-123,,,intestine,50990;LS-411N,,,intestine,50991;LS-513,,,intestine,50992;LU-134-A,,,lung,50993;LU-165,,,lung,50995;LXF-289,,,lung,50996;MFH-ino,,,miscellaneous,50997;MHH-CALL-2,,,blood,50998;MMAC-SF,,,skin,50999;MN-60,,,blood,51000;MPP-89,,,pleura,51002;MUTZ-1,,,blood,51003;MZ1-PC,,,pancreas,51004;MZ2-MEL,,,skin,51005;MZ7-mel,,,skin,51006;NB10,,,nervous system,51007;NB13,,,nervous system,51009;NB14,,,nervous system,51010;NB16,,,nervous system,51011;NB17,,,nervous system,51012;NB5,,,nervous system,51013;NB6,,,nervous system,51014;NB7,,,nervous system,51015;NCI-H1355,,,lung,51017;NCI-H157,,,lung,51018;NCI-H2126,,,lung,51019;NCI-H322M,,,lung,51020;NCI-H64,,,lung,51021;NCI-H716,,,intestine,51022;NCI-H747,,,intestine,51023;NKM-1,,,blood,51024;NMC-G1,,,brain,51025;no-10,,,brain,51026;no-11,,,brain,51027;NOMO-1,,,blood,51028;NOS-1,,,bone,51029;NTERA-S-cl-D1,,,testes,51030;OMC-1,,,cervix,51033;ONS-76,,,brain,51034;OS-RC-2,,,kidney,51035;QIMR-WIL,,,blood,51037;Ramos-2G6-4C10,,,lymphatic system,51038;RCC10RGB,,,kidney,51039;RKO,,,intestine,51041;RL95-2,,,uterus,51042;RPMI-8866,,,blood,51043;SF126,,,brain,51045;SF268,,,brain,51046;SF539,,,brain,51047;SH-4,,,skin,51048;SK-MM-2,,,blood,51053;SK-PN-DW,,,bone,51054;SK-UT-1,,,uterus,51055;SNU-C1,,,intestine,51056;SNU-C2B,,,intestine,51057;SW403,,,intestine,51058;SW684,,,miscellaneous,51059;SW872,,,miscellaneous,51060;SW954,,,vulva,51061;SW982,,,miscellaneous,51063;TE-1,,,esophagus,51064;TE-10,,,esophagus,51065;TE-441-T,,,muscle,51069;TE-5,,,esophagus,51070;TE-6,,,esophagus,51071;TGBC11TKB,,,stomach,51074;TGBC1TKB,,,biliary tract,51075;TK10,,,kidney,51077;UACC-257,,,skin,51078;ECC10,,,stomach,50919;JEG-3,,,miscellaneous,50961;697.0,,,blood,50877;LU-139,,,lung,50994;CTB-1,,,lymphatic system,50905;ES3,,,bone,50927;TE-11,,,esophagus,51066;IST-SL1,,,lung,50959;TGBC24TKB,,,biliary tract,51076;KLE,,,uterus,50968;LC-1F,,,lung,50986;HCE-4,,,esophagus,50953;A4-Fuk,,,skin,50883;SK-MEL-24,,,skin,51050;CP50-MEL-B,,,skin,50903;YH-13,,,brain,51080;OC-314,,,ovary,51031;RF-48,,,stomach,51040;SK-MG-1,,,brain,51052;B2-17,,,brain,50889;Mo-T,,,blood,51001;KP-N-YN,,,nervous system,50972;D-423MG,,,brain,50911;H9,,,lymphatic system,50949;D-566MG,,,brain,50914;SK-MEL-5,,,skin,51051;NBsusSR,,,nervous system,51016;A101D,,,skin,50879;A388,,,miscellaneous,50881;BB65-RCC,,,kidney,50892;D-502MG,,,brain,50912;GCIY,,,stomach,50944;HA7-RCC,,,kidney,50950;LC-2-ad,,,lung,50987;LS-1034,,,intestine,50989;NB12,,,nervous system,51008;OCUB-M,,,breast,51032;OVCAR-4,,,ovary,51036;RXF393,,,kidney,51044;SJSA-1,,,bone,51049;SW962,,,vulva,51062;TE-12,,,esophagus,51067;TE-15,,,esophagus,51068;TE-8,,,esophagus,51072;TE-9,,,esophagus,51073;VA-ES-BJ,,,miscellaneous,51079;CGTH-W-1,,,thyroid,50899;LB647-SCLC,,,lung,50982</t>
+  </si>
+  <si>
+    <t>1057\cell lines</t>
+  </si>
+  <si>
+    <t>AZD-6482,small molecule,10059-101,LSM-1059;JNK-9L,small molecule,10100-101,None;HG-6-64-01,small molecule,10017-101,LSM-6015</t>
+  </si>
+  <si>
+    <t>http://lincs.hms.harvard.edu/db/datasets/20009/</t>
+  </si>
+  <si>
+    <t>MGH (CMT) Growth Inhibition Assay Protocol (9 compound doses: 2.56 uM to 0.01 uM) -- DNA Staining</t>
+  </si>
+  <si>
+    <t>5637.0,epithelial,,urinary bladder,50001;647-V,epithelial-like,,urinary bladder,50002;A375.S2,epithelial,,skin,50003;AGS,epithelial,,stomach,50004;BPH-1,epitheloid,,prostate,50005;Ca Ski,epithelial,,cervix,50006;Ca9-22,epithelial-like,,head &amp; neck,50007;CAL-51,epithelial-like,,breast,50008;Calu-1,epithelial,,lung,50009;Calu-3,epithelial,,lung,50010;COLO-679,fibroblastic,,skin,50011;COLO-800,epithelial-like,,skin,50012;FU97,epithelial-like,,stomach,50013;HEC-1,,,uterus,50014;HLF,,,liver,50015;HUTU-80,epithelial,,intestine,50016;IA-LM,,,lung,50017;Ishikawa,epithelial-like,,uterus,50018;Ishikawa (Heraklio) 02 ER-,epithelial,,uterus,50019;IST-MEL1,epithelial-like,,skin,50020;JHH-6,epithelial-like,,liver,50021;KMRC-20,epithelial-like,,kidney,50023;KYSE-140,,,esophagus,50024;KYSE-150,epitheloid,,esophagus,50025;KYSE-180,epitheloid,,esophagus,50026;KYSE-450,epitheloid,,esophagus,50027;LNZTA3WT4,,,brain,50028;MCF7,epithelial,,breast,50029;MDA-MB-435S,melanocyte,,skin,50030;MT-3,epithelial,,breast,50031;NCI-H1648,,,lung,50032;NCI-H1651,epithelial,,lung,50033;NCI-H1703,epithelial,,lung,50034;NCI-H1915,large cell,,lung,50035;NCI-H2023,,,lung,50036;NCI-H810,epithelial,,lung,50037;PE/CA-PJ15,epithelial-like,,head &amp; neck,50039;SJCRH30,fibroblast,,muscle,50041;SK-LMS-1,,,uterus,50042;SK-MES,epithelial,,lung,50043;SK-OV-3,epithelial,,ovary,50044;SNB75,,,brain,50045;SW527,epithelial,,breast,50046;SW620,epithelial,,intestine,50047;T24,epithelial,,urinary bladder,50048;WiDr,epithelial,,intestine,50049;Hep 3B2.1-7,epithelial,,liver,50051;Hep G2,epithelial,,liver,50052;Huh7,,,liver,50055;SK-BR-3,epithelial,,breast,50057;MDA-MB-231,epithelial,,breast,50058;LNCaP,epithelial,,prostate,50059;A-375,epithelial,,skin,50060;HeLa,epithelial,,cervix,50061;1205Lu,,,skin,50062;1321N1,,,brain,50063;143B,,,bone,50064;143B PML BK TK,,,bone,50065;1A6,,,urinary bladder,50066;22RV1,,,prostate,50067;23132/87,,,stomach,50068;42-MG-BA,,,brain,50069;639-V,,,ureter,50071;769-P,,,kidney,50072;786-O,,,kidney,50073;8305C,,,thyroid,50074;8505C,,,thyroid,50075;A172,,,brain,50076;A-204,,,muscle,50077;A2058,,,skin,50078;A2780,,,ovary,50079;A2780ADR,,,ovary,50080;A373-C6,,,skin,50081;A-427,,,lung,50082;A431,,,skin,50083;A549,,,lung,50084;A673,,,muscle,50085;ABC-1,,,lung,50086;ACHN,,,kidney,50087;AN3CA,,,uterus,50088;ASH-3,,,thyroid,50089;AsPC-1,,,pancreas,50090;AU565,,,breast,50091;AZ-521,,,stomach,50092;B-CPAP,,,thyroid,50093;BE(2)-C,,,nervous system,50094;BEN,,,lung,50095;BeWo,,,miscellaneous,50096;BFTC-905,,,urinary bladder,50097;BFTC-909,,,kidney,50098;BHT-101,,,thyroid,50099;BHY,,,head &amp; neck,50100;BICR 10,,,head &amp; neck,50101;BICR 22,,,head &amp; neck,50102;BICR 31,,,head &amp; neck,50103;BICR 78,,,head &amp; neck,50104;BT-20,,,breast,50105;BT-474,,,breast,50106;BT-483,,,breast,50107;BT-549,,,breast,50108;BxPC-3,,,pancreas,50109;C170,,,intestine,50110;C2BBe1,,,intestine,50111;C32,,,skin,50112;C-33 A,,,cervix,50113;C3A,,,liver,50114;C-4 I,,,cervix,50115;C-4 II,,,cervix,50116;Caco-2,,,intestine,50117;Caki-1,,,kidney,50118;CAL 27,,,head &amp; neck,50119;CAL-120,,,breast,50120;CAL-12T,,,lung,50121;CAL-148,,,breast,50122;CAL-29,,,urinary bladder,50123;CAL-33,,,head &amp; neck,50124;CAL-39,,,vulva,50125;CAL-54,,,kidney,50126;CAL-62,,,thyroid,50127;CAL-72,,,bone,50128;CAL-78,,,bone,50129;CAL-85-1,,,breast,50130;CAMA-1,,,breast,50131;Caov-3,,,ovary,50132;Caov-4,,,ovary,50133;Capan-1,,,pancreas,50134;Capan-2,,,pancreas,50135;CaR-1,,,intestine,50136;CCF-STTG1,,,brain,50137;CCK-81,,,intestine,50138;CHP-212,,,nervous system,50139;CoCM-1,,,intestine,50141;COLO 201,,,intestine,50142;COLO 205,,,intestine,50143;COLO 320DM,,,intestine,50144;COLO 741,,,intestine,50145;COLO 792,,,skin,50146;COLO 853,,,skin,50147;COLO 857,,,skin,50148;COLO 858,,,skin,50149;COLO-206F,,,intestine,50150;COLO-320,,,intestine,50151;COLO-678,,,intestine,50152;COLO-680N,,,esophagus,50153;COLO-783,,,skin,50154;COLO-818,,,skin,50155;COLO-824,,,breast,50156;COLO-849,,,skin,50157;COR-L 105,,,lung,50158;COR-L 23/CPR,,,lung,50159;COR-L23,,,lung,50160;DAN-G,,,pancreas,50161;Daoy,,,brain,50162;DBTRG-05MG,,,brain,50163;Detroit 562,,,head &amp; neck,50164;DK-MG,,,brain,50165;DLD-1,,,intestine,50166;DMS 273,,,lung,50167;DMS 53,,,lung,50168;DOK,,,head &amp; neck,50169;DoTc2 4510,,,cervix,50170;DU 145,,,prostate,50171;DV-90,,,lung,50172;EBC-1,,,lung,50173;EFE-184,,,uterus,50174;EFM-19,,,breast,50175;EFM-192A,,,breast,50176;EFM-192B,,,breast,50177;EFM-192C,,,breast,50178;EFO-21,,,ovary,50179;EFO-27,,,ovary,50180;EGI-1,,,biliary tract,50181;EJ138,,,urinary bladder,50182;EN,,,uterus,50183;EPLC-272H,,,lung,50184;ES-2,,,ovary,50185;ESS-1,,,uterus,50186;EVSA-T,,,breast,50187;FaDu,,,head &amp; neck,50188;FLYA13,,,miscellaneous,50189;FTC-133,,,thyroid,50190;FTC-238,,,thyroid,50191;FU-OV-1,,,ovary,50192;G-292 Clone A141B1,,,bone,50193;G-361,,,skin,50194;G-401,,,kidney,50195;G-402,,,kidney,50196;GAMG,,,brain,50197;GCT,,,miscellaneous,50198;GMS-10,,,brain,50199;GOS-3,,,brain,50200;GP5d,,,intestine,50201;H4,,,brain,50202;HARA,,,lung,50204;HCC1143,,,breast,50205;HCC1395,,,breast,50206;HCC1419,,,breast,50207;HCC1428,,,breast,50208;HCC-15,,,lung,50209;HCC1569,,,breast,50210;HCC1806,,,breast,50211;HCC1937,,,breast,50212;HCC1954,,,breast,50213;HCC-366,,,lung,50215;HCC38,,,breast,50216;HCC-44,,,lung,50217;HCC-56,,,intestine,50218;HCC70,,,breast,50219;HCC-78,,,lung,50220;HCC-827,,,lung,50221;HCT 116,,,intestine,50222;HCT-15,,,intestine,50223;HCT-8,,,intestine,50224;HDQ-P1,,,breast,50225;H-EMC-SS,,,bone,50226;HGC-27,,,stomach,50227;HLE,,,liver,50228;HMVII,,,skin,50229;HN,,,head &amp; neck,50230;HO-1-N-1,,,head &amp; neck,50231;HO-1-u-1,,,head &amp; neck,50232;HOS,,,bone,50233;HPAC,,,pancreas,50234;HPAF-II,,,pancreas,50235;HRT-18,,,intestine,50236;Hs 257.T,,,intestine,50237;Hs 578T,,,breast,50238;Hs 588.T,,,cervix,50239;Hs 633T,,,miscellaneous,50240;Hs 683,,,brain,50241;Hs 746T,,,stomach,50242;Hs 766T,,,pancreas,50243;HSC-2,,,head &amp; neck,50244;HSC-3,,,head &amp; neck,50245;HSC-4,,,head &amp; neck,50246;HT 1080,,,miscellaneous,50247;HT 1376,,,urinary bladder,50248;HT115,,,intestine,50249;HT-1197,,,urinary bladder,50250;HT-29,,,intestine,50251;HT-3,,,cervix,50252;HT55,,,intestine,50253;HTC-C3,,,thyroid,50254;HuCCT1,,,biliary tract,50255;huH-1,,,liver,50256;HuO-3N1,,,bone,50257;HuO9,,,bone,50258;HuO9N2,,,bone,50259;HUP-T3,,,pancreas,50260;HUP-T4,,,pancreas,50261;IGR-1,,,skin,50262;IGR-37,,,skin,50263;IGR-39,,,skin,50264;IHH-4,,,thyroid,50265;IM-95,,,stomach,50266;IM-95m,,,stomach,50267;IMR-32,,,nervous system,50268;IPC-298,,,skin,50269;J82,,,urinary bladder,50270;JAR,,,miscellaneous,50271;JHH-1,,,liver,50272;JHH-2,,,liver,50273;JHH-4,,,liver,50274;JHH-7,,,liver,50275;JIMT-1,,,breast,50276;KELLY,,,nervous system,50277;KG-1-C,,,brain,50278;KHOS/NP,,,bone,50280;KHOS-240S,,,bone,50281;KHOS-312H,,,bone,50282;KMH-2,,,thyroid,50283;KMRC-1,,,kidney,50284;KON,,,head &amp; neck,50285;KOSC-2 cl3-43,,,head &amp; neck,50286;KP-2,,,pancreas,50287;KP-3,,,pancreas,50288;KP-3L,,,pancreas,50289;KP-4,,,pancreas,50290;KPL-1,,,breast,50291;KU-19-19,,,urinary bladder,50292;KYSE-220,,,esophagus,50293;KYSE-270,,,esophagus,50294;KYSE-30,,,esophagus,50295;KYSE-410,,,esophagus,50296;KYSE-50,,,esophagus,50297;KYSE-510,,,esophagus,50298;KYSE-520,,,esophagus,50299;KYSE-70,,,esophagus,50300;LC-1 sq,,,lung,50301;LCLC-103H,,,lung,50302;LCLC-97TM1,,,lung,50303;LK-2,,,lung,50304;LN-18,,,brain,50305;LN-229,,,brain,50306;LN-405,,,brain,50307;LNZTA3WT11,,,brain,50308;LOU-NH91,,,lung,50309;LoVo,,,intestine,50310;LS174T,,,intestine,50311;LS180,,,intestine,50312;Lu-135,,,lung,50314;LU65,,,lung,50315;LU65A,,,lung,50316;LU65B,,,lung,50317;LU65C,,,lung,50318;LU99A,,,lung,50319;LU99B,,,lung,50320;LU99C,,,lung,50321;LUDLU-1,,,lung,50322;M059J,,,brain,50323;MB 157,,,breast,50324;MCAS,,,ovary,50325;MC-IXC,,,nervous system,50326;MDA-MB-134-VI,,,breast,50327;MDA-MB-157,,,breast,50328;MDA-MB-175-VII,,,breast,50329;MDA-MB-330,,,breast,50330;MDA-MB-361,,,breast,50331;MDA-MB-415,,,breast,50332;MDA-MB-436,,,breast,50333;MDA-MB-453,,,breast,50334;MDA-MB-468,,,breast,50335;MDST8,,,intestine,50336;ME-180,,,cervix,50337;MEL-HO,,,skin,50338;MEL-JUSO,,,skin,50339;MES-SA,,,uterus,50340;MES-SA/Dx-5,,,uterus,50341;MEWO,,,skin,50342;MFE-280,,,uterus,50343;MFE-296,,,uterus,50344;MFE-319,,,uterus,50345;MFM-223,,,breast,50346;MG-63,,,bone,50347;MHH-ES-1,,,nervous system,50348;MIA PaCa-2,,,pancreas,50349;MKN1,,,stomach,50350;MKN28,,,stomach,50351;MKN45,,,stomach,50352;MKN7,,,stomach,50353;MKN74,,,stomach,50354;ML-1,,,thyroid,50355;MOG-G-CCM,,,brain,50356;MOG-G-UVW,,,brain,50357;MS751,,,cervix,50358;MSTO-211H,,,pleura,50359;NB69,,,nervous system,50360;NCC-IT-A3,,,testes,50361;NCI-H1048,,,lung,50362;NCI-H1299,,,lung,50363;NCI-H1435,,,lung,50364;NCI-H1437,,,lung,50365;NCI-H1568,,,lung,50366;NCI-H1573,,,lung,50367;NCI-H1581,,,lung,50368;NCI-H1623,,,lung,50369;NCI-H1650,,,lung,50370;NCI-H1688,,,lung,50371;NCI-H1693,,,lung,50372;NCI-H1734,,,lung,50373;NCI-H1755,,,lung,50374;NCI-H1781,,,lung,50375;NCI-H1792,,,lung,50376;NCI-H1793,,,lung,50377;NCI-H1869,,,lung,50378;NCI-H1876,,,lung,50379;NCI-H1944,,,lung,50380;NCI-H196,,,lung,50381;NCI-H1993,,,lung,50382;NCI-H2009,,,lung,50383;NCI-H2029,,,lung,50384;NCI-H2030,,,lung,50385;NCI-H2073,,,lung,50386;NCI-H2085,,,lung,50387;NCI-H2087,,,lung,50388;NCI-H2110,,,lung,50389;NCI-H2122,,,lung,50390;NCI-H2135,,,lung,50391;NCI-H2170,,,lung,50392;NCI-H2172,,,lung,50393;NCI-H2195,,,lung,50394;NCI-H2196,,,lung,50395;NCI-H2198,,,lung,50396;NCI-H2228,,,lung,50397;NCI-H2286,,,lung,50398;NCI-H2291,,,lung,50399;NCI-H23,,,lung,50400;NCI-H2342,,,lung,50401;NCI-H2347,,,lung,50402;NCI-H2405,,,lung,50403;NCI-H2444,,,lung,50404;NCI-H2452,,,lung,50405;NCI-H322,,,lung,50407;NCI-H358,,,lung,50408;NCI-H441,,,lung,50409;NCI-H460,,,lung,50410;NCI-H520,,,lung,50411;NCI-H522,,,lung,50412;NCI-H596,,,lung,50413;NCI-H630,,,intestine,50414;NCI-H647,,,lung,50415;NCI-H650,,,lung,50416;NCI-H661,,,lung,50417;NCI-H727,,,lung,50418;NCI-H838,,,lung,50419;NCI-H841,,,lung,50420;NCI-N87,,,stomach,50421;NIH:OVCAR-3,,,ovary,50422;NUGC-3,,,stomach,50424;NUGC-4,,,stomach,50425;NY,,,bone,50426;OAW28,,,ovary,50427;OAW42,,,ovary,50428;OCUG-1,,,gall bladder,50429;OCUM-1,,,stomach,50430;OE19,,,esophagus,50431;OE21,,,esophagus,50432;OE33,,,esophagus,50433;OSC-19,,,head &amp; neck,50434;OSC-20,,,head &amp; neck,50435;OUMS-23,,,intestine,50436;OV-90,,,ovary,50437;OVISE,,,ovary,50438;OVKATE,,,ovary,50439;OVMIU,,,ovary,50440;OVSAYO,,,ovary,50441;OVTOKO,,,ovary,50442;PA-1,,,ovary,50443;Panc 02.03,,,pancreas,50444;Panc 03.27,,,pancreas,50445;Panc 04.03,,,pancreas,50446;Panc 08.13,,,pancreas,50447;Panc 10.05,,,pancreas,50448;PANC-1,,,pancreas,50449;PA-TU-8902,,,pancreas,50450;PA-TU-8988S,,,pancreas,50451;PA-TU-8988T,,,pancreas,50452;PC-14,,,lung,50453;PC-3,,,prostate,50454;PFSK-1,,,brain,50455;PL45,,,pancreas,50456;PLC/PRF/5,,,liver,50457;RCM-1,,,intestine,50459;RD,,,muscle,50460;RD-ES,,,nervous system,50461;RERF-GC-1B,,,stomach,50462;RERF-LC-Ad1,,,lung,50463;RERF-LC-KJ,,,lung,50464;RERF-LC-MA,,,lung,50465;RERF-LC-Sq1,,,lung,50466;RKN,,,ovary,50467;RMG-I,,,ovary,50468;RO82-W-1,,,thyroid,50469;RPMI 2650,,,head &amp; neck,50470;RPMI-7951,,,skin,50471;RT-112,,,urinary bladder,50472;RT112/84,,,urinary bladder,50473;RT4,,,urinary bladder,50474;RVH-421,,,skin,50475;S-117,,,thyroid,50476;Saos-2,,,bone,50477;SAS,,,head &amp; neck,50478;SAT,,,head &amp; neck,50479;SBC-3,,,lung,50480;SBC-5,,,lung,50481;SCaBER,,,urinary bladder,50482;SCC-15,,,head &amp; neck,50483;SCC-25,,,head &amp; neck,50484;SCC-4,,,head &amp; neck,50485;SCC-9,,,head &amp; neck,50486;SCCH-26,,,nervous system,50488;SCH,,,stomach,50489;SCLC-21H,,,lung,50490;SHP-77,,,lung,50491;SiHa,,,cervix,50493;SISO,,,cervix,50494;SK-CO-1,,,intestine,50495;SK-ES-1,,,bone,50496;SKG-IIIa,,,cervix,50497;SKG-IIIb,,,cervix,50498;SK-HEP-1,,,liver,50499;SK-LU-1,,,lung,50500;SK-MEL-2,,,skin,50501;SK-MEL-30,,,skin,50502;SKN,,,uterus,50503;SKN-3,,,head &amp; neck,50504;SK-N-AS,,,nervous system,50505;SK-N-DZ,,,nervous system,50506;SK-NEP-1,,,kidney,50507;SK-N-SH,,,nervous system,50508;SNG-M,,,uterus,50509;SNU-1,,,stomach,50510;SNU-16,,,stomach,50511;SNU-182,,,liver,50512;SNU-387,,,liver,50513;SNU-398,,,liver,50514;SNU-423,,,liver,50515;SNU-449,,,liver,50516;SNU-475,,,liver,50517;SNU-5,,,stomach,50518;SU.86.86,,,pancreas,50520;SUIT-2,,,pancreas,50521;SW 1088,,,brain,50522;SW 1271,,,lung,50524;SW 13,,,adrenal gland,50525;SW 1417,,,intestine,50526;SW 1463,,,intestine,50527;SW 156,,,kidney,50528;SW 1573,,,lung,50529;SW 1783,,,brain,50530;SW 48,,,intestine,50531;SW 626,,,ovary,50532;SW 780,,,urinary bladder,50533;SW 900,,,lung,50534;SW-1710,,,urinary bladder,50535;SW756,,,cervix,50536;SW837,,,intestine,50537;SW-948,,,intestine,50538;T.T,,,esophagus,50539;T.Tn,,,esophagus,50540;T47D,,,breast,50541;T84,,,intestine,50542;T98G,,,brain,50543;TASK1,,,nervous system,50544;TCCSUP,,,urinary bladder,50545;TGW,,,adrenal gland,50546;TOV-112D,,,ovary,50547;TOV-21G,,,ovary,50548;TT2609-C02,,,thyroid,50549;TYK-nu,,,ovary,50550;U-118 MG,,,brain,50551;U-138 MG,,,brain,50552;U-2 OS,,,bone,50553;U-251 MG,,,brain,50554;U373 MG,,,brain,50555;UACC-812,,,breast,50556;UACC-893,,,breast,50557;UMC-11,,,lung,50558;UM-UC-3,,,urinary bladder,50559;VCaP,,,prostate,50560;VM-CUB1,,,urinary bladder,50561;VMRC-LCP,,,lung,50562;VMRC-MELG,,,skin,50563;VMRC-RCW,,,kidney,50564;VMRC-RCZ,,,kidney,50565;WM 266-4,,,skin,50566;WM-115,,,skin,50567;WM1552C,,,skin,50568;WM278,,,skin,50569;WM35,,,skin,50570;WM793B,,,skin,50571;YAPC,,,pancreas,50572;YKG-1,,,brain,50573;ZR-75-1,,,breast,50574;ZR-75-30,,,breast,50575;DU4475,epithelial,,breast,50577;HCC1187,epithelial,,breast,50578;HCC1500,epithelial,,breast,50579;HCC1599,epithelial,,breast,50580;HCC2157,epithelial,,breast,50581;HCC2218,epithelial,,breast,50582;2B8,,,lymphatic system,50585;A2780cis,,,ovary,50586;A3,,,blood,50587;A3/KAW,,,lymphatic system,50588;AGR-ON,,,blood,50589;ALL-SIL,,,blood,50590;AMO-1,,,lymphatic system,50591;ARH-77,,,blood,50592;BALL-1,,,blood,50593;BC-1,,,lymphatic system,50594;BC-2,,,lymphatic system,50595;BC-3,,,lymphatic system,50596;BDCM,,,blood,50597;BE(2)-M17,,,nervous system,50598;BL-41,,,lymphatic system,50599;BL-70,,,lymphatic system,50600;C8166,,,blood,50601;CA46,,,lymphatic system,50602;CCRF-CEM,,,blood,50603;CCRF-HSB-2,,,blood,50604;CCRF-SB,,,blood,50605;CEM/C1,,,blood,50606;CEM/C2,,,blood,50607;CESS,,,blood,50608;CFPAC-1,,,pancreas,50609;ChaGo-K-1,,,lung,50610;CHP-126,,,nervous system,50611;CI-1,,,lymphatic system,50612;CL-11,,,intestine,50613;Clone 15 HL-60,,,blood,50614;CMK,,,blood,50615;COLO 684,,,uterus,50616;COLO-704,,,ovary,50617;COR-L279,,,lung,50618;COR-L51,,,lung,50619;COR-L88,,,lung,50620;COR-L95,,,lung,50621;CPC-N,,,lung,50622;CTV-1,,,blood,50623;D283 Med,,,brain,50624;Daudi,,,lymphatic system,50625;DB,,,lymphatic system,50626;DERL-2,,,lymphatic system,50627;DG-75,,,lymphatic system,50628;DMS 114,,,lung,50629;DMS 153,,,lung,50630;DMS 79,,,lung,50631;DND-41,,,blood,50632;EB1,,,lymphatic system,50633;EB2,,,lymphatic system,50634;EB-3,,,lymphatic system,50635;EHEB,,,blood,50636;EJM,,,blood,50637;Eos-HL-60,,,blood,50638;Farage,,,lymphatic system,50639;GA-10,,,lymphatic system,50640;GA-10 (Clone 20),,,lymphatic system,50641;GDM-1,,,blood,50642;GOTO,,,nervous system,50643;Gp2D,,,intestine,50644;GRANTA-519,,,lymphatic system,50645;H33HJ-JA1,,,blood,50646;HC-1,,,blood,50647;HCC-33,,,lung,50648;HDLM-2,,,lymphatic system,50649;HD-MY-Z,,,lymphatic system,50650;HEL,,,blood,50651;HEL 92.1.7,,,blood,50652;HH,,,lymphatic system,50653;HL-60,,,blood,50654;HL60(S),,,blood,50655;HL-60/MX2,,,blood,50656;HL60RG,,,blood,50657;Hs 445,,,lymphatic system,50658;HS-Sultan,,,lymphatic system,50659;HT,,,lymphatic system,50660;HuT 78,,,lymphatic system,50661;I 2.1,,,blood,50662;I 9.2,,,blood,50663;IM-9,,,lymphatic system,50664;J.gamma1,,,blood,50665;J.gamma1.WT,,,blood,50666;J.RT3-T3.5,,,blood,50667;J45.01,,,blood,50668;Jiyoye,,,lymphatic system,50669;JJN-3,,,blood,50670;JKT-beta-del,,,blood,50671;JM1,,,lymphatic system,50672;JSC-1,,,lymphatic system,50673;Jurkat, Clone E6-1,,,blood,50674;JURL-MK1,,,blood,50675;JURL-MK2,,,blood,50676;K-562,,,blood,50677;K562/ADM,,,blood,50678;KARPAS-231,,,blood,50679;KARPAS-299,,,lymphatic system,50680;KARPAS-422,,,lymphatic system,50681;KARPAS-45,,,blood,50682;KARPAS-620,,,blood,50683;Kasumi-1,,,blood,50684;KCL-22,,,blood,50685;KE-37,,,blood,50686;KG-1,,,blood,50687;KG-1a,,,blood,50688;KM-H2,,,lymphatic system,50689;KMOE-2,,,blood,50690;KMS-12-BM,,,blood,50691;KMS-12-PE,,,blood,50692;KO52,,,blood,50693;KOPN-8,,,blood,50694;KP-1N,,,pancreas,50695;KP-1NL,,,pancreas,50696;KU812,,,blood,50697;KU812E,,,blood,50698;KU812F,,,blood,50699;KY821,,,blood,50700;KY821A3,,,blood,50701;KYM-1,,,muscle,50702;L-1236,,,lymphatic system,50703;L-363,,,blood,50704;L-428,,,lymphatic system,50705;L-540,,,lymphatic system,50706;LAMA-84,,,blood,50707;LC4-1,,,blood,50708;Loucy,,,blood,50709;LP-1,,,blood,50710;Lu-134-B,,,lung,50711;M059K,,,brain,50712;MC/CAR,,,lymphatic system,50713;MC116,,,lymphatic system,50714;ME-1,,,blood,50715;MEC-1,,,blood,50716;MEC-2,,,blood,50717;MEG-01,,,blood,50718;MHH-NB-11,,,nervous system,50719;MHH-PREB-1,,,lymphatic system,50720;MJ,,,lymphatic system,50721;ML-2,,,blood,50722;MLMA,,,blood,50723;MOLM-13,,,blood,50724;MOLP-8,,,blood,50725;MOLT-14,,,blood,50726;MOLT-16,,,blood,50727;MOLT-4,,,blood,50728;MOLT-4F,,,blood,50729;MONO-MAC-1,,,blood,50730;MONO-MAC-6,,,blood,50731;MRK-nu-1,,,breast,50732;MS-1-L,,,lung,50733;MV-4-11,,,blood,50734;MY,,,blood,50735;MY-M12,,,blood,50736;MY-M13,,,blood,50737;NALM-19,,,blood,50738;NALM-6,,,blood,50739;NAMALWA,,,lymphatic system,50740;NAMALWA.PNT,,,lymphatic system,50741;NB(TU)1-10,,,nervous system,50742;NB-1,,,nervous system,50743;NB-4,,,blood,50744;NC-37,,,lymphatic system,50745;NCI-H1092,,,lung,50746;NCI-H1155,,,lung,50747;NCI-H1304,,,lung,50748;NCI-H1385,,,lung,50749;NCI-H1395,,,lung,50750;NCI-H1404,,,lung,50751;NCI-H1417,,,lung,50752;NCI-H1436,,,lung,50753;NCI-H1522,,,lung,50754;NCI-H1563,,,lung,50755;NCI-H1618,,,lung,50756;NCI-H1666,,,lung,50757;NCI-H1694,,,lung,50758;NCI-H1770,,,lung,50759;NCI-H1836,,,lung,50760;NCI-H1838,,,lung,50761;NCI-H187,,,lung,50762;NCI-H1882,,,lung,50763;NCI-H1963,,,lung,50764;NCI-H1975,,,lung,50765;NCI-H2081,,,lung,50766;NCI-H209,,,lung,50767;NCI-H2106,,,lung,50768;NCI-H211,,,lung,50769;NCI-H2141,,,lung,50770;NCI-H2171,,,lung,50771;NCI-H220,,,lung,50772;NCI-H2227,,,lung,50773;NCI-H226,,,lung,50774;NCI-H345,,,lung,50775;NCI-H446,,,lung,50776;NCI-H510A,,,lung,50777;NCI-H524,,,lung,50778;NCI-H526,,,lung,50779;NCI-H69,,,lung,50780;NCI-H719,,,lung,50781;NCI-H720,,,lung,50782;NCI-H748,,,lung,50783;NCI-H82,,,lung,50784;NCI-H847,,,lung,50785;NCI-H889,,,lung,50786;NEC8,,,testes,50787;NH-12,,,nervous system,50788;NK-92MI,,,lymphatic system,50789;NOMO-1/ADM,,,blood,50790;NU-DUL-1,,,lymphatic system,50791;OCI-AML2,,,blood,50792;OCI-AML3,,,blood,50793;OCI-AML5,,,blood,50794;OCI-LY-19,,,lymphatic system,50795;OCI-M1,,,blood,50796;OPM-2,,,blood,50797;P116.cl39,,,blood,50798;P12-ICHIKAWA,,,blood,50799;P30/OHK,,,blood,50800;P31/FUJ,,,blood,50801;P32/ISH,,,lymphatic system,50802;P3HR-1,,,lymphatic system,50803;PC-3 [JPC-3],,,lung,50804;PEER,,,blood,50805;PF-382,,,blood,50806;Pfeiffer,,,lymphatic system,50807;PL-21,,,blood,50808;PSN1,,,pancreas,50809;Raji,,,lymphatic system,50810;Ramos (RA 1),,,blood,50811;RC-K8,,,lymphatic system,50812;REC-1,,,lymphatic system,50813;Reh,,,blood,50814;RERF-LC-MS,,,lung,50815;RH-1,,,bone,50816;RH-30,,,muscle,50817;RH-41,,,muscle,50818;RL,,,lymphatic system,50819;ROS-50,,,blood,50820;RPMI 1788,,,blood,50821;RPMI 6666,,,lymphatic system,50822;RPMI 8226,,,blood,50823;RPMI-8402,,,blood,50824;RS4;11,,,blood,50825;SBC-1,,,lung,50826;SBC-2,,,lung,50827;SC-1,,,lymphatic system,50828;SCC-3,,,lymphatic system,50829;Sci-1,,,lymphatic system,50830;SIG-M5,,,blood,50831;SIMA,,,nervous system,50832;SK-MEL-1,,,skin,50833;SK-MEL-3,,,skin,50834;SK-N-BE(2),,,nervous system,50835;SK-N-FI,,,nervous system,50836;SLVL,,,lymphatic system,50837;SNB-19,,,brain,50838;SR,,,lymphatic system,50839;ST486,,,lymphatic system,50840;SU-DHL-1,,,lymphatic system,50841;SU-DHL-10,,,lymphatic system,50842;SU-DHL-16,,,lymphatic system,50843;SU-DHL-4,,,lymphatic system,50844;SU-DHL-5,,,lymphatic system,50845;SU-DHL-6,,,lymphatic system,50846;SU-DHL-8,,,lymphatic system,50847;SUP-B15,,,blood,50848;SUP-HD1,,,lymphatic system,50849;SUP-M2,,,lymphatic system,50850;SUP-T1,,,blood,50851;SVG p12,,,brain,50852;SW 1990,,,pancreas,50853;TALL-1,,,blood,50854;TANOUE,,,blood,50855;TC-71,,,bone,50856;Tera-1,,,testes,50857;TF-1,,,blood,50858;TF-1.CN5a.1,,,blood,50859;TF-1a,,,blood,50860;THP-1,,,blood,50861;TK,,,lymphatic system,50862;Toledo,,,lymphatic system,50863;TT,,,thyroid,50864;TUR,,,lymphatic system,50865;U266B1,,,blood,50866;U-698-M,,,blood,50867;U-87 MG,,,brain,50868;U-937,,,lymphatic system,50869;VAL,,,lymphatic system,50870;WIL2 NS,,,lymphatic system,50871;WILCL,,,blood,50872;WSU-DLCL2,,,lymphatic system,50873;WSU-NHL,,,lymphatic system,50874;YMB-1,,,breast,50875;YT,,,lymphatic system,50876;HCC202,,,breast,50214;CGTH-W-1,,,thyroid,50899;LB647-SCLC,,,lung,50982;8-MG-BA,,,brain,50878;A253,,,head &amp; neck,50880;A498,,,kidney,50882;A704,,,kidney,50884;ACN,,,nervous system,50885;ALL-PO,,,blood,50886;AM-38,,,brain,50887;ATN-1,,,blood,50888;BB30-HNC,,,head &amp; neck,50890;BB49-HNC,,,head &amp; neck,50891;BE-13,,,blood,50893;Becker,,,brain,50894;BOKU,,,cervix,50895;BV-173,,,blood,50896;Calu-6,,,lung,50897;CAS-1,,,brain,50898;COLO-320-HSR,,,intestine,50900;COLO-668,,,lung,50901;COLO-829,,,skin,50902;CP66-MEL,,,skin,50904;CW-2,,,intestine,50906;D-247MG,,,brain,50907;D-263MG,,,brain,50908;D-336MG,,,brain,50909;D-392MG,,,brain,50910;D-542MG,,,brain,50913;DEL,,,blood,50915;DJM-1,,,skin,50916;DOHH-2,,,lymphatic system,50917;DSH1,,,urinary tract,50918;ECC12,,,stomach,50920;ECC4,,,intestine,50921;EC-GI-10,,,esophagus,50922;EKVX,,,lung,50923;EM-2,,,blood,50924;EoL-1-cell,,,blood,50925;ES1,,,bone,50926;ES4,,,bone,50928;ES5,,,bone,50929;ES6,,,bone,50930;ES7,,,bone,50931;ES8,,,bone,50932;ETK-1,,,biliary tract,50933;EW-1,,,bone,50934;EW-11,,,bone,50935;EW-13,,,bone,50936;EW-16,,,bone,50937;EW-18,,,bone,50938;EW-24,,,bone,50939;EW-3,,,bone,50940;EW-7,,,bone,50941;GAK,,,skin,50942;GB-1,,,brain,50943;GI-1,,,brain,50945;GI-ME-N,,,nervous system,50946;GR-ST,,,blood,50947;GT3TKB,,,stomach,50948;HAL-01,,,blood,50951;HCC2998,,,intestine,50952;HCE-T,,,head &amp; neck,50954;HOP-62,,,lung,50955;HT-144,,,skin,50956;IMR-5,,,nervous system,50957;IST-MES1,,,pleura,50958;IST-SL2,,,lung,50960;JVM-2,,,blood,50962;JVM-3,,,blood,50963;K5,,,thyroid,50964;KALS-1,,,brain,50965;KGN,,,ovary,50966;KINGS-1,,,brain,50967;KM12,,,intestine,50969;KNS-42,,,brain,50970;KNS-81-FD,,,brain,50971;KP-N-YS,,,nervous system,50973;KS-1,,,brain,50974;KURAMOCHI,,,ovary,50975;LAN-5,,,nervous system,50976;LAN-6,,,nervous system,50977;LB1047-RCC,,,kidney,50978;LB2241-RCC,,,kidney,50979;LB2518-MEL,,,skin,50980;LB373-MEL-D,,,skin,50981;LB771-HNC,,,head &amp; neck,50983;LB831-BLC,,,urinary tract,50984;LB996-RCC,,,kidney,50985;LOXIMVI,,,skin,50988;LS-123,,,intestine,50990;LS-411N,,,intestine,50991;LS-513,,,intestine,50992;LU-134-A,,,lung,50993;LU-165,,,lung,50995;LXF-289,,,lung,50996;MFH-ino,,,miscellaneous,50997;MHH-CALL-2,,,blood,50998;MMAC-SF,,,skin,50999;MN-60,,,blood,51000;MPP-89,,,pleura,51002;MUTZ-1,,,blood,51003;MZ1-PC,,,pancreas,51004;MZ2-MEL,,,skin,51005;MZ7-mel,,,skin,51006;NB10,,,nervous system,51007;NB13,,,nervous system,51009;NB14,,,nervous system,51010;NB16,,,nervous system,51011;NB17,,,nervous system,51012;NB5,,,nervous system,51013;NB6,,,nervous system,51014;NB7,,,nervous system,51015;NCI-H1355,,,lung,51017;NCI-H157,,,lung,51018;NCI-H2126,,,lung,51019;NCI-H322M,,,lung,51020;NCI-H64,,,lung,51021;NCI-H716,,,intestine,51022;NCI-H747,,,intestine,51023;NKM-1,,,blood,51024;NMC-G1,,,brain,51025;no-10,,,brain,51026;no-11,,,brain,51027;NOMO-1,,,blood,51028;NOS-1,,,bone,51029;NTERA-S-cl-D1,,,testes,51030;OMC-1,,,cervix,51033;ONS-76,,,brain,51034;OS-RC-2,,,kidney,51035;QIMR-WIL,,,blood,51037;Ramos-2G6-4C10,,,lymphatic system,51038;RCC10RGB,,,kidney,51039;RKO,,,intestine,51041;RL95-2,,,uterus,51042;RPMI-8866,,,blood,51043;SF126,,,brain,51045;SF268,,,brain,51046;SF539,,,brain,51047;SH-4,,,skin,51048;SK-MM-2,,,blood,51053;SK-PN-DW,,,bone,51054;SK-UT-1,,,uterus,51055;SNU-C1,,,intestine,51056;SNU-C2B,,,intestine,51057;SW403,,,intestine,51058;SW684,,,miscellaneous,51059;SW872,,,miscellaneous,51060;SW954,,,vulva,51061;SW982,,,miscellaneous,51063;TE-1,,,esophagus,51064;TE-10,,,esophagus,51065;TE-441-T,,,muscle,51069;TE-5,,,esophagus,51070;TE-6,,,esophagus,51071;TGBC11TKB,,,stomach,51074;TGBC1TKB,,,biliary tract,51075;TK10,,,kidney,51077;UACC-257,,,skin,51078;ECC10,,,stomach,50919;JEG-3,,,miscellaneous,50961;697.0,,,blood,50877;LU-139,,,lung,50994;CTB-1,,,lymphatic system,50905;ES3,,,bone,50927;TE-11,,,esophagus,51066;IST-SL1,,,lung,50959;TGBC24TKB,,,biliary tract,51076;KLE,,,uterus,50968;LC-1F,,,lung,50986;HCE-4,,,esophagus,50953;A4-Fuk,,,skin,50883;SK-MEL-24,,,skin,51050;CP50-MEL-B,,,skin,50903;YH-13,,,brain,51080;OC-314,,,ovary,51031;RF-48,,,stomach,51040;SK-MG-1,,,brain,51052;B2-17,,,brain,50889;Mo-T,,,blood,51001;KP-N-YN,,,nervous system,50972;D-423MG,,,brain,50911;H9,,,lymphatic system,50949;D-566MG,,,brain,50914;SK-MEL-5,,,skin,51051;NBsusSR,,,nervous system,51016;A101D,,,skin,50879;A388,,,miscellaneous,50881;BB65-RCC,,,kidney,50892;D-502MG,,,brain,50912;GCIY,,,stomach,50944;HA7-RCC,,,kidney,50950;LC-2-ad,,,lung,50987;LS-1034,,,intestine,50989;NB12,,,nervous system,51008;OCUB-M,,,breast,51032;OVCAR-4,,,ovary,51036;RXF393,,,kidney,51044;SJSA-1,,,bone,51049;SW962,,,vulva,51062;TE-12,,,esophagus,51067;TE-15,,,esophagus,51068;TE-8,,,esophagus,51072;TE-9,,,esophagus,51073;VA-ES-BJ,,,miscellaneous,51079;NUGC-2,,,stomach,50423;QGP-1,,,pancreas,50458;SW 1116,,,intestine,50523</t>
+  </si>
+  <si>
+    <t>1061\cell lines</t>
+  </si>
+  <si>
+    <t>CHIR-99021,small molecule,10180-101,LSM-1181;PF562271,small molecule,10072-101,LSM-1072;OSI 906,small molecule,10135-101,LSM-1135;Sigma A6730,small molecule,10035-109,LSM-1035;GSK1070916,small molecule,10062-101,LSM-1062;BMS-754807,small molecule,10290-101,LSM-6218</t>
+  </si>
+  <si>
+    <t>http://lincs.hms.harvard.edu/db/datasets/20010/</t>
+  </si>
+  <si>
+    <t>MGH (CMT) Growth Inhibition Assay Protocol (9 compound doses: 1.024 uM to 0.004 uM) -- DNA Staining</t>
+  </si>
+  <si>
+    <t>5637.0,epithelial,,urinary bladder,50001;647-V,epithelial-like,,urinary bladder,50002;A375.S2,epithelial,,skin,50003;AGS,epithelial,,stomach,50004;BPH-1,epitheloid,,prostate,50005;Ca Ski,epithelial,,cervix,50006;Ca9-22,epithelial-like,,head &amp; neck,50007;CAL-51,epithelial-like,,breast,50008;Calu-1,epithelial,,lung,50009;Calu-3,epithelial,,lung,50010;COLO-679,fibroblastic,,skin,50011;COLO-800,epithelial-like,,skin,50012;HEC-1,,,uterus,50014;HLF,,,liver,50015;HUTU-80,epithelial,,intestine,50016;IA-LM,,,lung,50017;Ishikawa,epithelial-like,,uterus,50018;Ishikawa (Heraklio) 02 ER-,epithelial,,uterus,50019;IST-MEL1,epithelial-like,,skin,50020;JHH-6,epithelial-like,,liver,50021;KYSE-140,,,esophagus,50024;KYSE-150,epitheloid,,esophagus,50025;KYSE-180,epitheloid,,esophagus,50026;KYSE-450,epitheloid,,esophagus,50027;LNZTA3WT4,,,brain,50028;MCF7,epithelial,,breast,50029;MDA-MB-435S,melanocyte,,skin,50030;MT-3,epithelial,,breast,50031;NCI-H1648,,,lung,50032;NCI-H1651,epithelial,,lung,50033;NCI-H1703,epithelial,,lung,50034;NCI-H1915,large cell,,lung,50035;NCI-H2023,,,lung,50036;NCI-H810,epithelial,,lung,50037;PE/CA-PJ15,epithelial-like,,head &amp; neck,50039;SK-LMS-1,,,uterus,50042;SK-MES,epithelial,,lung,50043;SK-OV-3,epithelial,,ovary,50044;SNB75,,,brain,50045;SW527,epithelial,,breast,50046;SW620,epithelial,,intestine,50047;T24,epithelial,,urinary bladder,50048;WiDr,epithelial,,intestine,50049;Hep 3B2.1-7,epithelial,,liver,50051;Hep G2,epithelial,,liver,50052;Huh7,,,liver,50055;SK-BR-3,epithelial,,breast,50057;MDA-MB-231,epithelial,,breast,50058;A-375,epithelial,,skin,50060;HeLa,epithelial,,cervix,50061;1205Lu,,,skin,50062;1321N1,,,brain,50063;143B,,,bone,50064;143B PML BK TK,,,bone,50065;1A6,,,urinary bladder,50066;22RV1,,,prostate,50067;23132/87,,,stomach,50068;42-MG-BA,,,brain,50069;639-V,,,ureter,50071;769-P,,,kidney,50072;786-O,,,kidney,50073;8305C,,,thyroid,50074;8505C,,,thyroid,50075;A172,,,brain,50076;A-204,,,muscle,50077;A2058,,,skin,50078;A2780,,,ovary,50079;A2780ADR,,,ovary,50080;A373-C6,,,skin,50081;A-427,,,lung,50082;A549,,,lung,50084;A673,,,muscle,50085;ABC-1,,,lung,50086;ACHN,,,kidney,50087;AN3CA,,,uterus,50088;ASH-3,,,thyroid,50089;AsPC-1,,,pancreas,50090;AU565,,,breast,50091;AZ-521,,,stomach,50092;B-CPAP,,,thyroid,50093;BE(2)-C,,,nervous system,50094;BEN,,,lung,50095;BeWo,,,miscellaneous,50096;BFTC-905,,,urinary bladder,50097;BFTC-909,,,kidney,50098;BHT-101,,,thyroid,50099;BHY,,,head &amp; neck,50100;BICR 10,,,head &amp; neck,50101;BICR 22,,,head &amp; neck,50102;BICR 31,,,head &amp; neck,50103;BICR 78,,,head &amp; neck,50104;BT-20,,,breast,50105;BT-474,,,breast,50106;BT-483,,,breast,50107;BT-549,,,breast,50108;BxPC-3,,,pancreas,50109;C170,,,intestine,50110;C2BBe1,,,intestine,50111;C32,,,skin,50112;C-33 A,,,cervix,50113;C3A,,,liver,50114;C-4 I,,,cervix,50115;C-4 II,,,cervix,50116;Caco-2,,,intestine,50117;Caki-1,,,kidney,50118;CAL 27,,,head &amp; neck,50119;CAL-120,,,breast,50120;CAL-12T,,,lung,50121;CAL-29,,,urinary bladder,50123;CAL-33,,,head &amp; neck,50124;CAL-39,,,vulva,50125;CAL-62,,,thyroid,50127;CAL-72,,,bone,50128;CAL-78,,,bone,50129;CAL-85-1,,,breast,50130;CAMA-1,,,breast,50131;Caov-3,,,ovary,50132;Caov-4,,,ovary,50133;Capan-2,,,pancreas,50135;CaR-1,,,intestine,50136;CCF-STTG1,,,brain,50137;CCK-81,,,intestine,50138;CHP-212,,,nervous system,50139;CoCM-1,,,intestine,50141;COLO 201,,,intestine,50142;COLO 205,,,intestine,50143;COLO 741,,,intestine,50145;COLO 792,,,skin,50146;COLO 853,,,skin,50147;COLO 857,,,skin,50148;COLO 858,,,skin,50149;COLO-678,,,intestine,50152;COLO-680N,,,esophagus,50153;COLO-783,,,skin,50154;COLO-818,,,skin,50155;COLO-849,,,skin,50157;COR-L 105,,,lung,50158;COR-L23,,,lung,50160;DAN-G,,,pancreas,50161;Daoy,,,brain,50162;DBTRG-05MG,,,brain,50163;Detroit 562,,,head &amp; neck,50164;DK-MG,,,brain,50165;DMS 273,,,lung,50167;DMS 53,,,lung,50168;DOK,,,head &amp; neck,50169;DoTc2 4510,,,cervix,50170;DU 145,,,prostate,50171;DV-90,,,lung,50172;EBC-1,,,lung,50173;EFE-184,,,uterus,50174;EFM-19,,,breast,50175;EFM-192A,,,breast,50176;EFM-192B,,,breast,50177;EFM-192C,,,breast,50178;EFO-21,,,ovary,50179;EFO-27,,,ovary,50180;EGI-1,,,biliary tract,50181;EJ138,,,urinary bladder,50182;EN,,,uterus,50183;EPLC-272H,,,lung,50184;ESS-1,,,uterus,50186;FaDu,,,head &amp; neck,50188;FLYA13,,,miscellaneous,50189;FTC-133,,,thyroid,50190;FTC-238,,,thyroid,50191;FU-OV-1,,,ovary,50192;G-292 Clone A141B1,,,bone,50193;G-401,,,kidney,50195;G-402,,,kidney,50196;GAMG,,,brain,50197;GCT,,,miscellaneous,50198;GMS-10,,,brain,50199;GOS-3,,,brain,50200;GP5d,,,intestine,50201;H4,,,brain,50202;HARA,,,lung,50204;HCC1143,,,breast,50205;HCC1395,,,breast,50206;HCC1419,,,breast,50207;HCC1428,,,breast,50208;HCC-15,,,lung,50209;HCC1569,,,breast,50210;HCC1806,,,breast,50211;HCC1937,,,breast,50212;HCC1954,,,breast,50213;HCC-366,,,lung,50215;HCC38,,,breast,50216;HCC-44,,,lung,50217;HCC-56,,,intestine,50218;HCC70,,,breast,50219;HCC-78,,,lung,50220;HCC-827,,,lung,50221;HCT 116,,,intestine,50222;HCT-15,,,intestine,50223;HCT-8,,,intestine,50224;HDQ-P1,,,breast,50225;HGC-27,,,stomach,50227;HLE,,,liver,50228;HMVII,,,skin,50229;HN,,,head &amp; neck,50230;HO-1-N-1,,,head &amp; neck,50231;HO-1-u-1,,,head &amp; neck,50232;HOS,,,bone,50233;HPAC,,,pancreas,50234;HPAF-II,,,pancreas,50235;HRT-18,,,intestine,50236;Hs 257.T,,,intestine,50237;Hs 578T,,,breast,50238;Hs 588.T,,,cervix,50239;Hs 633T,,,miscellaneous,50240;Hs 683,,,brain,50241;Hs 746T,,,stomach,50242;Hs 766T,,,pancreas,50243;HSC-2,,,head &amp; neck,50244;HSC-3,,,head &amp; neck,50245;HSC-4,,,head &amp; neck,50246;HT 1080,,,miscellaneous,50247;HT 1376,,,urinary bladder,50248;HT115,,,intestine,50249;HT-1197,,,urinary bladder,50250;HT-29,,,intestine,50251;HT-3,,,cervix,50252;HT55,,,intestine,50253;HTC-C3,,,thyroid,50254;HuCCT1,,,biliary tract,50255;huH-1,,,liver,50256;HuO9,,,bone,50258;HuO9N2,,,bone,50259;HUP-T3,,,pancreas,50260;HUP-T4,,,pancreas,50261;IGR-1,,,skin,50262;IGR-37,,,skin,50263;IGR-39,,,skin,50264;IHH-4,,,thyroid,50265;IM-95,,,stomach,50266;IM-95m,,,stomach,50267;IPC-298,,,skin,50269;J82,,,urinary bladder,50270;JHH-1,,,liver,50272;JHH-2,,,liver,50273;JHH-4,,,liver,50274;JHH-7,,,liver,50275;JIMT-1,,,breast,50276;KELLY,,,nervous system,50277;KG-1-C,,,brain,50278;KHOS/NP,,,bone,50280;KHOS-240S,,,bone,50281;KHOS-312H,,,bone,50282;KMH-2,,,thyroid,50283;KMRC-1,,,kidney,50284;KON,,,head &amp; neck,50285;KOSC-2 cl3-43,,,head &amp; neck,50286;KP-2,,,pancreas,50287;KPL-1,,,breast,50291;KU-19-19,,,urinary bladder,50292;KYSE-220,,,esophagus,50293;KYSE-270,,,esophagus,50294;KYSE-30,,,esophagus,50295;KYSE-410,,,esophagus,50296;KYSE-50,,,esophagus,50297;KYSE-510,,,esophagus,50298;KYSE-520,,,esophagus,50299;KYSE-70,,,esophagus,50300;LC-1 sq,,,lung,50301;LCLC-103H,,,lung,50302;LCLC-97TM1,,,lung,50303;LK-2,,,lung,50304;LN-18,,,brain,50305;LN-229,,,brain,50306;LN-405,,,brain,50307;LNZTA3WT11,,,brain,50308;LoVo,,,intestine,50310;LS174T,,,intestine,50311;LS180,,,intestine,50312;Lu-135,,,lung,50314;LU65A,,,lung,50316;LU65B,,,lung,50317;LU65C,,,lung,50318;LU99A,,,lung,50319;LU99B,,,lung,50320;LU99C,,,lung,50321;LUDLU-1,,,lung,50322;M059J,,,brain,50323;MB 157,,,breast,50324;MCAS,,,ovary,50325;MC-IXC,,,nervous system,50326;MDA-MB-134-VI,,,breast,50327;MDA-MB-175-VII,,,breast,50329;MDA-MB-330,,,breast,50330;MDA-MB-361,,,breast,50331;MDA-MB-415,,,breast,50332;MDA-MB-436,,,breast,50333;MDA-MB-453,,,breast,50334;MDA-MB-468,,,breast,50335;ME-180,,,cervix,50337;MEL-HO,,,skin,50338;MEL-JUSO,,,skin,50339;MES-SA,,,uterus,50340;MES-SA/Dx-5,,,uterus,50341;MEWO,,,skin,50342;MFE-280,,,uterus,50343;MFE-296,,,uterus,50344;MFE-319,,,uterus,50345;MFM-223,,,breast,50346;MG-63,,,bone,50347;MHH-ES-1,,,nervous system,50348;MIA PaCa-2,,,pancreas,50349;MKN1,,,stomach,50350;MKN28,,,stomach,50351;MKN45,,,stomach,50352;MKN7,,,stomach,50353;MKN74,,,stomach,50354;ML-1,,,thyroid,50355;MOG-G-CCM,,,brain,50356;MOG-G-UVW,,,brain,50357;MS751,,,cervix,50358;NB69,,,nervous system,50360;NCC-IT-A3,,,testes,50361;NCI-H1048,,,lung,50362;NCI-H1299,,,lung,50363;NCI-H1435,,,lung,50364;NCI-H1437,,,lung,50365;NCI-H1568,,,lung,50366;NCI-H1573,,,lung,50367;NCI-H1623,,,lung,50369;NCI-H1650,,,lung,50370;NCI-H1688,,,lung,50371;NCI-H1693,,,lung,50372;NCI-H1734,,,lung,50373;NCI-H1755,,,lung,50374;NCI-H1781,,,lung,50375;NCI-H1792,,,lung,50376;NCI-H1793,,,lung,50377;NCI-H1944,,,lung,50380;NCI-H196,,,lung,50381;NCI-H1993,,,lung,50382;NCI-H2009,,,lung,50383;NCI-H2029,,,lung,50384;NCI-H2030,,,lung,50385;NCI-H2073,,,lung,50386;NCI-H2085,,,lung,50387;NCI-H2110,,,lung,50389;NCI-H2122,,,lung,50390;NCI-H2135,,,lung,50391;NCI-H2170,,,lung,50392;NCI-H2172,,,lung,50393;NCI-H2195,,,lung,50394;NCI-H2198,,,lung,50396;NCI-H2228,,,lung,50397;NCI-H2286,,,lung,50398;NCI-H2291,,,lung,50399;NCI-H23,,,lung,50400;NCI-H2342,,,lung,50401;NCI-H2347,,,lung,50402;NCI-H2405,,,lung,50403;NCI-H2444,,,lung,50404;NCI-H2452,,,lung,50405;NCI-H322,,,lung,50407;NCI-H358,,,lung,50408;NCI-H441,,,lung,50409;NCI-H460,,,lung,50410;NCI-H520,,,lung,50411;NCI-H522,,,lung,50412;NCI-H596,,,lung,50413;NCI-H630,,,intestine,50414;NCI-H647,,,lung,50415;NCI-H650,,,lung,50416;NCI-H661,,,lung,50417;NCI-H727,,,lung,50418;NCI-H838,,,lung,50419;NCI-H841,,,lung,50420;NCI-N87,,,stomach,50421;NIH:OVCAR-3,,,ovary,50422;NUGC-3,,,stomach,50424;NUGC-4,,,stomach,50425;NY,,,bone,50426;OAW28,,,ovary,50427;OAW42,,,ovary,50428;OE19,,,esophagus,50431;OE21,,,esophagus,50432;OE33,,,esophagus,50433;OSC-19,,,head &amp; neck,50434;OSC-20,,,head &amp; neck,50435;OUMS-23,,,intestine,50436;OV-90,,,ovary,50437;OVISE,,,ovary,50438;OVKATE,,,ovary,50439;OVMIU,,,ovary,50440;OVSAYO,,,ovary,50441;OVTOKO,,,ovary,50442;PA-1,,,ovary,50443;Panc 02.03,,,pancreas,50444;Panc 03.27,,,pancreas,50445;Panc 04.03,,,pancreas,50446;Panc 08.13,,,pancreas,50447;Panc 10.05,,,pancreas,50448;PANC-1,,,pancreas,50449;PA-TU-8902,,,pancreas,50450;PA-TU-8988S,,,pancreas,50451;PA-TU-8988T,,,pancreas,50452;PC-14,,,lung,50453;PC-3,,,prostate,50454;PFSK-1,,,brain,50455;PL45,,,pancreas,50456;PLC/PRF/5,,,liver,50457;RCM-1,,,intestine,50459;RD,,,muscle,50460;RERF-GC-1B,,,stomach,50462;RERF-LC-Ad1,,,lung,50463;RERF-LC-KJ,,,lung,50464;RERF-LC-Sq1,,,lung,50466;RKN,,,ovary,50467;RMG-I,,,ovary,50468;RO82-W-1,,,thyroid,50469;RPMI 2650,,,head &amp; neck,50470;RPMI-7951,,,skin,50471;RT-112,,,urinary bladder,50472;RT112/84,,,urinary bladder,50473;RT4,,,urinary bladder,50474;RVH-421,,,skin,50475;S-117,,,thyroid,50476;Saos-2,,,bone,50477;SAS,,,head &amp; neck,50478;SAT,,,head &amp; neck,50479;SBC-3,,,lung,50480;SBC-5,,,lung,50481;SCaBER,,,urinary bladder,50482;SCC-15,,,head &amp; neck,50483;SCC-25,,,head &amp; neck,50484;SCC-4,,,head &amp; neck,50485;SCC-9,,,head &amp; neck,50486;SCCH-26,,,nervous system,50488;SiHa,,,cervix,50493;SISO,,,cervix,50494;SK-CO-1,,,intestine,50495;SKG-IIIa,,,cervix,50497;SKG-IIIb,,,cervix,50498;SK-HEP-1,,,liver,50499;SK-LU-1,,,lung,50500;SK-MEL-2,,,skin,50501;SK-MEL-30,,,skin,50502;SKN,,,uterus,50503;SKN-3,,,head &amp; neck,50504;SK-N-AS,,,nervous system,50505;SK-N-SH,,,nervous system,50508;SNG-M,,,uterus,50509;SNU-182,,,liver,50512;SNU-387,,,liver,50513;SNU-398,,,liver,50514;SNU-423,,,liver,50515;SNU-449,,,liver,50516;SNU-475,,,liver,50517;SU.86.86,,,pancreas,50520;SUIT-2,,,pancreas,50521;SW 1088,,,brain,50522;SW 1271,,,lung,50524;SW 13,,,adrenal gland,50525;SW 1463,,,intestine,50527;SW 156,,,kidney,50528;SW 1573,,,lung,50529;SW 1783,,,brain,50530;SW 48,,,intestine,50531;SW 626,,,ovary,50532;SW 780,,,urinary bladder,50533;SW 900,,,lung,50534;SW-1710,,,urinary bladder,50535;SW756,,,cervix,50536;SW837,,,intestine,50537;SW-948,,,intestine,50538;T.T,,,esophagus,50539;T.Tn,,,esophagus,50540;T47D,,,breast,50541;T84,,,intestine,50542;T98G,,,brain,50543;TASK1,,,nervous system,50544;TCCSUP,,,urinary bladder,50545;TOV-112D,,,ovary,50547;TOV-21G,,,ovary,50548;TT2609-C02,,,thyroid,50549;TYK-nu,,,ovary,50550;U-118 MG,,,brain,50551;U-138 MG,,,brain,50552;U-2 OS,,,bone,50553;U-251 MG,,,brain,50554;U373 MG,,,brain,50555;UACC-893,,,breast,50557;UMC-11,,,lung,50558;UM-UC-3,,,urinary bladder,50559;VMRC-LCP,,,lung,50562;VMRC-MELG,,,skin,50563;VMRC-RCZ,,,kidney,50565;WM 266-4,,,skin,50566;WM-115,,,skin,50567;WM1552C,,,skin,50568;WM278,,,skin,50569;WM35,,,skin,50570;WM793B,,,skin,50571;YAPC,,,pancreas,50572;YKG-1,,,brain,50573;ZR-75-1,,,breast,50574;ZR-75-30,,,breast,50575;DU4475,epithelial,,breast,50577;HCC1500,epithelial,,breast,50579;A2780cis,,,ovary,50586;A3,,,blood,50587;BC-2,,,lymphatic system,50595;BC-3,,,lymphatic system,50596;CEM/C2,,,blood,50607;CFPAC-1,,,pancreas,50609;ChaGo-K-1,,,lung,50610;COLO-704,,,ovary,50617;COR-L95,,,lung,50621;DMS 114,,,lung,50629;EJM,,,blood,50637;GA-10 (Clone 20),,,lymphatic system,50641;Gp2D,,,intestine,50644;HCC-33,,,lung,50648;HEL 92.1.7,,,blood,50652;HL60(S),,,blood,50655;HL-60/MX2,,,blood,50656;I 2.1,,,blood,50662;I 9.2,,,blood,50663;IM-9,,,lymphatic system,50664;J.gamma1,,,blood,50665;JM1,,,lymphatic system,50672;Jurkat, Clone E6-1,,,blood,50674;KARPAS-231,,,blood,50679;KMOE-2,,,blood,50690;KP-1N,,,pancreas,50695;KP-1NL,,,pancreas,50696;KU812,,,blood,50697;KU812E,,,blood,50698;KYM-1,,,muscle,50702;Lu-134-B,,,lung,50711;M059K,,,brain,50712;MHH-NB-11,,,nervous system,50719;NCI-H1385,,,lung,50749;NCI-H1563,,,lung,50755;NCI-H1618,,,lung,50756;NCI-H1666,,,lung,50757;NCI-H1836,,,lung,50760;NCI-H1838,,,lung,50761;NCI-H1963,,,lung,50764;NCI-H1975,,,lung,50765;NCI-H2081,,,lung,50766;NCI-H2106,,,lung,50768;NCI-H211,,,lung,50769;NCI-H220,,,lung,50772;NCI-H2227,,,lung,50773;NCI-H719,,,lung,50781;NCI-H720,,,lung,50782;NCI-H748,,,lung,50783;OCI-AML3,,,blood,50793;P116.cl39,,,blood,50798;PC-3 [JPC-3],,,lung,50804;PEER,,,blood,50805;Pfeiffer,,,lymphatic system,50807;PSN1,,,pancreas,50809;RERF-LC-MS,,,lung,50815;RH-30,,,muscle,50817;ROS-50,,,blood,50820;SBC-2,,,lung,50827;SC-1,,,lymphatic system,50828;SK-MEL-3,,,skin,50834;SK-N-BE(2),,,nervous system,50835;SNB-19,,,brain,50838;SU-DHL-16,,,lymphatic system,50843;SUP-HD1,,,lymphatic system,50849;SVG p12,,,brain,50852;SW 1990,,,pancreas,50853;TALL-1,,,blood,50854;Tera-1,,,testes,50857;TF-1,,,blood,50858;TF-1.CN5a.1,,,blood,50859;Toledo,,,lymphatic system,50863;TT,,,thyroid,50864;YMB-1,,,breast,50875;FU97,epithelial-like,,stomach,50013;KMRC-20,epithelial-like,,kidney,50023;SJCRH30,fibroblast,,muscle,50041;LNCaP,epithelial,,prostate,50059;A431,,,skin,50083;CAL-148,,,breast,50122;CAL-54,,,kidney,50126;Capan-1,,,pancreas,50134;COLO 320DM,,,intestine,50144;COLO-206F,,,intestine,50150;COLO-320,,,intestine,50151;COLO-824,,,breast,50156;COR-L 23/CPR,,,lung,50159;DLD-1,,,intestine,50166;ES-2,,,ovary,50185;EVSA-T,,,breast,50187;G-361,,,skin,50194;HCC202,,,breast,50214;H-EMC-SS,,,bone,50226;HuO-3N1,,,bone,50257;IMR-32,,,nervous system,50268;JAR,,,miscellaneous,50271;KP-3,,,pancreas,50288;KP-3L,,,pancreas,50289;KP-4,,,pancreas,50290;LOU-NH91,,,lung,50309;LU65,,,lung,50315;MDA-MB-157,,,breast,50328;MDST8,,,intestine,50336;MSTO-211H,,,pleura,50359;NCI-H1581,,,lung,50368;NCI-H1869,,,lung,50378;NCI-H1876,,,lung,50379;NCI-H2087,,,lung,50388;NCI-H2196,,,lung,50395;OCUG-1,,,gall bladder,50429;OCUM-1,,,stomach,50430;RD-ES,,,nervous system,50461;RERF-LC-MA,,,lung,50465;SCH,,,stomach,50489;SCLC-21H,,,lung,50490;SHP-77,,,lung,50491;SK-ES-1,,,bone,50496;SK-N-DZ,,,nervous system,50506;SK-NEP-1,,,kidney,50507;SNU-1,,,stomach,50510;SNU-16,,,stomach,50511;SNU-5,,,stomach,50518;SW 1417,,,intestine,50526;TGW,,,adrenal gland,50546;UACC-812,,,breast,50556;VCaP,,,prostate,50560;VM-CUB1,,,urinary bladder,50561;VMRC-RCW,,,kidney,50564;HCC1187,epithelial,,breast,50578;HCC1599,epithelial,,breast,50580;HCC2157,epithelial,,breast,50581;HCC2218,epithelial,,breast,50582;2B8,,,lymphatic system,50585;A3/KAW,,,lymphatic system,50588;AGR-ON,,,blood,50589;ALL-SIL,,,blood,50590;AMO-1,,,lymphatic system,50591;ARH-77,,,blood,50592;BALL-1,,,blood,50593;BC-1,,,lymphatic system,50594;BDCM,,,blood,50597;BE(2)-M17,,,nervous system,50598;BL-41,,,lymphatic system,50599;BL-70,,,lymphatic system,50600;C8166,,,blood,50601;CA46,,,lymphatic system,50602;CCRF-CEM,,,blood,50603;CCRF-HSB-2,,,blood,50604;CCRF-SB,,,blood,50605;CEM/C1,,,blood,50606;CESS,,,blood,50608;CHP-126,,,nervous system,50611;CI-1,,,lymphatic system,50612;CL-11,,,intestine,50613;Clone 15 HL-60,,,blood,50614;CMK,,,blood,50615;COLO 684,,,uterus,50616;COR-L279,,,lung,50618;COR-L51,,,lung,50619;COR-L88,,,lung,50620;CPC-N,,,lung,50622;CTV-1,,,blood,50623;D283 Med,,,brain,50624;Daudi,,,lymphatic system,50625;DB,,,lymphatic system,50626;DERL-2,,,lymphatic system,50627;DG-75,,,lymphatic system,50628;DMS 153,,,lung,50630;DMS 79,,,lung,50631;DND-41,,,blood,50632;EB1,,,lymphatic system,50633;EB2,,,lymphatic system,50634;EB-3,,,lymphatic system,50635;EHEB,,,blood,50636;Eos-HL-60,,,blood,50638;Farage,,,lymphatic system,50639;GDM-1,,,blood,50642;GOTO,,,nervous system,50643;GRANTA-519,,,lymphatic system,50645;H33HJ-JA1,,,blood,50646;HC-1,,,blood,50647;HDLM-2,,,lymphatic system,50649;HD-MY-Z,,,lymphatic system,50650;HEL,,,blood,50651;HH,,,lymphatic system,50653;HL-60,,,blood,50654;HL60RG,,,blood,50657;Hs 445,,,lymphatic system,50658;HS-Sultan,,,lymphatic system,50659;HT,,,lymphatic system,50660;HuT 78,,,lymphatic system,50661;J.gamma1.WT,,,blood,50666;J.RT3-T3.5,,,blood,50667;J45.01,,,blood,50668;Jiyoye,,,lymphatic system,50669;JJN-3,,,blood,50670;JKT-beta-del,,,blood,50671;JSC-1,,,lymphatic system,50673;JURL-MK1,,,blood,50675;JURL-MK2,,,blood,50676;K-562,,,blood,50677;K562/ADM,,,blood,50678;KARPAS-299,,,lymphatic system,50680;KARPAS-422,,,lymphatic system,50681;KARPAS-45,,,blood,50682;KARPAS-620,,,blood,50683;KCL-22,,,blood,50685;KE-37,,,blood,50686;KG-1,,,blood,50687;KG-1a,,,blood,50688;KM-H2,,,lymphatic system,50689;KMS-12-BM,,,blood,50691;KMS-12-PE,,,blood,50692;KO52,,,blood,50693;KOPN-8,,,blood,50694;KU812F,,,blood,50699;KY821,,,blood,50700;KY821A3,,,blood,50701;L-1236,,,lymphatic system,50703;L-363,,,blood,50704;L-428,,,lymphatic system,50705;L-540,,,lymphatic system,50706;LAMA-84,,,blood,50707;LC4-1,,,blood,50708;Loucy,,,blood,50709;LP-1,,,blood,50710;MC/CAR,,,lymphatic system,50713;MC116,,,lymphatic system,50714;ME-1,,,blood,50715;MEC-1,,,blood,50716;MEC-2,,,blood,50717;MEG-01,,,blood,50718;MHH-PREB-1,,,lymphatic system,50720;MJ,,,lymphatic system,50721;ML-2,,,blood,50722;MLMA,,,blood,50723;MOLM-13,,,blood,50724;MOLP-8,,,blood,50725;MOLT-14,,,blood,50726;MOLT-16,,,blood,50727;MOLT-4,,,blood,50728;MOLT-4F,,,blood,50729;MONO-MAC-1,,,blood,50730;MONO-MAC-6,,,blood,50731;MRK-nu-1,,,breast,50732;MS-1-L,,,lung,50733;MV-4-11,,,blood,50734;MY,,,blood,50735;MY-M12,,,blood,50736;MY-M13,,,blood,50737;NALM-19,,,blood,50738;NALM-6,,,blood,50739;NAMALWA,,,lymphatic system,50740;NAMALWA.PNT,,,lymphatic system,50741;NB(TU)1-10,,,nervous system,50742;NB-1,,,nervous system,50743;NB-4,,,blood,50744;NC-37,,,lymphatic system,50745;NCI-H1092,,,lung,50746;NCI-H1155,,,lung,50747;NCI-H1304,,,lung,50748;NCI-H1395,,,lung,50750;NCI-H1404,,,lung,50751;NCI-H1417,,,lung,50752;NCI-H1436,,,lung,50753;NCI-H1522,,,lung,50754;NCI-H1694,,,lung,50758;NCI-H1770,,,lung,50759;NCI-H187,,,lung,50762;NCI-H1882,,,lung,50763;NCI-H209,,,lung,50767;NCI-H2141,,,lung,50770;NCI-H2171,,,lung,50771;NCI-H226,,,lung,50774;NCI-H345,,,lung,50775;NCI-H446,,,lung,50776;NCI-H510A,,,lung,50777;NCI-H524,,,lung,50778;NCI-H526,,,lung,50779;NCI-H69,,,lung,50780;NCI-H82,,,lung,50784;NCI-H847,,,lung,50785;NCI-H889,,,lung,50786;NEC8,,,testes,50787;NH-12,,,nervous system,50788;NK-92MI,,,lymphatic system,50789;NOMO-1/ADM,,,blood,50790;NU-DUL-1,,,lymphatic system,50791;OCI-AML2,,,blood,50792;OCI-AML5,,,blood,50794;OCI-LY-19,,,lymphatic system,50795;OCI-M1,,,blood,50796;OPM-2,,,blood,50797;P12-ICHIKAWA,,,blood,50799;P30/OHK,,,blood,50800;P31/FUJ,,,blood,50801;P32/ISH,,,lymphatic system,50802;P3HR-1,,,lymphatic system,50803;PF-382,,,blood,50806;PL-21,,,blood,50808;Raji,,,lymphatic system,50810;Ramos (RA 1),,,blood,50811;RC-K8,,,lymphatic system,50812;REC-1,,,lymphatic system,50813;Reh,,,blood,50814;RH-1,,,bone,50816;RH-41,,,muscle,50818;RL,,,lymphatic system,50819;RPMI 1788,,,blood,50821;RPMI 6666,,,lymphatic system,50822;RPMI 8226,,,blood,50823;RPMI-8402,,,blood,50824;RS4;11,,,blood,50825;SBC-1,,,lung,50826;SCC-3,,,lymphatic system,50829;Sci-1,,,lymphatic system,50830;SIG-M5,,,blood,50831;SIMA,,,nervous system,50832;SK-MEL-1,,,skin,50833;SK-N-FI,,,nervous system,50836;SLVL,,,lymphatic system,50837;SR,,,lymphatic system,50839;ST486,,,lymphatic system,50840;SU-DHL-1,,,lymphatic system,50841;SU-DHL-4,,,lymphatic system,50844;SU-DHL-5,,,lymphatic system,50845;SU-DHL-6,,,lymphatic system,50846;SU-DHL-8,,,lymphatic system,50847;SUP-B15,,,blood,50848;SUP-M2,,,lymphatic system,50850;SUP-T1,,,blood,50851;TANOUE,,,blood,50855;TC-71,,,bone,50856;TF-1a,,,blood,50860;THP-1,,,blood,50861;TK,,,lymphatic system,50862;TUR,,,lymphatic system,50865;U266B1,,,blood,50866;U-698-M,,,blood,50867;U-87 MG,,,brain,50868;U-937,,,lymphatic system,50869;VAL,,,lymphatic system,50870;WIL2 NS,,,lymphatic system,50871;WILCL,,,blood,50872;WSU-DLCL2,,,lymphatic system,50873;WSU-NHL,,,lymphatic system,50874;YT,,,lymphatic system,50876;CGTH-W-1,,,thyroid,50899;8-MG-BA,,,brain,50878;A253,,,head &amp; neck,50880;A498,,,kidney,50882;A704,,,kidney,50884;ACN,,,nervous system,50885;BB30-HNC,,,head &amp; neck,50890;BE-13,,,blood,50893;Becker,,,brain,50894;BV-173,,,blood,50896;Calu-6,,,lung,50897;COLO-320-HSR,,,intestine,50900;COLO-668,,,lung,50901;COLO-829,,,skin,50902;CP66-MEL,,,skin,50904;CW-2,,,intestine,50906;D-247MG,,,brain,50907;D-263MG,,,brain,50908;D-336MG,,,brain,50909;D-392MG,,,brain,50910;D-542MG,,,brain,50913;DJM-1,,,skin,50916;DSH1,,,urinary tract,50918;ECC12,,,stomach,50920;EC-GI-10,,,esophagus,50922;EKVX,,,lung,50923;ES1,,,bone,50926;ES4,,,bone,50928;ES5,,,bone,50929;ES6,,,bone,50930;ES7,,,bone,50931;ES8,,,bone,50932;ETK-1,,,biliary tract,50933;EW-1,,,bone,50934;EW-11,,,bone,50935;EW-13,,,bone,50936;EW-16,,,bone,50937;EW-24,,,bone,50939;EW-3,,,bone,50940;EW-7,,,bone,50941;GAK,,,skin,50942;GB-1,,,brain,50943;GI-1,,,brain,50945;GI-ME-N,,,nervous system,50946;GT3TKB,,,stomach,50948;HAL-01,,,blood,50951;HCC2998,,,intestine,50952;HCE-T,,,head &amp; neck,50954;HOP-62,,,lung,50955;HT-144,,,skin,50956;IMR-5,,,nervous system,50957;IST-MES1,,,pleura,50958;IST-SL2,,,lung,50960;JVM-3,,,blood,50963;K5,,,thyroid,50964;KALS-1,,,brain,50965;KGN,,,ovary,50966;KINGS-1,,,brain,50967;KNS-42,,,brain,50970;KNS-81-FD,,,brain,50971;KP-N-YS,,,nervous system,50973;KS-1,,,brain,50974;KURAMOCHI,,,ovary,50975;LAN-5,,,nervous system,50976;LAN-6,,,nervous system,50977;LB1047-RCC,,,kidney,50978;LB2241-RCC,,,kidney,50979;LB2518-MEL,,,skin,50980;LB373-MEL-D,,,skin,50981;LB771-HNC,,,head &amp; neck,50983;LB831-BLC,,,urinary tract,50984;LB996-RCC,,,kidney,50985;LS-123,,,intestine,50990;LS-411N,,,intestine,50991;LS-513,,,intestine,50992;LXF-289,,,lung,50996;MFH-ino,,,miscellaneous,50997;MMAC-SF,,,skin,50999;MPP-89,,,pleura,51002;MZ1-PC,,,pancreas,51004;MZ2-MEL,,,skin,51005;MZ7-mel,,,skin,51006;NB10,,,nervous system,51007;NB13,,,nervous system,51009;NB14,,,nervous system,51010;NB16,,,nervous system,51011;NB17,,,nervous system,51012;NB5,,,nervous system,51013;NB6,,,nervous system,51014;NB7,,,nervous system,51015;NCI-H1355,,,lung,51017;NCI-H157,,,lung,51018;NCI-H2126,,,lung,51019;NCI-H322M,,,lung,51020;NCI-H64,,,lung,51021;NCI-H716,,,intestine,51022;NCI-H747,,,intestine,51023;NKM-1,,,blood,51024;no-10,,,brain,51026;no-11,,,brain,51027;NOS-1,,,bone,51029;NTERA-S-cl-D1,,,testes,51030;OMC-1,,,cervix,51033;ONS-76,,,brain,51034;OS-RC-2,,,kidney,51035;RCC10RGB,,,kidney,51039;RKO,,,intestine,51041;RL95-2,,,uterus,51042;SF126,,,brain,51045;SF268,,,brain,51046;SF539,,,brain,51047;SH-4,,,skin,51048;SK-PN-DW,,,bone,51054;SK-UT-1,,,uterus,51055;SNU-C1,,,intestine,51056;SNU-C2B,,,intestine,51057;SW403,,,intestine,51058;SW684,,,miscellaneous,51059;SW872,,,miscellaneous,51060;SW954,,,vulva,51061;SW982,,,miscellaneous,51063;TE-1,,,esophagus,51064;TE-10,,,esophagus,51065;TE-441-T,,,muscle,51069;TE-5,,,esophagus,51070;TE-6,,,esophagus,51071;TGBC11TKB,,,stomach,51074;TGBC1TKB,,,biliary tract,51075;TK10,,,kidney,51077;UACC-257,,,skin,51078;ECC10,,,stomach,50919;JEG-3,,,miscellaneous,50961;697.0,,,blood,50877;LU-139,,,lung,50994;CTB-1,,,lymphatic system,50905;ES3,,,bone,50927;TE-11,,,esophagus,51066;TGBC24TKB,,,biliary tract,51076;KLE,,,uterus,50968;LC-1F,,,lung,50986;HCE-4,,,esophagus,50953;A4-Fuk,,,skin,50883;SK-MEL-24,,,skin,51050;CP50-MEL-B,,,skin,50903;YH-13,,,brain,51080;OC-314,,,ovary,51031;RF-48,,,stomach,51040;SK-MG-1,,,brain,51052;B2-17,,,brain,50889;Mo-T,,,blood,51001;KP-N-YN,,,nervous system,50972;D-423MG,,,brain,50911;H9,,,lymphatic system,50949;D-566MG,,,brain,50914;SK-MEL-5,,,skin,51051;NBsusSR,,,nervous system,51016;A101D,,,skin,50879;A388,,,miscellaneous,50881;BB65-RCC,,,kidney,50892;BOKU,,,cervix,50895;D-502MG,,,brain,50912;GCIY,,,stomach,50944;HA7-RCC,,,kidney,50950;LC-2-ad,,,lung,50987;LS-1034,,,intestine,50989;NB12,,,nervous system,51008;OCUB-M,,,breast,51032;OVCAR-4,,,ovary,51036;RXF393,,,kidney,51044;SJSA-1,,,bone,51049;SW962,,,vulva,51062;TE-12,,,esophagus,51067;TE-15,,,esophagus,51068;TE-8,,,esophagus,51072;TE-9,,,esophagus,51073;VA-ES-BJ,,,miscellaneous,51079;LB647-SCLC,,,lung,50982;ALL-PO,,,blood,50886;AM-38,,,brain,50887;ATN-1,,,blood,50888;BB49-HNC,,,head &amp; neck,50891;CAS-1,,,brain,50898;DEL,,,blood,50915;DOHH-2,,,lymphatic system,50917;ECC4,,,intestine,50921;EM-2,,,blood,50924;EoL-1-cell,,,blood,50925;EW-18,,,bone,50938;GR-ST,,,blood,50947;JVM-2,,,blood,50962;KM12,,,intestine,50969;LOXIMVI,,,skin,50988;LU-134-A,,,lung,50993;LU-165,,,lung,50995;MHH-CALL-2,,,blood,50998;MN-60,,,blood,51000;MUTZ-1,,,blood,51003;NMC-G1,,,brain,51025;NOMO-1,,,blood,51028;QIMR-WIL,,,blood,51037;Ramos-2G6-4C10,,,lymphatic system,51038;RPMI-8866,,,blood,51043;SK-MM-2,,,blood,51053;IST-SL1,,,lung,50959</t>
+  </si>
+  <si>
+    <t>1055\cell lines</t>
+  </si>
+  <si>
+    <t>A 769662,small molecule,10174-101,LSM-1175;GSK1904529A,small molecule,10134-101,LSM-1134;Doxorubicin,small molecule,10248-101,LSM-4062;Gemcitabine,small molecule,10252-101,LSM-5333</t>
+  </si>
+  <si>
+    <t>false\small molecules,4</t>
+  </si>
+  <si>
+    <t>http://lincs.hms.harvard.edu/db/datasets/20011/</t>
+  </si>
+  <si>
+    <t>MGH (CMT) Growth Inhibition Assay Protocol (9 compound doses: 0.512 uM to 0.002 uM) -- DNA Staining</t>
+  </si>
+  <si>
+    <t>5637.0,epithelial,,urinary bladder,50001;647-V,epithelial-like,,urinary bladder,50002;A375.S2,epithelial,,skin,50003;AGS,epithelial,,stomach,50004;BPH-1,epitheloid,,prostate,50005;Ca Ski,epithelial,,cervix,50006;Ca9-22,epithelial-like,,head &amp; neck,50007;CAL-51,epithelial-like,,breast,50008;Calu-1,epithelial,,lung,50009;Calu-3,epithelial,,lung,50010;COLO-679,fibroblastic,,skin,50011;COLO-800,epithelial-like,,skin,50012;FU97,epithelial-like,,stomach,50013;HEC-1,,,uterus,50014;HLF,,,liver,50015;HUTU-80,epithelial,,intestine,50016;IA-LM,,,lung,50017;Ishikawa,epithelial-like,,uterus,50018;Ishikawa (Heraklio) 02 ER-,epithelial,,uterus,50019;IST-MEL1,epithelial-like,,skin,50020;JHH-6,epithelial-like,,liver,50021;KMRC-20,epithelial-like,,kidney,50023;KYSE-140,,,esophagus,50024;KYSE-150,epitheloid,,esophagus,50025;KYSE-180,epitheloid,,esophagus,50026;KYSE-450,epitheloid,,esophagus,50027;LNZTA3WT4,,,brain,50028;MCF7,epithelial,,breast,50029;MDA-MB-435S,melanocyte,,skin,50030;MT-3,epithelial,,breast,50031;NCI-H1648,,,lung,50032;NCI-H1651,epithelial,,lung,50033;NCI-H1703,epithelial,,lung,50034;NCI-H1915,large cell,,lung,50035;NCI-H2023,,,lung,50036;NCI-H810,epithelial,,lung,50037;PE/CA-PJ15,epithelial-like,,head &amp; neck,50039;SJCRH30,fibroblast,,muscle,50041;SK-LMS-1,,,uterus,50042;SK-OV-3,epithelial,,ovary,50044;SNB75,,,brain,50045;SW527,epithelial,,breast,50046;SW620,epithelial,,intestine,50047;T24,epithelial,,urinary bladder,50048;WiDr,epithelial,,intestine,50049;Hep 3B2.1-7,epithelial,,liver,50051;Hep G2,epithelial,,liver,50052;Huh7,,,liver,50055;1205Lu,,,skin,50062;1321N1,,,brain,50063;143B,,,bone,50064;143B PML BK TK,,,bone,50065;1A6,,,urinary bladder,50066;22RV1,,,prostate,50067;23132/87,,,stomach,50068;42-MG-BA,,,brain,50069;639-V,,,ureter,50071;769-P,,,kidney,50072;786-O,,,kidney,50073;8305C,,,thyroid,50074;8505C,,,thyroid,50075;A172,,,brain,50076;A-204,,,muscle,50077;A2058,,,skin,50078;A2780,,,ovary,50079;A2780ADR,,,ovary,50080;A373-C6,,,skin,50081;A-427,,,lung,50082;A431,,,skin,50083;A549,,,lung,50084;A673,,,muscle,50085;ABC-1,,,lung,50086;ACHN,,,kidney,50087;AN3CA,,,uterus,50088;ASH-3,,,thyroid,50089;AsPC-1,,,pancreas,50090;AU565,,,breast,50091;AZ-521,,,stomach,50092;B-CPAP,,,thyroid,50093;BE(2)-C,,,nervous system,50094;BEN,,,lung,50095;BeWo,,,miscellaneous,50096;BFTC-905,,,urinary bladder,50097;BFTC-909,,,kidney,50098;BHT-101,,,thyroid,50099;BHY,,,head &amp; neck,50100;BICR 10,,,head &amp; neck,50101;BICR 22,,,head &amp; neck,50102;BICR 31,,,head &amp; neck,50103;BICR 78,,,head &amp; neck,50104;BT-20,,,breast,50105;BT-474,,,breast,50106;BT-483,,,breast,50107;BT-549,,,breast,50108;BxPC-3,,,pancreas,50109;C170,,,intestine,50110;C2BBe1,,,intestine,50111;C32,,,skin,50112;C-33 A,,,cervix,50113;C3A,,,liver,50114;C-4 I,,,cervix,50115;C-4 II,,,cervix,50116;Caco-2,,,intestine,50117;Caki-1,,,kidney,50118;CAL 27,,,head &amp; neck,50119;CAL-120,,,breast,50120;CAL-12T,,,lung,50121;CAL-148,,,breast,50122;CAL-29,,,urinary bladder,50123;CAL-33,,,head &amp; neck,50124;CAL-39,,,vulva,50125;CAL-54,,,kidney,50126;CAL-62,,,thyroid,50127;CAL-72,,,bone,50128;CAL-78,,,bone,50129;CAL-85-1,,,breast,50130;CAMA-1,,,breast,50131;Caov-3,,,ovary,50132;Caov-4,,,ovary,50133;Capan-1,,,pancreas,50134;Capan-2,,,pancreas,50135;CaR-1,,,intestine,50136;CCF-STTG1,,,brain,50137;CCK-81,,,intestine,50138;CHP-212,,,nervous system,50139;CoCM-1,,,intestine,50141;COLO 201,,,intestine,50142;COLO 205,,,intestine,50143;COLO 320DM,,,intestine,50144;COLO 741,,,intestine,50145;COLO 792,,,skin,50146;COLO 853,,,skin,50147;COLO 857,,,skin,50148;COLO 858,,,skin,50149;COLO-206F,,,intestine,50150;COLO-320,,,intestine,50151;COLO-678,,,intestine,50152;COLO-680N,,,esophagus,50153;COLO-783,,,skin,50154;COLO-818,,,skin,50155;COLO-824,,,breast,50156;COLO-849,,,skin,50157;COR-L 105,,,lung,50158;COR-L 23/CPR,,,lung,50159;COR-L23,,,lung,50160;DAN-G,,,pancreas,50161;Daoy,,,brain,50162;DBTRG-05MG,,,brain,50163;Detroit 562,,,head &amp; neck,50164;DK-MG,,,brain,50165;DLD-1,,,intestine,50166;DMS 273,,,lung,50167;DMS 53,,,lung,50168;DOK,,,head &amp; neck,50169;DoTc2 4510,,,cervix,50170;DU 145,,,prostate,50171;DV-90,,,lung,50172;EBC-1,,,lung,50173;EFE-184,,,uterus,50174;EFM-19,,,breast,50175;EFM-192A,,,breast,50176;EFM-192B,,,breast,50177;EFM-192C,,,breast,50178;EFO-21,,,ovary,50179;EFO-27,,,ovary,50180;EGI-1,,,biliary tract,50181;EJ138,,,urinary bladder,50182;EN,,,uterus,50183;EPLC-272H,,,lung,50184;ES-2,,,ovary,50185;ESS-1,,,uterus,50186;EVSA-T,,,breast,50187;FaDu,,,head &amp; neck,50188;FLYA13,,,miscellaneous,50189;FTC-133,,,thyroid,50190;FTC-238,,,thyroid,50191;FU-OV-1,,,ovary,50192;G-292 Clone A141B1,,,bone,50193;G-361,,,skin,50194;G-401,,,kidney,50195;G-402,,,kidney,50196;GAMG,,,brain,50197;GCT,,,miscellaneous,50198;GMS-10,,,brain,50199;GOS-3,,,brain,50200;GP5d,,,intestine,50201;H4,,,brain,50202;HARA,,,lung,50204;HCC1143,,,breast,50205;HCC1395,,,breast,50206;HCC1419,,,breast,50207;HCC1428,,,breast,50208;HCC-15,,,lung,50209;HCC1569,,,breast,50210;HCC1806,,,breast,50211;HCC1937,,,breast,50212;HCC1954,,,breast,50213;HCC-366,,,lung,50215;HCC38,,,breast,50216;HCC-44,,,lung,50217;HCC-56,,,intestine,50218;HCC70,,,breast,50219;HCC-78,,,lung,50220;HCC-827,,,lung,50221;HCT 116,,,intestine,50222;HCT-15,,,intestine,50223;HCT-8,,,intestine,50224;HDQ-P1,,,breast,50225;H-EMC-SS,,,bone,50226;HGC-27,,,stomach,50227;HLE,,,liver,50228;HMVII,,,skin,50229;HN,,,head &amp; neck,50230;HO-1-N-1,,,head &amp; neck,50231;HO-1-u-1,,,head &amp; neck,50232;HOS,,,bone,50233;HPAC,,,pancreas,50234;HPAF-II,,,pancreas,50235;HRT-18,,,intestine,50236;Hs 257.T,,,intestine,50237;Hs 578T,,,breast,50238;Hs 588.T,,,cervix,50239;Hs 633T,,,miscellaneous,50240;Hs 683,,,brain,50241;Hs 746T,,,stomach,50242;Hs 766T,,,pancreas,50243;HSC-2,,,head &amp; neck,50244;HSC-3,,,head &amp; neck,50245;HSC-4,,,head &amp; neck,50246;HT 1080,,,miscellaneous,50247;HT 1376,,,urinary bladder,50248;HT115,,,intestine,50249;HT-1197,,,urinary bladder,50250;HT-29,,,intestine,50251;HT-3,,,cervix,50252;HT55,,,intestine,50253;HTC-C3,,,thyroid,50254;HuCCT1,,,biliary tract,50255;huH-1,,,liver,50256;HuO-3N1,,,bone,50257;HuO9,,,bone,50258;HuO9N2,,,bone,50259;HUP-T3,,,pancreas,50260;HUP-T4,,,pancreas,50261;IGR-1,,,skin,50262;IGR-37,,,skin,50263;IGR-39,,,skin,50264;IHH-4,,,thyroid,50265;IM-95,,,stomach,50266;IM-95m,,,stomach,50267;IMR-32,,,nervous system,50268;IPC-298,,,skin,50269;J82,,,urinary bladder,50270;JAR,,,miscellaneous,50271;JHH-1,,,liver,50272;JHH-2,,,liver,50273;JHH-4,,,liver,50274;JHH-7,,,liver,50275;JIMT-1,,,breast,50276;KELLY,,,nervous system,50277;KG-1-C,,,brain,50278;KHOS/NP,,,bone,50280;KHOS-240S,,,bone,50281;KHOS-312H,,,bone,50282;KMH-2,,,thyroid,50283;KMRC-1,,,kidney,50284;KON,,,head &amp; neck,50285;KOSC-2 cl3-43,,,head &amp; neck,50286;KP-2,,,pancreas,50287;KP-3,,,pancreas,50288;KP-3L,,,pancreas,50289;KP-4,,,pancreas,50290;KPL-1,,,breast,50291;KU-19-19,,,urinary bladder,50292;KYSE-220,,,esophagus,50293;KYSE-270,,,esophagus,50294;KYSE-30,,,esophagus,50295;KYSE-410,,,esophagus,50296;KYSE-50,,,esophagus,50297;KYSE-510,,,esophagus,50298;KYSE-520,,,esophagus,50299;KYSE-70,,,esophagus,50300;LC-1 sq,,,lung,50301;LCLC-103H,,,lung,50302;LCLC-97TM1,,,lung,50303;LK-2,,,lung,50304;LN-18,,,brain,50305;LN-229,,,brain,50306;LN-405,,,brain,50307;LNZTA3WT11,,,brain,50308;LOU-NH91,,,lung,50309;LoVo,,,intestine,50310;LS174T,,,intestine,50311;LS180,,,intestine,50312;Lu-135,,,lung,50314;LU65,,,lung,50315;LU65A,,,lung,50316;LU65B,,,lung,50317;LU65C,,,lung,50318;LU99A,,,lung,50319;LU99B,,,lung,50320;LU99C,,,lung,50321;LUDLU-1,,,lung,50322;M059J,,,brain,50323;MB 157,,,breast,50324;MCAS,,,ovary,50325;MC-IXC,,,nervous system,50326;MDA-MB-134-VI,,,breast,50327;MDA-MB-157,,,breast,50328;MDA-MB-175-VII,,,breast,50329;MDA-MB-330,,,breast,50330;MDA-MB-361,,,breast,50331;MDA-MB-415,,,breast,50332;MDA-MB-436,,,breast,50333;MDA-MB-453,,,breast,50334;MDA-MB-468,,,breast,50335;MDST8,,,intestine,50336;ME-180,,,cervix,50337;MEL-HO,,,skin,50338;MEL-JUSO,,,skin,50339;MES-SA,,,uterus,50340;MES-SA/Dx-5,,,uterus,50341;MEWO,,,skin,50342;MFE-280,,,uterus,50343;MFE-296,,,uterus,50344;MFE-319,,,uterus,50345;MFM-223,,,breast,50346;MG-63,,,bone,50347;MHH-ES-1,,,nervous system,50348;MIA PaCa-2,,,pancreas,50349;MKN1,,,stomach,50350;MKN28,,,stomach,50351;MKN45,,,stomach,50352;MKN7,,,stomach,50353;MKN74,,,stomach,50354;ML-1,,,thyroid,50355;MOG-G-CCM,,,brain,50356;MOG-G-UVW,,,brain,50357;MS751,,,cervix,50358;MSTO-211H,,,pleura,50359;NB69,,,nervous system,50360;NCC-IT-A3,,,testes,50361;NCI-H1048,,,lung,50362;NCI-H1299,,,lung,50363;NCI-H1435,,,lung,50364;NCI-H1437,,,lung,50365;NCI-H1568,,,lung,50366;NCI-H1573,,,lung,50367;NCI-H1581,,,lung,50368;NCI-H1623,,,lung,50369;NCI-H1650,,,lung,50370;NCI-H1688,,,lung,50371;NCI-H1693,,,lung,50372;NCI-H1734,,,lung,50373;NCI-H1755,,,lung,50374;NCI-H1781,,,lung,50375;NCI-H1792,,,lung,50376;NCI-H1793,,,lung,50377;NCI-H1869,,,lung,50378;NCI-H1876,,,lung,50379;NCI-H1944,,,lung,50380;NCI-H196,,,lung,50381;NCI-H1993,,,lung,50382;NCI-H2009,,,lung,50383;NCI-H2029,,,lung,50384;NCI-H2030,,,lung,50385;NCI-H2073,,,lung,50386;NCI-H2085,,,lung,50387;NCI-H2087,,,lung,50388;NCI-H2110,,,lung,50389;NCI-H2122,,,lung,50390;NCI-H2135,,,lung,50391;NCI-H2170,,,lung,50392;NCI-H2172,,,lung,50393;NCI-H2195,,,lung,50394;NCI-H2196,,,lung,50395;NCI-H2198,,,lung,50396;NCI-H2228,,,lung,50397;NCI-H2286,,,lung,50398;NCI-H2291,,,lung,50399;NCI-H23,,,lung,50400;NCI-H2342,,,lung,50401;NCI-H2347,,,lung,50402;NCI-H2405,,,lung,50403;NCI-H2444,,,lung,50404;NCI-H2452,,,lung,50405;NCI-H322,,,lung,50407;NCI-H358,,,lung,50408;NCI-H441,,,lung,50409;NCI-H460,,,lung,50410;NCI-H520,,,lung,50411;NCI-H522,,,lung,50412;NCI-H596,,,lung,50413;NCI-H630,,,intestine,50414;NCI-H647,,,lung,50415;NCI-H650,,,lung,50416;NCI-H661,,,lung,50417;NCI-H727,,,lung,50418;NCI-H838,,,lung,50419;NCI-H841,,,lung,50420;NCI-N87,,,stomach,50421;NIH:OVCAR-3,,,ovary,50422;NUGC-3,,,stomach,50424;NUGC-4,,,stomach,50425;NY,,,bone,50426;OAW28,,,ovary,50427;OAW42,,,ovary,50428;OCUG-1,,,gall bladder,50429;OCUM-1,,,stomach,50430;OE19,,,esophagus,50431;OE21,,,esophagus,50432;OE33,,,esophagus,50433;OSC-19,,,head &amp; neck,50434;OSC-20,,,head &amp; neck,50435;OUMS-23,,,intestine,50436;OV-90,,,ovary,50437;OVISE,,,ovary,50438;OVKATE,,,ovary,50439;OVMIU,,,ovary,50440;OVSAYO,,,ovary,50441;OVTOKO,,,ovary,50442;PA-1,,,ovary,50443;Panc 02.03,,,pancreas,50444;Panc 03.27,,,pancreas,50445;Panc 04.03,,,pancreas,50446;Panc 08.13,,,pancreas,50447;Panc 10.05,,,pancreas,50448;PANC-1,,,pancreas,50449;PA-TU-8902,,,pancreas,50450;PA-TU-8988S,,,pancreas,50451;PA-TU-8988T,,,pancreas,50452;PC-14,,,lung,50453;PC-3,,,prostate,50454;PFSK-1,,,brain,50455;PL45,,,pancreas,50456;PLC/PRF/5,,,liver,50457;RCM-1,,,intestine,50459;RD,,,muscle,50460;RD-ES,,,nervous system,50461;RERF-GC-1B,,,stomach,50462;RERF-LC-Ad1,,,lung,50463;RERF-LC-KJ,,,lung,50464;RERF-LC-MA,,,lung,50465;RERF-LC-Sq1,,,lung,50466;RKN,,,ovary,50467;RMG-I,,,ovary,50468;RO82-W-1,,,thyroid,50469;RPMI 2650,,,head &amp; neck,50470;RPMI-7951,,,skin,50471;RT-112,,,urinary bladder,50472;RT112/84,,,urinary bladder,50473;RT4,,,urinary bladder,50474;RVH-421,,,skin,50475;S-117,,,thyroid,50476;Saos-2,,,bone,50477;SAS,,,head &amp; neck,50478;SAT,,,head &amp; neck,50479;SBC-3,,,lung,50480;SBC-5,,,lung,50481;SCaBER,,,urinary bladder,50482;SCC-15,,,head &amp; neck,50483;SCC-25,,,head &amp; neck,50484;SCC-4,,,head &amp; neck,50485;SCC-9,,,head &amp; neck,50486;SCCH-26,,,nervous system,50488;SCH,,,stomach,50489;SCLC-21H,,,lung,50490;SHP-77,,,lung,50491;SiHa,,,cervix,50493;SISO,,,cervix,50494;SK-CO-1,,,intestine,50495;SK-ES-1,,,bone,50496;SKG-IIIa,,,cervix,50497;SKG-IIIb,,,cervix,50498;SK-HEP-1,,,liver,50499;SK-LU-1,,,lung,50500;SK-MEL-2,,,skin,50501;SK-MEL-30,,,skin,50502;SKN,,,uterus,50503;SKN-3,,,head &amp; neck,50504;SK-N-AS,,,nervous system,50505;SK-N-DZ,,,nervous system,50506;SK-NEP-1,,,kidney,50507;SK-N-SH,,,nervous system,50508;SNG-M,,,uterus,50509;SNU-1,,,stomach,50510;SNU-16,,,stomach,50511;SNU-182,,,liver,50512;SNU-387,,,liver,50513;SNU-398,,,liver,50514;SNU-423,,,liver,50515;SNU-449,,,liver,50516;SNU-475,,,liver,50517;SNU-5,,,stomach,50518;SU.86.86,,,pancreas,50520;SUIT-2,,,pancreas,50521;SW 1088,,,brain,50522;SW 1271,,,lung,50524;SW 13,,,adrenal gland,50525;SW 1417,,,intestine,50526;SW 1463,,,intestine,50527;SW 156,,,kidney,50528;SW 1573,,,lung,50529;SW 1783,,,brain,50530;SW 48,,,intestine,50531;SW 626,,,ovary,50532;SW 780,,,urinary bladder,50533;SW 900,,,lung,50534;SW-1710,,,urinary bladder,50535;SW756,,,cervix,50536;SW837,,,intestine,50537;SW-948,,,intestine,50538;T.T,,,esophagus,50539;T.Tn,,,esophagus,50540;T47D,,,breast,50541;T84,,,intestine,50542;T98G,,,brain,50543;TASK1,,,nervous system,50544;TCCSUP,,,urinary bladder,50545;TGW,,,adrenal gland,50546;TOV-112D,,,ovary,50547;TOV-21G,,,ovary,50548;TT2609-C02,,,thyroid,50549;TYK-nu,,,ovary,50550;U-118 MG,,,brain,50551;U-138 MG,,,brain,50552;U-2 OS,,,bone,50553;U-251 MG,,,brain,50554;U373 MG,,,brain,50555;UACC-812,,,breast,50556;UACC-893,,,breast,50557;UMC-11,,,lung,50558;UM-UC-3,,,urinary bladder,50559;VCaP,,,prostate,50560;VM-CUB1,,,urinary bladder,50561;VMRC-LCP,,,lung,50562;VMRC-MELG,,,skin,50563;VMRC-RCW,,,kidney,50564;VMRC-RCZ,,,kidney,50565;WM 266-4,,,skin,50566;WM-115,,,skin,50567;WM1552C,,,skin,50568;WM278,,,skin,50569;WM35,,,skin,50570;WM793B,,,skin,50571;YAPC,,,pancreas,50572;YKG-1,,,brain,50573;ZR-75-1,,,breast,50574;ZR-75-30,,,breast,50575;2B8,,,lymphatic system,50585;A2780cis,,,ovary,50586;A3,,,blood,50587;A3/KAW,,,lymphatic system,50588;AGR-ON,,,blood,50589;ALL-SIL,,,blood,50590;AMO-1,,,lymphatic system,50591;ARH-77,,,blood,50592;BALL-1,,,blood,50593;BC-1,,,lymphatic system,50594;BC-2,,,lymphatic system,50595;BC-3,,,lymphatic system,50596;BDCM,,,blood,50597;BE(2)-M17,,,nervous system,50598;BL-41,,,lymphatic system,50599;BL-70,,,lymphatic system,50600;C8166,,,blood,50601;CA46,,,lymphatic system,50602;CCRF-CEM,,,blood,50603;CCRF-HSB-2,,,blood,50604;CCRF-SB,,,blood,50605;CEM/C1,,,blood,50606;CEM/C2,,,blood,50607;CESS,,,blood,50608;CFPAC-1,,,pancreas,50609;ChaGo-K-1,,,lung,50610;CHP-126,,,nervous system,50611;CI-1,,,lymphatic system,50612;CL-11,,,intestine,50613;Clone 15 HL-60,,,blood,50614;CMK,,,blood,50615;COLO 684,,,uterus,50616;COLO-704,,,ovary,50617;COR-L279,,,lung,50618;COR-L51,,,lung,50619;COR-L88,,,lung,50620;COR-L95,,,lung,50621;CPC-N,,,lung,50622;CTV-1,,,blood,50623;D283 Med,,,brain,50624;Daudi,,,lymphatic system,50625;DB,,,lymphatic system,50626;DERL-2,,,lymphatic system,50627;DG-75,,,lymphatic system,50628;DMS 114,,,lung,50629;DMS 153,,,lung,50630;DMS 79,,,lung,50631;DND-41,,,blood,50632;EB1,,,lymphatic system,50633;EB2,,,lymphatic system,50634;EB-3,,,lymphatic system,50635;EHEB,,,blood,50636;EJM,,,blood,50637;Eos-HL-60,,,blood,50638;Farage,,,lymphatic system,50639;GA-10,,,lymphatic system,50640;GA-10 (Clone 20),,,lymphatic system,50641;GDM-1,,,blood,50642;GOTO,,,nervous system,50643;Gp2D,,,intestine,50644;GRANTA-519,,,lymphatic system,50645;H33HJ-JA1,,,blood,50646;HC-1,,,blood,50647;HCC-33,,,lung,50648;HDLM-2,,,lymphatic system,50649;HD-MY-Z,,,lymphatic system,50650;HEL,,,blood,50651;HEL 92.1.7,,,blood,50652;HH,,,lymphatic system,50653;HL-60,,,blood,50654;HL60(S),,,blood,50655;HL-60/MX2,,,blood,50656;HL60RG,,,blood,50657;Hs 445,,,lymphatic system,50658;HS-Sultan,,,lymphatic system,50659;HT,,,lymphatic system,50660;HuT 78,,,lymphatic system,50661;I 2.1,,,blood,50662;I 9.2,,,blood,50663;IM-9,,,lymphatic system,50664;J.gamma1,,,blood,50665;J.gamma1.WT,,,blood,50666;J.RT3-T3.5,,,blood,50667;J45.01,,,blood,50668;Jiyoye,,,lymphatic system,50669;JJN-3,,,blood,50670;JKT-beta-del,,,blood,50671;JM1,,,lymphatic system,50672;JSC-1,,,lymphatic system,50673;Jurkat, Clone E6-1,,,blood,50674;JURL-MK1,,,blood,50675;JURL-MK2,,,blood,50676;K-562,,,blood,50677;K562/ADM,,,blood,50678;KARPAS-231,,,blood,50679;KARPAS-299,,,lymphatic system,50680;KARPAS-422,,,lymphatic system,50681;KARPAS-45,,,blood,50682;KARPAS-620,,,blood,50683;Kasumi-1,,,blood,50684;KCL-22,,,blood,50685;KE-37,,,blood,50686;KG-1,,,blood,50687;KG-1a,,,blood,50688;KM-H2,,,lymphatic system,50689;KMOE-2,,,blood,50690;KMS-12-BM,,,blood,50691;KMS-12-PE,,,blood,50692;KO52,,,blood,50693;KOPN-8,,,blood,50694;KP-1N,,,pancreas,50695;KP-1NL,,,pancreas,50696;KU812,,,blood,50697;KU812E,,,blood,50698;KU812F,,,blood,50699;KY821,,,blood,50700;KY821A3,,,blood,50701;KYM-1,,,muscle,50702;L-1236,,,lymphatic system,50703;L-363,,,blood,50704;L-428,,,lymphatic system,50705;L-540,,,lymphatic system,50706;LAMA-84,,,blood,50707;LC4-1,,,blood,50708;Loucy,,,blood,50709;LP-1,,,blood,50710;Lu-134-B,,,lung,50711;M059K,,,brain,50712;MC/CAR,,,lymphatic system,50713;MC116,,,lymphatic system,50714;ME-1,,,blood,50715;MEC-1,,,blood,50716;MEC-2,,,blood,50717;MEG-01,,,blood,50718;MHH-NB-11,,,nervous system,50719;MHH-PREB-1,,,lymphatic system,50720;MJ,,,lymphatic system,50721;ML-2,,,blood,50722;MLMA,,,blood,50723;MOLM-13,,,blood,50724;MOLP-8,,,blood,50725;MOLT-14,,,blood,50726;MOLT-16,,,blood,50727;MOLT-4,,,blood,50728;MOLT-4F,,,blood,50729;MONO-MAC-1,,,blood,50730;MONO-MAC-6,,,blood,50731;MRK-nu-1,,,breast,50732;MS-1-L,,,lung,50733;MV-4-11,,,blood,50734;MY,,,blood,50735;MY-M12,,,blood,50736;MY-M13,,,blood,50737;NALM-19,,,blood,50738;NALM-6,,,blood,50739;NAMALWA,,,lymphatic system,50740;NAMALWA.PNT,,,lymphatic system,50741;NB(TU)1-10,,,nervous system,50742;NB-1,,,nervous system,50743;NB-4,,,blood,50744;NC-37,,,lymphatic system,50745;NCI-H1092,,,lung,50746;NCI-H1155,,,lung,50747;NCI-H1304,,,lung,50748;NCI-H1385,,,lung,50749;NCI-H1395,,,lung,50750;NCI-H1404,,,lung,50751;NCI-H1417,,,lung,50752;NCI-H1436,,,lung,50753;NCI-H1522,,,lung,50754;NCI-H1563,,,lung,50755;NCI-H1618,,,lung,50756;NCI-H1666,,,lung,50757;NCI-H1694,,,lung,50758;NCI-H1770,,,lung,50759;NCI-H1836,,,lung,50760;NCI-H1838,,,lung,50761;NCI-H187,,,lung,50762;NCI-H1882,,,lung,50763;NCI-H1963,,,lung,50764;NCI-H1975,,,lung,50765;NCI-H2081,,,lung,50766;NCI-H209,,,lung,50767;NCI-H2106,,,lung,50768;NCI-H211,,,lung,50769;NCI-H2141,,,lung,50770;NCI-H2171,,,lung,50771;NCI-H220,,,lung,50772;NCI-H2227,,,lung,50773;NCI-H226,,,lung,50774;NCI-H345,,,lung,50775;NCI-H446,,,lung,50776;NCI-H510A,,,lung,50777;NCI-H524,,,lung,50778;NCI-H526,,,lung,50779;NCI-H69,,,lung,50780;NCI-H719,,,lung,50781;NCI-H720,,,lung,50782;NCI-H748,,,lung,50783;NCI-H82,,,lung,50784;NCI-H847,,,lung,50785;NCI-H889,,,lung,50786;NEC8,,,testes,50787;NH-12,,,nervous system,50788;NK-92MI,,,lymphatic system,50789;NOMO-1/ADM,,,blood,50790;NU-DUL-1,,,lymphatic system,50791;OCI-AML2,,,blood,50792;OCI-AML3,,,blood,50793;OCI-AML5,,,blood,50794;OCI-LY-19,,,lymphatic system,50795;OCI-M1,,,blood,50796;OPM-2,,,blood,50797;P116.cl39,,,blood,50798;P12-ICHIKAWA,,,blood,50799;P30/OHK,,,blood,50800;P31/FUJ,,,blood,50801;P32/ISH,,,lymphatic system,50802;P3HR-1,,,lymphatic system,50803;PC-3 [JPC-3],,,lung,50804;PEER,,,blood,50805;PF-382,,,blood,50806;Pfeiffer,,,lymphatic system,50807;PL-21,,,blood,50808;PSN1,,,pancreas,50809;Raji,,,lymphatic system,50810;Ramos (RA 1),,,blood,50811;RC-K8,,,lymphatic system,50812;REC-1,,,lymphatic system,50813;Reh,,,blood,50814;RERF-LC-MS,,,lung,50815;RH-1,,,bone,50816;RH-30,,,muscle,50817;RH-41,,,muscle,50818;RL,,,lymphatic system,50819;ROS-50,,,blood,50820;RPMI 1788,,,blood,50821;RPMI 6666,,,lymphatic system,50822;RPMI 8226,,,blood,50823;RPMI-8402,,,blood,50824;RS4;11,,,blood,50825;SBC-1,,,lung,50826;SBC-2,,,lung,50827;SC-1,,,lymphatic system,50828;SCC-3,,,lymphatic system,50829;Sci-1,,,lymphatic system,50830;SIG-M5,,,blood,50831;SIMA,,,nervous system,50832;SK-MEL-1,,,skin,50833;SK-MEL-3,,,skin,50834;SK-N-BE(2),,,nervous system,50835;SK-N-FI,,,nervous system,50836;SLVL,,,lymphatic system,50837;SNB-19,,,brain,50838;SR,,,lymphatic system,50839;ST486,,,lymphatic system,50840;SU-DHL-1,,,lymphatic system,50841;SU-DHL-10,,,lymphatic system,50842;SU-DHL-16,,,lymphatic system,50843;SU-DHL-4,,,lymphatic system,50844;SU-DHL-5,,,lymphatic system,50845;SU-DHL-6,,,lymphatic system,50846;SU-DHL-8,,,lymphatic system,50847;SUP-B15,,,blood,50848;SUP-HD1,,,lymphatic system,50849;SUP-M2,,,lymphatic system,50850;SUP-T1,,,blood,50851;SVG p12,,,brain,50852;SW 1990,,,pancreas,50853;TALL-1,,,blood,50854;TANOUE,,,blood,50855;TC-71,,,bone,50856;Tera-1,,,testes,50857;TF-1,,,blood,50858;TF-1.CN5a.1,,,blood,50859;TF-1a,,,blood,50860;THP-1,,,blood,50861;TK,,,lymphatic system,50862;Toledo,,,lymphatic system,50863;TT,,,thyroid,50864;TUR,,,lymphatic system,50865;U266B1,,,blood,50866;U-698-M,,,blood,50867;U-87 MG,,,brain,50868;U-937,,,lymphatic system,50869;VAL,,,lymphatic system,50870;WIL2 NS,,,lymphatic system,50871;WILCL,,,blood,50872;WSU-DLCL2,,,lymphatic system,50873;WSU-NHL,,,lymphatic system,50874;YMB-1,,,breast,50875;YT,,,lymphatic system,50876;A-375,epithelial,,skin,50060;DU4475,epithelial,,breast,50577;HCC1187,epithelial,,breast,50578;HCC1500,epithelial,,breast,50579;HCC1599,epithelial,,breast,50580;HCC2157,epithelial,,breast,50581;HCC2218,epithelial,,breast,50582;HeLa,epithelial,,cervix,50061;LNCaP,epithelial,,prostate,50059;MDA-MB-231,epithelial,,breast,50058;SK-BR-3,epithelial,,breast,50057;SK-MES,epithelial,,lung,50043;CGTH-W-1,,,thyroid,50899;LB647-SCLC,,,lung,50982;8-MG-BA,,,brain,50878;A253,,,head &amp; neck,50880;A498,,,kidney,50882;A704,,,kidney,50884;ACN,,,nervous system,50885;ALL-PO,,,blood,50886;AM-38,,,brain,50887;ATN-1,,,blood,50888;BB30-HNC,,,head &amp; neck,50890;BB49-HNC,,,head &amp; neck,50891;BE-13,,,blood,50893;Becker,,,brain,50894;BOKU,,,cervix,50895;BV-173,,,blood,50896;Calu-6,,,lung,50897;CAS-1,,,brain,50898;COLO-320-HSR,,,intestine,50900;COLO-668,,,lung,50901;COLO-829,,,skin,50902;CP66-MEL,,,skin,50904;CW-2,,,intestine,50906;D-247MG,,,brain,50907;D-263MG,,,brain,50908;D-336MG,,,brain,50909;D-392MG,,,brain,50910;D-542MG,,,brain,50913;DEL,,,blood,50915;DJM-1,,,skin,50916;DOHH-2,,,lymphatic system,50917;DSH1,,,urinary tract,50918;ECC12,,,stomach,50920;ECC4,,,intestine,50921;EC-GI-10,,,esophagus,50922;EKVX,,,lung,50923;EM-2,,,blood,50924;EoL-1-cell,,,blood,50925;ES1,,,bone,50926;ES4,,,bone,50928;ES5,,,bone,50929;ES6,,,bone,50930;ES7,,,bone,50931;ES8,,,bone,50932;ETK-1,,,biliary tract,50933;EW-1,,,bone,50934;EW-11,,,bone,50935;EW-13,,,bone,50936;EW-16,,,bone,50937;EW-18,,,bone,50938;EW-24,,,bone,50939;EW-3,,,bone,50940;EW-7,,,bone,50941;GAK,,,skin,50942;GB-1,,,brain,50943;GI-1,,,brain,50945;GI-ME-N,,,nervous system,50946;GR-ST,,,blood,50947;GT3TKB,,,stomach,50948;HAL-01,,,blood,50951;HCC2998,,,intestine,50952;HCE-T,,,head &amp; neck,50954;HOP-62,,,lung,50955;HT-144,,,skin,50956;IMR-5,,,nervous system,50957;IST-MES1,,,pleura,50958;IST-SL2,,,lung,50960;JVM-2,,,blood,50962;JVM-3,,,blood,50963;K5,,,thyroid,50964;KALS-1,,,brain,50965;KGN,,,ovary,50966;KINGS-1,,,brain,50967;KM12,,,intestine,50969;KNS-42,,,brain,50970;KNS-81-FD,,,brain,50971;KP-N-YS,,,nervous system,50973;KS-1,,,brain,50974;KURAMOCHI,,,ovary,50975;LAN-5,,,nervous system,50976;LAN-6,,,nervous system,50977;LB1047-RCC,,,kidney,50978;LB2241-RCC,,,kidney,50979;LB2518-MEL,,,skin,50980;LB373-MEL-D,,,skin,50981;LB771-HNC,,,head &amp; neck,50983;LB831-BLC,,,urinary tract,50984;LB996-RCC,,,kidney,50985;LOXIMVI,,,skin,50988;LS-123,,,intestine,50990;LS-411N,,,intestine,50991;LS-513,,,intestine,50992;LU-134-A,,,lung,50993;LU-165,,,lung,50995;LXF-289,,,lung,50996;MFH-ino,,,miscellaneous,50997;MHH-CALL-2,,,blood,50998;MMAC-SF,,,skin,50999;MN-60,,,blood,51000;MPP-89,,,pleura,51002;MUTZ-1,,,blood,51003;MZ1-PC,,,pancreas,51004;MZ2-MEL,,,skin,51005;MZ7-mel,,,skin,51006;NB10,,,nervous system,51007;NB13,,,nervous system,51009;NB14,,,nervous system,51010;NB16,,,nervous system,51011;NB17,,,nervous system,51012;NB5,,,nervous system,51013;NB6,,,nervous system,51014;NB7,,,nervous system,51015;NCI-H1355,,,lung,51017;NCI-H157,,,lung,51018;NCI-H2126,,,lung,51019;NCI-H322M,,,lung,51020;NCI-H64,,,lung,51021;NCI-H716,,,intestine,51022;NCI-H747,,,intestine,51023;NKM-1,,,blood,51024;NMC-G1,,,brain,51025;no-10,,,brain,51026;no-11,,,brain,51027;NOMO-1,,,blood,51028;NOS-1,,,bone,51029;NTERA-S-cl-D1,,,testes,51030;OMC-1,,,cervix,51033;ONS-76,,,brain,51034;OS-RC-2,,,kidney,51035;QIMR-WIL,,,blood,51037;Ramos-2G6-4C10,,,lymphatic system,51038;RCC10RGB,,,kidney,51039;RKO,,,intestine,51041;RL95-2,,,uterus,51042;RPMI-8866,,,blood,51043;SF126,,,brain,51045;SF268,,,brain,51046;SF539,,,brain,51047;SH-4,,,skin,51048;SK-MM-2,,,blood,51053;SK-PN-DW,,,bone,51054;SK-UT-1,,,uterus,51055;SNU-C1,,,intestine,51056;SNU-C2B,,,intestine,51057;SW403,,,intestine,51058;SW684,,,miscellaneous,51059;SW872,,,miscellaneous,51060;SW954,,,vulva,51061;SW982,,,miscellaneous,51063;TE-1,,,esophagus,51064;TE-10,,,esophagus,51065;TE-441-T,,,muscle,51069;TE-5,,,esophagus,51070;TE-6,,,esophagus,51071;TGBC11TKB,,,stomach,51074;TGBC1TKB,,,biliary tract,51075;TK10,,,kidney,51077;UACC-257,,,skin,51078;ECC10,,,stomach,50919;JEG-3,,,miscellaneous,50961;697.0,,,blood,50877;LU-139,,,lung,50994;CTB-1,,,lymphatic system,50905;ES3,,,bone,50927;TE-11,,,esophagus,51066;IST-SL1,,,lung,50959;TGBC24TKB,,,biliary tract,51076;KLE,,,uterus,50968;LC-1F,,,lung,50986;HCE-4,,,esophagus,50953;A4-Fuk,,,skin,50883;SK-MEL-24,,,skin,51050;CP50-MEL-B,,,skin,50903;YH-13,,,brain,51080;OC-314,,,ovary,51031;RF-48,,,stomach,51040;SK-MG-1,,,brain,51052;B2-17,,,brain,50889;Mo-T,,,blood,51001;KP-N-YN,,,nervous system,50972;D-423MG,,,brain,50911;H9,,,lymphatic system,50949;D-566MG,,,brain,50914;SK-MEL-5,,,skin,51051;NBsusSR,,,nervous system,51016;A101D,,,skin,50879;A388,,,miscellaneous,50881;BB65-RCC,,,kidney,50892;D-502MG,,,brain,50912;GCIY,,,stomach,50944;HA7-RCC,,,kidney,50950;LC-2-ad,,,lung,50987;LS-1034,,,intestine,50989;NB12,,,nervous system,51008;OCUB-M,,,breast,51032;OVCAR-4,,,ovary,51036;RXF393,,,kidney,51044;SJSA-1,,,bone,51049;SW962,,,vulva,51062;TE-12,,,esophagus,51067;TE-15,,,esophagus,51068;TE-8,,,esophagus,51072;TE-9,,,esophagus,51073;VA-ES-BJ,,,miscellaneous,51079;HCC202,,,breast,50214</t>
+  </si>
+  <si>
+    <t>1058\cell lines</t>
+  </si>
+  <si>
+    <t>PKC412,small molecule,10220-101,LSM-1221;Ponatinib,small molecule,10150-101,LSM-1151;Thapsigargin,small molecule,10293-101,LSM-3545</t>
+  </si>
+  <si>
+    <t>http://lincs.hms.harvard.edu/db/datasets/20012/</t>
+  </si>
+  <si>
+    <t>MGH (CMT) Growth Inhibition Assay Protocol (9 compound doses: 8 nM to 0.03125 nM) -- DNA Staining</t>
+  </si>
+  <si>
+    <t>5637.0,epithelial,,urinary bladder,50001;647-V,epithelial-like,,urinary bladder,50002;A375.S2,epithelial,,skin,50003;AGS,epithelial,,stomach,50004;BPH-1,epitheloid,,prostate,50005;Ca Ski,epithelial,,cervix,50006;Ca9-22,epithelial-like,,head &amp; neck,50007;CAL-51,epithelial-like,,breast,50008;Calu-1,epithelial,,lung,50009;Calu-3,epithelial,,lung,50010;COLO-679,fibroblastic,,skin,50011;COLO-800,epithelial-like,,skin,50012;FU97,epithelial-like,,stomach,50013;HEC-1,,,uterus,50014;HLF,,,liver,50015;HUTU-80,epithelial,,intestine,50016;IA-LM,,,lung,50017;Ishikawa,epithelial-like,,uterus,50018;Ishikawa (Heraklio) 02 ER-,epithelial,,uterus,50019;IST-MEL1,epithelial-like,,skin,50020;JHH-6,epithelial-like,,liver,50021;KMRC-20,epithelial-like,,kidney,50023;KYSE-140,,,esophagus,50024;KYSE-150,epitheloid,,esophagus,50025;KYSE-180,epitheloid,,esophagus,50026;KYSE-450,epitheloid,,esophagus,50027;LNZTA3WT4,,,brain,50028;MCF7,epithelial,,breast,50029;MDA-MB-435S,melanocyte,,skin,50030;MT-3,epithelial,,breast,50031;NCI-H1648,,,lung,50032;NCI-H1651,epithelial,,lung,50033;NCI-H1703,epithelial,,lung,50034;NCI-H1915,large cell,,lung,50035;NCI-H2023,,,lung,50036;NCI-H810,epithelial,,lung,50037;PE/CA-PJ15,epithelial-like,,head &amp; neck,50039;SJCRH30,fibroblast,,muscle,50041;SK-LMS-1,,,uterus,50042;SK-MES,epithelial,,lung,50043;SK-OV-3,epithelial,,ovary,50044;SNB75,,,brain,50045;SW527,epithelial,,breast,50046;SW620,epithelial,,intestine,50047;T24,epithelial,,urinary bladder,50048;WiDr,epithelial,,intestine,50049;Hep 3B2.1-7,epithelial,,liver,50051;Hep G2,epithelial,,liver,50052;Huh7,,,liver,50055;SK-BR-3,epithelial,,breast,50057;MDA-MB-231,epithelial,,breast,50058;LNCaP,epithelial,,prostate,50059;A-375,epithelial,,skin,50060;HeLa,epithelial,,cervix,50061;1205Lu,,,skin,50062;1321N1,,,brain,50063;143B,,,bone,50064;143B PML BK TK,,,bone,50065;1A6,,,urinary bladder,50066;22RV1,,,prostate,50067;23132/87,,,stomach,50068;42-MG-BA,,,brain,50069;639-V,,,ureter,50071;769-P,,,kidney,50072;786-O,,,kidney,50073;8305C,,,thyroid,50074;8505C,,,thyroid,50075;A172,,,brain,50076;A-204,,,muscle,50077;A2058,,,skin,50078;A2780,,,ovary,50079;A2780ADR,,,ovary,50080;A373-C6,,,skin,50081;A-427,,,lung,50082;A431,,,skin,50083;A549,,,lung,50084;A673,,,muscle,50085;ABC-1,,,lung,50086;ACHN,,,kidney,50087;AN3CA,,,uterus,50088;ASH-3,,,thyroid,50089;AsPC-1,,,pancreas,50090;AU565,,,breast,50091;AZ-521,,,stomach,50092;B-CPAP,,,thyroid,50093;BE(2)-C,,,nervous system,50094;BEN,,,lung,50095;BeWo,,,miscellaneous,50096;BFTC-905,,,urinary bladder,50097;BFTC-909,,,kidney,50098;BHT-101,,,thyroid,50099;BHY,,,head &amp; neck,50100;BICR 10,,,head &amp; neck,50101;BICR 22,,,head &amp; neck,50102;BICR 31,,,head &amp; neck,50103;BICR 78,,,head &amp; neck,50104;BT-20,,,breast,50105;BT-474,,,breast,50106;BT-483,,,breast,50107;BT-549,,,breast,50108;BxPC-3,,,pancreas,50109;C170,,,intestine,50110;C2BBe1,,,intestine,50111;C32,,,skin,50112;C-33 A,,,cervix,50113;C3A,,,liver,50114;C-4 I,,,cervix,50115;C-4 II,,,cervix,50116;Caco-2,,,intestine,50117;Caki-1,,,kidney,50118;CAL 27,,,head &amp; neck,50119;CAL-120,,,breast,50120;CAL-12T,,,lung,50121;CAL-148,,,breast,50122;CAL-29,,,urinary bladder,50123;CAL-33,,,head &amp; neck,50124;CAL-39,,,vulva,50125;CAL-54,,,kidney,50126;CAL-62,,,thyroid,50127;CAL-72,,,bone,50128;CAL-78,,,bone,50129;CAL-85-1,,,breast,50130;CAMA-1,,,breast,50131;Caov-3,,,ovary,50132;Caov-4,,,ovary,50133;Capan-1,,,pancreas,50134;Capan-2,,,pancreas,50135;CaR-1,,,intestine,50136;CCF-STTG1,,,brain,50137;CCK-81,,,intestine,50138;CHP-212,,,nervous system,50139;CoCM-1,,,intestine,50141;COLO 201,,,intestine,50142;COLO 205,,,intestine,50143;COLO 320DM,,,intestine,50144;COLO 741,,,intestine,50145;COLO 792,,,skin,50146;COLO 853,,,skin,50147;COLO 857,,,skin,50148;COLO 858,,,skin,50149;COLO-206F,,,intestine,50150;COLO-320,,,intestine,50151;COLO-678,,,intestine,50152;COLO-680N,,,esophagus,50153;COLO-783,,,skin,50154;COLO-824,,,breast,50156;COLO-849,,,skin,50157;COR-L 105,,,lung,50158;COR-L 23/CPR,,,lung,50159;COR-L23,,,lung,50160;DAN-G,,,pancreas,50161;Daoy,,,brain,50162;DBTRG-05MG,,,brain,50163;Detroit 562,,,head &amp; neck,50164;DK-MG,,,brain,50165;DLD-1,,,intestine,50166;DMS 273,,,lung,50167;DMS 53,,,lung,50168;DOK,,,head &amp; neck,50169;DoTc2 4510,,,cervix,50170;DU 145,,,prostate,50171;DV-90,,,lung,50172;EBC-1,,,lung,50173;EFE-184,,,uterus,50174;EFM-19,,,breast,50175;EFM-192A,,,breast,50176;EFM-192B,,,breast,50177;EFM-192C,,,breast,50178;EFO-21,,,ovary,50179;EFO-27,,,ovary,50180;EGI-1,,,biliary tract,50181;EJ138,,,urinary bladder,50182;EN,,,uterus,50183;EPLC-272H,,,lung,50184;ES-2,,,ovary,50185;ESS-1,,,uterus,50186;EVSA-T,,,breast,50187;FaDu,,,head &amp; neck,50188;FLYA13,,,miscellaneous,50189;FTC-133,,,thyroid,50190;FTC-238,,,thyroid,50191;FU-OV-1,,,ovary,50192;G-292 Clone A141B1,,,bone,50193;G-361,,,skin,50194;G-401,,,kidney,50195;G-402,,,kidney,50196;GAMG,,,brain,50197;GCT,,,miscellaneous,50198;GMS-10,,,brain,50199;GOS-3,,,brain,50200;GP5d,,,intestine,50201;H4,,,brain,50202;HARA,,,lung,50204;HCC1143,,,breast,50205;HCC1395,,,breast,50206;HCC1419,,,breast,50207;HCC1428,,,breast,50208;HCC-15,,,lung,50209;HCC1569,,,breast,50210;HCC1806,,,breast,50211;HCC1937,,,breast,50212;HCC1954,,,breast,50213;HCC202,,,breast,50214;HCC-366,,,lung,50215;HCC38,,,breast,50216;HCC-44,,,lung,50217;HCC-56,,,intestine,50218;HCC70,,,breast,50219;HCC-78,,,lung,50220;HCC-827,,,lung,50221;HCT 116,,,intestine,50222;HCT-15,,,intestine,50223;HCT-8,,,intestine,50224;HDQ-P1,,,breast,50225;H-EMC-SS,,,bone,50226;HGC-27,,,stomach,50227;HLE,,,liver,50228;HMVII,,,skin,50229;HN,,,head &amp; neck,50230;HO-1-N-1,,,head &amp; neck,50231;HO-1-u-1,,,head &amp; neck,50232;HOS,,,bone,50233;HPAC,,,pancreas,50234;HPAF-II,,,pancreas,50235;HRT-18,,,intestine,50236;Hs 257.T,,,intestine,50237;Hs 578T,,,breast,50238;Hs 588.T,,,cervix,50239;Hs 633T,,,miscellaneous,50240;Hs 683,,,brain,50241;Hs 766T,,,pancreas,50243;HSC-2,,,head &amp; neck,50244;HSC-3,,,head &amp; neck,50245;HSC-4,,,head &amp; neck,50246;HT 1080,,,miscellaneous,50247;HT 1376,,,urinary bladder,50248;HT115,,,intestine,50249;HT-1197,,,urinary bladder,50250;HT-29,,,intestine,50251;HT-3,,,cervix,50252;HT55,,,intestine,50253;HTC-C3,,,thyroid,50254;HuCCT1,,,biliary tract,50255;huH-1,,,liver,50256;HuO-3N1,,,bone,50257;HuO9,,,bone,50258;HuO9N2,,,bone,50259;HUP-T3,,,pancreas,50260;HUP-T4,,,pancreas,50261;IGR-1,,,skin,50262;IGR-37,,,skin,50263;IGR-39,,,skin,50264;IHH-4,,,thyroid,50265;IM-95,,,stomach,50266;IM-95m,,,stomach,50267;IMR-32,,,nervous system,50268;IPC-298,,,skin,50269;J82,,,urinary bladder,50270;JAR,,,miscellaneous,50271;JHH-1,,,liver,50272;JHH-2,,,liver,50273;JHH-4,,,liver,50274;JHH-7,,,liver,50275;JIMT-1,,,breast,50276;KELLY,,,nervous system,50277;KG-1-C,,,brain,50278;KHOS/NP,,,bone,50280;KHOS-240S,,,bone,50281;KHOS-312H,,,bone,50282;KMH-2,,,thyroid,50283;KMRC-1,,,kidney,50284;KON,,,head &amp; neck,50285;KOSC-2 cl3-43,,,head &amp; neck,50286;KP-2,,,pancreas,50287;KP-3,,,pancreas,50288;KP-3L,,,pancreas,50289;KP-4,,,pancreas,50290;KPL-1,,,breast,50291;KU-19-19,,,urinary bladder,50292;KYSE-220,,,esophagus,50293;KYSE-270,,,esophagus,50294;KYSE-30,,,esophagus,50295;KYSE-410,,,esophagus,50296;KYSE-50,,,esophagus,50297;KYSE-510,,,esophagus,50298;KYSE-520,,,esophagus,50299;KYSE-70,,,esophagus,50300;LC-1 sq,,,lung,50301;LCLC-103H,,,lung,50302;LCLC-97TM1,,,lung,50303;LK-2,,,lung,50304;LN-18,,,brain,50305;LN-229,,,brain,50306;LN-405,,,brain,50307;LNZTA3WT11,,,brain,50308;LOU-NH91,,,lung,50309;LoVo,,,intestine,50310;LS174T,,,intestine,50311;LS180,,,intestine,50312;Lu-135,,,lung,50314;LU65,,,lung,50315;LU65A,,,lung,50316;LU65B,,,lung,50317;LU65C,,,lung,50318;LU99A,,,lung,50319;LU99B,,,lung,50320;LU99C,,,lung,50321;LUDLU-1,,,lung,50322;M059J,,,brain,50323;MB 157,,,breast,50324;MCAS,,,ovary,50325;MC-IXC,,,nervous system,50326;MDA-MB-134-VI,,,breast,50327;MDA-MB-157,,,breast,50328;MDA-MB-175-VII,,,breast,50329;MDA-MB-330,,,breast,50330;MDA-MB-361,,,breast,50331;MDA-MB-415,,,breast,50332;MDA-MB-436,,,breast,50333;MDA-MB-453,,,breast,50334;MDA-MB-468,,,breast,50335;MDST8,,,intestine,50336;ME-180,,,cervix,50337;MEL-HO,,,skin,50338;MEL-JUSO,,,skin,50339;MES-SA,,,uterus,50340;MES-SA/Dx-5,,,uterus,50341;MEWO,,,skin,50342;MFE-280,,,uterus,50343;MFE-296,,,uterus,50344;MFE-319,,,uterus,50345;MFM-223,,,breast,50346;MG-63,,,bone,50347;MHH-ES-1,,,nervous system,50348;MIA PaCa-2,,,pancreas,50349;MKN1,,,stomach,50350;MKN28,,,stomach,50351;MKN45,,,stomach,50352;MKN7,,,stomach,50353;MKN74,,,stomach,50354;ML-1,,,thyroid,50355;MOG-G-CCM,,,brain,50356;MOG-G-UVW,,,brain,50357;MS751,,,cervix,50358;MSTO-211H,,,pleura,50359;NB69,,,nervous system,50360;NCC-IT-A3,,,testes,50361;NCI-H1048,,,lung,50362;NCI-H1299,,,lung,50363;NCI-H1435,,,lung,50364;NCI-H1437,,,lung,50365;NCI-H1568,,,lung,50366;NCI-H1573,,,lung,50367;NCI-H1581,,,lung,50368;NCI-H1623,,,lung,50369;NCI-H1650,,,lung,50370;NCI-H1688,,,lung,50371;NCI-H1693,,,lung,50372;NCI-H1734,,,lung,50373;NCI-H1755,,,lung,50374;NCI-H1781,,,lung,50375;NCI-H1792,,,lung,50376;NCI-H1793,,,lung,50377;NCI-H1869,,,lung,50378;NCI-H1876,,,lung,50379;NCI-H1944,,,lung,50380;NCI-H196,,,lung,50381;NCI-H1993,,,lung,50382;NCI-H2009,,,lung,50383;NCI-H2029,,,lung,50384;NCI-H2030,,,lung,50385;NCI-H2073,,,lung,50386;NCI-H2085,,,lung,50387;NCI-H2087,,,lung,50388;NCI-H2110,,,lung,50389;NCI-H2122,,,lung,50390;NCI-H2135,,,lung,50391;NCI-H2170,,,lung,50392;NCI-H2172,,,lung,50393;NCI-H2195,,,lung,50394;NCI-H2196,,,lung,50395;NCI-H2198,,,lung,50396;NCI-H2228,,,lung,50397;NCI-H2286,,,lung,50398;NCI-H2291,,,lung,50399;NCI-H23,,,lung,50400;NCI-H2342,,,lung,50401;NCI-H2347,,,lung,50402;NCI-H2405,,,lung,50403;NCI-H2444,,,lung,50404;NCI-H2452,,,lung,50405;NCI-H322,,,lung,50407;NCI-H358,,,lung,50408;NCI-H441,,,lung,50409;NCI-H460,,,lung,50410;NCI-H520,,,lung,50411;NCI-H522,,,lung,50412;NCI-H596,,,lung,50413;NCI-H647,,,lung,50415;NCI-H650,,,lung,50416;NCI-H661,,,lung,50417;NCI-H727,,,lung,50418;NCI-H838,,,lung,50419;NCI-H841,,,lung,50420;NCI-N87,,,stomach,50421;NIH:OVCAR-3,,,ovary,50422;NUGC-3,,,stomach,50424;NUGC-4,,,stomach,50425;NY,,,bone,50426;OAW28,,,ovary,50427;OAW42,,,ovary,50428;OCUG-1,,,gall bladder,50429;OCUM-1,,,stomach,50430;OE19,,,esophagus,50431;OE21,,,esophagus,50432;OE33,,,esophagus,50433;OSC-19,,,head &amp; neck,50434;OSC-20,,,head &amp; neck,50435;OUMS-23,,,intestine,50436;OV-90,,,ovary,50437;OVISE,,,ovary,50438;OVKATE,,,ovary,50439;OVMIU,,,ovary,50440;OVSAYO,,,ovary,50441;OVTOKO,,,ovary,50442;PA-1,,,ovary,50443;Panc 02.03,,,pancreas,50444;Panc 03.27,,,pancreas,50445;Panc 04.03,,,pancreas,50446;Panc 08.13,,,pancreas,50447;Panc 10.05,,,pancreas,50448;PANC-1,,,pancreas,50449;PA-TU-8902,,,pancreas,50450;PA-TU-8988S,,,pancreas,50451;PA-TU-8988T,,,pancreas,50452;PC-14,,,lung,50453;PC-3,,,prostate,50454;PFSK-1,,,brain,50455;PL45,,,pancreas,50456;PLC/PRF/5,,,liver,50457;RCM-1,,,intestine,50459;RD,,,muscle,50460;RD-ES,,,nervous system,50461;RERF-GC-1B,,,stomach,50462;RERF-LC-Ad1,,,lung,50463;RERF-LC-KJ,,,lung,50464;RERF-LC-MA,,,lung,50465;RERF-LC-Sq1,,,lung,50466;RKN,,,ovary,50467;RMG-I,,,ovary,50468;RO82-W-1,,,thyroid,50469;RPMI 2650,,,head &amp; neck,50470;RPMI-7951,,,skin,50471;RT-112,,,urinary bladder,50472;RT112/84,,,urinary bladder,50473;RT4,,,urinary bladder,50474;RVH-421,,,skin,50475;S-117,,,thyroid,50476;Saos-2,,,bone,50477;SAS,,,head &amp; neck,50478;SAT,,,head &amp; neck,50479;SBC-3,,,lung,50480;SBC-5,,,lung,50481;SCaBER,,,urinary bladder,50482;SCC-15,,,head &amp; neck,50483;SCC-25,,,head &amp; neck,50484;SCC-4,,,head &amp; neck,50485;SCC-9,,,head &amp; neck,50486;SCCH-26,,,nervous system,50488;SCH,,,stomach,50489;SCLC-21H,,,lung,50490;SHP-77,,,lung,50491;SiHa,,,cervix,50493;SISO,,,cervix,50494;SK-CO-1,,,intestine,50495;SK-ES-1,,,bone,50496;SKG-IIIa,,,cervix,50497;SKG-IIIb,,,cervix,50498;SK-HEP-1,,,liver,50499;SK-LU-1,,,lung,50500;SK-MEL-2,,,skin,50501;SK-MEL-30,,,skin,50502;SKN,,,uterus,50503;SKN-3,,,head &amp; neck,50504;SK-N-AS,,,nervous system,50505;SK-N-DZ,,,nervous system,50506;SK-NEP-1,,,kidney,50507;SK-N-SH,,,nervous system,50508;SNG-M,,,uterus,50509;SNU-1,,,stomach,50510;SNU-16,,,stomach,50511;SNU-182,,,liver,50512;SNU-387,,,liver,50513;SNU-398,,,liver,50514;SNU-423,,,liver,50515;SNU-449,,,liver,50516;SNU-475,,,liver,50517;SNU-5,,,stomach,50518;SU.86.86,,,pancreas,50520;SUIT-2,,,pancreas,50521;SW 1088,,,brain,50522;SW 1271,,,lung,50524;SW 13,,,adrenal gland,50525;SW 1417,,,intestine,50526;SW 1463,,,intestine,50527;SW 156,,,kidney,50528;SW 1573,,,lung,50529;SW 1783,,,brain,50530;SW 48,,,intestine,50531;SW 626,,,ovary,50532;SW 780,,,urinary bladder,50533;SW 900,,,lung,50534;SW-1710,,,urinary bladder,50535;SW756,,,cervix,50536;SW837,,,intestine,50537;SW-948,,,intestine,50538;T.T,,,esophagus,50539;T.Tn,,,esophagus,50540;T47D,,,breast,50541;T84,,,intestine,50542;T98G,,,brain,50543;TASK1,,,nervous system,50544;TCCSUP,,,urinary bladder,50545;TGW,,,adrenal gland,50546;TOV-112D,,,ovary,50547;TOV-21G,,,ovary,50548;TT2609-C02,,,thyroid,50549;TYK-nu,,,ovary,50550;U-118 MG,,,brain,50551;U-138 MG,,,brain,50552;U-2 OS,,,bone,50553;U-251 MG,,,brain,50554;U373 MG,,,brain,50555;UACC-812,,,breast,50556;UACC-893,,,breast,50557;UMC-11,,,lung,50558;UM-UC-3,,,urinary bladder,50559;VCaP,,,prostate,50560;VM-CUB1,,,urinary bladder,50561;VMRC-LCP,,,lung,50562;VMRC-MELG,,,skin,50563;VMRC-RCW,,,kidney,50564;VMRC-RCZ,,,kidney,50565;WM 266-4,,,skin,50566;WM-115,,,skin,50567;WM1552C,,,skin,50568;WM278,,,skin,50569;WM35,,,skin,50570;WM793B,,,skin,50571;YAPC,,,pancreas,50572;YKG-1,,,brain,50573;ZR-75-1,,,breast,50574;ZR-75-30,,,breast,50575;DU4475,epithelial,,breast,50577;HCC1187,epithelial,,breast,50578;HCC1500,epithelial,,breast,50579;HCC1599,epithelial,,breast,50580;HCC2157,epithelial,,breast,50581;HCC2218,epithelial,,breast,50582;2B8,,,lymphatic system,50585;A2780cis,,,ovary,50586;A3,,,blood,50587;A3/KAW,,,lymphatic system,50588;AGR-ON,,,blood,50589;ALL-SIL,,,blood,50590;AMO-1,,,lymphatic system,50591;ARH-77,,,blood,50592;BALL-1,,,blood,50593;BC-1,,,lymphatic system,50594;BC-2,,,lymphatic system,50595;BC-3,,,lymphatic system,50596;BDCM,,,blood,50597;BE(2)-M17,,,nervous system,50598;BL-41,,,lymphatic system,50599;BL-70,,,lymphatic system,50600;C8166,,,blood,50601;CA46,,,lymphatic system,50602;CCRF-CEM,,,blood,50603;CCRF-HSB-2,,,blood,50604;CCRF-SB,,,blood,50605;CEM/C1,,,blood,50606;CEM/C2,,,blood,50607;CESS,,,blood,50608;CFPAC-1,,,pancreas,50609;ChaGo-K-1,,,lung,50610;CHP-126,,,nervous system,50611;CI-1,,,lymphatic system,50612;CL-11,,,intestine,50613;Clone 15 HL-60,,,blood,50614;CMK,,,blood,50615;COLO 684,,,uterus,50616;COLO-704,,,ovary,50617;COR-L279,,,lung,50618;COR-L51,,,lung,50619;COR-L88,,,lung,50620;COR-L95,,,lung,50621;CPC-N,,,lung,50622;CTV-1,,,blood,50623;D283 Med,,,brain,50624;Daudi,,,lymphatic system,50625;DB,,,lymphatic system,50626;DERL-2,,,lymphatic system,50627;DG-75,,,lymphatic system,50628;DMS 114,,,lung,50629;DMS 153,,,lung,50630;DMS 79,,,lung,50631;DND-41,,,blood,50632;EB1,,,lymphatic system,50633;EB2,,,lymphatic system,50634;EB-3,,,lymphatic system,50635;EHEB,,,blood,50636;EJM,,,blood,50637;Eos-HL-60,,,blood,50638;Farage,,,lymphatic system,50639;GA-10 (Clone 20),,,lymphatic system,50641;GDM-1,,,blood,50642;GOTO,,,nervous system,50643;Gp2D,,,intestine,50644;GRANTA-519,,,lymphatic system,50645;H33HJ-JA1,,,blood,50646;HC-1,,,blood,50647;HCC-33,,,lung,50648;HDLM-2,,,lymphatic system,50649;HD-MY-Z,,,lymphatic system,50650;HEL,,,blood,50651;HEL 92.1.7,,,blood,50652;HH,,,lymphatic system,50653;HL-60,,,blood,50654;HL60(S),,,blood,50655;HL-60/MX2,,,blood,50656;HL60RG,,,blood,50657;Hs 445,,,lymphatic system,50658;HS-Sultan,,,lymphatic system,50659;HT,,,lymphatic system,50660;HuT 78,,,lymphatic system,50661;I 2.1,,,blood,50662;I 9.2,,,blood,50663;IM-9,,,lymphatic system,50664;J.gamma1,,,blood,50665;J.gamma1.WT,,,blood,50666;J.RT3-T3.5,,,blood,50667;J45.01,,,blood,50668;Jiyoye,,,lymphatic system,50669;JJN-3,,,blood,50670;JKT-beta-del,,,blood,50671;JM1,,,lymphatic system,50672;JSC-1,,,lymphatic system,50673;Jurkat, Clone E6-1,,,blood,50674;JURL-MK1,,,blood,50675;JURL-MK2,,,blood,50676;K-562,,,blood,50677;K562/ADM,,,blood,50678;KARPAS-231,,,blood,50679;KARPAS-299,,,lymphatic system,50680;KARPAS-422,,,lymphatic system,50681;KARPAS-45,,,blood,50682;KARPAS-620,,,blood,50683;KCL-22,,,blood,50685;KE-37,,,blood,50686;KG-1,,,blood,50687;KG-1a,,,blood,50688;KM-H2,,,lymphatic system,50689;KMOE-2,,,blood,50690;KMS-12-BM,,,blood,50691;KMS-12-PE,,,blood,50692;KO52,,,blood,50693;KOPN-8,,,blood,50694;KP-1N,,,pancreas,50695;KP-1NL,,,pancreas,50696;KU812,,,blood,50697;KU812E,,,blood,50698;KU812F,,,blood,50699;KY821,,,blood,50700;KY821A3,,,blood,50701;KYM-1,,,muscle,50702;L-1236,,,lymphatic system,50703;L-363,,,blood,50704;L-428,,,lymphatic system,50705;L-540,,,lymphatic system,50706;LAMA-84,,,blood,50707;LC4-1,,,blood,50708;Loucy,,,blood,50709;LP-1,,,blood,50710;Lu-134-B,,,lung,50711;M059K,,,brain,50712;MC/CAR,,,lymphatic system,50713;MC116,,,lymphatic system,50714;ME-1,,,blood,50715;MEC-1,,,blood,50716;MEC-2,,,blood,50717;MEG-01,,,blood,50718;MHH-NB-11,,,nervous system,50719;MHH-PREB-1,,,lymphatic system,50720;MJ,,,lymphatic system,50721;ML-2,,,blood,50722;MLMA,,,blood,50723;MOLM-13,,,blood,50724;MOLP-8,,,blood,50725;MOLT-14,,,blood,50726;MOLT-16,,,blood,50727;MOLT-4,,,blood,50728;MOLT-4F,,,blood,50729;MONO-MAC-1,,,blood,50730;MONO-MAC-6,,,blood,50731;MRK-nu-1,,,breast,50732;MS-1-L,,,lung,50733;MV-4-11,,,blood,50734;MY,,,blood,50735;MY-M12,,,blood,50736;MY-M13,,,blood,50737;NALM-19,,,blood,50738;NALM-6,,,blood,50739;NAMALWA,,,lymphatic system,50740;NAMALWA.PNT,,,lymphatic system,50741;NB(TU)1-10,,,nervous system,50742;NB-1,,,nervous system,50743;NB-4,,,blood,50744;NC-37,,,lymphatic system,50745;NCI-H1092,,,lung,50746;NCI-H1155,,,lung,50747;NCI-H1304,,,lung,50748;NCI-H1385,,,lung,50749;NCI-H1395,,,lung,50750;NCI-H1404,,,lung,50751;NCI-H1417,,,lung,50752;NCI-H1436,,,lung,50753;NCI-H1522,,,lung,50754;NCI-H1563,,,lung,50755;NCI-H1618,,,lung,50756;NCI-H1666,,,lung,50757;NCI-H1694,,,lung,50758;NCI-H1770,,,lung,50759;NCI-H1836,,,lung,50760;NCI-H1838,,,lung,50761;NCI-H187,,,lung,50762;NCI-H1882,,,lung,50763;NCI-H1963,,,lung,50764;NCI-H1975,,,lung,50765;NCI-H2081,,,lung,50766;NCI-H209,,,lung,50767;NCI-H2106,,,lung,50768;NCI-H211,,,lung,50769;NCI-H2141,,,lung,50770;NCI-H2171,,,lung,50771;NCI-H220,,,lung,50772;NCI-H2227,,,lung,50773;NCI-H226,,,lung,50774;NCI-H345,,,lung,50775;NCI-H446,,,lung,50776;NCI-H510A,,,lung,50777;NCI-H524,,,lung,50778;NCI-H526,,,lung,50779;NCI-H69,,,lung,50780;NCI-H719,,,lung,50781;NCI-H720,,,lung,50782;NCI-H748,,,lung,50783;NCI-H82,,,lung,50784;NCI-H847,,,lung,50785;NCI-H889,,,lung,50786;NEC8,,,testes,50787;NH-12,,,nervous system,50788;NK-92MI,,,lymphatic system,50789;NOMO-1/ADM,,,blood,50790;NU-DUL-1,,,lymphatic system,50791;OCI-AML2,,,blood,50792;OCI-AML3,,,blood,50793;OCI-AML5,,,blood,50794;OCI-LY-19,,,lymphatic system,50795;OCI-M1,,,blood,50796;OPM-2,,,blood,50797;P116.cl39,,,blood,50798;P12-ICHIKAWA,,,blood,50799;P30/OHK,,,blood,50800;P31/FUJ,,,blood,50801;P32/ISH,,,lymphatic system,50802;P3HR-1,,,lymphatic system,50803;PC-3 [JPC-3],,,lung,50804;PEER,,,blood,50805;PF-382,,,blood,50806;Pfeiffer,,,lymphatic system,50807;PL-21,,,blood,50808;PSN1,,,pancreas,50809;Raji,,,lymphatic system,50810;Ramos (RA 1),,,blood,50811;RC-K8,,,lymphatic system,50812;REC-1,,,lymphatic system,50813;Reh,,,blood,50814;RERF-LC-MS,,,lung,50815;RH-1,,,bone,50816;RH-30,,,muscle,50817;RH-41,,,muscle,50818;RL,,,lymphatic system,50819;ROS-50,,,blood,50820;RPMI 1788,,,blood,50821;RPMI 6666,,,lymphatic system,50822;RPMI 8226,,,blood,50823;RPMI-8402,,,blood,50824;RS4;11,,,blood,50825;SBC-1,,,lung,50826;SBC-2,,,lung,50827;SC-1,,,lymphatic system,50828;SCC-3,,,lymphatic system,50829;Sci-1,,,lymphatic system,50830;SIG-M5,,,blood,50831;SIMA,,,nervous system,50832;SK-MEL-1,,,skin,50833;SK-MEL-3,,,skin,50834;SK-N-BE(2),,,nervous system,50835;SK-N-FI,,,nervous system,50836;SLVL,,,lymphatic system,50837;SNB-19,,,brain,50838;SR,,,lymphatic system,50839;ST486,,,lymphatic system,50840;SU-DHL-1,,,lymphatic system,50841;SU-DHL-16,,,lymphatic system,50843;SU-DHL-4,,,lymphatic system,50844;SU-DHL-5,,,lymphatic system,50845;SU-DHL-6,,,lymphatic system,50846;SU-DHL-8,,,lymphatic system,50847;SUP-B15,,,blood,50848;SUP-HD1,,,lymphatic system,50849;SUP-M2,,,lymphatic system,50850;SUP-T1,,,blood,50851;SW 1990,,,pancreas,50853;TALL-1,,,blood,50854;TANOUE,,,blood,50855;TC-71,,,bone,50856;Tera-1,,,testes,50857;TF-1,,,blood,50858;TF-1.CN5a.1,,,blood,50859;TF-1a,,,blood,50860;THP-1,,,blood,50861;TK,,,lymphatic system,50862;Toledo,,,lymphatic system,50863;TT,,,thyroid,50864;TUR,,,lymphatic system,50865;U266B1,,,blood,50866;U-698-M,,,blood,50867;U-87 MG,,,brain,50868;U-937,,,lymphatic system,50869;VAL,,,lymphatic system,50870;WIL2 NS,,,lymphatic system,50871;WILCL,,,blood,50872;WSU-DLCL2,,,lymphatic system,50873;WSU-NHL,,,lymphatic system,50874;YMB-1,,,breast,50875;YT,,,lymphatic system,50876;697.0,,,blood,50877;8-MG-BA,,,brain,50878;A101D,,,skin,50879;A253,,,head &amp; neck,50880;A388,,,miscellaneous,50881;A498,,,kidney,50882;A4-Fuk,,,skin,50883;A704,,,kidney,50884;ACN,,,nervous system,50885;ALL-PO,,,blood,50886;AM-38,,,brain,50887;ATN-1,,,blood,50888;B2-17,,,brain,50889;BB30-HNC,,,head &amp; neck,50890;BB49-HNC,,,head &amp; neck,50891;BB65-RCC,,,kidney,50892;BE-13,,,blood,50893;Becker,,,brain,50894;BOKU,,,cervix,50895;BV-173,,,blood,50896;Calu-6,,,lung,50897;CAS-1,,,brain,50898;CGTH-W-1,,,thyroid,50899;COLO-320-HSR,,,intestine,50900;COLO-668,,,lung,50901;COLO-829,,,skin,50902;CP50-MEL-B,,,skin,50903;CP66-MEL,,,skin,50904;CTB-1,,,lymphatic system,50905;CW-2,,,intestine,50906;D-263MG,,,brain,50908;D-392MG,,,brain,50910;D-423MG,,,brain,50911;D-502MG,,,brain,50912;D-542MG,,,brain,50913;D-566MG,,,brain,50914;DEL,,,blood,50915;DJM-1,,,skin,50916;DOHH-2,,,lymphatic system,50917;DSH1,,,urinary tract,50918;ECC10,,,stomach,50919;ECC4,,,intestine,50921;EC-GI-10,,,esophagus,50922;EKVX,,,lung,50923;EM-2,,,blood,50924;EoL-1-cell,,,blood,50925;ES1,,,bone,50926;ES3,,,bone,50927;ES4,,,bone,50928;ES5,,,bone,50929;ES6,,,bone,50930;ES7,,,bone,50931;ES8,,,bone,50932;ETK-1,,,biliary tract,50933;EW-1,,,bone,50934;EW-11,,,bone,50935;EW-13,,,bone,50936;EW-16,,,bone,50937;EW-18,,,bone,50938;EW-24,,,bone,50939;EW-3,,,bone,50940;EW-7,,,bone,50941;GAK,,,skin,50942;GB-1,,,brain,50943;GCIY,,,stomach,50944;GI-1,,,brain,50945;GI-ME-N,,,nervous system,50946;GR-ST,,,blood,50947;GT3TKB,,,stomach,50948;H9,,,lymphatic system,50949;HA7-RCC,,,kidney,50950;HAL-01,,,blood,50951;HCC2998,,,intestine,50952;HCE-4,,,esophagus,50953;HCE-T,,,head &amp; neck,50954;HOP-62,,,lung,50955;HT-144,,,skin,50956;IMR-5,,,nervous system,50957;IST-MES1,,,pleura,50958;IST-SL1,,,lung,50959;IST-SL2,,,lung,50960;JEG-3,,,miscellaneous,50961;JVM-2,,,blood,50962;JVM-3,,,blood,50963;K5,,,thyroid,50964;KALS-1,,,brain,50965;KGN,,,ovary,50966;KINGS-1,,,brain,50967;KLE,,,uterus,50968;KM12,,,intestine,50969;KNS-42,,,brain,50970;KNS-81-FD,,,brain,50971;KP-N-YN,,,nervous system,50972;KP-N-YS,,,nervous system,50973;KS-1,,,brain,50974;KURAMOCHI,,,ovary,50975;LAN-5,,,nervous system,50976;LAN-6,,,nervous system,50977;LB1047-RCC,,,kidney,50978;LB2241-RCC,,,kidney,50979;LB2518-MEL,,,skin,50980;LB373-MEL-D,,,skin,50981;LB647-SCLC,,,lung,50982;LB771-HNC,,,head &amp; neck,50983;LB831-BLC,,,urinary tract,50984;LB996-RCC,,,kidney,50985;LC-1F,,,lung,50986;LC-2-ad,,,lung,50987;LOXIMVI,,,skin,50988;LS-1034,,,intestine,50989;LS-123,,,intestine,50990;LS-411N,,,intestine,50991;LS-513,,,intestine,50992;LU-134-A,,,lung,50993;LU-139,,,lung,50994;LU-165,,,lung,50995;LXF-289,,,lung,50996;MFH-ino,,,miscellaneous,50997;MHH-CALL-2,,,blood,50998;MMAC-SF,,,skin,50999;MN-60,,,blood,51000;Mo-T,,,blood,51001;MPP-89,,,pleura,51002;MUTZ-1,,,blood,51003;MZ1-PC,,,pancreas,51004;MZ2-MEL,,,skin,51005;MZ7-mel,,,skin,51006;NB10,,,nervous system,51007;NB12,,,nervous system,51008;NB13,,,nervous system,51009;NB14,,,nervous system,51010;NB16,,,nervous system,51011;NB5,,,nervous system,51013;NB6,,,nervous system,51014;NB7,,,nervous system,51015;NBsusSR,,,nervous system,51016;NCI-H1355,,,lung,51017;NCI-H157,,,lung,51018;NCI-H2126,,,lung,51019;NCI-H322M,,,lung,51020;NCI-H64,,,lung,51021;NCI-H716,,,intestine,51022;NCI-H747,,,intestine,51023;NKM-1,,,blood,51024;NMC-G1,,,brain,51025;no-10,,,brain,51026;no-11,,,brain,51027;NOMO-1,,,blood,51028;NOS-1,,,bone,51029;NTERA-S-cl-D1,,,testes,51030;OC-314,,,ovary,51031;OCUB-M,,,breast,51032;OMC-1,,,cervix,51033;ONS-76,,,brain,51034;OS-RC-2,,,kidney,51035;OVCAR-4,,,ovary,51036;QIMR-WIL,,,blood,51037;Ramos-2G6-4C10,,,lymphatic system,51038;RCC10RGB,,,kidney,51039;RF-48,,,stomach,51040;RKO,,,intestine,51041;RPMI-8866,,,blood,51043;RXF393,,,kidney,51044;SF126,,,brain,51045;SF268,,,brain,51046;SF539,,,brain,51047;SH-4,,,skin,51048;SJSA-1,,,bone,51049;SK-MEL-24,,,skin,51050;SK-MEL-5,,,skin,51051;SK-MG-1,,,brain,51052;SK-MM-2,,,blood,51053;SK-PN-DW,,,bone,51054;SK-UT-1,,,uterus,51055;SNU-C1,,,intestine,51056;SNU-C2B,,,intestine,51057;SW403,,,intestine,51058;SW684,,,miscellaneous,51059;SW872,,,miscellaneous,51060;SW954,,,vulva,51061;SW962,,,vulva,51062;SW982,,,miscellaneous,51063;TE-1,,,esophagus,51064;TE-10,,,esophagus,51065;TE-11,,,esophagus,51066;TE-12,,,esophagus,51067;TE-15,,,esophagus,51068;TE-441-T,,,muscle,51069;TE-5,,,esophagus,51070;TE-6,,,esophagus,51071;TE-8,,,esophagus,51072;TE-9,,,esophagus,51073;TGBC11TKB,,,stomach,51074;TGBC1TKB,,,biliary tract,51075;TGBC24TKB,,,biliary tract,51076;TK10,,,kidney,51077;UACC-257,,,skin,51078;VA-ES-BJ,,,miscellaneous,51079;YH-13,,,brain,51080</t>
+  </si>
+  <si>
+    <t>Bryostatin 1,small molecule,10296-101,LSM-6313</t>
+  </si>
+  <si>
+    <t>http://lincs.hms.harvard.edu/db/datasets/20013/</t>
+  </si>
+  <si>
+    <t>MGH (CMT) Growth Inhibition Assay Protocol (9 compound doses: 64 nM to 0.25 nM) -- DNA Staining</t>
+  </si>
+  <si>
+    <t>5637.0,epithelial,,urinary bladder,50001;647-V,epithelial-like,,urinary bladder,50002;A375.S2,epithelial,,skin,50003;AGS,epithelial,,stomach,50004;BPH-1,epitheloid,,prostate,50005;Ca Ski,epithelial,,cervix,50006;Ca9-22,epithelial-like,,head &amp; neck,50007;CAL-51,epithelial-like,,breast,50008;Calu-1,epithelial,,lung,50009;Calu-3,epithelial,,lung,50010;COLO-679,fibroblastic,,skin,50011;COLO-800,epithelial-like,,skin,50012;FU97,epithelial-like,,stomach,50013;HEC-1,,,uterus,50014;HLF,,,liver,50015;HUTU-80,epithelial,,intestine,50016;IA-LM,,,lung,50017;Ishikawa,epithelial-like,,uterus,50018;Ishikawa (Heraklio) 02 ER-,epithelial,,uterus,50019;IST-MEL1,epithelial-like,,skin,50020;JHH-6,epithelial-like,,liver,50021;KMRC-20,epithelial-like,,kidney,50023;KYSE-140,,,esophagus,50024;KYSE-150,epitheloid,,esophagus,50025;KYSE-180,epitheloid,,esophagus,50026;KYSE-450,epitheloid,,esophagus,50027;LNZTA3WT4,,,brain,50028;MCF7,epithelial,,breast,50029;MDA-MB-435S,melanocyte,,skin,50030;MT-3,epithelial,,breast,50031;NCI-H1648,,,lung,50032;NCI-H1651,epithelial,,lung,50033;NCI-H1703,epithelial,,lung,50034;NCI-H1915,large cell,,lung,50035;NCI-H2023,,,lung,50036;NCI-H810,epithelial,,lung,50037;PE/CA-PJ15,epithelial-like,,head &amp; neck,50039;SJCRH30,fibroblast,,muscle,50041;SK-LMS-1,,,uterus,50042;SK-MES,epithelial,,lung,50043;SK-OV-3,epithelial,,ovary,50044;SNB75,,,brain,50045;SW527,epithelial,,breast,50046;SW620,epithelial,,intestine,50047;T24,epithelial,,urinary bladder,50048;WiDr,epithelial,,intestine,50049;Hep 3B2.1-7,epithelial,,liver,50051;Hep G2,epithelial,,liver,50052;Huh7,,,liver,50055;SK-BR-3,epithelial,,breast,50057;MDA-MB-231,epithelial,,breast,50058;LNCaP,epithelial,,prostate,50059;A-375,epithelial,,skin,50060;HeLa,epithelial,,cervix,50061;1205Lu,,,skin,50062;1321N1,,,brain,50063;143B,,,bone,50064;143B PML BK TK,,,bone,50065;1A6,,,urinary bladder,50066;22RV1,,,prostate,50067;23132/87,,,stomach,50068;42-MG-BA,,,brain,50069;639-V,,,ureter,50071;769-P,,,kidney,50072;786-O,,,kidney,50073;8305C,,,thyroid,50074;8505C,,,thyroid,50075;A172,,,brain,50076;A-204,,,muscle,50077;A2058,,,skin,50078;A2780,,,ovary,50079;A2780ADR,,,ovary,50080;A373-C6,,,skin,50081;A-427,,,lung,50082;A431,,,skin,50083;A549,,,lung,50084;A673,,,muscle,50085;ABC-1,,,lung,50086;ACHN,,,kidney,50087;AN3CA,,,uterus,50088;ASH-3,,,thyroid,50089;AsPC-1,,,pancreas,50090;AU565,,,breast,50091;AZ-521,,,stomach,50092;B-CPAP,,,thyroid,50093;BE(2)-C,,,nervous system,50094;BEN,,,lung,50095;BeWo,,,miscellaneous,50096;BFTC-905,,,urinary bladder,50097;BFTC-909,,,kidney,50098;BHT-101,,,thyroid,50099;BHY,,,head &amp; neck,50100;BICR 10,,,head &amp; neck,50101;BICR 22,,,head &amp; neck,50102;BICR 31,,,head &amp; neck,50103;BICR 78,,,head &amp; neck,50104;BT-20,,,breast,50105;BT-474,,,breast,50106;BT-483,,,breast,50107;BT-549,,,breast,50108;BxPC-3,,,pancreas,50109;C170,,,intestine,50110;C2BBe1,,,intestine,50111;C32,,,skin,50112;C-33 A,,,cervix,50113;C3A,,,liver,50114;C-4 I,,,cervix,50115;C-4 II,,,cervix,50116;Caco-2,,,intestine,50117;Caki-1,,,kidney,50118;CAL 27,,,head &amp; neck,50119;CAL-120,,,breast,50120;CAL-12T,,,lung,50121;CAL-148,,,breast,50122;CAL-29,,,urinary bladder,50123;CAL-33,,,head &amp; neck,50124;CAL-39,,,vulva,50125;CAL-54,,,kidney,50126;CAL-62,,,thyroid,50127;CAL-72,,,bone,50128;CAL-78,,,bone,50129;CAL-85-1,,,breast,50130;CAMA-1,,,breast,50131;Caov-3,,,ovary,50132;Caov-4,,,ovary,50133;Capan-1,,,pancreas,50134;Capan-2,,,pancreas,50135;CaR-1,,,intestine,50136;CCF-STTG1,,,brain,50137;CCK-81,,,intestine,50138;CHP-212,,,nervous system,50139;CoCM-1,,,intestine,50141;COLO 201,,,intestine,50142;COLO 205,,,intestine,50143;COLO 320DM,,,intestine,50144;COLO 741,,,intestine,50145;COLO 792,,,skin,50146;COLO 853,,,skin,50147;COLO 857,,,skin,50148;COLO 858,,,skin,50149;COLO-206F,,,intestine,50150;COLO-320,,,intestine,50151;COLO-678,,,intestine,50152;COLO-680N,,,esophagus,50153;COLO-783,,,skin,50154;COLO-818,,,skin,50155;COLO-824,,,breast,50156;COLO-849,,,skin,50157;COR-L 105,,,lung,50158;COR-L 23/CPR,,,lung,50159;COR-L23,,,lung,50160;DAN-G,,,pancreas,50161;Daoy,,,brain,50162;DBTRG-05MG,,,brain,50163;Detroit 562,,,head &amp; neck,50164;DK-MG,,,brain,50165;DLD-1,,,intestine,50166;DMS 273,,,lung,50167;DMS 53,,,lung,50168;DOK,,,head &amp; neck,50169;DoTc2 4510,,,cervix,50170;DU 145,,,prostate,50171;DV-90,,,lung,50172;EBC-1,,,lung,50173;EFE-184,,,uterus,50174;EFM-19,,,breast,50175;EFM-192A,,,breast,50176;EFM-192B,,,breast,50177;EFM-192C,,,breast,50178;EFO-21,,,ovary,50179;EFO-27,,,ovary,50180;EGI-1,,,biliary tract,50181;EJ138,,,urinary bladder,50182;EN,,,uterus,50183;EPLC-272H,,,lung,50184;ES-2,,,ovary,50185;ESS-1,,,uterus,50186;EVSA-T,,,breast,50187;FaDu,,,head &amp; neck,50188;FLYA13,,,miscellaneous,50189;FTC-133,,,thyroid,50190;FTC-238,,,thyroid,50191;FU-OV-1,,,ovary,50192;G-292 Clone A141B1,,,bone,50193;G-361,,,skin,50194;G-401,,,kidney,50195;G-402,,,kidney,50196;GAMG,,,brain,50197;GCT,,,miscellaneous,50198;GMS-10,,,brain,50199;GOS-3,,,brain,50200;GP5d,,,intestine,50201;H4,,,brain,50202;HARA,,,lung,50204;HCC1143,,,breast,50205;HCC1395,,,breast,50206;HCC1419,,,breast,50207;HCC1428,,,breast,50208;HCC-15,,,lung,50209;HCC1569,,,breast,50210;HCC1806,,,breast,50211;HCC1937,,,breast,50212;HCC1954,,,breast,50213;HCC-366,,,lung,50215;HCC38,,,breast,50216;HCC-44,,,lung,50217;HCC-56,,,intestine,50218;HCC70,,,breast,50219;HCC-78,,,lung,50220;HCC-827,,,lung,50221;HCT 116,,,intestine,50222;HCT-15,,,intestine,50223;HCT-8,,,intestine,50224;HDQ-P1,,,breast,50225;H-EMC-SS,,,bone,50226;HGC-27,,,stomach,50227;HLE,,,liver,50228;HMVII,,,skin,50229;HN,,,head &amp; neck,50230;HO-1-N-1,,,head &amp; neck,50231;HO-1-u-1,,,head &amp; neck,50232;HOS,,,bone,50233;HPAC,,,pancreas,50234;HPAF-II,,,pancreas,50235;HRT-18,,,intestine,50236;Hs 257.T,,,intestine,50237;Hs 578T,,,breast,50238;Hs 588.T,,,cervix,50239;Hs 633T,,,miscellaneous,50240;Hs 683,,,brain,50241;Hs 746T,,,stomach,50242;Hs 766T,,,pancreas,50243;HSC-2,,,head &amp; neck,50244;HSC-3,,,head &amp; neck,50245;HSC-4,,,head &amp; neck,50246;HT 1080,,,miscellaneous,50247;HT 1376,,,urinary bladder,50248;HT115,,,intestine,50249;HT-1197,,,urinary bladder,50250;HT-29,,,intestine,50251;HT-3,,,cervix,50252;HT55,,,intestine,50253;HTC-C3,,,thyroid,50254;HuCCT1,,,biliary tract,50255;huH-1,,,liver,50256;HuO-3N1,,,bone,50257;HuO9,,,bone,50258;HuO9N2,,,bone,50259;HUP-T3,,,pancreas,50260;HUP-T4,,,pancreas,50261;IGR-1,,,skin,50262;IGR-37,,,skin,50263;IGR-39,,,skin,50264;IHH-4,,,thyroid,50265;IM-95,,,stomach,50266;IM-95m,,,stomach,50267;IMR-32,,,nervous system,50268;IPC-298,,,skin,50269;J82,,,urinary bladder,50270;JAR,,,miscellaneous,50271;JHH-1,,,liver,50272;JHH-2,,,liver,50273;JHH-4,,,liver,50274;JHH-7,,,liver,50275;JIMT-1,,,breast,50276;KELLY,,,nervous system,50277;KG-1-C,,,brain,50278;KHOS/NP,,,bone,50280;KHOS-240S,,,bone,50281;KHOS-312H,,,bone,50282;KMH-2,,,thyroid,50283;KMRC-1,,,kidney,50284;KON,,,head &amp; neck,50285;KOSC-2 cl3-43,,,head &amp; neck,50286;KP-2,,,pancreas,50287;KP-3,,,pancreas,50288;KP-3L,,,pancreas,50289;KP-4,,,pancreas,50290;KPL-1,,,breast,50291;KU-19-19,,,urinary bladder,50292;KYSE-220,,,esophagus,50293;KYSE-270,,,esophagus,50294;KYSE-30,,,esophagus,50295;KYSE-410,,,esophagus,50296;KYSE-50,,,esophagus,50297;KYSE-510,,,esophagus,50298;KYSE-520,,,esophagus,50299;KYSE-70,,,esophagus,50300;LC-1 sq,,,lung,50301;LCLC-103H,,,lung,50302;LCLC-97TM1,,,lung,50303;LK-2,,,lung,50304;LN-18,,,brain,50305;LN-229,,,brain,50306;LN-405,,,brain,50307;LNZTA3WT11,,,brain,50308;LOU-NH91,,,lung,50309;LoVo,,,intestine,50310;LS174T,,,intestine,50311;LS180,,,intestine,50312;Lu-135,,,lung,50314;LU65,,,lung,50315;LU65A,,,lung,50316;LU65B,,,lung,50317;LU65C,,,lung,50318;LU99A,,,lung,50319;LU99B,,,lung,50320;LU99C,,,lung,50321;LUDLU-1,,,lung,50322;M059J,,,brain,50323;MB 157,,,breast,50324;MCAS,,,ovary,50325;MC-IXC,,,nervous system,50326;MDA-MB-134-VI,,,breast,50327;MDA-MB-157,,,breast,50328;MDA-MB-175-VII,,,breast,50329;MDA-MB-330,,,breast,50330;MDA-MB-361,,,breast,50331;MDA-MB-415,,,breast,50332;MDA-MB-436,,,breast,50333;MDA-MB-453,,,breast,50334;MDA-MB-468,,,breast,50335;MDST8,,,intestine,50336;ME-180,,,cervix,50337;MEL-HO,,,skin,50338;MEL-JUSO,,,skin,50339;MES-SA,,,uterus,50340;MES-SA/Dx-5,,,uterus,50341;MEWO,,,skin,50342;MFE-280,,,uterus,50343;MFE-296,,,uterus,50344;MFE-319,,,uterus,50345;MFM-223,,,breast,50346;MG-63,,,bone,50347;MHH-ES-1,,,nervous system,50348;MIA PaCa-2,,,pancreas,50349;MKN1,,,stomach,50350;MKN28,,,stomach,50351;MKN45,,,stomach,50352;MKN7,,,stomach,50353;MKN74,,,stomach,50354;ML-1,,,thyroid,50355;MOG-G-CCM,,,brain,50356;MOG-G-UVW,,,brain,50357;MS751,,,cervix,50358;MSTO-211H,,,pleura,50359;NB69,,,nervous system,50360;NCC-IT-A3,,,testes,50361;NCI-H1048,,,lung,50362;NCI-H1299,,,lung,50363;NCI-H1435,,,lung,50364;NCI-H1437,,,lung,50365;NCI-H1568,,,lung,50366;NCI-H1573,,,lung,50367;NCI-H1581,,,lung,50368;NCI-H1623,,,lung,50369;NCI-H1650,,,lung,50370;NCI-H1688,,,lung,50371;NCI-H1693,,,lung,50372;NCI-H1734,,,lung,50373;NCI-H1755,,,lung,50374;NCI-H1781,,,lung,50375;NCI-H1792,,,lung,50376;NCI-H1793,,,lung,50377;NCI-H1869,,,lung,50378;NCI-H1876,,,lung,50379;NCI-H1944,,,lung,50380;NCI-H196,,,lung,50381;NCI-H1993,,,lung,50382;NCI-H2009,,,lung,50383;NCI-H2029,,,lung,50384;NCI-H2030,,,lung,50385;NCI-H2073,,,lung,50386;NCI-H2085,,,lung,50387;NCI-H2087,,,lung,50388;NCI-H2110,,,lung,50389;NCI-H2122,,,lung,50390;NCI-H2135,,,lung,50391;NCI-H2170,,,lung,50392;NCI-H2172,,,lung,50393;NCI-H2195,,,lung,50394;NCI-H2196,,,lung,50395;NCI-H2198,,,lung,50396;NCI-H2228,,,lung,50397;NCI-H2286,,,lung,50398;NCI-H2291,,,lung,50399;NCI-H23,,,lung,50400;NCI-H2342,,,lung,50401;NCI-H2347,,,lung,50402;NCI-H2405,,,lung,50403;NCI-H2444,,,lung,50404;NCI-H2452,,,lung,50405;NCI-H322,,,lung,50407;NCI-H358,,,lung,50408;NCI-H441,,,lung,50409;NCI-H460,,,lung,50410;NCI-H520,,,lung,50411;NCI-H522,,,lung,50412;NCI-H596,,,lung,50413;NCI-H630,,,intestine,50414;NCI-H647,,,lung,50415;NCI-H650,,,lung,50416;NCI-H661,,,lung,50417;NCI-H727,,,lung,50418;NCI-H838,,,lung,50419;NCI-H841,,,lung,50420;NCI-N87,,,stomach,50421;NIH:OVCAR-3,,,ovary,50422;NUGC-3,,,stomach,50424;NUGC-4,,,stomach,50425;NY,,,bone,50426;OAW28,,,ovary,50427;OAW42,,,ovary,50428;OCUG-1,,,gall bladder,50429;OCUM-1,,,stomach,50430;OE19,,,esophagus,50431;OE21,,,esophagus,50432;OE33,,,esophagus,50433;OSC-19,,,head &amp; neck,50434;OSC-20,,,head &amp; neck,50435;OUMS-23,,,intestine,50436;OV-90,,,ovary,50437;OVISE,,,ovary,50438;OVKATE,,,ovary,50439;OVMIU,,,ovary,50440;OVSAYO,,,ovary,50441;OVTOKO,,,ovary,50442;PA-1,,,ovary,50443;Panc 02.03,,,pancreas,50444;Panc 03.27,,,pancreas,50445;Panc 04.03,,,pancreas,50446;Panc 08.13,,,pancreas,50447;Panc 10.05,,,pancreas,50448;PANC-1,,,pancreas,50449;PA-TU-8902,,,pancreas,50450;PA-TU-8988S,,,pancreas,50451;PA-TU-8988T,,,pancreas,50452;PC-14,,,lung,50453;PC-3,,,prostate,50454;PFSK-1,,,brain,50455;PL45,,,pancreas,50456;PLC/PRF/5,,,liver,50457;RCM-1,,,intestine,50459;RD,,,muscle,50460;RD-ES,,,nervous system,50461;RERF-GC-1B,,,stomach,50462;RERF-LC-Ad1,,,lung,50463;RERF-LC-KJ,,,lung,50464;RERF-LC-MA,,,lung,50465;RERF-LC-Sq1,,,lung,50466;RKN,,,ovary,50467;RMG-I,,,ovary,50468;RO82-W-1,,,thyroid,50469;RPMI 2650,,,head &amp; neck,50470;RPMI-7951,,,skin,50471;RT-112,,,urinary bladder,50472;RT112/84,,,urinary bladder,50473;RT4,,,urinary bladder,50474;RVH-421,,,skin,50475;S-117,,,thyroid,50476;Saos-2,,,bone,50477;SAS,,,head &amp; neck,50478;SAT,,,head &amp; neck,50479;SBC-3,,,lung,50480;SBC-5,,,lung,50481;SCaBER,,,urinary bladder,50482;SCC-15,,,head &amp; neck,50483;SCC-25,,,head &amp; neck,50484;SCC-4,,,head &amp; neck,50485;SCC-9,,,head &amp; neck,50486;SCCH-26,,,nervous system,50488;SCH,,,stomach,50489;SCLC-21H,,,lung,50490;SHP-77,,,lung,50491;SiHa,,,cervix,50493;SISO,,,cervix,50494;SK-CO-1,,,intestine,50495;SK-ES-1,,,bone,50496;SKG-IIIa,,,cervix,50497;SKG-IIIb,,,cervix,50498;SK-HEP-1,,,liver,50499;SK-LU-1,,,lung,50500;SK-MEL-2,,,skin,50501;SK-MEL-30,,,skin,50502;SKN,,,uterus,50503;SKN-3,,,head &amp; neck,50504;SK-N-AS,,,nervous system,50505;SK-N-DZ,,,nervous system,50506;SK-NEP-1,,,kidney,50507;SK-N-SH,,,nervous system,50508;SNG-M,,,uterus,50509;SNU-1,,,stomach,50510;SNU-16,,,stomach,50511;SNU-182,,,liver,50512;SNU-387,,,liver,50513;SNU-398,,,liver,50514;SNU-423,,,liver,50515;SNU-449,,,liver,50516;SNU-475,,,liver,50517;SNU-5,,,stomach,50518;SU.86.86,,,pancreas,50520;SUIT-2,,,pancreas,50521;SW 1088,,,brain,50522;SW 1271,,,lung,50524;SW 13,,,adrenal gland,50525;SW 1417,,,intestine,50526;SW 1463,,,intestine,50527;SW 156,,,kidney,50528;SW 1573,,,lung,50529;SW 1783,,,brain,50530;SW 48,,,intestine,50531;SW 626,,,ovary,50532;SW 780,,,urinary bladder,50533;SW 900,,,lung,50534;SW-1710,,,urinary bladder,50535;SW756,,,cervix,50536;SW837,,,intestine,50537;SW-948,,,intestine,50538;T.T,,,esophagus,50539;T.Tn,,,esophagus,50540;T47D,,,breast,50541;T84,,,intestine,50542;T98G,,,brain,50543;TASK1,,,nervous system,50544;TCCSUP,,,urinary bladder,50545;TGW,,,adrenal gland,50546;TOV-112D,,,ovary,50547;TOV-21G,,,ovary,50548;TT2609-C02,,,thyroid,50549;TYK-nu,,,ovary,50550;U-118 MG,,,brain,50551;U-138 MG,,,brain,50552;U-2 OS,,,bone,50553;U-251 MG,,,brain,50554;U373 MG,,,brain,50555;UACC-812,,,breast,50556;UACC-893,,,breast,50557;UMC-11,,,lung,50558;UM-UC-3,,,urinary bladder,50559;VCaP,,,prostate,50560;VM-CUB1,,,urinary bladder,50561;VMRC-LCP,,,lung,50562;VMRC-MELG,,,skin,50563;VMRC-RCW,,,kidney,50564;VMRC-RCZ,,,kidney,50565;WM 266-4,,,skin,50566;WM-115,,,skin,50567;WM1552C,,,skin,50568;WM278,,,skin,50569;WM35,,,skin,50570;WM793B,,,skin,50571;YAPC,,,pancreas,50572;YKG-1,,,brain,50573;ZR-75-1,,,breast,50574;ZR-75-30,,,breast,50575;DU4475,epithelial,,breast,50577;HCC1187,epithelial,,breast,50578;HCC1500,epithelial,,breast,50579;HCC1599,epithelial,,breast,50580;HCC2157,epithelial,,breast,50581;HCC2218,epithelial,,breast,50582;2B8,,,lymphatic system,50585;A2780cis,,,ovary,50586;A3,,,blood,50587;A3/KAW,,,lymphatic system,50588;AGR-ON,,,blood,50589;ALL-SIL,,,blood,50590;AMO-1,,,lymphatic system,50591;ARH-77,,,blood,50592;BALL-1,,,blood,50593;BC-1,,,lymphatic system,50594;BC-2,,,lymphatic system,50595;BC-3,,,lymphatic system,50596;BDCM,,,blood,50597;BE(2)-M17,,,nervous system,50598;BL-41,,,lymphatic system,50599;BL-70,,,lymphatic system,50600;C8166,,,blood,50601;CA46,,,lymphatic system,50602;CCRF-CEM,,,blood,50603;CCRF-HSB-2,,,blood,50604;CCRF-SB,,,blood,50605;CEM/C1,,,blood,50606;CEM/C2,,,blood,50607;CESS,,,blood,50608;CFPAC-1,,,pancreas,50609;ChaGo-K-1,,,lung,50610;CHP-126,,,nervous system,50611;CI-1,,,lymphatic system,50612;CL-11,,,intestine,50613;Clone 15 HL-60,,,blood,50614;CMK,,,blood,50615;COLO 684,,,uterus,50616;COLO-704,,,ovary,50617;COR-L279,,,lung,50618;COR-L51,,,lung,50619;COR-L88,,,lung,50620;COR-L95,,,lung,50621;CPC-N,,,lung,50622;CTV-1,,,blood,50623;D283 Med,,,brain,50624;Daudi,,,lymphatic system,50625;DB,,,lymphatic system,50626;DERL-2,,,lymphatic system,50627;DG-75,,,lymphatic system,50628;DMS 114,,,lung,50629;DMS 153,,,lung,50630;DMS 79,,,lung,50631;DND-41,,,blood,50632;EB1,,,lymphatic system,50633;EB2,,,lymphatic system,50634;EB-3,,,lymphatic system,50635;EHEB,,,blood,50636;EJM,,,blood,50637;Eos-HL-60,,,blood,50638;Farage,,,lymphatic system,50639;GA-10,,,lymphatic system,50640;GA-10 (Clone 20),,,lymphatic system,50641;GDM-1,,,blood,50642;GOTO,,,nervous system,50643;Gp2D,,,intestine,50644;GRANTA-519,,,lymphatic system,50645;H33HJ-JA1,,,blood,50646;HC-1,,,blood,50647;HCC-33,,,lung,50648;HDLM-2,,,lymphatic system,50649;HD-MY-Z,,,lymphatic system,50650;HEL,,,blood,50651;HEL 92.1.7,,,blood,50652;HH,,,lymphatic system,50653;HL-60,,,blood,50654;HL60(S),,,blood,50655;HL-60/MX2,,,blood,50656;HL60RG,,,blood,50657;Hs 445,,,lymphatic system,50658;HS-Sultan,,,lymphatic system,50659;HT,,,lymphatic system,50660;HuT 78,,,lymphatic system,50661;I 2.1,,,blood,50662;I 9.2,,,blood,50663;IM-9,,,lymphatic system,50664;J.gamma1,,,blood,50665;J.gamma1.WT,,,blood,50666;J.RT3-T3.5,,,blood,50667;J45.01,,,blood,50668;Jiyoye,,,lymphatic system,50669;JJN-3,,,blood,50670;JKT-beta-del,,,blood,50671;JM1,,,lymphatic system,50672;JSC-1,,,lymphatic system,50673;Jurkat, Clone E6-1,,,blood,50674;JURL-MK1,,,blood,50675;JURL-MK2,,,blood,50676;K-562,,,blood,50677;K562/ADM,,,blood,50678;KARPAS-231,,,blood,50679;KARPAS-299,,,lymphatic system,50680;KARPAS-422,,,lymphatic system,50681;KARPAS-45,,,blood,50682;KARPAS-620,,,blood,50683;Kasumi-1,,,blood,50684;KCL-22,,,blood,50685;KE-37,,,blood,50686;KG-1,,,blood,50687;KG-1a,,,blood,50688;KM-H2,,,lymphatic system,50689;KMOE-2,,,blood,50690;KMS-12-BM,,,blood,50691;KMS-12-PE,,,blood,50692;KO52,,,blood,50693;KOPN-8,,,blood,50694;KP-1N,,,pancreas,50695;KP-1NL,,,pancreas,50696;KU812,,,blood,50697;KU812E,,,blood,50698;KU812F,,,blood,50699;KY821,,,blood,50700;KY821A3,,,blood,50701;KYM-1,,,muscle,50702;L-1236,,,lymphatic system,50703;L-363,,,blood,50704;L-428,,,lymphatic system,50705;L-540,,,lymphatic system,50706;LAMA-84,,,blood,50707;LC4-1,,,blood,50708;Loucy,,,blood,50709;LP-1,,,blood,50710;Lu-134-B,,,lung,50711;M059K,,,brain,50712;MC/CAR,,,lymphatic system,50713;MC116,,,lymphatic system,50714;ME-1,,,blood,50715;MEC-1,,,blood,50716;MEC-2,,,blood,50717;MEG-01,,,blood,50718;MHH-NB-11,,,nervous system,50719;MHH-PREB-1,,,lymphatic system,50720;MJ,,,lymphatic system,50721;ML-2,,,blood,50722;MLMA,,,blood,50723;MOLM-13,,,blood,50724;MOLP-8,,,blood,50725;MOLT-14,,,blood,50726;MOLT-16,,,blood,50727;MOLT-4,,,blood,50728;MOLT-4F,,,blood,50729;MONO-MAC-1,,,blood,50730;MONO-MAC-6,,,blood,50731;MRK-nu-1,,,breast,50732;MS-1-L,,,lung,50733;MV-4-11,,,blood,50734;MY,,,blood,50735;MY-M12,,,blood,50736;MY-M13,,,blood,50737;NALM-19,,,blood,50738;NALM-6,,,blood,50739;NAMALWA,,,lymphatic system,50740;NAMALWA.PNT,,,lymphatic system,50741;NB(TU)1-10,,,nervous system,50742;NB-1,,,nervous system,50743;NB-4,,,blood,50744;NC-37,,,lymphatic system,50745;NCI-H1092,,,lung,50746;NCI-H1155,,,lung,50747;NCI-H1304,,,lung,50748;NCI-H1385,,,lung,50749;NCI-H1395,,,lung,50750;NCI-H1404,,,lung,50751;NCI-H1417,,,lung,50752;NCI-H1436,,,lung,50753;NCI-H1522,,,lung,50754;NCI-H1563,,,lung,50755;NCI-H1618,,,lung,50756;NCI-H1666,,,lung,50757;NCI-H1694,,,lung,50758;NCI-H1770,,,lung,50759;NCI-H1836,,,lung,50760;NCI-H1838,,,lung,50761;NCI-H187,,,lung,50762;NCI-H1882,,,lung,50763;NCI-H1963,,,lung,50764;NCI-H1975,,,lung,50765;NCI-H2081,,,lung,50766;NCI-H209,,,lung,50767;NCI-H2106,,,lung,50768;NCI-H211,,,lung,50769;NCI-H2141,,,lung,50770;NCI-H2171,,,lung,50771;NCI-H220,,,lung,50772;NCI-H2227,,,lung,50773;NCI-H226,,,lung,50774;NCI-H345,,,lung,50775;NCI-H446,,,lung,50776;NCI-H510A,,,lung,50777;NCI-H524,,,lung,50778;NCI-H526,,,lung,50779;NCI-H69,,,lung,50780;NCI-H719,,,lung,50781;NCI-H720,,,lung,50782;NCI-H748,,,lung,50783;NCI-H82,,,lung,50784;NCI-H847,,,lung,50785;NCI-H889,,,lung,50786;NEC8,,,testes,50787;NH-12,,,nervous system,50788;NK-92MI,,,lymphatic system,50789;NOMO-1/ADM,,,blood,50790;NU-DUL-1,,,lymphatic system,50791;OCI-AML2,,,blood,50792;OCI-AML3,,,blood,50793;OCI-AML5,,,blood,50794;OCI-LY-19,,,lymphatic system,50795;OCI-M1,,,blood,50796;OPM-2,,,blood,50797;P116.cl39,,,blood,50798;P12-ICHIKAWA,,,blood,50799;P30/OHK,,,blood,50800;P31/FUJ,,,blood,50801;P32/ISH,,,lymphatic system,50802;P3HR-1,,,lymphatic system,50803;PC-3 [JPC-3],,,lung,50804;PEER,,,blood,50805;PF-382,,,blood,50806;Pfeiffer,,,lymphatic system,50807;PL-21,,,blood,50808;PSN1,,,pancreas,50809;Raji,,,lymphatic system,50810;Ramos (RA 1),,,blood,50811;RC-K8,,,lymphatic system,50812;REC-1,,,lymphatic system,50813;Reh,,,blood,50814;RERF-LC-MS,,,lung,50815;RH-1,,,bone,50816;RH-30,,,muscle,50817;RH-41,,,muscle,50818;RL,,,lymphatic system,50819;ROS-50,,,blood,50820;RPMI 1788,,,blood,50821;RPMI 6666,,,lymphatic system,50822;RPMI 8226,,,blood,50823;RPMI-8402,,,blood,50824;RS4;11,,,blood,50825;SBC-1,,,lung,50826;SBC-2,,,lung,50827;SC-1,,,lymphatic system,50828;SCC-3,,,lymphatic system,50829;Sci-1,,,lymphatic system,50830;SIG-M5,,,blood,50831;SIMA,,,nervous system,50832;SK-MEL-1,,,skin,50833;SK-MEL-3,,,skin,50834;SK-N-BE(2),,,nervous system,50835;SK-N-FI,,,nervous system,50836;SLVL,,,lymphatic system,50837;SNB-19,,,brain,50838;SR,,,lymphatic system,50839;ST486,,,lymphatic system,50840;SU-DHL-1,,,lymphatic system,50841;SU-DHL-10,,,lymphatic system,50842;SU-DHL-16,,,lymphatic system,50843;SU-DHL-4,,,lymphatic system,50844;SU-DHL-5,,,lymphatic system,50845;SU-DHL-6,,,lymphatic system,50846;SU-DHL-8,,,lymphatic system,50847;SUP-B15,,,blood,50848;SUP-HD1,,,lymphatic system,50849;SUP-M2,,,lymphatic system,50850;SUP-T1,,,blood,50851;SVG p12,,,brain,50852;SW 1990,,,pancreas,50853;TALL-1,,,blood,50854;TANOUE,,,blood,50855;TC-71,,,bone,50856;Tera-1,,,testes,50857;TF-1,,,blood,50858;TF-1.CN5a.1,,,blood,50859;TF-1a,,,blood,50860;THP-1,,,blood,50861;TK,,,lymphatic system,50862;Toledo,,,lymphatic system,50863;TT,,,thyroid,50864;TUR,,,lymphatic system,50865;U266B1,,,blood,50866;U-698-M,,,blood,50867;U-87 MG,,,brain,50868;U-937,,,lymphatic system,50869;VAL,,,lymphatic system,50870;WIL2 NS,,,lymphatic system,50871;WILCL,,,blood,50872;WSU-DLCL2,,,lymphatic system,50873;WSU-NHL,,,lymphatic system,50874;YMB-1,,,breast,50875;YT,,,lymphatic system,50876;697.0,,,blood,50877;8-MG-BA,,,brain,50878;A101D,,,skin,50879;A253,,,head &amp; neck,50880;A388,,,miscellaneous,50881;A498,,,kidney,50882;A4-Fuk,,,skin,50883;A704,,,kidney,50884;ACN,,,nervous system,50885;ALL-PO,,,blood,50886;AM-38,,,brain,50887;ATN-1,,,blood,50888;B2-17,,,brain,50889;BB30-HNC,,,head &amp; neck,50890;BB49-HNC,,,head &amp; neck,50891;BB65-RCC,,,kidney,50892;BE-13,,,blood,50893;Becker,,,brain,50894;BOKU,,,cervix,50895;BV-173,,,blood,50896;Calu-6,,,lung,50897;CAS-1,,,brain,50898;CGTH-W-1,,,thyroid,50899;COLO-320-HSR,,,intestine,50900;COLO-668,,,lung,50901;COLO-829,,,skin,50902;CP50-MEL-B,,,skin,50903;CP66-MEL,,,skin,50904;CTB-1,,,lymphatic system,50905;CW-2,,,intestine,50906;D-247MG,,,brain,50907;D-263MG,,,brain,50908;D-336MG,,,brain,50909;D-392MG,,,brain,50910;D-423MG,,,brain,50911;D-502MG,,,brain,50912;D-542MG,,,brain,50913;D-566MG,,,brain,50914;DEL,,,blood,50915;DJM-1,,,skin,50916;DOHH-2,,,lymphatic system,50917;DSH1,,,urinary tract,50918;ECC10,,,stomach,50919;ECC12,,,stomach,50920;ECC4,,,intestine,50921;EC-GI-10,,,esophagus,50922;EKVX,,,lung,50923;EM-2,,,blood,50924;EoL-1-cell,,,blood,50925;ES1,,,bone,50926;ES3,,,bone,50927;ES4,,,bone,50928;ES5,,,bone,50929;ES6,,,bone,50930;ES7,,,bone,50931;ES8,,,bone,50932;ETK-1,,,biliary tract,50933;EW-1,,,bone,50934;EW-11,,,bone,50935;EW-13,,,bone,50936;EW-16,,,bone,50937;EW-18,,,bone,50938;EW-24,,,bone,50939;EW-3,,,bone,50940;EW-7,,,bone,50941;GAK,,,skin,50942;GB-1,,,brain,50943;GCIY,,,stomach,50944;GI-1,,,brain,50945;GI-ME-N,,,nervous system,50946;GR-ST,,,blood,50947;GT3TKB,,,stomach,50948;H9,,,lymphatic system,50949;HA7-RCC,,,kidney,50950;HAL-01,,,blood,50951;HCC2998,,,intestine,50952;HCE-4,,,esophagus,50953;HCE-T,,,head &amp; neck,50954;HOP-62,,,lung,50955;HT-144,,,skin,50956;IMR-5,,,nervous system,50957;IST-MES1,,,pleura,50958;IST-SL1,,,lung,50959;IST-SL2,,,lung,50960;JEG-3,,,miscellaneous,50961;JVM-2,,,blood,50962;JVM-3,,,blood,50963;K5,,,thyroid,50964;KALS-1,,,brain,50965;KGN,,,ovary,50966;KINGS-1,,,brain,50967;KLE,,,uterus,50968;KM12,,,intestine,50969;KNS-42,,,brain,50970;KNS-81-FD,,,brain,50971;KP-N-YN,,,nervous system,50972;KP-N-YS,,,nervous system,50973;KS-1,,,brain,50974;KURAMOCHI,,,ovary,50975;LAN-5,,,nervous system,50976;LAN-6,,,nervous system,50977;LB1047-RCC,,,kidney,50978;LB2241-RCC,,,kidney,50979;LB2518-MEL,,,skin,50980;LB373-MEL-D,,,skin,50981;LB647-SCLC,,,lung,50982;LB771-HNC,,,head &amp; neck,50983;LB831-BLC,,,urinary tract,50984;LB996-RCC,,,kidney,50985;LC-1F,,,lung,50986;LC-2-ad,,,lung,50987;LOXIMVI,,,skin,50988;LS-1034,,,intestine,50989;LS-123,,,intestine,50990;LS-411N,,,intestine,50991;LS-513,,,intestine,50992;LU-134-A,,,lung,50993;LU-139,,,lung,50994;LU-165,,,lung,50995;LXF-289,,,lung,50996;MFH-ino,,,miscellaneous,50997;MHH-CALL-2,,,blood,50998;MMAC-SF,,,skin,50999;MN-60,,,blood,51000;Mo-T,,,blood,51001;MPP-89,,,pleura,51002;MUTZ-1,,,blood,51003;MZ1-PC,,,pancreas,51004;MZ2-MEL,,,skin,51005;MZ7-mel,,,skin,51006;NB10,,,nervous system,51007;NB12,,,nervous system,51008;NB13,,,nervous system,51009;NB14,,,nervous system,51010;NB16,,,nervous system,51011;NB17,,,nervous system,51012;NB5,,,nervous system,51013;NB6,,,nervous system,51014;NB7,,,nervous system,51015;NBsusSR,,,nervous system,51016;NCI-H1355,,,lung,51017;NCI-H157,,,lung,51018;NCI-H2126,,,lung,51019;NCI-H322M,,,lung,51020;NCI-H64,,,lung,51021;NCI-H716,,,intestine,51022;NCI-H747,,,intestine,51023;NKM-1,,,blood,51024;NMC-G1,,,brain,51025;no-10,,,brain,51026;no-11,,,brain,51027;NOMO-1,,,blood,51028;NOS-1,,,bone,51029;NTERA-S-cl-D1,,,testes,51030;OC-314,,,ovary,51031;OCUB-M,,,breast,51032;OMC-1,,,cervix,51033;ONS-76,,,brain,51034;OS-RC-2,,,kidney,51035;OVCAR-4,,,ovary,51036;QIMR-WIL,,,blood,51037;Ramos-2G6-4C10,,,lymphatic system,51038;RCC10RGB,,,kidney,51039;RF-48,,,stomach,51040;RKO,,,intestine,51041;RL95-2,,,uterus,51042;RPMI-8866,,,blood,51043;RXF393,,,kidney,51044;SF126,,,brain,51045;SF268,,,brain,51046;SF539,,,brain,51047;SH-4,,,skin,51048;SJSA-1,,,bone,51049;SK-MEL-24,,,skin,51050;SK-MEL-5,,,skin,51051;SK-MG-1,,,brain,51052;SK-MM-2,,,blood,51053;SK-PN-DW,,,bone,51054;SK-UT-1,,,uterus,51055;SNU-C1,,,intestine,51056;SNU-C2B,,,intestine,51057;SW403,,,intestine,51058;SW684,,,miscellaneous,51059;SW872,,,miscellaneous,51060;SW954,,,vulva,51061;SW962,,,vulva,51062;SW982,,,miscellaneous,51063;TE-1,,,esophagus,51064;TE-10,,,esophagus,51065;TE-11,,,esophagus,51066;TE-12,,,esophagus,51067;TE-15,,,esophagus,51068;TE-441-T,,,muscle,51069;TE-5,,,esophagus,51070;TE-6,,,esophagus,51071;TE-8,,,esophagus,51072;TE-9,,,esophagus,51073;TGBC11TKB,,,stomach,51074;TGBC1TKB,,,biliary tract,51075;TGBC24TKB,,,biliary tract,51076;TK10,,,kidney,51077;UACC-257,,,skin,51078;VA-ES-BJ,,,miscellaneous,51079;YH-13,,,brain,51080</t>
+  </si>
+  <si>
+    <t>Vinorelbine,small molecule,10281-101,LSM-6302</t>
+  </si>
+  <si>
+    <t>http://lincs.hms.harvard.edu/db/datasets/20014/</t>
+  </si>
+  <si>
+    <t>MGH (CMT) Growth Inhibition Assay Protocol (9 compound doses: 16 uM to 0.0625 uM) -- DNA Staining</t>
+  </si>
+  <si>
+    <t>A375.S2,epithelial,,skin,50003;CAL-51,epithelial-like,,breast,50008;Calu-1,epithelial,,lung,50009;Calu-3,epithelial,,lung,50010;COLO-800,epithelial-like,,skin,50012;FU97,epithelial-like,,stomach,50013;HUTU-80,epithelial,,intestine,50016;IA-LM,,,lung,50017;IST-MEL1,epithelial-like,,skin,50020;KMRC-20,epithelial-like,,kidney,50023;KYSE-150,epitheloid,,esophagus,50025;LNZTA3WT4,,,brain,50028;MCF7,epithelial,,breast,50029;MDA-MB-435S,melanocyte,,skin,50030;MT-3,epithelial,,breast,50031;NCI-H1648,,,lung,50032;NCI-H1651,epithelial,,lung,50033;NCI-H1703,epithelial,,lung,50034;NCI-H1915,large cell,,lung,50035;NCI-H2023,,,lung,50036;NCI-H810,epithelial,,lung,50037;PE/CA-PJ15,epithelial-like,,head &amp; neck,50039;SJCRH30,fibroblast,,muscle,50041;SK-MES,epithelial,,lung,50043;SK-OV-3,epithelial,,ovary,50044;SNB75,,,brain,50045;SW527,epithelial,,breast,50046;SW620,epithelial,,intestine,50047;Hep G2,epithelial,,liver,50052;SK-BR-3,epithelial,,breast,50057;MDA-MB-231,epithelial,,breast,50058;A-375,epithelial,,skin,50060;HeLa,epithelial,,cervix,50061;1321N1,,,brain,50063;143B,,,bone,50064;143B PML BK TK,,,bone,50065;42-MG-BA,,,brain,50069;639-V,,,ureter,50071;769-P,,,kidney,50072;786-O,,,kidney,50073;A172,,,brain,50076;A2058,,,skin,50078;A2780,,,ovary,50079;A2780ADR,,,ovary,50080;A373-C6,,,skin,50081;A-427,,,lung,50082;A431,,,skin,50083;A549,,,lung,50084;A673,,,muscle,50085;ABC-1,,,lung,50086;ACHN,,,kidney,50087;ASH-3,,,thyroid,50089;AsPC-1,,,pancreas,50090;AU565,,,breast,50091;BE(2)-C,,,nervous system,50094;BEN,,,lung,50095;BFTC-905,,,urinary bladder,50097;BFTC-909,,,kidney,50098;BT-20,,,breast,50105;BT-474,,,breast,50106;BT-483,,,breast,50107;BT-549,,,breast,50108;BxPC-3,,,pancreas,50109;C2BBe1,,,intestine,50111;C32,,,skin,50112;C-33 A,,,cervix,50113;Caco-2,,,intestine,50117;Caki-1,,,kidney,50118;CAL-120,,,breast,50120;CAL-12T,,,lung,50121;CAL-148,,,breast,50122;CAL-54,,,kidney,50126;CAL-72,,,bone,50128;CAL-78,,,bone,50129;CAL-85-1,,,breast,50130;CAMA-1,,,breast,50131;Caov-3,,,ovary,50132;Capan-1,,,pancreas,50134;Capan-2,,,pancreas,50135;CaR-1,,,intestine,50136;CCF-STTG1,,,brain,50137;CCK-81,,,intestine,50138;CHP-212,,,nervous system,50139;COLO 205,,,intestine,50143;COLO 320DM,,,intestine,50144;COLO 741,,,intestine,50145;COLO 792,,,skin,50146;COLO 853,,,skin,50147;COLO 857,,,skin,50148;COLO 858,,,skin,50149;COLO-206F,,,intestine,50150;COLO-320,,,intestine,50151;COLO-678,,,intestine,50152;COLO-783,,,skin,50154;COLO-818,,,skin,50155;COLO-824,,,breast,50156;COR-L 105,,,lung,50158;COR-L 23/CPR,,,lung,50159;COR-L23,,,lung,50160;DAN-G,,,pancreas,50161;Daoy,,,brain,50162;DBTRG-05MG,,,brain,50163;DK-MG,,,brain,50165;DLD-1,,,intestine,50166;DMS 273,,,lung,50167;DMS 53,,,lung,50168;DoTc2 4510,,,cervix,50170;DV-90,,,lung,50172;EBC-1,,,lung,50173;EFM-19,,,breast,50175;EFM-192A,,,breast,50176;EFM-192B,,,breast,50177;EFM-192C,,,breast,50178;EFO-21,,,ovary,50179;EFO-27,,,ovary,50180;EGI-1,,,biliary tract,50181;EN,,,uterus,50183;EPLC-272H,,,lung,50184;ES-2,,,ovary,50185;EVSA-T,,,breast,50187;FaDu,,,head &amp; neck,50188;FU-OV-1,,,ovary,50192;G-292 Clone A141B1,,,bone,50193;G-361,,,skin,50194;G-401,,,kidney,50195;G-402,,,kidney,50196;GAMG,,,brain,50197;GMS-10,,,brain,50199;GOS-3,,,brain,50200;GP5d,,,intestine,50201;H4,,,brain,50202;HARA,,,lung,50204;HCC1143,,,breast,50205;HCC1395,,,breast,50206;HCC1419,,,breast,50207;HCC1428,,,breast,50208;HCC-15,,,lung,50209;HCC1569,,,breast,50210;HCC1806,,,breast,50211;HCC1937,,,breast,50212;HCC1954,,,breast,50213;HCC202,,,breast,50214;HCC-366,,,lung,50215;HCC38,,,breast,50216;HCC-44,,,lung,50217;HCC-56,,,intestine,50218;HCC70,,,breast,50219;HCC-78,,,lung,50220;HCC-827,,,lung,50221;HCT 116,,,intestine,50222;HCT-15,,,intestine,50223;HDQ-P1,,,breast,50225;HLE,,,liver,50228;HMVII,,,skin,50229;HN,,,head &amp; neck,50230;HO-1-u-1,,,head &amp; neck,50232;HOS,,,bone,50233;HPAC,,,pancreas,50234;HPAF-II,,,pancreas,50235;Hs 578T,,,breast,50238;Hs 683,,,brain,50241;Hs 766T,,,pancreas,50243;HSC-4,,,head &amp; neck,50246;HT 1376,,,urinary bladder,50248;HT-29,,,intestine,50251;HT-3,,,cervix,50252;HT55,,,intestine,50253;HuCCT1,,,biliary tract,50255;HuO-3N1,,,bone,50257;HuO9,,,bone,50258;HuO9N2,,,bone,50259;HUP-T3,,,pancreas,50260;HUP-T4,,,pancreas,50261;IGR-1,,,skin,50262;IGR-37,,,skin,50263;IGR-39,,,skin,50264;IHH-4,,,thyroid,50265;IM-95,,,stomach,50266;IPC-298,,,skin,50269;J82,,,urinary bladder,50270;JHH-1,,,liver,50272;JHH-2,,,liver,50273;JHH-4,,,liver,50274;JHH-7,,,liver,50275;JIMT-1,,,breast,50276;KG-1-C,,,brain,50278;KHOS/NP,,,bone,50280;KHOS-240S,,,bone,50281;KHOS-312H,,,bone,50282;KMH-2,,,thyroid,50283;KMRC-1,,,kidney,50284;KP-2,,,pancreas,50287;KP-3,,,pancreas,50288;KP-3L,,,pancreas,50289;KP-4,,,pancreas,50290;KPL-1,,,breast,50291;KU-19-19,,,urinary bladder,50292;KYSE-220,,,esophagus,50293;KYSE-410,,,esophagus,50296;KYSE-510,,,esophagus,50298;LC-1 sq,,,lung,50301;LCLC-103H,,,lung,50302;LCLC-97TM1,,,lung,50303;LK-2,,,lung,50304;LN-18,,,brain,50305;LN-229,,,brain,50306;LN-405,,,brain,50307;LNZTA3WT11,,,brain,50308;LOU-NH91,,,lung,50309;LoVo,,,intestine,50310;LS174T,,,intestine,50311;LS180,,,intestine,50312;LU65,,,lung,50315;LU65A,,,lung,50316;LU65B,,,lung,50317;LU65C,,,lung,50318;LU99A,,,lung,50319;LU99B,,,lung,50320;LU99C,,,lung,50321;LUDLU-1,,,lung,50322;M059J,,,brain,50323;MB 157,,,breast,50324;MCAS,,,ovary,50325;MDA-MB-134-VI,,,breast,50327;MDA-MB-157,,,breast,50328;MDA-MB-175-VII,,,breast,50329;MDA-MB-330,,,breast,50330;MDA-MB-361,,,breast,50331;MDA-MB-415,,,breast,50332;MDA-MB-436,,,breast,50333;MDA-MB-453,,,breast,50334;MDA-MB-468,,,breast,50335;MEL-HO,,,skin,50338;MEL-JUSO,,,skin,50339;MES-SA,,,uterus,50340;MES-SA/Dx-5,,,uterus,50341;MEWO,,,skin,50342;MFE-319,,,uterus,50345;MFM-223,,,breast,50346;MG-63,,,bone,50347;MHH-ES-1,,,nervous system,50348;MIA PaCa-2,,,pancreas,50349;ML-1,,,thyroid,50355;MOG-G-CCM,,,brain,50356;MOG-G-UVW,,,brain,50357;MS751,,,cervix,50358;NB69,,,nervous system,50360;NCI-H1048,,,lung,50362;NCI-H1299,,,lung,50363;NCI-H1435,,,lung,50364;NCI-H1437,,,lung,50365;NCI-H1568,,,lung,50366;NCI-H1573,,,lung,50367;NCI-H1581,,,lung,50368;NCI-H1623,,,lung,50369;NCI-H1650,,,lung,50370;NCI-H1688,,,lung,50371;NCI-H1693,,,lung,50372;NCI-H1734,,,lung,50373;NCI-H1781,,,lung,50375;NCI-H1792,,,lung,50376;NCI-H1793,,,lung,50377;NCI-H1869,,,lung,50378;NCI-H1876,,,lung,50379;NCI-H1944,,,lung,50380;NCI-H196,,,lung,50381;NCI-H1993,,,lung,50382;NCI-H2009,,,lung,50383;NCI-H2030,,,lung,50385;NCI-H2073,,,lung,50386;NCI-H2085,,,lung,50387;NCI-H2087,,,lung,50388;NCI-H2110,,,lung,50389;NCI-H2122,,,lung,50390;NCI-H2170,,,lung,50392;NCI-H2172,,,lung,50393;NCI-H2196,,,lung,50395;NCI-H2198,,,lung,50396;NCI-H2228,,,lung,50397;NCI-H2286,,,lung,50398;NCI-H2291,,,lung,50399;NCI-H23,,,lung,50400;NCI-H2347,,,lung,50402;NCI-H2405,,,lung,50403;NCI-H2444,,,lung,50404;NCI-H2452,,,lung,50405;NCI-H322,,,lung,50407;NCI-H358,,,lung,50408;NCI-H441,,,lung,50409;NCI-H460,,,lung,50410;NCI-H520,,,lung,50411;NCI-H522,,,lung,50412;NCI-H596,,,lung,50413;NCI-H630,,,intestine,50414;NCI-H647,,,lung,50415;NCI-H650,,,lung,50416;NCI-H661,,,lung,50417;NCI-H727,,,lung,50418;NCI-H838,,,lung,50419;NCI-H841,,,lung,50420;NIH:OVCAR-3,,,ovary,50422;NUGC-2,,,stomach,50423;NY,,,bone,50426;OAW28,,,ovary,50427;OAW42,,,ovary,50428;OCUG-1,,,gall bladder,50429;OCUM-1,,,stomach,50430;OE21,,,esophagus,50432;OSC-20,,,head &amp; neck,50435;OUMS-23,,,intestine,50436;OV-90,,,ovary,50437;OVISE,,,ovary,50438;OVKATE,,,ovary,50439;OVMIU,,,ovary,50440;OVSAYO,,,ovary,50441;OVTOKO,,,ovary,50442;PA-1,,,ovary,50443;Panc 02.03,,,pancreas,50444;Panc 03.27,,,pancreas,50445;Panc 04.03,,,pancreas,50446;Panc 08.13,,,pancreas,50447;Panc 10.05,,,pancreas,50448;PANC-1,,,pancreas,50449;PA-TU-8902,,,pancreas,50450;PA-TU-8988S,,,pancreas,50451;PA-TU-8988T,,,pancreas,50452;PC-14,,,lung,50453;PC-3,,,prostate,50454;PFSK-1,,,brain,50455;PL45,,,pancreas,50456;QGP-1,,,pancreas,50458;RCM-1,,,intestine,50459;RD-ES,,,nervous system,50461;RERF-GC-1B,,,stomach,50462;RERF-LC-Ad1,,,lung,50463;RERF-LC-KJ,,,lung,50464;RERF-LC-MA,,,lung,50465;RERF-LC-Sq1,,,lung,50466;RKN,,,ovary,50467;RMG-I,,,ovary,50468;RPMI-7951,,,skin,50471;RT4,,,urinary bladder,50474;RVH-421,,,skin,50475;Saos-2,,,bone,50477;SAS,,,head &amp; neck,50478;SBC-3,,,lung,50480;SBC-5,,,lung,50481;SCaBER,,,urinary bladder,50482;SCC-15,,,head &amp; neck,50483;SCLC-21H,,,lung,50490;SHP-77,,,lung,50491;SiHa,,,cervix,50493;SISO,,,cervix,50494;SK-CO-1,,,intestine,50495;SK-ES-1,,,bone,50496;SKG-IIIa,,,cervix,50497;SK-LU-1,,,lung,50500;SK-MEL-2,,,skin,50501;SK-MEL-30,,,skin,50502;SKN,,,uterus,50503;SK-N-AS,,,nervous system,50505;SNG-M,,,uterus,50509;SNU-182,,,liver,50512;SNU-449,,,liver,50516;SU.86.86,,,pancreas,50520;SUIT-2,,,pancreas,50521;SW 1088,,,brain,50522;SW 1116,,,intestine,50523;SW 1271,,,lung,50524;SW 13,,,adrenal gland,50525;SW 1417,,,intestine,50526;SW 1463,,,intestine,50527;SW 156,,,kidney,50528;SW 1573,,,lung,50529;SW 1783,,,brain,50530;SW 48,,,intestine,50531;SW 626,,,ovary,50532;SW 780,,,urinary bladder,50533;SW 900,,,lung,50534;SW837,,,intestine,50537;SW-948,,,intestine,50538;T47D,,,breast,50541;T84,,,intestine,50542;T98G,,,brain,50543;TOV-112D,,,ovary,50547;TOV-21G,,,ovary,50548;TYK-nu,,,ovary,50550;U-118 MG,,,brain,50551;U-138 MG,,,brain,50552;U-2 OS,,,bone,50553;U-251 MG,,,brain,50554;U373 MG,,,brain,50555;UACC-812,,,breast,50556;UACC-893,,,breast,50557;UMC-11,,,lung,50558;UM-UC-3,,,urinary bladder,50559;VM-CUB1,,,urinary bladder,50561;VMRC-LCP,,,lung,50562;VMRC-RCW,,,kidney,50564;VMRC-RCZ,,,kidney,50565;WM 266-4,,,skin,50566;WM-115,,,skin,50567;WM1552C,,,skin,50568;WM278,,,skin,50569;WM35,,,skin,50570;WM793B,,,skin,50571;YAPC,,,pancreas,50572;YKG-1,,,brain,50573;ZR-75-1,,,breast,50574;ZR-75-30,,,breast,50575;DU4475,epithelial,,breast,50577;HCC1187,epithelial,,breast,50578;HCC1500,epithelial,,breast,50579;HCC1599,epithelial,,breast,50580;HCC2157,epithelial,,breast,50581;HCC2218,epithelial,,breast,50582;A3/KAW,,,lymphatic system,50588;AGR-ON,,,blood,50589;ALL-SIL,,,blood,50590;AMO-1,,,lymphatic system,50591;ARH-77,,,blood,50592;BALL-1,,,blood,50593;BC-2,,,lymphatic system,50595;BC-3,,,lymphatic system,50596;BDCM,,,blood,50597;BL-41,,,lymphatic system,50599;BL-70,,,lymphatic system,50600;C8166,,,blood,50601;CA46,,,lymphatic system,50602;CCRF-CEM,,,blood,50603;CCRF-HSB-2,,,blood,50604;CCRF-SB,,,blood,50605;CEM/C1,,,blood,50606;CEM/C2,,,blood,50607;CESS,,,blood,50608;CFPAC-1,,,pancreas,50609;ChaGo-K-1,,,lung,50610;CI-1,,,lymphatic system,50612;Clone 15 HL-60,,,blood,50614;CMK,,,blood,50615;COLO-704,,,ovary,50617;COR-L279,,,lung,50618;COR-L88,,,lung,50620;COR-L95,,,lung,50621;CPC-N,,,lung,50622;CTV-1,,,blood,50623;D283 Med,,,brain,50624;Daudi,,,lymphatic system,50625;DB,,,lymphatic system,50626;DERL-2,,,lymphatic system,50627;DG-75,,,lymphatic system,50628;DMS 114,,,lung,50629;DMS 79,,,lung,50631;DND-41,,,blood,50632;EB1,,,lymphatic system,50633;EB2,,,lymphatic system,50634;EB-3,,,lymphatic system,50635;EJM,,,blood,50637;Eos-HL-60,,,blood,50638;Farage,,,lymphatic system,50639;GA-10 (Clone 20),,,lymphatic system,50641;GDM-1,,,blood,50642;GRANTA-519,,,lymphatic system,50645;H33HJ-JA1,,,blood,50646;HC-1,,,blood,50647;HCC-33,,,lung,50648;HDLM-2,,,lymphatic system,50649;HD-MY-Z,,,lymphatic system,50650;HEL,,,blood,50651;HEL 92.1.7,,,blood,50652;HH,,,lymphatic system,50653;HL-60,,,blood,50654;HL60(S),,,blood,50655;HL-60/MX2,,,blood,50656;HL60RG,,,blood,50657;Hs 445,,,lymphatic system,50658;HS-Sultan,,,lymphatic system,50659;HT,,,lymphatic system,50660;HuT 78,,,lymphatic system,50661;I 2.1,,,blood,50662;J.gamma1,,,blood,50665;J.gamma1.WT,,,blood,50666;J.RT3-T3.5,,,blood,50667;J45.01,,,blood,50668;Jiyoye,,,lymphatic system,50669;JJN-3,,,blood,50670;JKT-beta-del,,,blood,50671;JSC-1,,,lymphatic system,50673;JURL-MK1,,,blood,50675;JURL-MK2,,,blood,50676;K-562,,,blood,50677;K562/ADM,,,blood,50678;KARPAS-299,,,lymphatic system,50680;KARPAS-422,,,lymphatic system,50681;KARPAS-45,,,blood,50682;KARPAS-620,,,blood,50683;Kasumi-1,,,blood,50684;KCL-22,,,blood,50685;KE-37,,,blood,50686;KG-1,,,blood,50687;KG-1a,,,blood,50688;KM-H2,,,lymphatic system,50689;KMOE-2,,,blood,50690;KMS-12-BM,,,blood,50691;KMS-12-PE,,,blood,50692;KO52,,,blood,50693;KOPN-8,,,blood,50694;KP-1N,,,pancreas,50695;KP-1NL,,,pancreas,50696;KU812,,,blood,50697;KU812E,,,blood,50698;KU812F,,,blood,50699;KY821,,,blood,50700;KY821A3,,,blood,50701;L-1236,,,lymphatic system,50703;L-363,,,blood,50704;L-428,,,lymphatic system,50705;L-540,,,lymphatic system,50706;LAMA-84,,,blood,50707;LC4-1,,,blood,50708;Loucy,,,blood,50709;LP-1,,,blood,50710;M059K,,,brain,50712;MC/CAR,,,lymphatic system,50713;MC116,,,lymphatic system,50714;ME-1,,,blood,50715;MEC-1,,,blood,50716;MEC-2,,,blood,50717;MEG-01,,,blood,50718;MHH-PREB-1,,,lymphatic system,50720;MJ,,,lymphatic system,50721;ML-2,,,blood,50722;MLMA,,,blood,50723;MOLM-13,,,blood,50724;MOLP-8,,,blood,50725;MOLT-14,,,blood,50726;MOLT-16,,,blood,50727;MOLT-4,,,blood,50728;MOLT-4F,,,blood,50729;MONO-MAC-1,,,blood,50730;MONO-MAC-6,,,blood,50731;MRK-nu-1,,,breast,50732;MS-1-L,,,lung,50733;MV-4-11,,,blood,50734;MY,,,blood,50735;MY-M13,,,blood,50737;NALM-19,,,blood,50738;NALM-6,,,blood,50739;NAMALWA,,,lymphatic system,50740;NAMALWA.PNT,,,lymphatic system,50741;NB-4,,,blood,50744;NC-37,,,lymphatic system,50745;NCI-H1155,,,lung,50747;NCI-H1385,,,lung,50749;NCI-H1395,,,lung,50750;NCI-H1417,,,lung,50752;NCI-H1436,,,lung,50753;NCI-H1563,,,lung,50755;NCI-H1666,,,lung,50757;NCI-H1694,,,lung,50758;NCI-H1770,,,lung,50759;NCI-H1836,,,lung,50760;NCI-H1838,,,lung,50761;NCI-H1882,,,lung,50763;NCI-H1975,,,lung,50765;NCI-H211,,,lung,50769;NCI-H2171,,,lung,50771;NCI-H226,,,lung,50774;NCI-H446,,,lung,50776;NCI-H524,,,lung,50778;NCI-H526,,,lung,50779;NCI-H720,,,lung,50782;NCI-H847,,,lung,50785;NOMO-1/ADM,,,blood,50790;NU-DUL-1,,,lymphatic system,50791;OCI-AML2,,,blood,50792;OCI-AML3,,,blood,50793;OCI-AML5,,,blood,50794;OCI-LY-19,,,lymphatic system,50795;OCI-M1,,,blood,50796;OPM-2,,,blood,50797;P116.cl39,,,blood,50798;P12-ICHIKAWA,,,blood,50799;P30/OHK,,,blood,50800;P31/FUJ,,,blood,50801;P3HR-1,,,lymphatic system,50803;PC-3 [JPC-3],,,lung,50804;PEER,,,blood,50805;PF-382,,,blood,50806;Pfeiffer,,,lymphatic system,50807;PL-21,,,blood,50808;PSN1,,,pancreas,50809;Raji,,,lymphatic system,50810;Ramos (RA 1),,,blood,50811;RC-K8,,,lymphatic system,50812;REC-1,,,lymphatic system,50813;Reh,,,blood,50814;RH-30,,,muscle,50817;RL,,,lymphatic system,50819;ROS-50,,,blood,50820;RPMI 6666,,,lymphatic system,50822;RPMI 8226,,,blood,50823;RPMI-8402,,,blood,50824;RS4;11,,,blood,50825;SBC-2,,,lung,50827;SCC-3,,,lymphatic system,50829;Sci-1,,,lymphatic system,50830;SIG-M5,,,blood,50831;SK-MEL-1,,,skin,50833;SK-MEL-3,,,skin,50834;SLVL,,,lymphatic system,50837;SR,,,lymphatic system,50839;ST486,,,lymphatic system,50840;SU-DHL-1,,,lymphatic system,50841;SU-DHL-10,,,lymphatic system,50842;SU-DHL-16,,,lymphatic system,50843;SU-DHL-4,,,lymphatic system,50844;SU-DHL-5,,,lymphatic system,50845;SU-DHL-6,,,lymphatic system,50846;SU-DHL-8,,,lymphatic system,50847;SUP-B15,,,blood,50848;SUP-HD1,,,lymphatic system,50849;SUP-M2,,,lymphatic system,50850;SUP-T1,,,blood,50851;SW 1990,,,pancreas,50853;TALL-1,,,blood,50854;TANOUE,,,blood,50855;TC-71,,,bone,50856;TF-1,,,blood,50858;TF-1.CN5a.1,,,blood,50859;TF-1a,,,blood,50860;THP-1,,,blood,50861;TK,,,lymphatic system,50862;Toledo,,,lymphatic system,50863;TUR,,,lymphatic system,50865;U266B1,,,blood,50866;U-698-M,,,blood,50867;U-87 MG,,,brain,50868;U-937,,,lymphatic system,50869;VAL,,,lymphatic system,50870;WIL2 NS,,,lymphatic system,50871;WSU-DLCL2,,,lymphatic system,50873;WSU-NHL,,,lymphatic system,50874;YMB-1,,,breast,50875;YT,,,lymphatic system,50876;697.0,,,blood,50877;8-MG-BA,,,brain,50878;A101D,,,skin,50879;A4-Fuk,,,skin,50883;A704,,,kidney,50884;ACN,,,nervous system,50885;ALL-PO,,,blood,50886;AM-38,,,brain,50887;ATN-1,,,blood,50888;BB49-HNC,,,head &amp; neck,50891;BB65-RCC,,,kidney,50892;BE-13,,,blood,50893;Becker,,,brain,50894;BOKU,,,cervix,50895;BV-173,,,blood,50896;Calu-6,,,lung,50897;CAS-1,,,brain,50898;COLO-320-HSR,,,intestine,50900;COLO-668,,,lung,50901;CP50-MEL-B,,,skin,50903;CP66-MEL,,,skin,50904;CW-2,,,intestine,50906;D-247MG,,,brain,50907;D-263MG,,,brain,50908;D-336MG,,,brain,50909;D-392MG,,,brain,50910;D-423MG,,,brain,50911;D-502MG,,,brain,50912;D-542MG,,,brain,50913;DEL,,,blood,50915;ECC4,,,intestine,50921;EKVX,,,lung,50923;EM-2,,,blood,50924;EoL-1-cell,,,blood,50925;ES1,,,bone,50926;ES3,,,bone,50927;ES4,,,bone,50928;ES5,,,bone,50929;ES6,,,bone,50930;ES7,,,bone,50931;ES8,,,bone,50932;ETK-1,,,biliary tract,50933;EW-1,,,bone,50934;EW-11,,,bone,50935;EW-13,,,bone,50936;EW-16,,,bone,50937;EW-18,,,bone,50938;EW-24,,,bone,50939;EW-3,,,bone,50940;EW-7,,,bone,50941;GAK,,,skin,50942;GB-1,,,brain,50943;GI-1,,,brain,50945;GI-ME-N,,,nervous system,50946;GR-ST,,,blood,50947;H9,,,lymphatic system,50949;HA7-RCC,,,kidney,50950;HAL-01,,,blood,50951;HCC2998,,,intestine,50952;HCE-4,,,esophagus,50953;HOP-62,,,lung,50955;HT-144,,,skin,50956;JVM-2,,,blood,50962;JVM-3,,,blood,50963;KALS-1,,,brain,50965;KGN,,,ovary,50966;KINGS-1,,,brain,50967;KM12,,,intestine,50969;KNS-42,,,brain,50970;KNS-81-FD,,,brain,50971;KS-1,,,brain,50974;KURAMOCHI,,,ovary,50975;LB1047-RCC,,,kidney,50978;LB2241-RCC,,,kidney,50979;LB2518-MEL,,,skin,50980;LB373-MEL-D,,,skin,50981;LB647-SCLC,,,lung,50982;LB996-RCC,,,kidney,50985;LC-1F,,,lung,50986;LC-2-ad,,,lung,50987;LOXIMVI,,,skin,50988;LS-1034,,,intestine,50989;LS-123,,,intestine,50990;LS-411N,,,intestine,50991;LS-513,,,intestine,50992;LU-134-A,,,lung,50993;LU-139,,,lung,50994;LXF-289,,,lung,50996;MHH-CALL-2,,,blood,50998;MMAC-SF,,,skin,50999;MN-60,,,blood,51000;Mo-T,,,blood,51001;MUTZ-1,,,blood,51003;MZ1-PC,,,pancreas,51004;MZ2-MEL,,,skin,51005;MZ7-mel,,,skin,51006;NCI-H1355,,,lung,51017;NCI-H157,,,lung,51018;NCI-H2126,,,lung,51019;NCI-H322M,,,lung,51020;NCI-H716,,,intestine,51022;NCI-H747,,,intestine,51023;NKM-1,,,blood,51024;NMC-G1,,,brain,51025;no-10,,,brain,51026;no-11,,,brain,51027;NOMO-1,,,blood,51028;NOS-1,,,bone,51029;OC-314,,,ovary,51031;OCUB-M,,,breast,51032;OMC-1,,,cervix,51033;ONS-76,,,brain,51034;OS-RC-2,,,kidney,51035;OVCAR-4,,,ovary,51036;QIMR-WIL,,,blood,51037;Ramos-2G6-4C10,,,lymphatic system,51038;RCC10RGB,,,kidney,51039;RKO,,,intestine,51041;RPMI-8866,,,blood,51043;RXF393,,,kidney,51044;SF126,,,brain,51045;SF268,,,brain,51046;SF539,,,brain,51047;SH-4,,,skin,51048;SJSA-1,,,bone,51049;SK-MEL-24,,,skin,51050;SK-MEL-5,,,skin,51051;SK-MG-1,,,brain,51052;SK-MM-2,,,blood,51053;SK-PN-DW,,,bone,51054;SNU-C1,,,intestine,51056;SNU-C2B,,,intestine,51057;TE-10,,,esophagus,51065;TE-11,,,esophagus,51066;TE-5,,,esophagus,51070;TE-6,,,esophagus,51071;TGBC1TKB,,,biliary tract,51075;TGBC24TKB,,,biliary tract,51076;TK10,,,kidney,51077;UACC-257,,,skin,51078;YH-13,,,brain,51080;5637.0,epithelial,,urinary bladder,50001;647-V,epithelial-like,,urinary bladder,50002;AGS,epithelial,,stomach,50004;BPH-1,epitheloid,,prostate,50005;Ca Ski,epithelial,,cervix,50006;Ca9-22,epithelial-like,,head &amp; neck,50007;COLO-679,fibroblastic,,skin,50011;HEC-1,,,uterus,50014;HLF,,,liver,50015;Ishikawa,epithelial-like,,uterus,50018;Ishikawa (Heraklio) 02 ER-,epithelial,,uterus,50019;JHH-6,epithelial-like,,liver,50021;KYSE-140,,,esophagus,50024;KYSE-180,epitheloid,,esophagus,50026;KYSE-450,epitheloid,,esophagus,50027;SK-LMS-1,,,uterus,50042;T24,epithelial,,urinary bladder,50048;WiDr,epithelial,,intestine,50049;Hep 3B2.1-7,epithelial,,liver,50051;Huh7,,,liver,50055;LNCaP,epithelial,,prostate,50059;1205Lu,,,skin,50062;1A6,,,urinary bladder,50066;22RV1,,,prostate,50067;23132/87,,,stomach,50068;8305C,,,thyroid,50074;8505C,,,thyroid,50075;A-204,,,muscle,50077;AN3CA,,,uterus,50088;AZ-521,,,stomach,50092;B-CPAP,,,thyroid,50093;BeWo,,,miscellaneous,50096;BHT-101,,,thyroid,50099;BHY,,,head &amp; neck,50100;BICR 10,,,head &amp; neck,50101;BICR 22,,,head &amp; neck,50102;BICR 31,,,head &amp; neck,50103;BICR 78,,,head &amp; neck,50104;C170,,,intestine,50110;C3A,,,liver,50114;C-4 I,,,cervix,50115;C-4 II,,,cervix,50116;CAL 27,,,head &amp; neck,50119;CAL-29,,,urinary bladder,50123;CAL-33,,,head &amp; neck,50124;CAL-39,,,vulva,50125;CAL-62,,,thyroid,50127;Caov-4,,,ovary,50133;CoCM-1,,,intestine,50141;COLO 201,,,intestine,50142;COLO-680N,,,esophagus,50153;COLO-849,,,skin,50157;Detroit 562,,,head &amp; neck,50164;DOK,,,head &amp; neck,50169;DU 145,,,prostate,50171;EFE-184,,,uterus,50174;EJ138,,,urinary bladder,50182;ESS-1,,,uterus,50186;FLYA13,,,miscellaneous,50189;FTC-133,,,thyroid,50190;FTC-238,,,thyroid,50191;GCT,,,miscellaneous,50198;HCT-8,,,intestine,50224;H-EMC-SS,,,bone,50226;HGC-27,,,stomach,50227;HO-1-N-1,,,head &amp; neck,50231;HRT-18,,,intestine,50236;Hs 257.T,,,intestine,50237;Hs 588.T,,,cervix,50239;Hs 633T,,,miscellaneous,50240;Hs 746T,,,stomach,50242;HSC-2,,,head &amp; neck,50244;HSC-3,,,head &amp; neck,50245;HT 1080,,,miscellaneous,50247;HT115,,,intestine,50249;HT-1197,,,urinary bladder,50250;HTC-C3,,,thyroid,50254;huH-1,,,liver,50256;IM-95m,,,stomach,50267;IMR-32,,,nervous system,50268;JAR,,,miscellaneous,50271;KELLY,,,nervous system,50277;KON,,,head &amp; neck,50285;KOSC-2 cl3-43,,,head &amp; neck,50286;KYSE-270,,,esophagus,50294;KYSE-30,,,esophagus,50295;KYSE-50,,,esophagus,50297;KYSE-520,,,esophagus,50299;KYSE-70,,,esophagus,50300;Lu-135,,,lung,50314;MC-IXC,,,nervous system,50326;MDST8,,,intestine,50336;ME-180,,,cervix,50337;MFE-280,,,uterus,50343;MFE-296,,,uterus,50344;MKN1,,,stomach,50350;MKN28,,,stomach,50351;MKN45,,,stomach,50352;MKN7,,,stomach,50353;MKN74,,,stomach,50354;MSTO-211H,,,pleura,50359;NCC-IT-A3,,,testes,50361;NCI-H1755,,,lung,50374;NCI-H2029,,,lung,50384;NCI-H2135,,,lung,50391;NCI-H2195,,,lung,50394;NCI-H2342,,,lung,50401;NCI-N87,,,stomach,50421;NUGC-3,,,stomach,50424;NUGC-4,,,stomach,50425;OE19,,,esophagus,50431;OE33,,,esophagus,50433;OSC-19,,,head &amp; neck,50434;PLC/PRF/5,,,liver,50457;RD,,,muscle,50460;RO82-W-1,,,thyroid,50469;RPMI 2650,,,head &amp; neck,50470;RT-112,,,urinary bladder,50472;RT112/84,,,urinary bladder,50473;S-117,,,thyroid,50476;SAT,,,head &amp; neck,50479;SCC-25,,,head &amp; neck,50484;SCC-4,,,head &amp; neck,50485;SCC-9,,,head &amp; neck,50486;SCCH-26,,,nervous system,50488;SCH,,,stomach,50489;SKG-IIIb,,,cervix,50498;SK-HEP-1,,,liver,50499;SKN-3,,,head &amp; neck,50504;SK-N-DZ,,,nervous system,50506;SK-NEP-1,,,kidney,50507;SK-N-SH,,,nervous system,50508;SNU-1,,,stomach,50510;SNU-16,,,stomach,50511;SNU-387,,,liver,50513;SNU-398,,,liver,50514;SNU-423,,,liver,50515;SNU-475,,,liver,50517;SNU-5,,,stomach,50518;SW-1710,,,urinary bladder,50535;SW756,,,cervix,50536;T.T,,,esophagus,50539;T.Tn,,,esophagus,50540;TASK1,,,nervous system,50544;TCCSUP,,,urinary bladder,50545;TGW,,,adrenal gland,50546;TT2609-C02,,,thyroid,50549;VCaP,,,prostate,50560;VMRC-MELG,,,skin,50563;2B8,,,lymphatic system,50585;A2780cis,,,ovary,50586;A3,,,blood,50587;BC-1,,,lymphatic system,50594;BE(2)-M17,,,nervous system,50598;CHP-126,,,nervous system,50611;CL-11,,,intestine,50613;COLO 684,,,uterus,50616;COR-L51,,,lung,50619;DMS 153,,,lung,50630;EHEB,,,blood,50636;GA-10,,,lymphatic system,50640;GOTO,,,nervous system,50643;Gp2D,,,intestine,50644;I 9.2,,,blood,50663;IM-9,,,lymphatic system,50664;JM1,,,lymphatic system,50672;Jurkat, Clone E6-1,,,blood,50674;KARPAS-231,,,blood,50679;KYM-1,,,muscle,50702;Lu-134-B,,,lung,50711;MHH-NB-11,,,nervous system,50719;MY-M12,,,blood,50736;NB(TU)1-10,,,nervous system,50742;NB-1,,,nervous system,50743;NCI-H1092,,,lung,50746;NCI-H1304,,,lung,50748;NCI-H1404,,,lung,50751;NCI-H1522,,,lung,50754;NCI-H1618,,,lung,50756;NCI-H187,,,lung,50762;NCI-H1963,,,lung,50764;NCI-H2081,,,lung,50766;NCI-H209,,,lung,50767;NCI-H2106,,,lung,50768;NCI-H2141,,,lung,50770;NCI-H220,,,lung,50772;NCI-H2227,,,lung,50773;NCI-H345,,,lung,50775;NCI-H510A,,,lung,50777;NCI-H69,,,lung,50780;NCI-H719,,,lung,50781;NCI-H748,,,lung,50783;NCI-H82,,,lung,50784;NCI-H889,,,lung,50786;NEC8,,,testes,50787;NH-12,,,nervous system,50788;NK-92MI,,,lymphatic system,50789;P32/ISH,,,lymphatic system,50802;RERF-LC-MS,,,lung,50815;RH-1,,,bone,50816;RH-41,,,muscle,50818;RPMI 1788,,,blood,50821;SBC-1,,,lung,50826;SC-1,,,lymphatic system,50828;SIMA,,,nervous system,50832;SK-N-BE(2),,,nervous system,50835;SK-N-FI,,,nervous system,50836;SNB-19,,,brain,50838;SVG p12,,,brain,50852;Tera-1,,,testes,50857;TT,,,thyroid,50864;WILCL,,,blood,50872;A253,,,head &amp; neck,50880;A388,,,miscellaneous,50881;A498,,,kidney,50882;B2-17,,,brain,50889;BB30-HNC,,,head &amp; neck,50890;CGTH-W-1,,,thyroid,50899;COLO-829,,,skin,50902;CTB-1,,,lymphatic system,50905;D-566MG,,,brain,50914;DJM-1,,,skin,50916;DOHH-2,,,lymphatic system,50917;DSH1,,,urinary tract,50918;ECC10,,,stomach,50919;ECC12,,,stomach,50920;EC-GI-10,,,esophagus,50922;GCIY,,,stomach,50944;GT3TKB,,,stomach,50948;HCE-T,,,head &amp; neck,50954;IMR-5,,,nervous system,50957;IST-MES1,,,pleura,50958;IST-SL1,,,lung,50959;IST-SL2,,,lung,50960;JEG-3,,,miscellaneous,50961;K5,,,thyroid,50964;KLE,,,uterus,50968;KP-N-YN,,,nervous system,50972;KP-N-YS,,,nervous system,50973;LAN-5,,,nervous system,50976;LAN-6,,,nervous system,50977;LB771-HNC,,,head &amp; neck,50983;LB831-BLC,,,urinary tract,50984;LU-165,,,lung,50995;MFH-ino,,,miscellaneous,50997;MPP-89,,,pleura,51002;NB10,,,nervous system,51007;NB12,,,nervous system,51008;NB13,,,nervous system,51009;NB14,,,nervous system,51010;NB16,,,nervous system,51011;NB17,,,nervous system,51012;NB5,,,nervous system,51013;NB6,,,nervous system,51014;NB7,,,nervous system,51015;NBsusSR,,,nervous system,51016;NCI-H64,,,lung,51021;NTERA-S-cl-D1,,,testes,51030;RF-48,,,stomach,51040;RL95-2,,,uterus,51042;SK-UT-1,,,uterus,51055;SW403,,,intestine,51058;SW684,,,miscellaneous,51059;SW872,,,miscellaneous,51060;SW954,,,vulva,51061;SW962,,,vulva,51062;SW982,,,miscellaneous,51063;TE-1,,,esophagus,51064;TE-12,,,esophagus,51067;TE-15,,,esophagus,51068;TE-441-T,,,muscle,51069;TE-8,,,esophagus,51072;TE-9,,,esophagus,51073;TGBC11TKB,,,stomach,51074;VA-ES-BJ,,,miscellaneous,51079</t>
+  </si>
+  <si>
+    <t>CP466722,small molecule,10009-101,LSM-1009;BMS345541,small molecule,10028-102,LSM-1028;Etoposide,small molecule,10250-101,LSM-6348;Shikonin,small molecule,10291-101,LSM-6309;Mitomycin C,small molecule,10292-101,LSM-6310;NSC-87877,small molecule,10297-101,LSM-6314;LFM-A13/DDE-28,small molecule,10298-101,LSM-6315;GSK650394,small molecule,10299-101,LSM-6316</t>
+  </si>
+  <si>
+    <t>http://lincs.hms.harvard.edu/db/datasets/20016/</t>
+  </si>
+  <si>
+    <t>MGH (CMT) Growth Inhibition Assay Protocol (9 compound doses: 32 uM to 0.125 uM) -- DNA Staining</t>
+  </si>
+  <si>
+    <t>Embelin,small molecule,10294-101,LSM-6311;IPA-3,small molecule,10295-101,LSM-6312</t>
+  </si>
+  <si>
+    <t>false\small molecules,2</t>
+  </si>
+  <si>
+    <t>http://lincs.hms.harvard.edu/db/datasets/20017/</t>
+  </si>
+  <si>
+    <t>Metrics other than potency reveal systematic variation in responses to cancer drugs: Data published in Fallahi-Sichani et al. (2013) Nature Chemical Biology. PMID: 24013279</t>
+  </si>
+  <si>
+    <t>The following is the abstract from Fallahi-Sichani et al. (2013) Nature Chemical Biology: &lt;i&gt;Large-scale analysis of cellular response to anticancer drugs typically focuses on variation in potency (half-maximum inhibitory concentration, (IC50)), assuming that it is the most important difference between effective and ineffective drugs or sensitive and resistant cells. We took a multiparametric approach involving analysis of the slope of the dose-response curve, the area under the curve and the maximum effect (Emax). We found that some of these parameters vary systematically with cell line and others with drug class. For cell-cycle inhibitors, Emax often but not always correlated with cell proliferation rate. For drugs targeting the Akt/PI3K/mTOR pathway, dose-response curves were unusually shallow. Classical pharmacology has no ready explanation for this phenomenon, but single-cell analysis showed that it correlated with significant and heritable cell-to-cell variability in the extent of target inhibition. We conclude that parameters other than potency should be considered in the comparative analysis of drug response, particularly at clinically relevant concentrations near and above the IC50.&lt;/i)</t>
+  </si>
+  <si>
+    <t>MCF7,epithelial,,breast,50029;SK-BR-3,epithelial,,breast,50057;MDA-MB-231,epithelial,,breast,50058;AU565,,,breast,50091;BT-20,,,breast,50105;BT-474,,,breast,50106;BT-483,,,breast,50107;BT-549,,,breast,50108;CAMA-1,,,breast,50131;HCC1143,,,breast,50205;HCC1395,,,breast,50206;HCC1419,,,breast,50207;HCC1428,,,breast,50208;HCC1569,,,breast,50210;HCC1806,,,breast,50211;HCC1937,,,breast,50212;HCC1954,,,breast,50213;HCC202,,,breast,50214;HCC38,,,breast,50216;HCC70,,,breast,50219;Hs 578T,,,breast,50238;MB 157,,,breast,50324;MDA-MB-134-VI,,,breast,50327;MDA-MB-157,,,breast,50328;MDA-MB-175-VII,,,breast,50329;MDA-MB-361,,,breast,50331;MDA-MB-436,,,breast,50333;MDA-MB-453,,,breast,50334;MDA-MB-468,,,breast,50335;T47D,,,breast,50541;UACC-812,,,breast,50556;UACC-893,,,breast,50557;ZR-75-1,,,breast,50574;184B5,epithelial,,breast,50576;HCC1187,epithelial,,breast,50578;MCF 10A,epithelial,,breast,50583;MCF 10F,epithelial,,breast,50584;SUM1315MO2,,,breast,51081;SUM149PT,,,breast,51082;SUM159PT,,,breast,51083;SUM185PE,,,breast,51084;SUM225CWN,,,breast,51085;SUM229PE,,,breast,51086;SUM52PE,,,breast,51087;184A1,,,breast,51088;MCF12A,,,breast,51089;MX1,,,breast,51090;T47DKBLUC,,,breast,51091;600MPE,,,breast,51092;HCC2185,,,breast,51093;HCC3153,,,breast,51094;LY2,,,breast,51095;ZR75B,,,breast,51096</t>
+  </si>
+  <si>
+    <t>53\cell lines</t>
+  </si>
+  <si>
+    <t>GSK461364,small molecule,10013-101,LSM-1013;Tozasertib,small molecule,10021-101,LSM-1021;Imatinib,small molecule,10023-103,LSM-1023;PD173074,small molecule,10026-101,LSM-1026;Sigma A6730,small molecule,10035-101,LSM-1035;GSK1070916,small molecule,10062-101,LSM-1062;Erlotinib,small molecule,10097-101,LSM-1097;Gefitinib,small molecule,10098-101,LSM-1098;Taxol,small molecule,10102-101,LSM-1102;MG-132,small molecule,10107-101,LSM-1107;Geldanamycin,small molecule,10108-101,LSM-1108;Afatinib,small molecule,10133-101,LSM-5742;Trametinib,small molecule,10142-101,LSM-1143;GSK2126458,small molecule,10146-101,LSM-1147;GSK1059615,small molecule,10172-101,LSM-1173;Sunitinib malate,small molecule,10175-106,LSM-1176;Bosutinib,small molecule,10189-101,LSM-1190;AG1478,small molecule,10223-101,LSM-1224;IKK16,small molecule,10228-102,LSM-2309;Lestaurtinib,small molecule,10230-101,LSM-1231;RAD001,small molecule,10235-101,LSM-4258;17-AAG,small molecule,10236-101,LSM-5870;5-DFUR,small molecule,10237-101,LSM-6359;5-FU,small molecule,10238-101,LSM-4261;Bortezomib,small molecule,10241-101,LSM-6281;Carboplatin,small molecule,10242-101,LSM-4265;CGC-11047,small molecule,10243-101,LSM-4266;CGC-11144,small molecule,10244-999,LSM-4267;Cisplatin,small molecule,10245-999,LSM-4268;CPT-11,small molecule,10246-999,LSM-2167;Docetaxel,small molecule,10247-101,LSM-6360;Doxorubicin,small molecule,10248-101,LSM-4062;Epirubicin,small molecule,10249-101,LSM-2078;Etoposide,small molecule,10250-101,LSM-6348;Fascaplysin,small molecule,10251-112,LSM-4272;Gemcitabine,small molecule,10252-101,LSM-5333;GSK1838705,small molecule,10255-101,LSM-4276;GSK923295,small molecule,10257-101,LSM-4278;Ibandronate sodium salt,small molecule,10258-110,LSM-4279;Ispinesib,small molecule,10260-999,LSM-5732;Ixabepilone,small molecule,10261-101,LSM-6350;LBH589,small molecule,10263-101,LSM-4284;MLN4924,small molecule,10265-101,LSM-6263;NSC 663284,small molecule,10266-101,LSM-2042;NU6102,small molecule,10267-101,LSM-4287;Nutlin 3a,small molecule,10268-101,LSM-6351;Oxaliplatin,small molecule,10269-999,LSM-6352;Oxamflatin,small molecule,10270-101,LSM-4290;(Z)-4-Hydroxytamoxifen,small molecule,10275-101,LSM-6361;TCS 2312,small molecule,10276-101,LSM-6362;Temsirolimus,small molecule,10277-101,LSM-4295;Topotecan,small molecule,10278-999,LSM-5662;Trichostatin A,small molecule,10279-101,LSM-3524;Triciribine,small molecule,10280-101,LSM-3810;Vinorelbine,small molecule,10281-101,LSM-6302;Vorinostat,small molecule,10282-101,LSM-3828;XRP44X,small molecule,10283-101,LSM-4298;Baicalein,small molecule,10343-101,LSM-6355;Olomoucine II,small molecule,10344-101,LSM-6356;PP242 hydrate,small molecule,10345-111,LSM-6357;Valproic acid,small molecule,10346-110,LSM-6363;Z-Leu-Leu-Norvalinal,small molecule,10348-101,LSM-6358</t>
+  </si>
+  <si>
+    <t>false\small molecules,62</t>
+  </si>
+  <si>
+    <t>http://lincs.hms.harvard.edu/db/datasets/20120/</t>
+  </si>
+  <si>
+    <t>Basal profile of receptor tyrosine kinase signaling network measured by ELISA: Data published in Niepel, Hafner et al. (2013) Science Signaling. PMID: 24065145</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Here, basal profiles for cells are the data for the abundance and basal phosphorylation of 22 receptors and 3 downstream kinases, as well as for the abundance of estrogen receptor (ER) and progesterone receptor (PR). In this dataset, basal profiles were obtained for approximately 40 breast cancer cell lines. All basal phosphorylation and protein abundance data were obtained by ELISA and, where possible, we estimated steady-state levels of molecules per cell using calibrated, recombinant standards. For the receptor tyrosine kinase phosphorylation data, we measured the amount of total phosphotyrosine rather than of individual phosphorylation sites, with the exception of IGF1R, for which we measured phosphorylation of Tyr1131. </t>
+  </si>
+  <si>
+    <t>184B5,epithelial,,breast,50576;AU565,,,breast,50091;BT-20,,,breast,50105;BT-474,,,breast,50106;BT-483,,,breast,50107;BT-549,,,breast,50108;CAMA-1,,,breast,50131;HCC1187,epithelial,,breast,50578;HCC1395,,,breast,50206;HCC1419,,,breast,50207;HCC1428,,,breast,50208;HCC1500,epithelial,,breast,50579;HCC1569,,,breast,50210;HCC1806,,,breast,50211;HCC1937,,,breast,50212;HCC1954,,,breast,50213;HCC202,,,breast,50214;HCC38,,,breast,50216;HCC70,,,breast,50219;Hs 578T,,,breast,50238;MCF 10A,epithelial,,breast,50583;MCF 10F,epithelial,,breast,50584;MCF12A,,,breast,51089;MCF7,epithelial,,breast,50029;MDA-MB-134-VI,,,breast,50327;MDA-MB-157,,,breast,50328;MDA-MB-175-VII,,,breast,50329;MDA-MB-231,epithelial,,breast,50058;MDA-MB-361,,,breast,50331;MDA-MB-415,,,breast,50332;MDA-MB-436,,,breast,50333;MDA-MB-453,,,breast,50334;MDA-MB-468,,,breast,50335;SK-BR-3,epithelial,,breast,50057;T47D,,,breast,50541;UACC-812,,,breast,50556;UACC-893,,,breast,50557;ZR-75-1,,,breast,50574;ZR-75-30,,,breast,50575</t>
+  </si>
+  <si>
+    <t>39\cell lines</t>
+  </si>
+  <si>
+    <t>http://lincs.hms.harvard.edu/db/datasets/20137/</t>
+  </si>
+  <si>
+    <t>Cell signaling response to growth factors measured by high throughput microscopy: Data published in Niepel, Hafner et al. (2013) Science Signaling. PMID: 24065145</t>
+  </si>
+  <si>
+    <t>To generate the growth factor __signaling profile__ set, we exposed approximately 40 breast cancer cell lines individually to fifteen different growth factors (protein ligands) for 10, 30, or 90 min. We monitored the response by measuring the phosphorylation state of ERK1/2, Akt, p38, and JNK using high throughput immunofluorescence microscopy.</t>
+  </si>
+  <si>
+    <t>184B5,epithelial,,breast,50576;AU565,,,breast,50091;BT-20,,,breast,50105;BT-474,,,breast,50106;BT-483,,,breast,50107;BT-549,,,breast,50108;CAMA-1,,,breast,50131;HCC1187,epithelial,,breast,50578;HCC1395,,,breast,50206;HCC1419,,,breast,50207;HCC1428,,,breast,50208;HCC1500,epithelial,,breast,50579;HCC1569,,,breast,50210;HCC1806,,,breast,50211;HCC1937,,,breast,50212;HCC1954,,,breast,50213;HCC202,,,breast,50214;HCC38,,,breast,50216;HCC70,,,breast,50219;Hs 578T,,,breast,50238;MCF 10A,epithelial,,breast,50583;MCF 10F,epithelial,,breast,50584;MCF12A,,,breast,51089;MCF7,epithelial,,breast,50029;MDA-MB-134-VI,,,breast,50327;MDA-MB-157,,,breast,50328;MDA-MB-175-VII,,,breast,50329;MDA-MB-231,epithelial,,breast,50058;MDA-MB-361,,,breast,50331;MDA-MB-415,,,breast,50332;MDA-MB-436,,,breast,50333;MDA-MB-453,,,breast,50334;SK-BR-3,epithelial,,breast,50057;T47D,,,breast,50541;UACC-812,,,breast,50556;UACC-893,,,breast,50557;ZR-75-1,,,breast,50574;ZR-75-30,,,breast,50575</t>
+  </si>
+  <si>
+    <t>38\cell lines</t>
+  </si>
+  <si>
+    <t>http://lincs.hms.harvard.edu/db/datasets/20138/</t>
+  </si>
+  <si>
+    <t>15\proteins</t>
+  </si>
+  <si>
+    <t>Cell signaling response to cytokines measured by high throughput microscopy: Data published in Niepel, Hafner et al. (2013) Science Signaling. PMID: 24065145</t>
+  </si>
+  <si>
+    <t>To generate the cytokine __signaling profile__ set, we exposed approximately 40 breast cancer cell lines individually to seven different cytokines (protein ligands or LPS) for 10, 30, or 90 min. We monitored the response by measuring the phosphorylation state of ERK1/2, STAT1, and STAT3 and the nuclear translocation of NF-kappaB using high throughput immunofluorescence microscopy.</t>
+  </si>
+  <si>
+    <t>184B5,epithelial,,breast,50576;AU565,,,breast,50091;BT-20,,,breast,50105;BT-474,,,breast,50106;BT-483,,,breast,50107;BT-549,,,breast,50108;CAMA-1,,,breast,50131;HCC1187,epithelial,,breast,50578;HCC1395,,,breast,50206;HCC1419,,,breast,50207;HCC1428,,,breast,50208;HCC1500,epithelial,,breast,50579;HCC1569,,,breast,50210;HCC1806,,,breast,50211;HCC1937,,,breast,50212;HCC1954,,,breast,50213;HCC202,,,breast,50214;HCC38,,,breast,50216;HCC70,,,breast,50219;Hs 578T,,,breast,50238;MCF 10A,epithelial,,breast,50583;MCF 10F,epithelial,,breast,50584;MCF12A,,,breast,51089;MCF7,epithelial,,breast,50029;MDA-MB-134-VI,,,breast,50327;MDA-MB-157,,,breast,50328;MDA-MB-175-VII,,,breast,50329;MDA-MB-231,epithelial,,breast,50058;MDA-MB-361,,,breast,50331;MDA-MB-415,,,breast,50332;MDA-MB-453,,,breast,50334;SK-BR-3,epithelial,,breast,50057;T47D,,,breast,50541;UACC-812,,,breast,50556;UACC-893,,,breast,50557;ZR-75-1,,,breast,50574;ZR-75-30,,,breast,50575</t>
+  </si>
+  <si>
+    <t>37\cell lines</t>
+  </si>
+  <si>
+    <t>http://lincs.hms.harvard.edu/db/datasets/20139/</t>
+  </si>
+  <si>
+    <t>6\proteins</t>
+  </si>
+  <si>
+    <t>Cell signaling response to growth factors measured by ELISA: Data published in Niepel, Hafner et al. (2013) Science Signaling. PMID: 24065145</t>
+  </si>
+  <si>
+    <t>To generate the growth factor __signaling profile__ set, we exposed approximately 40 breast cancer cell lines individually to fifteen different growth factors (protein ligands) for 10, 30, or 90 min. We monitored the response by measuring the phosphorylation state of ERK1/2 and Akt using ELISA.</t>
+  </si>
+  <si>
+    <t>MCF7,epithelial,,breast,50029;SK-BR-3,epithelial,,breast,50057;MDA-MB-231,epithelial,,breast,50058;AU565,,,breast,50091;BT-20,,,breast,50105;BT-474,,,breast,50106;BT-483,,,breast,50107;BT-549,,,breast,50108;CAMA-1,,,breast,50131;HCC1395,,,breast,50206;HCC1419,,,breast,50207;HCC1428,,,breast,50208;HCC1569,,,breast,50210;HCC1806,,,breast,50211;HCC1937,,,breast,50212;HCC1954,,,breast,50213;HCC202,,,breast,50214;HCC38,,,breast,50216;HCC70,,,breast,50219;Hs 578T,,,breast,50238;MDA-MB-134-VI,,,breast,50327;MDA-MB-157,,,breast,50328;MDA-MB-175-VII,,,breast,50329;MDA-MB-361,,,breast,50331;MDA-MB-415,,,breast,50332;MDA-MB-436,,,breast,50333;MDA-MB-453,,,breast,50334;MDA-MB-468,,,breast,50335;T47D,,,breast,50541;UACC-812,,,breast,50556;UACC-893,,,breast,50557;ZR-75-1,,,breast,50574;ZR-75-30,,,breast,50575;184B5,epithelial,,breast,50576;HCC1187,epithelial,,breast,50578;HCC1500,epithelial,,breast,50579;MCF 10A,epithelial,,breast,50583;MCF 10F,epithelial,,breast,50584;MCF12A,,,breast,51089</t>
+  </si>
+  <si>
+    <t>http://lincs.hms.harvard.edu/db/datasets/20140/</t>
+  </si>
+  <si>
+    <t>KINOMEscan</t>
+  </si>
+  <si>
+    <t>The KINOMEscan assay platform is based on a competition binding assay that is run for a compound of interest against each of a panel of 317 to 456 kinases. The assay has three components: a kinase-tagged phage, a test compound, and an immobilized ligand that the compound competes with to displace the kinase. The amount of kinase bound to the immobilized ligand is determined using quantitative PCR of the DNA tag.  Results for each kinase are reported as "Percent of control", where the control is DMSO and where a 100% result means no inhibition of kinase binding to the ligand in the presence of the compound, and where low percent results mean strong inhibition. The KINOMEscan data are presented graphically on TREEspot Kinase Dendrograms (http://www.discoverx.com/services/drug-discovery-development-services/treespot-data-analysis). For this study, HMS LINCS investigators have graphed results for kinases classified as 35 "percent of control" (in the presence of the compound, the kinase is 35% as active for binding ligand in the presence of DMSO), 5 "percent of control" and 1 "percent of control".</t>
+  </si>
+  <si>
+    <t>Sorafenib,small molecule,10008-101,LSM-1008;HG-6-64-01,small molecule,10017-101,LSM-6015;GW-5074,small molecule,10029-101,LSM-1029;SB590885,small molecule,10046-101,LSM-1046;PLX-4720,small molecule,10049-101,LSM-1049;AZ-628,small molecule,10050-101,LSM-1050;PLX4032,small molecule,10068-101,LSM-1068;AZD7762,small molecule,10006-101,LSM-1006;CP466722,small molecule,10009-101,LSM-1009;CP724714,small molecule,10010-101,LSM-1010;GSK429286A,small molecule,10012-101,LSM-1012;GSK461364,small molecule,10013-101,LSM-1013;GW843682,small molecule,10014-101,LSM-1014;Crizotinib,small molecule,10027-101,LSM-1027;BMS345541,small molecule,10028-102,LSM-1028;WH-4-023,small molecule,10038-101,LSM-5613;BX-912,small molecule,10055-101,LSM-1055;AZD-6482,small molecule,10059-101,LSM-1059;TAK-715,small molecule,10060-101,LSM-1060;NU7441,small molecule,10061-101,LSM-1061;KIN001-220,small molecule,10065-101,LSM-1065;MLN8054,small molecule,10066-101,LSM-1066;Barasertib,small molecule,10067-101,LSM-1067;PD0332991,small molecule,10071-101,LSM-1071;JWE-035,small molecule,10092-101,LSM-1092;ZM-447439,small molecule,10096-101,LSM-1096;JNK-9L,small molecule,10100-101,None;ALW-II-38-3,small molecule,10002-101,LSM-1002;ALW-II-49-7,small molecule,10003-101,LSM-1003;HG-5-113-01,small molecule,10015-101,LSM-5982;HG-5-88-01,small molecule,10016-101,LSM-5245;Neratinib,small molecule,10018-101,LSM-1018;CGP60474,small molecule,10025-101,LSM-1025;PD173074,small molecule,10026-101,LSM-1026;WH-4-025,small molecule,10039-101,LSM-5431;BI-2536,small molecule,10041-101,LSM-1041;KIN001-127,small molecule,10043-101,LSM-1043;A443654,small molecule,10045-101,LSM-1045;GDC-0941,small molecule,10047-101,LSM-1047;NPK76-II-72-1,small molecule,10070-101,LSM-1070;QL-X-138,small molecule,10075-101,LSM-5803;QL-XI-92,small molecule,10076-101,LSM-5394;Torin1,small molecule,10079-101,LSM-1079;Torin2,small molecule,10080-101,LSM-1080;WZ-4-145,small molecule,10082-101,LSM-5545;WZ-7043,small molecule,10083-101,LSM-5749;WZ3105,small molecule,10084-101,LSM-5970;WZ4002,small molecule,10085-101,LSM-1085;XMD11-50,small molecule,10086-101,LSM-1086;XMD11-85h,small molecule,10087-101,LSM-5577;XMD13-2,small molecule,10088-101,LSM-6296;XMD14-99,small molecule,10089-101,LSM-6297;XMD15-27,small molecule,10090-101,LSM-6298;XMD16-144,small molecule,10091-101,LSM-6299;XMD8-85,small molecule,10093-101,LSM-1093;XMD8-92,small molecule,10094-101,LSM-1094;ZG-10,small molecule,10095-101,LSM-6300;WYE-125132,small molecule,10064-101,LSM-1064;PD0325901,small molecule,10101-101,LSM-1101;JNK-IN-5A,small molecule,10208-101,LSM-1209;Momelotinib,small molecule,10140-101,LSM-1141;Sigma A6730,small molecule,10035-101,LSM-1035;GSK2126458,small molecule,10146-101,LSM-1147;GSK1059615,small molecule,10172-101,LSM-1173;AG1478,small molecule,10223-101,LSM-1224;BEZ235,small molecule,10232-101,LSM-4255;Lapatinib,small molecule,10051-104,LSM-1051;JW-7-24-1,small molecule,10019-101,LSM-5674;NVP-TAE684,small molecule,10024-101,LSM-1024;R406,small molecule,10040-101,LSM-1040;SP600125,small molecule,10162-101,LSM-1163;BMS-536924, KIN001-126,small molecule,10209-101,LSM-1210;KIN001-111/A770041,small molecule,10213-101,LSM-1214;CG-930,small molecule,10058-101,LSM-1058;XMD-12,small molecule,10106-101,LSM-1106;Bosutinib,small molecule,10189-101,LSM-1190;KU63794,small molecule,10229-101,LSM-1230;Canertinib,small molecule,10120-102,LSM-1120;KIN001-123/WZ-1-84,small molecule,10214-101,LSM-1215;(R)- Roscovitine,small molecule,10001-101,LSM-1001;PHA-793887,small molecule,10073-101,LSM-1073;PHA-767491,small molecule,10285-101,LSM-6304;BS-181,small molecule,10286-102,LSM-6305;Dinaciclib,small molecule,10287-101,LSM-6306;AZD4547,small molecule,10289-101,LSM-6308;OTSSP167,small molecule,10337-102,LSM-6340;Dabrafenib,small molecule,10284-101,LSM-6303;HG-9-91-01,small molecule,10340-101,LSM-6343;HG-14-8-02,small molecule,10341-101,LSM-6344;HG-14-10-04,small molecule,10342-101,LSM-6345;AZD 5438,small molecule,10158-101,LSM-1159;BMS345541,small molecule,10028-102,LSM-1028;AC220,small molecule,10037-101,LSM-1037;R406,small molecule,10040-101,LSM-1040;BI-2536,small molecule,10041-101,LSM-1041;Motesanib,small molecule,10042-101,LSM-1042;KIN001-242,small molecule,10044-104,LSM-1044;GDC-0941,small molecule,10047-101,LSM-1047;PD184352,small molecule,10048-101,LSM-1048;PLX-4720,small molecule,10049-101,LSM-1049;Lapatinib,small molecule,10051-104,LSM-1051;Selumetinib,small molecule,10056-101,LSM-1056;MLN8054,small molecule,10066-101,LSM-1066;Barasertib,small molecule,10067-101,LSM-1067;Enzastaurin,small molecule,10069-101,LSM-1069;Erlotinib,small molecule,10097-101,LSM-1097;Gefitinib,small molecule,10098-101,LSM-1098;Nilotinib,small molecule,10099-101,LSM-1099;Pazopanib,small molecule,10114-101,LSM-1114;Canertinib,small molecule,10120-102,LSM-1120;SGX523,small molecule,10123-101,LSM-1123;PHA-665752,small molecule,10125-101,LSM-1125;PI103,small molecule,10126-101,LSM-1126;Dovitinib,small molecule,10127-101,LSM-1127;GSK 690693,small molecule,10128-101,LSM-1128;Masitinib,small molecule,10130-101,LSM-1130;BMS-387032,small molecule,10132-101,LSM-1132;Afatinib,small molecule,10133-101,LSM-5742;Ruxolitinib,small molecule,10138-101,LSM-1139;TG 101348,small molecule,10141-101,LSM-1142;BIBF-1120,small molecule,10151-101,LSM-1152;Foretinib,small molecule,10157-101,LSM-1158;SB 203580,small molecule,10167-101,LSM-1168;VX-745,small molecule,10168-101,LSM-1169;Sunitinib,small molecule,10175-101,LSM-1176;Brivanib,small molecule,10177-101,LSM-1178;GDC-0879,small molecule,10181-101,LSM-1182;Linifanib,small molecule,10182-101,LSM-1183;Ki20227,small molecule,10187-101,LSM-1188;Bosutinib,small molecule,10189-101,LSM-1190;KW2449,small molecule,10192-101,LSM-1193;Vandetanib,small molecule,10198-101,LSM-1199;PKC412,small molecule,10220-101,LSM-1221;Tofacitinib,small molecule,10226-108,LSM-1227;Lestaurtinib,small molecule,10230-101,LSM-1231;GSK1838705,small molecule,10255-101,LSM-4276;AT-7519,small molecule,10004-101,LSM-1004;Sorafenib,small molecule,10008-101,LSM-1008;Flavopiridol,small molecule,10011-101,LSM-1011;GSK461364,small molecule,10013-101,LSM-1013;Neratinib,small molecule,10018-101,LSM-1018;Dasatinib,small molecule,10020-101,LSM-1020;Tozasertib,small molecule,10021-101,LSM-1021;Imatinib,small molecule,10023-103,LSM-1023;NVP-TAE684,small molecule,10024-101,LSM-1024;Crizotinib,small molecule,10027-101,LSM-1027;RAF 265,small molecule,10206-101,LSM-1207;RO-3306,small molecule,10104-101,LSM-1104;CGP74514A,small molecule,10355-101,LSM-6711;5z-7-oxozeaenol,small molecule,10356-101,LSM-6712</t>
+  </si>
+  <si>
+    <t>false\small molecules,150</t>
+  </si>
+  <si>
+    <t>http://lincs.hms.harvard.edu/data/kinomescan/</t>
+  </si>
+  <si>
+    <t>482\proteins</t>
+  </si>
+  <si>
+    <t>KiNativ</t>
+  </si>
+  <si>
+    <t>The KiNativ assay platform is based on the use of biotinylated acyl phosphates of ATP or ADP that act as probes by reacting with protein kinases on conserved lysine residues in the ATP binding pocket to covalently attach a biotin moiety.  Using these probes, cell lysates treated with a kinase inhibitor can be labeled with BHAcATP or BHAcADP, with kinases inhibited by the compound of interest exhibiting reduced or no labeling.  This is followed by digestion with trypsin, isolation of biotinylated peptides, and analysis by mass spectrometry to determine the extent of labeling of peptides from each kinase.</t>
+  </si>
+  <si>
+    <t>A-375,epithelial,,skin,50060;HeLa,epithelial,,cervix,50061;PC-3,,,prostate,50454;BCWM.1,,,blood,51097;Ramos (RA 1),,,blood,50811;NGP,,,nervous system,51099;MDA-MB-468,,,breast,50335</t>
+  </si>
+  <si>
+    <t>Sorafenib,small molecule,10008-101,LSM-1008;GW-5074,small molecule,10029-101,LSM-1029;SB590885,small molecule,10046-101,LSM-1046;PLX-4720,small molecule,10049-101,LSM-1049;AZ-628,small molecule,10050-101,LSM-1050;PLX4032,small molecule,10068-101,LSM-1068;HG-6-64-01,small molecule,10017-101,LSM-6015;Torin1,small molecule,10079-101,LSM-1079;Torin2,small molecule,10080-101,LSM-1080;XMD11-50,small molecule,10086-101,LSM-1086;XMD11-85h,small molecule,10087-101,LSM-5577;XMD16-144,small molecule,10091-101,LSM-6299;JWE-035,small molecule,10092-101,LSM-1092;XMD8-85,small molecule,10093-101,LSM-1093;XMD8-92,small molecule,10094-101,LSM-1094;XMD-12,small molecule,10106-101,LSM-1106;NVP-BHG712,small molecule,10200-101,LSM-1201;CH5424802,small molecule,10201-101,LSM-1202;NPK76-II-72-1,small molecule,10070-101,LSM-1070;QL-X-138,small molecule,10075-101,LSM-5803;Ibrutinib,small molecule,10129-101,LSM-1129;BX795,small molecule,10188-101,LSM-1189;OTSSP167,small molecule,10337-102,LSM-6340;DCC-2036,small molecule,10351-101,LSM-6708</t>
+  </si>
+  <si>
+    <t>false\small molecules,24</t>
+  </si>
+  <si>
+    <t>http://lincs.hms.harvard.edu/db/datasets/?search=&amp;extra_form_shown=true&amp;dataset_type=KiNativ</t>
+  </si>
+  <si>
+    <t>326\proteins</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -911,8 +1316,14 @@
       <color rgb="FF000000"/>
       <name val="Calibri (Body)"/>
     </font>
+    <font>
+      <sz val="24"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -945,6 +1356,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1670,7 +2087,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1738,6 +2155,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="659">
     <cellStyle name="Bad" xfId="43" builtinId="27"/>
@@ -2735,10 +3163,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y101"/>
+  <dimension ref="A1:BQ101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="B80" sqref="B80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="17" customHeight="1" x14ac:dyDescent="0"/>
@@ -6013,22 +6441,1052 @@
       <c r="X64" s="17"/>
       <c r="Y64" s="22"/>
     </row>
-    <row r="91" spans="1:1" ht="17" customHeight="1">
+    <row r="65" spans="1:69" ht="33">
+      <c r="A65" s="23" t="s">
+        <v>271</v>
+      </c>
+      <c r="B65" s="24"/>
+      <c r="C65" s="24"/>
+      <c r="D65" s="24"/>
+      <c r="E65" s="24"/>
+      <c r="F65" s="24"/>
+      <c r="G65" s="24"/>
+      <c r="H65" s="24"/>
+      <c r="I65" s="24"/>
+      <c r="J65" s="24"/>
+      <c r="K65" s="24"/>
+      <c r="L65" s="24"/>
+      <c r="M65" s="24"/>
+      <c r="N65" s="24"/>
+      <c r="O65" s="24"/>
+      <c r="P65" s="24"/>
+      <c r="Q65" s="24"/>
+      <c r="R65" s="24"/>
+      <c r="S65" s="24"/>
+      <c r="T65" s="24"/>
+      <c r="U65" s="24"/>
+      <c r="V65" s="24"/>
+      <c r="W65" s="24"/>
+      <c r="X65" s="24"/>
+      <c r="Y65" s="24"/>
+      <c r="Z65" s="24"/>
+      <c r="AA65" s="24"/>
+      <c r="AB65" s="24"/>
+      <c r="AC65" s="24"/>
+      <c r="AD65" s="24"/>
+      <c r="AE65" s="24"/>
+      <c r="AF65" s="24"/>
+      <c r="AG65" s="24"/>
+      <c r="AH65" s="24"/>
+      <c r="AI65" s="24"/>
+      <c r="AJ65" s="24"/>
+      <c r="AK65" s="24"/>
+      <c r="AL65" s="24"/>
+      <c r="AM65" s="24"/>
+      <c r="AN65" s="24"/>
+      <c r="AO65" s="24"/>
+      <c r="AP65" s="24"/>
+      <c r="AQ65" s="24"/>
+      <c r="AR65" s="24"/>
+      <c r="AS65" s="24"/>
+      <c r="AT65" s="24"/>
+      <c r="AU65" s="24"/>
+      <c r="AV65" s="24"/>
+      <c r="AW65" s="24"/>
+      <c r="AX65" s="24"/>
+      <c r="AY65" s="24"/>
+      <c r="AZ65" s="24"/>
+      <c r="BA65" s="24"/>
+      <c r="BB65" s="24"/>
+      <c r="BC65" s="24"/>
+      <c r="BD65" s="24"/>
+      <c r="BE65" s="24"/>
+      <c r="BF65" s="24"/>
+      <c r="BG65" s="24"/>
+      <c r="BH65" s="24"/>
+      <c r="BI65" s="24"/>
+      <c r="BJ65" s="24"/>
+      <c r="BK65" s="24"/>
+      <c r="BL65" s="24"/>
+      <c r="BM65" s="24"/>
+      <c r="BN65" s="24"/>
+      <c r="BO65" s="24"/>
+      <c r="BP65" s="24"/>
+      <c r="BQ65" s="25"/>
+    </row>
+    <row r="66" spans="1:69" ht="17" customHeight="1">
+      <c r="A66" s="26" t="s">
+        <v>254</v>
+      </c>
+      <c r="B66" s="26" t="s">
+        <v>272</v>
+      </c>
+      <c r="C66" s="26" t="s">
+        <v>273</v>
+      </c>
+      <c r="D66" s="26" t="s">
+        <v>274</v>
+      </c>
+      <c r="E66" s="26" t="s">
+        <v>232</v>
+      </c>
+      <c r="F66" s="26" t="s">
+        <v>275</v>
+      </c>
+      <c r="G66" s="26" t="s">
+        <v>276</v>
+      </c>
+      <c r="H66" s="27">
+        <v>41677</v>
+      </c>
+      <c r="I66" s="26"/>
+      <c r="J66" s="26"/>
+      <c r="K66" s="26" t="s">
+        <v>277</v>
+      </c>
+      <c r="L66" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="M66" s="26"/>
+      <c r="N66" s="26"/>
+      <c r="O66" s="26">
+        <v>20001</v>
+      </c>
+    </row>
+    <row r="67" spans="1:69" ht="17" customHeight="1">
+      <c r="A67" s="26" t="s">
+        <v>254</v>
+      </c>
+      <c r="B67" s="26" t="s">
+        <v>279</v>
+      </c>
+      <c r="C67" s="26" t="s">
+        <v>280</v>
+      </c>
+      <c r="D67" s="26" t="s">
+        <v>281</v>
+      </c>
+      <c r="E67" s="26" t="s">
+        <v>228</v>
+      </c>
+      <c r="F67" s="26" t="s">
+        <v>275</v>
+      </c>
+      <c r="G67" s="26" t="s">
+        <v>276</v>
+      </c>
+      <c r="H67" s="27">
+        <v>41677</v>
+      </c>
+      <c r="I67" s="26"/>
+      <c r="J67" s="26"/>
+      <c r="K67" s="26" t="s">
+        <v>282</v>
+      </c>
+      <c r="L67" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="M67" s="26"/>
+      <c r="N67" s="26"/>
+      <c r="O67" s="26">
+        <v>20002</v>
+      </c>
+    </row>
+    <row r="68" spans="1:69" ht="17" customHeight="1">
+      <c r="A68" s="26" t="s">
+        <v>254</v>
+      </c>
+      <c r="B68" s="26" t="s">
+        <v>283</v>
+      </c>
+      <c r="C68" s="26" t="s">
+        <v>284</v>
+      </c>
+      <c r="D68" s="26" t="s">
+        <v>285</v>
+      </c>
+      <c r="E68" s="26" t="s">
+        <v>286</v>
+      </c>
+      <c r="F68" s="26" t="s">
+        <v>287</v>
+      </c>
+      <c r="G68" s="26" t="s">
+        <v>276</v>
+      </c>
+      <c r="H68" s="27">
+        <v>41677</v>
+      </c>
+      <c r="I68" s="26"/>
+      <c r="J68" s="26"/>
+      <c r="K68" s="26" t="s">
+        <v>288</v>
+      </c>
+      <c r="L68" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="M68" s="26"/>
+      <c r="N68" s="26"/>
+      <c r="O68" s="26">
+        <v>20003</v>
+      </c>
+    </row>
+    <row r="69" spans="1:69" ht="17" customHeight="1">
+      <c r="A69" s="26" t="s">
+        <v>254</v>
+      </c>
+      <c r="B69" s="26" t="s">
+        <v>289</v>
+      </c>
+      <c r="C69" s="26" t="s">
+        <v>290</v>
+      </c>
+      <c r="D69" s="26" t="s">
+        <v>291</v>
+      </c>
+      <c r="E69" s="26" t="s">
+        <v>292</v>
+      </c>
+      <c r="F69" s="26" t="s">
+        <v>275</v>
+      </c>
+      <c r="G69" s="26" t="s">
+        <v>276</v>
+      </c>
+      <c r="H69" s="27">
+        <v>41677</v>
+      </c>
+      <c r="I69" s="26"/>
+      <c r="J69" s="26"/>
+      <c r="K69" s="26" t="s">
+        <v>293</v>
+      </c>
+      <c r="L69" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="M69" s="26"/>
+      <c r="N69" s="26"/>
+      <c r="O69" s="26">
+        <v>20004</v>
+      </c>
+    </row>
+    <row r="70" spans="1:69" ht="17" customHeight="1">
+      <c r="A70" s="26" t="s">
+        <v>254</v>
+      </c>
+      <c r="B70" s="26" t="s">
+        <v>294</v>
+      </c>
+      <c r="C70" s="26" t="s">
+        <v>295</v>
+      </c>
+      <c r="D70" s="26" t="s">
+        <v>296</v>
+      </c>
+      <c r="E70" s="26" t="s">
+        <v>297</v>
+      </c>
+      <c r="F70" s="26" t="s">
+        <v>298</v>
+      </c>
+      <c r="G70" s="26" t="s">
+        <v>181</v>
+      </c>
+      <c r="H70" s="27">
+        <v>41677</v>
+      </c>
+      <c r="I70" s="26"/>
+      <c r="J70" s="26"/>
+      <c r="K70" s="26" t="s">
+        <v>299</v>
+      </c>
+      <c r="L70" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="M70" s="26"/>
+      <c r="N70" s="26"/>
+      <c r="O70" s="26">
+        <v>20015</v>
+      </c>
+    </row>
+    <row r="71" spans="1:69" ht="17" customHeight="1">
+      <c r="A71" s="26" t="s">
+        <v>254</v>
+      </c>
+      <c r="B71" s="26" t="s">
+        <v>300</v>
+      </c>
+      <c r="C71" s="26" t="s">
+        <v>301</v>
+      </c>
+      <c r="D71" s="26" t="s">
+        <v>302</v>
+      </c>
+      <c r="E71" s="26" t="s">
+        <v>231</v>
+      </c>
+      <c r="F71" s="26"/>
+      <c r="G71" s="26"/>
+      <c r="H71" s="27">
+        <v>41677</v>
+      </c>
+      <c r="I71" s="26"/>
+      <c r="J71" s="26"/>
+      <c r="K71" s="26" t="s">
+        <v>303</v>
+      </c>
+      <c r="L71" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="M71" s="26"/>
+      <c r="N71" s="26"/>
+      <c r="O71" s="26">
+        <v>20121</v>
+      </c>
+    </row>
+    <row r="72" spans="1:69" ht="17" customHeight="1">
+      <c r="A72" s="26" t="s">
+        <v>254</v>
+      </c>
+      <c r="B72" s="26" t="s">
+        <v>304</v>
+      </c>
+      <c r="C72" s="26" t="s">
+        <v>305</v>
+      </c>
+      <c r="D72" s="26" t="s">
+        <v>306</v>
+      </c>
+      <c r="E72" s="26" t="s">
+        <v>226</v>
+      </c>
+      <c r="F72" s="26" t="s">
+        <v>307</v>
+      </c>
+      <c r="G72" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="H72" s="27">
+        <v>41677</v>
+      </c>
+      <c r="I72" s="26"/>
+      <c r="J72" s="26"/>
+      <c r="K72" s="26" t="s">
+        <v>309</v>
+      </c>
+      <c r="L72" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="M72" s="26"/>
+      <c r="N72" s="26"/>
+      <c r="O72" s="26">
+        <v>20136</v>
+      </c>
+    </row>
+    <row r="73" spans="1:69" ht="17" customHeight="1">
+      <c r="A73" s="26" t="s">
+        <v>254</v>
+      </c>
+      <c r="B73" s="26" t="s">
+        <v>310</v>
+      </c>
+      <c r="C73" s="26" t="s">
+        <v>311</v>
+      </c>
+      <c r="D73" s="26" t="s">
+        <v>312</v>
+      </c>
+      <c r="E73" s="26" t="s">
+        <v>313</v>
+      </c>
+      <c r="F73" s="26" t="s">
+        <v>314</v>
+      </c>
+      <c r="G73" s="26" t="s">
+        <v>315</v>
+      </c>
+      <c r="H73" s="27">
+        <v>41677</v>
+      </c>
+      <c r="I73" s="26"/>
+      <c r="J73" s="26"/>
+      <c r="K73" s="26" t="s">
+        <v>316</v>
+      </c>
+      <c r="L73" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="M73" s="26"/>
+      <c r="N73" s="26"/>
+      <c r="O73" s="26">
+        <v>20006</v>
+      </c>
+    </row>
+    <row r="74" spans="1:69" ht="17" customHeight="1">
+      <c r="A74" s="26" t="s">
+        <v>254</v>
+      </c>
+      <c r="B74" s="26" t="s">
+        <v>317</v>
+      </c>
+      <c r="C74" s="26" t="s">
+        <v>311</v>
+      </c>
+      <c r="D74" s="26" t="s">
+        <v>318</v>
+      </c>
+      <c r="E74" s="26" t="s">
+        <v>319</v>
+      </c>
+      <c r="F74" s="26" t="s">
+        <v>320</v>
+      </c>
+      <c r="G74" s="26" t="s">
+        <v>321</v>
+      </c>
+      <c r="H74" s="27">
+        <v>41677</v>
+      </c>
+      <c r="I74" s="26"/>
+      <c r="J74" s="26"/>
+      <c r="K74" s="26" t="s">
+        <v>322</v>
+      </c>
+      <c r="L74" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="M74" s="26"/>
+      <c r="N74" s="26"/>
+      <c r="O74" s="26">
+        <v>20007</v>
+      </c>
+    </row>
+    <row r="75" spans="1:69" ht="17" customHeight="1">
+      <c r="A75" s="26" t="s">
+        <v>254</v>
+      </c>
+      <c r="B75" s="26" t="s">
+        <v>323</v>
+      </c>
+      <c r="C75" s="26" t="s">
+        <v>295</v>
+      </c>
+      <c r="D75" s="26" t="s">
+        <v>324</v>
+      </c>
+      <c r="E75" s="26" t="s">
+        <v>325</v>
+      </c>
+      <c r="F75" s="26" t="s">
+        <v>326</v>
+      </c>
+      <c r="G75" s="26" t="s">
+        <v>174</v>
+      </c>
+      <c r="H75" s="27">
+        <v>41677</v>
+      </c>
+      <c r="I75" s="26"/>
+      <c r="J75" s="26"/>
+      <c r="K75" s="26" t="s">
+        <v>327</v>
+      </c>
+      <c r="L75" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="M75" s="26"/>
+      <c r="N75" s="26"/>
+      <c r="O75" s="26">
+        <v>20008</v>
+      </c>
+    </row>
+    <row r="76" spans="1:69" ht="17" customHeight="1">
+      <c r="A76" s="26" t="s">
+        <v>254</v>
+      </c>
+      <c r="B76" s="26" t="s">
+        <v>328</v>
+      </c>
+      <c r="C76" s="26" t="s">
+        <v>295</v>
+      </c>
+      <c r="D76" s="26" t="s">
+        <v>329</v>
+      </c>
+      <c r="E76" s="26" t="s">
+        <v>330</v>
+      </c>
+      <c r="F76" s="26" t="s">
+        <v>331</v>
+      </c>
+      <c r="G76" s="26" t="s">
+        <v>174</v>
+      </c>
+      <c r="H76" s="27">
+        <v>41677</v>
+      </c>
+      <c r="I76" s="26"/>
+      <c r="J76" s="26"/>
+      <c r="K76" s="26" t="s">
+        <v>332</v>
+      </c>
+      <c r="L76" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="M76" s="26"/>
+      <c r="N76" s="26"/>
+      <c r="O76" s="26">
+        <v>20009</v>
+      </c>
+    </row>
+    <row r="77" spans="1:69" ht="17" customHeight="1">
+      <c r="A77" s="26" t="s">
+        <v>254</v>
+      </c>
+      <c r="B77" s="26" t="s">
+        <v>333</v>
+      </c>
+      <c r="C77" s="26" t="s">
+        <v>295</v>
+      </c>
+      <c r="D77" s="26" t="s">
+        <v>334</v>
+      </c>
+      <c r="E77" s="26" t="s">
+        <v>335</v>
+      </c>
+      <c r="F77" s="26" t="s">
+        <v>336</v>
+      </c>
+      <c r="G77" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="H77" s="27">
+        <v>41677</v>
+      </c>
+      <c r="I77" s="26"/>
+      <c r="J77" s="26"/>
+      <c r="K77" s="26" t="s">
+        <v>337</v>
+      </c>
+      <c r="L77" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="M77" s="26"/>
+      <c r="N77" s="26"/>
+      <c r="O77" s="26">
+        <v>20010</v>
+      </c>
+    </row>
+    <row r="78" spans="1:69" ht="17" customHeight="1">
+      <c r="A78" s="26" t="s">
+        <v>254</v>
+      </c>
+      <c r="B78" s="26" t="s">
+        <v>338</v>
+      </c>
+      <c r="C78" s="26" t="s">
+        <v>295</v>
+      </c>
+      <c r="D78" s="26" t="s">
+        <v>339</v>
+      </c>
+      <c r="E78" s="26" t="s">
+        <v>340</v>
+      </c>
+      <c r="F78" s="26" t="s">
+        <v>341</v>
+      </c>
+      <c r="G78" s="26" t="s">
+        <v>342</v>
+      </c>
+      <c r="H78" s="27">
+        <v>41677</v>
+      </c>
+      <c r="I78" s="26"/>
+      <c r="J78" s="26"/>
+      <c r="K78" s="26" t="s">
+        <v>343</v>
+      </c>
+      <c r="L78" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="M78" s="26"/>
+      <c r="N78" s="26"/>
+      <c r="O78" s="26">
+        <v>20011</v>
+      </c>
+    </row>
+    <row r="79" spans="1:69" ht="17" customHeight="1">
+      <c r="A79" s="26" t="s">
+        <v>254</v>
+      </c>
+      <c r="B79" s="26" t="s">
+        <v>344</v>
+      </c>
+      <c r="C79" s="26" t="s">
+        <v>295</v>
+      </c>
+      <c r="D79" s="26" t="s">
+        <v>345</v>
+      </c>
+      <c r="E79" s="26" t="s">
+        <v>346</v>
+      </c>
+      <c r="F79" s="26" t="s">
+        <v>347</v>
+      </c>
+      <c r="G79" s="26" t="s">
+        <v>174</v>
+      </c>
+      <c r="H79" s="27">
+        <v>41677</v>
+      </c>
+      <c r="I79" s="26"/>
+      <c r="J79" s="26"/>
+      <c r="K79" s="26" t="s">
+        <v>348</v>
+      </c>
+      <c r="L79" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="M79" s="26"/>
+      <c r="N79" s="26"/>
+      <c r="O79" s="26">
+        <v>20012</v>
+      </c>
+    </row>
+    <row r="80" spans="1:69" ht="17" customHeight="1">
+      <c r="A80" s="26" t="s">
+        <v>254</v>
+      </c>
+      <c r="B80" s="26" t="s">
+        <v>349</v>
+      </c>
+      <c r="C80" s="26" t="s">
+        <v>295</v>
+      </c>
+      <c r="D80" s="26" t="s">
+        <v>350</v>
+      </c>
+      <c r="E80" s="26" t="s">
+        <v>325</v>
+      </c>
+      <c r="F80" s="26" t="s">
+        <v>351</v>
+      </c>
+      <c r="G80" s="26" t="s">
+        <v>181</v>
+      </c>
+      <c r="H80" s="27">
+        <v>41677</v>
+      </c>
+      <c r="I80" s="26"/>
+      <c r="J80" s="26"/>
+      <c r="K80" s="26" t="s">
+        <v>352</v>
+      </c>
+      <c r="L80" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="M80" s="26"/>
+      <c r="N80" s="26"/>
+      <c r="O80" s="26">
+        <v>20013</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" ht="17" customHeight="1">
+      <c r="A81" s="26" t="s">
+        <v>254</v>
+      </c>
+      <c r="B81" s="26" t="s">
+        <v>353</v>
+      </c>
+      <c r="C81" s="26" t="s">
+        <v>295</v>
+      </c>
+      <c r="D81" s="26" t="s">
+        <v>354</v>
+      </c>
+      <c r="E81" s="26" t="s">
+        <v>330</v>
+      </c>
+      <c r="F81" s="26" t="s">
+        <v>355</v>
+      </c>
+      <c r="G81" s="26" t="s">
+        <v>181</v>
+      </c>
+      <c r="H81" s="27">
+        <v>41677</v>
+      </c>
+      <c r="I81" s="26"/>
+      <c r="J81" s="26"/>
+      <c r="K81" s="26" t="s">
+        <v>356</v>
+      </c>
+      <c r="L81" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="M81" s="26"/>
+      <c r="N81" s="26"/>
+      <c r="O81" s="26">
+        <v>20014</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15" ht="17" customHeight="1">
+      <c r="A82" s="26" t="s">
+        <v>254</v>
+      </c>
+      <c r="B82" s="26" t="s">
+        <v>357</v>
+      </c>
+      <c r="C82" s="26" t="s">
+        <v>295</v>
+      </c>
+      <c r="D82" s="26" t="s">
+        <v>358</v>
+      </c>
+      <c r="E82" s="26" t="s">
+        <v>335</v>
+      </c>
+      <c r="F82" s="26" t="s">
+        <v>359</v>
+      </c>
+      <c r="G82" s="26" t="s">
+        <v>276</v>
+      </c>
+      <c r="H82" s="27">
+        <v>41677</v>
+      </c>
+      <c r="I82" s="26"/>
+      <c r="J82" s="26"/>
+      <c r="K82" s="26" t="s">
+        <v>360</v>
+      </c>
+      <c r="L82" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="M82" s="26"/>
+      <c r="N82" s="26"/>
+      <c r="O82" s="26">
+        <v>20016</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" ht="17" customHeight="1">
+      <c r="A83" s="26" t="s">
+        <v>254</v>
+      </c>
+      <c r="B83" s="26" t="s">
+        <v>361</v>
+      </c>
+      <c r="C83" s="26" t="s">
+        <v>295</v>
+      </c>
+      <c r="D83" s="26" t="s">
+        <v>350</v>
+      </c>
+      <c r="E83" s="26" t="s">
+        <v>325</v>
+      </c>
+      <c r="F83" s="26" t="s">
+        <v>362</v>
+      </c>
+      <c r="G83" s="26" t="s">
+        <v>363</v>
+      </c>
+      <c r="H83" s="27">
+        <v>41677</v>
+      </c>
+      <c r="I83" s="26"/>
+      <c r="J83" s="26"/>
+      <c r="K83" s="26" t="s">
+        <v>364</v>
+      </c>
+      <c r="L83" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="M83" s="26"/>
+      <c r="N83" s="26"/>
+      <c r="O83" s="26">
+        <v>20017</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" ht="17" customHeight="1">
+      <c r="A84" s="26" t="s">
+        <v>254</v>
+      </c>
+      <c r="B84" s="26" t="s">
+        <v>365</v>
+      </c>
+      <c r="C84" s="26" t="s">
+        <v>366</v>
+      </c>
+      <c r="D84" s="26" t="s">
+        <v>367</v>
+      </c>
+      <c r="E84" s="26" t="s">
+        <v>368</v>
+      </c>
+      <c r="F84" s="26" t="s">
+        <v>369</v>
+      </c>
+      <c r="G84" s="26" t="s">
+        <v>370</v>
+      </c>
+      <c r="H84" s="27">
+        <v>41761</v>
+      </c>
+      <c r="I84" s="26"/>
+      <c r="J84" s="26"/>
+      <c r="K84" s="26" t="s">
+        <v>371</v>
+      </c>
+      <c r="L84" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="M84" s="26"/>
+      <c r="N84" s="26"/>
+      <c r="O84" s="26">
+        <v>20120</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" ht="17" customHeight="1">
+      <c r="A85" s="26" t="s">
+        <v>254</v>
+      </c>
+      <c r="B85" s="26" t="s">
+        <v>372</v>
+      </c>
+      <c r="C85" s="26" t="s">
+        <v>373</v>
+      </c>
+      <c r="D85" s="26" t="s">
+        <v>374</v>
+      </c>
+      <c r="E85" s="26" t="s">
+        <v>375</v>
+      </c>
+      <c r="F85" s="26"/>
+      <c r="G85" s="26"/>
+      <c r="H85" s="27">
+        <v>41677</v>
+      </c>
+      <c r="I85" s="26"/>
+      <c r="J85" s="26"/>
+      <c r="K85" s="26" t="s">
+        <v>376</v>
+      </c>
+      <c r="L85" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="M85" s="26"/>
+      <c r="N85" s="26"/>
+      <c r="O85" s="26">
+        <v>20137</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" ht="17" customHeight="1">
+      <c r="A86" s="26" t="s">
+        <v>254</v>
+      </c>
+      <c r="B86" s="26" t="s">
+        <v>377</v>
+      </c>
+      <c r="C86" s="26" t="s">
+        <v>378</v>
+      </c>
+      <c r="D86" s="26" t="s">
+        <v>379</v>
+      </c>
+      <c r="E86" s="26" t="s">
+        <v>380</v>
+      </c>
+      <c r="F86" s="26"/>
+      <c r="G86" s="26"/>
+      <c r="H86" s="27">
+        <v>41781</v>
+      </c>
+      <c r="I86" s="26"/>
+      <c r="J86" s="26"/>
+      <c r="K86" s="26" t="s">
+        <v>381</v>
+      </c>
+      <c r="L86" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="M86" s="26"/>
+      <c r="N86" s="26" t="s">
+        <v>382</v>
+      </c>
+      <c r="O86" s="26">
+        <v>20138</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" ht="17" customHeight="1">
+      <c r="A87" s="26" t="s">
+        <v>254</v>
+      </c>
+      <c r="B87" s="26" t="s">
+        <v>383</v>
+      </c>
+      <c r="C87" s="26" t="s">
+        <v>384</v>
+      </c>
+      <c r="D87" s="26" t="s">
+        <v>385</v>
+      </c>
+      <c r="E87" s="26" t="s">
+        <v>386</v>
+      </c>
+      <c r="F87" s="26"/>
+      <c r="G87" s="26"/>
+      <c r="H87" s="27">
+        <v>41781</v>
+      </c>
+      <c r="I87" s="26"/>
+      <c r="J87" s="26"/>
+      <c r="K87" s="26" t="s">
+        <v>387</v>
+      </c>
+      <c r="L87" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="M87" s="26"/>
+      <c r="N87" s="26" t="s">
+        <v>388</v>
+      </c>
+      <c r="O87" s="26">
+        <v>20139</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15" ht="17" customHeight="1">
+      <c r="A88" s="26" t="s">
+        <v>254</v>
+      </c>
+      <c r="B88" s="26" t="s">
+        <v>389</v>
+      </c>
+      <c r="C88" s="26" t="s">
+        <v>390</v>
+      </c>
+      <c r="D88" s="26" t="s">
+        <v>391</v>
+      </c>
+      <c r="E88" s="26" t="s">
+        <v>375</v>
+      </c>
+      <c r="F88" s="26"/>
+      <c r="G88" s="26"/>
+      <c r="H88" s="27">
+        <v>41677</v>
+      </c>
+      <c r="I88" s="26"/>
+      <c r="J88" s="26"/>
+      <c r="K88" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="L88" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="M88" s="26"/>
+      <c r="N88" s="26" t="s">
+        <v>382</v>
+      </c>
+      <c r="O88" s="26">
+        <v>20140</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15" ht="17" customHeight="1">
+      <c r="A89" s="26" t="s">
+        <v>254</v>
+      </c>
+      <c r="B89" s="26" t="s">
+        <v>393</v>
+      </c>
+      <c r="C89" s="26" t="s">
+        <v>394</v>
+      </c>
+      <c r="D89" s="26"/>
+      <c r="E89" s="26"/>
+      <c r="F89" s="26" t="s">
+        <v>395</v>
+      </c>
+      <c r="G89" s="26" t="s">
+        <v>396</v>
+      </c>
+      <c r="H89" s="27">
+        <v>41947</v>
+      </c>
+      <c r="I89" s="26"/>
+      <c r="J89" s="26"/>
+      <c r="K89" s="26" t="s">
+        <v>397</v>
+      </c>
+      <c r="L89" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="M89" s="26"/>
+      <c r="N89" s="26" t="s">
+        <v>398</v>
+      </c>
+      <c r="O89" s="26"/>
+    </row>
+    <row r="90" spans="1:15" ht="17" customHeight="1">
+      <c r="A90" s="26" t="s">
+        <v>254</v>
+      </c>
+      <c r="B90" s="26" t="s">
+        <v>399</v>
+      </c>
+      <c r="C90" s="26" t="s">
+        <v>400</v>
+      </c>
+      <c r="D90" s="26" t="s">
+        <v>401</v>
+      </c>
+      <c r="E90" s="26" t="s">
+        <v>228</v>
+      </c>
+      <c r="F90" s="26" t="s">
+        <v>402</v>
+      </c>
+      <c r="G90" s="26" t="s">
+        <v>403</v>
+      </c>
+      <c r="H90" s="27">
+        <v>41816</v>
+      </c>
+      <c r="I90" s="26"/>
+      <c r="J90" s="26"/>
+      <c r="K90" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="L90" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="M90" s="26"/>
+      <c r="N90" s="26" t="s">
+        <v>405</v>
+      </c>
+      <c r="O90" s="26"/>
+    </row>
+    <row r="91" spans="1:15" ht="17" customHeight="1">
       <c r="A91" s="21"/>
     </row>
-    <row r="92" spans="1:1" ht="17" customHeight="1">
+    <row r="92" spans="1:15" ht="17" customHeight="1">
       <c r="A92" s="21"/>
     </row>
-    <row r="93" spans="1:1" ht="17" customHeight="1">
+    <row r="93" spans="1:15" ht="17" customHeight="1">
       <c r="A93" s="21"/>
     </row>
-    <row r="94" spans="1:1" ht="17" customHeight="1">
+    <row r="94" spans="1:15" ht="17" customHeight="1">
       <c r="A94" s="21"/>
     </row>
-    <row r="95" spans="1:1" ht="17" customHeight="1">
+    <row r="95" spans="1:15" ht="17" customHeight="1">
       <c r="A95" s="21"/>
     </row>
-    <row r="96" spans="1:1" ht="17" customHeight="1">
+    <row r="96" spans="1:15" ht="17" customHeight="1">
       <c r="A96" s="21"/>
     </row>
     <row r="97" spans="1:1" ht="17" customHeight="1">
@@ -6047,6 +7505,9 @@
       <c r="A101" s="21"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A65:BQ65"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="R28" r:id="rId1"/>
     <hyperlink ref="R29" r:id="rId2"/>

</xml_diff>

<commit_message>
Released DTOXs RNASeq and Broad's P100 & GCP
</commit_message>
<xml_diff>
--- a/milestones-consolidated.xlsx
+++ b/milestones-consolidated.xlsx
@@ -1456,7 +1456,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="677">
+  <cellStyleXfs count="679">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2117,6 +2117,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2179,7 +2181,7 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="677">
+  <cellStyles count="679">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2531,6 +2533,8 @@
     <cellStyle name="Followed Hyperlink" xfId="674" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="675" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="676" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="677" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="678" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3196,7 +3200,7 @@
   <dimension ref="A1:BQ105"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="17" customHeight="1" x14ac:dyDescent="0"/>
@@ -3398,16 +3402,16 @@
         <v>79</v>
       </c>
       <c r="N4" s="5">
-        <v>42185</v>
+        <v>42124</v>
       </c>
       <c r="O4" s="5">
-        <v>42185</v>
+        <v>42124</v>
       </c>
       <c r="P4" s="5">
-        <v>42185</v>
+        <v>42124</v>
       </c>
       <c r="Q4" s="5">
-        <v>42185</v>
+        <v>42124</v>
       </c>
       <c r="R4" s="4" t="s">
         <v>422</v>

</xml_diff>